<commit_message>
Work in paper in winter break MX
</commit_message>
<xml_diff>
--- a/Tables/SS.xlsx
+++ b/Tables/SS.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21901"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21929"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\xps-seira\Dropbox\Apps\ShareLaTeX\Donde 2019\Tables\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\xps-seira\Dropbox\Apps\ShareLaTeX\Donde2019\Tables\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FFED6895-98F6-40F1-B8F7-8ABC34F3C846}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A7A61369-5D1D-47EA-8FB6-1A1819A3AF1B}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12600" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -229,19 +229,19 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -1355,8 +1355,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A2:G61"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A31" workbookViewId="0">
-      <selection activeCell="J6" sqref="J6"/>
+    <sheetView tabSelected="1" topLeftCell="A34" workbookViewId="0">
+      <selection activeCell="G60" sqref="A35:G60"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
@@ -1371,26 +1371,26 @@
   <sheetData>
     <row r="2" spans="1:7">
       <c r="A2" s="6"/>
-      <c r="B2" s="14" t="s">
+      <c r="B2" s="19" t="s">
         <v>13</v>
       </c>
-      <c r="C2" s="14"/>
-      <c r="D2" s="14"/>
-      <c r="E2" s="14"/>
-      <c r="F2" s="14"/>
+      <c r="C2" s="19"/>
+      <c r="D2" s="19"/>
+      <c r="E2" s="19"/>
+      <c r="F2" s="19"/>
       <c r="G2" s="7"/>
     </row>
     <row r="3" spans="1:7" ht="15" thickBot="1">
       <c r="A3" s="2"/>
       <c r="B3" s="4"/>
-      <c r="C3" s="15" t="s">
+      <c r="C3" s="18" t="s">
         <v>0</v>
       </c>
-      <c r="D3" s="15"/>
-      <c r="E3" s="15" t="s">
+      <c r="D3" s="18"/>
+      <c r="E3" s="18" t="s">
         <v>1</v>
       </c>
-      <c r="F3" s="15"/>
+      <c r="F3" s="18"/>
       <c r="G3" s="4"/>
     </row>
     <row r="4" spans="1:7" ht="15" thickTop="1">
@@ -1415,14 +1415,14 @@
     </row>
     <row r="5" spans="1:7" ht="15" thickBot="1">
       <c r="A5" s="2"/>
-      <c r="B5" s="15" t="s">
+      <c r="B5" s="18" t="s">
         <v>4</v>
       </c>
-      <c r="C5" s="15"/>
-      <c r="D5" s="15"/>
-      <c r="E5" s="15"/>
-      <c r="F5" s="15"/>
-      <c r="G5" s="15"/>
+      <c r="C5" s="18"/>
+      <c r="D5" s="18"/>
+      <c r="E5" s="18"/>
+      <c r="F5" s="18"/>
+      <c r="G5" s="18"/>
     </row>
     <row r="6" spans="1:7" ht="15" thickTop="1">
       <c r="A6" t="s">
@@ -1579,33 +1579,33 @@
       <c r="G11" s="11"/>
     </row>
     <row r="12" spans="1:7">
-      <c r="A12" s="19" t="s">
+      <c r="A12" s="16" t="s">
         <v>23</v>
       </c>
-      <c r="B12" s="20">
+      <c r="B12" s="17">
         <f>SS_admin!B8</f>
         <v>84</v>
       </c>
-      <c r="C12" s="20">
+      <c r="C12" s="17">
         <f>SS_admin!C8</f>
         <v>80</v>
       </c>
-      <c r="D12" s="20">
+      <c r="D12" s="17">
         <f>SS_admin!D8</f>
         <v>68</v>
       </c>
-      <c r="E12" s="20">
+      <c r="E12" s="17">
         <f>SS_admin!E8</f>
         <v>93</v>
       </c>
-      <c r="F12" s="20">
+      <c r="F12" s="17">
         <f>SS_admin!F8</f>
         <v>82</v>
       </c>
-      <c r="G12" s="20"/>
+      <c r="G12" s="17"/>
     </row>
     <row r="13" spans="1:7">
-      <c r="A13" s="18" t="s">
+      <c r="A13" s="15" t="s">
         <v>12</v>
       </c>
       <c r="B13" s="8">
@@ -1632,14 +1632,14 @@
     </row>
     <row r="14" spans="1:7" ht="15" thickBot="1">
       <c r="A14" s="2"/>
-      <c r="B14" s="15" t="s">
+      <c r="B14" s="18" t="s">
         <v>7</v>
       </c>
-      <c r="C14" s="15"/>
-      <c r="D14" s="15"/>
-      <c r="E14" s="15"/>
-      <c r="F14" s="15"/>
-      <c r="G14" s="15"/>
+      <c r="C14" s="18"/>
+      <c r="D14" s="18"/>
+      <c r="E14" s="18"/>
+      <c r="F14" s="18"/>
+      <c r="G14" s="18"/>
     </row>
     <row r="15" spans="1:7" ht="15" thickTop="1">
       <c r="A15" t="s">
@@ -2027,26 +2027,26 @@
     </row>
     <row r="30" spans="1:7" ht="15" thickTop="1"/>
     <row r="35" spans="1:7" ht="15" thickBot="1">
-      <c r="A35" s="15" t="s">
+      <c r="A35" s="18" t="s">
         <v>25</v>
       </c>
-      <c r="B35" s="15"/>
-      <c r="C35" s="15"/>
-      <c r="D35" s="15"/>
-      <c r="E35" s="15"/>
-      <c r="F35" s="15"/>
-      <c r="G35" s="15"/>
+      <c r="B35" s="18"/>
+      <c r="C35" s="18"/>
+      <c r="D35" s="18"/>
+      <c r="E35" s="18"/>
+      <c r="F35" s="18"/>
+      <c r="G35" s="18"/>
     </row>
     <row r="36" spans="1:7" ht="15.6" thickTop="1" thickBot="1">
-      <c r="A36" s="16"/>
-      <c r="B36" s="17" t="s">
+      <c r="A36" s="14"/>
+      <c r="B36" s="20" t="s">
         <v>26</v>
       </c>
-      <c r="C36" s="17"/>
-      <c r="D36" s="17"/>
-      <c r="E36" s="17"/>
-      <c r="F36" s="17"/>
-      <c r="G36" s="17"/>
+      <c r="C36" s="20"/>
+      <c r="D36" s="20"/>
+      <c r="E36" s="20"/>
+      <c r="F36" s="20"/>
+      <c r="G36" s="20"/>
     </row>
     <row r="37" spans="1:7" ht="15" thickTop="1">
       <c r="A37" s="10" t="s">
@@ -2262,14 +2262,14 @@
     </row>
     <row r="45" spans="1:7" ht="15" thickBot="1">
       <c r="A45" s="2"/>
-      <c r="B45" s="15" t="s">
+      <c r="B45" s="18" t="s">
         <v>27</v>
       </c>
-      <c r="C45" s="15"/>
-      <c r="D45" s="15"/>
-      <c r="E45" s="15"/>
-      <c r="F45" s="15"/>
-      <c r="G45" s="15"/>
+      <c r="C45" s="18"/>
+      <c r="D45" s="18"/>
+      <c r="E45" s="18"/>
+      <c r="F45" s="18"/>
+      <c r="G45" s="18"/>
     </row>
     <row r="46" spans="1:7" ht="15" thickTop="1">
       <c r="A46" s="10" t="s">

</xml_diff>

<commit_message>
update ss table - panel c
</commit_message>
<xml_diff>
--- a/Tables/SS.xlsx
+++ b/Tables/SS.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\xps-seira\Dropbox\Apps\ShareLaTeX\Donde2020\Tables\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7145EFF5-54C2-49FD-9313-E254A53F4948}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A3C2CBA4-0CAB-489C-AF5A-38DFBE5118E1}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12600" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -589,18 +589,18 @@
         <v>2197.3231220764928</v>
       </c>
       <c r="J2">
-        <v>0.32446131464480021</v>
+        <v>0.32446131464480321</v>
       </c>
     </row>
     <row r="3" spans="2:10">
       <c r="B3">
-        <v>79.41696803972188</v>
+        <v>79.416968039721894</v>
       </c>
       <c r="C3">
-        <v>71.911953944693536</v>
+        <v>71.911953944693508</v>
       </c>
       <c r="D3">
-        <v>74.033283407617617</v>
+        <v>74.033283407617645</v>
       </c>
       <c r="E3">
         <v>65.120503781670294</v>
@@ -799,362 +799,365 @@
   <sheetData>
     <row r="2" spans="2:10">
       <c r="B2">
-        <v>0.80701754385964908</v>
+        <v>0.75564409030544488</v>
       </c>
       <c r="C2">
-        <v>0.75268817204301075</v>
+        <v>0.72237196765498657</v>
       </c>
       <c r="D2">
-        <v>0.73333333333333328</v>
+        <v>0.72575250836120397</v>
       </c>
       <c r="E2">
-        <v>0.68949771689497719</v>
+        <v>0.71847070506454813</v>
       </c>
       <c r="F2">
-        <v>0.70499999999999996</v>
+        <v>0.74042027194066751</v>
       </c>
       <c r="G2">
-        <v>0.75014836795252227</v>
+        <v>0.74980252764612954</v>
       </c>
       <c r="H2">
-        <v>0.74777348344815997</v>
+        <v>0.73901568079490765</v>
       </c>
       <c r="J2">
-        <v>0.27253817439857192</v>
+        <v>0.3199816408066643</v>
       </c>
     </row>
     <row r="3" spans="2:10">
       <c r="B3">
-        <v>3.0947583995281136E-2</v>
+        <v>1.644910941444085E-2</v>
       </c>
       <c r="C3">
-        <v>3.7425461066832984E-2</v>
+        <v>1.609110026524976E-2</v>
       </c>
       <c r="D3">
-        <v>5.2078157637573702E-2</v>
+        <v>2.0205125736203776E-2</v>
       </c>
       <c r="E3">
-        <v>4.9354046174029359E-2</v>
+        <v>1.5011614271560187E-2</v>
       </c>
       <c r="F3">
-        <v>3.9752655213095241E-2</v>
+        <v>1.2844826313395475E-2</v>
       </c>
       <c r="G3">
-        <v>9.0179307184721242E-3</v>
+        <v>9.0149695175873682E-3</v>
       </c>
       <c r="H3">
-        <v>8.2565940982977423E-3</v>
+        <v>5.6636661229594034E-3</v>
       </c>
     </row>
     <row r="4" spans="2:10">
       <c r="B4">
-        <v>42.748427672955977</v>
+        <v>43.197724039829303</v>
       </c>
       <c r="C4">
-        <v>45.674285714285716</v>
+        <v>43.214285714285715</v>
       </c>
       <c r="D4">
-        <v>45.424778761061944</v>
+        <v>43.012808783165596</v>
       </c>
       <c r="E4">
-        <v>45.306930693069305</v>
+        <v>44.068702290076338</v>
       </c>
       <c r="F4">
-        <v>44.654450261780106</v>
+        <v>43.071663379355684</v>
       </c>
       <c r="G4">
-        <v>43.047860004216737</v>
+        <v>43.05681818181818</v>
       </c>
       <c r="H4">
-        <v>43.306466057675088</v>
+        <v>43.244162775183455</v>
       </c>
       <c r="J4">
-        <v>0.1078174600917928</v>
+        <v>0.78677267826023056</v>
       </c>
     </row>
     <row r="5" spans="2:10">
       <c r="B5">
-        <v>1.1409080237609841</v>
+        <v>0.56403599075095434</v>
       </c>
       <c r="C5">
-        <v>1.3073041730865835</v>
+        <v>0.77069700997930002</v>
       </c>
       <c r="D5">
-        <v>1.2652298792794539</v>
+        <v>0.65952524226845821</v>
       </c>
       <c r="E5">
-        <v>1.8811523967071297</v>
+        <v>0.60510467478567853</v>
       </c>
       <c r="F5">
-        <v>1.4229499642197045</v>
+        <v>0.51494995970101298</v>
       </c>
       <c r="G5">
-        <v>0.31618634602892209</v>
+        <v>0.31582069920051548</v>
       </c>
       <c r="H5">
-        <v>0.28692690707414531</v>
+        <v>0.21147020058714425</v>
       </c>
     </row>
     <row r="6" spans="2:10">
       <c r="B6">
-        <v>2682</v>
+        <v>3144.9910089163509</v>
       </c>
       <c r="C6">
-        <v>3335.7142857142858</v>
+        <v>2985.0461656208972</v>
       </c>
       <c r="D6">
-        <v>5200</v>
+        <v>3010.0226498567731</v>
       </c>
       <c r="E6">
-        <v>2925.9183673469388</v>
+        <v>3110.5951057232041</v>
       </c>
       <c r="F6">
-        <v>3473.3333333333335</v>
+        <v>3082.4794570266222</v>
       </c>
       <c r="G6">
-        <v>3194.8117466579006</v>
+        <v>3192.3475956420366</v>
       </c>
       <c r="H6">
-        <v>3198.042951307676</v>
+        <v>3111.5831964531485</v>
       </c>
       <c r="J6">
-        <v>0.1006580967852901</v>
+        <v>0.40587608283675952</v>
       </c>
     </row>
     <row r="7" spans="2:10">
       <c r="B7">
-        <v>335.96044290957826</v>
+        <v>68.21540163415446</v>
       </c>
       <c r="C7">
-        <v>378.58488600641124</v>
+        <v>88.350791604799952</v>
       </c>
       <c r="D7">
-        <v>821.84712222389157</v>
+        <v>76.46623124498781</v>
       </c>
       <c r="E7">
-        <v>666.26858017619622</v>
+        <v>84.456979102137012</v>
       </c>
       <c r="F7">
-        <v>784.15912629614616</v>
+        <v>99.018458366442971</v>
       </c>
       <c r="G7">
-        <v>75.304940461651896</v>
+        <v>75.187904829259352</v>
       </c>
       <c r="H7">
-        <v>73.549896044432629</v>
+        <v>35.73867184340029</v>
       </c>
     </row>
     <row r="8" spans="2:10">
       <c r="B8">
-        <v>0.87730061349693256</v>
+        <v>0.8904494382022472</v>
       </c>
       <c r="C8">
-        <v>0.92613636363636365</v>
+        <v>0.89978828510938602</v>
       </c>
       <c r="D8">
-        <v>0.92660550458715596</v>
+        <v>0.89142335766423353</v>
       </c>
       <c r="E8">
-        <v>0.97058823529411764</v>
+        <v>0.91065662002152847</v>
       </c>
       <c r="F8">
-        <v>0.92737430167597767</v>
+        <v>0.89407061958694201</v>
       </c>
       <c r="G8">
-        <v>0.88400739067953193</v>
+        <v>0.88422131147540983</v>
       </c>
       <c r="H8">
-        <v>0.89038933707471057</v>
+        <v>0.89265768725361372</v>
       </c>
       <c r="J8">
-        <v>4.9438636024099996E-6</v>
+        <v>0.55584000072208539</v>
       </c>
     </row>
     <row r="9" spans="2:10">
       <c r="B9">
-        <v>3.2306220014917099E-2</v>
+        <v>1.1507748187866138E-2</v>
       </c>
       <c r="C9">
-        <v>2.4994882760703128E-2</v>
+        <v>1.057909469617015E-2</v>
       </c>
       <c r="D9">
-        <v>2.6485822251702658E-2</v>
+        <v>1.4552389380818403E-2</v>
       </c>
       <c r="E9">
-        <v>1.1442327160377134E-2</v>
+        <v>9.9277590884214503E-3</v>
       </c>
       <c r="F9">
-        <v>2.3029153839256255E-2</v>
+        <v>9.4668089479309457E-3</v>
       </c>
       <c r="G9">
-        <v>1.055166642140079E-2</v>
+        <v>1.0533724370448033E-2</v>
       </c>
       <c r="H9">
-        <v>9.2082053183496181E-3</v>
+        <v>5.2053730841606369E-3</v>
       </c>
     </row>
     <row r="10" spans="2:10">
       <c r="B10">
-        <v>91.818181818181813</v>
+        <v>92.725089422585597</v>
       </c>
       <c r="C10">
-        <v>93.541666666666671</v>
+        <v>92.193231441048042</v>
       </c>
       <c r="D10">
-        <v>97.391304347826093</v>
+        <v>93.658892128279888</v>
       </c>
       <c r="E10">
-        <v>95.714285714285708</v>
+        <v>93.714012982054214</v>
       </c>
       <c r="F10">
-        <v>97.083333333333329</v>
+        <v>93.339202965708992</v>
       </c>
       <c r="G10">
-        <v>91.82910170749814</v>
+        <v>91.835829749369722</v>
       </c>
       <c r="H10">
-        <v>91.909090909090907</v>
+        <v>92.639685150375939</v>
       </c>
       <c r="J10">
-        <v>1.9649063146056E-3</v>
+        <v>4.6684240622125997E-3</v>
       </c>
     </row>
     <row r="11" spans="2:10">
       <c r="B11">
-        <v>3.1491565103378409</v>
+        <v>0.54084732630950216</v>
       </c>
       <c r="C11">
-        <v>2.1129000718349262</v>
+        <v>0.83856879215694513</v>
       </c>
       <c r="D11">
-        <v>1.8905836350662679</v>
+        <v>0.59084286834349808</v>
       </c>
       <c r="E11">
-        <v>1.9162351424188104</v>
+        <v>0.45528703025952877</v>
       </c>
       <c r="F11">
-        <v>2.0524420542122304</v>
+        <v>0.5948733338915928</v>
       </c>
       <c r="G11">
-        <v>0.30851148428900949</v>
+        <v>0.30818777366122263</v>
       </c>
       <c r="H11">
-        <v>0.30206336539853695</v>
+        <v>0.20479038611903611</v>
       </c>
     </row>
     <row r="12" spans="2:10">
       <c r="B12">
-        <v>0.67500000000000004</v>
+        <v>0.65949820788530467</v>
       </c>
       <c r="C12">
-        <v>0.64457831325301207</v>
+        <v>0.66884057971014488</v>
       </c>
       <c r="D12">
-        <v>0.8165137614678899</v>
+        <v>0.64749536178107603</v>
       </c>
       <c r="E12">
-        <v>0.59113300492610843</v>
+        <v>0.66257668711656437</v>
       </c>
       <c r="F12">
-        <v>0.5722543352601156</v>
+        <v>0.64335180055401664</v>
       </c>
       <c r="G12">
-        <v>0.59660875026167048</v>
+        <v>0.59694943585457583</v>
       </c>
       <c r="H12">
-        <v>0.6036148890479599</v>
+        <v>0.63278881778376561</v>
       </c>
       <c r="J12">
-        <v>3.0724202076669999E-4</v>
+        <v>6.6108847471301998E-3</v>
       </c>
     </row>
     <row r="13" spans="2:10">
       <c r="B13">
-        <v>4.3584554155909276E-2</v>
+        <v>1.9536506277868428E-2</v>
       </c>
       <c r="C13">
-        <v>4.3191949023352355E-2</v>
+        <v>1.9329841394817811E-2</v>
       </c>
       <c r="D13">
-        <v>4.7352286079552948E-2</v>
+        <v>2.4043222313478024E-2</v>
       </c>
       <c r="E13">
-        <v>5.6026042414491113E-2</v>
+        <v>1.6894823421726591E-2</v>
       </c>
       <c r="F13">
-        <v>5.8987003569326089E-2</v>
+        <v>1.6696589416796935E-2</v>
       </c>
       <c r="G13">
-        <v>1.2972763993953407E-2</v>
+        <v>1.2957951584969644E-2</v>
       </c>
       <c r="H13">
-        <v>1.1669989403791306E-2</v>
+        <v>7.4863193792611979E-3</v>
       </c>
     </row>
     <row r="14" spans="2:10">
       <c r="B14">
-        <v>0</v>
+        <v>0.98280098280098283</v>
       </c>
       <c r="C14">
-        <v>0</v>
+        <v>0.97273203985317247</v>
       </c>
       <c r="D14">
-        <v>0</v>
+        <v>0.98577120091064319</v>
       </c>
       <c r="E14">
-        <v>0</v>
+        <v>0.97859778597785974</v>
       </c>
       <c r="F14">
-        <v>0</v>
+        <v>0.98827772768259692</v>
       </c>
       <c r="G14">
-        <v>0</v>
+        <v>1.3007660066483597E-3</v>
       </c>
       <c r="H14">
-        <v>0</v>
+        <v>0.59500740909609029</v>
+      </c>
+      <c r="J14">
+        <v>0.2454321833124756</v>
       </c>
     </row>
     <row r="15" spans="2:10">
       <c r="B15">
-        <v>0</v>
+        <v>4.0156175496241656E-3</v>
       </c>
       <c r="C15">
-        <v>0</v>
+        <v>7.3961905116490204E-3</v>
       </c>
       <c r="D15">
-        <v>0</v>
+        <v>3.380162850677099E-3</v>
       </c>
       <c r="E15">
-        <v>0</v>
+        <v>5.9663991659335853E-3</v>
       </c>
       <c r="F15">
-        <v>0</v>
+        <v>3.007259722267115E-3</v>
       </c>
       <c r="G15">
-        <v>0</v>
+        <v>7.2827849166321888E-4</v>
       </c>
       <c r="H15">
-        <v>0</v>
+        <v>2.0884546392501639E-2</v>
       </c>
     </row>
     <row r="16" spans="2:10">
       <c r="B16">
-        <v>35</v>
+        <v>2035</v>
       </c>
       <c r="C16">
-        <v>52</v>
+        <v>1907</v>
       </c>
       <c r="D16">
-        <v>23</v>
+        <v>1757</v>
       </c>
       <c r="E16">
-        <v>58</v>
+        <v>2710</v>
       </c>
       <c r="F16">
-        <v>26</v>
+        <v>2218</v>
       </c>
       <c r="G16">
-        <v>6910</v>
+        <v>6919</v>
       </c>
     </row>
   </sheetData>
@@ -1174,48 +1177,48 @@
   <sheetData>
     <row r="2" spans="2:9">
       <c r="B2">
-        <v>0.75706594885598921</v>
+        <v>0.75757575757575757</v>
       </c>
       <c r="C2">
         <v>0.72451790633608815</v>
       </c>
       <c r="D2">
-        <v>0.72527472527472525</v>
+        <v>0.72504230118443314</v>
       </c>
       <c r="E2">
-        <v>0.71775417298937783</v>
+        <v>0.71811740890688258</v>
       </c>
       <c r="F2">
         <v>0.74094881398252188</v>
       </c>
       <c r="G2">
-        <v>0.73259740259740258</v>
+        <v>0.732753020657399</v>
       </c>
       <c r="H2">
         <v>0.73239071215462448</v>
       </c>
       <c r="I2">
-        <v>0.42180795324654552</v>
+        <v>0.41285083973109971</v>
       </c>
     </row>
     <row r="3" spans="2:9">
       <c r="B3">
-        <v>1.6329938660297399E-2</v>
+        <v>1.6353148457536527E-2</v>
       </c>
       <c r="C3">
         <v>1.6037712453979815E-2</v>
       </c>
       <c r="D3">
-        <v>2.0704066804602267E-2</v>
+        <v>2.0714850878795654E-2</v>
       </c>
       <c r="E3">
-        <v>1.5845064022229488E-2</v>
+        <v>1.5694316621148546E-2</v>
       </c>
       <c r="F3">
         <v>1.2961944419642095E-2</v>
       </c>
       <c r="G3">
-        <v>7.3811280869818512E-3</v>
+        <v>7.3610489260520747E-3</v>
       </c>
       <c r="H3">
         <v>7.3732935414456838E-3</v>
@@ -1223,48 +1226,48 @@
     </row>
     <row r="4" spans="2:9">
       <c r="B4">
-        <v>43.164866810655148</v>
+        <v>43.164985590778095</v>
       </c>
       <c r="C4">
         <v>43.174778761061944</v>
       </c>
       <c r="D4">
-        <v>42.960185185185182</v>
+        <v>42.961075069508802</v>
       </c>
       <c r="E4">
-        <v>43.95550611790879</v>
+        <v>43.956037840845852</v>
       </c>
       <c r="F4">
         <v>43.058471760797339</v>
       </c>
       <c r="G4">
-        <v>43.312710437710436</v>
+        <v>43.312982456140354</v>
       </c>
       <c r="H4">
         <v>43.318341039652516</v>
       </c>
       <c r="I4">
-        <v>0.78892398827320342</v>
+        <v>0.78911299773387222</v>
       </c>
     </row>
     <row r="5" spans="2:9">
       <c r="B5">
-        <v>0.57302039418728512</v>
+        <v>0.5734678785745746</v>
       </c>
       <c r="C5">
         <v>0.78693411412047953</v>
       </c>
       <c r="D5">
-        <v>0.65161383087213032</v>
+        <v>0.65217105015255705</v>
       </c>
       <c r="E5">
-        <v>0.61205771211875071</v>
+        <v>0.6123643223001326</v>
       </c>
       <c r="F5">
         <v>0.51624441834800938</v>
       </c>
       <c r="G5">
-        <v>0.28312963398438279</v>
+        <v>0.28324945753639863</v>
       </c>
       <c r="H5">
         <v>0.28291232956547702</v>
@@ -1272,48 +1275,48 @@
     </row>
     <row r="6" spans="2:9">
       <c r="B6">
-        <v>3151.8311879330831</v>
+        <v>3151.4645968486266</v>
       </c>
       <c r="C6">
-        <v>2977.8080010068757</v>
+        <v>2977.5760595933448</v>
       </c>
       <c r="D6">
-        <v>2987.6091755578368</v>
+        <v>2985.3601239472823</v>
       </c>
       <c r="E6">
-        <v>3114.8420998012557</v>
+        <v>3114.4788654572976</v>
       </c>
       <c r="F6">
-        <v>3079.6578772628068</v>
+        <v>3079.4527104367407</v>
       </c>
       <c r="G6">
-        <v>3069.0155901265421</v>
+        <v>3068.4022871033972</v>
       </c>
       <c r="H6">
         <v>3067.9203108635979</v>
       </c>
       <c r="I6">
-        <v>0.41322068028366221</v>
+        <v>0.40512608371464598</v>
       </c>
     </row>
     <row r="7" spans="2:9">
       <c r="B7">
-        <v>68.633705702668763</v>
+        <v>68.625662226643939</v>
       </c>
       <c r="C7">
-        <v>90.821567649747081</v>
+        <v>90.810127072547061</v>
       </c>
       <c r="D7">
-        <v>76.019238973365518</v>
+        <v>75.7749764033302</v>
       </c>
       <c r="E7">
-        <v>84.55291310515976</v>
+        <v>84.539006543944083</v>
       </c>
       <c r="F7">
-        <v>99.521101344569345</v>
+        <v>99.50770961838613</v>
       </c>
       <c r="G7">
-        <v>38.659700392067194</v>
+        <v>38.646858824752861</v>
       </c>
       <c r="H7">
         <v>38.640982667796216</v>
@@ -1321,48 +1324,48 @@
     </row>
     <row r="8" spans="2:9">
       <c r="B8">
-        <v>0.89102564102564108</v>
+        <v>0.89094796863863146</v>
       </c>
       <c r="C8">
         <v>0.89841498559077815</v>
       </c>
       <c r="D8">
-        <v>0.89289012003693446</v>
+        <v>0.89279112754158962</v>
       </c>
       <c r="E8">
-        <v>0.91063596491228072</v>
+        <v>0.91058694459681844</v>
       </c>
       <c r="F8">
         <v>0.89367429340511439</v>
       </c>
       <c r="G8">
-        <v>0.89826026443980511</v>
+        <v>0.89821776663881925</v>
       </c>
       <c r="H8">
         <v>0.89838754517653596</v>
       </c>
       <c r="I8">
-        <v>0.67959038571202313</v>
+        <v>0.67936345560508071</v>
       </c>
     </row>
     <row r="9" spans="2:9">
       <c r="B9">
-        <v>1.1699017063997981E-2</v>
+        <v>1.1702510413535415E-2</v>
       </c>
       <c r="C9">
-        <v>1.0536449576402313E-2</v>
+        <v>1.0536449576402311E-2</v>
       </c>
       <c r="D9">
-        <v>1.4414244480650894E-2</v>
+        <v>1.441850449267084E-2</v>
       </c>
       <c r="E9">
-        <v>9.9893832545590311E-3</v>
+        <v>9.9874959754338993E-3</v>
       </c>
       <c r="F9">
         <v>9.5208878346407667E-3</v>
       </c>
       <c r="G9">
-        <v>4.9470435011570342E-3</v>
+        <v>4.9467781608944564E-3</v>
       </c>
       <c r="H9">
         <v>4.9392865548329125E-3</v>
@@ -1376,22 +1379,22 @@
         <v>92.156950672645735</v>
       </c>
       <c r="D10">
-        <v>93.604376108811351</v>
+        <v>93.600591715976336</v>
       </c>
       <c r="E10">
-        <v>93.67277691107644</v>
+        <v>93.670308232539995</v>
       </c>
       <c r="F10">
         <v>93.297094657919402</v>
       </c>
       <c r="G10">
-        <v>93.136476181043875</v>
+        <v>93.135116394254581</v>
       </c>
       <c r="H10">
         <v>93.139930727362696</v>
       </c>
       <c r="I10">
-        <v>0.45299974490804878</v>
+        <v>0.45561209600109898</v>
       </c>
     </row>
     <row r="11" spans="2:9">
@@ -1402,16 +1405,16 @@
         <v>0.85746436976065976</v>
       </c>
       <c r="D11">
-        <v>0.59648670007090776</v>
+        <v>0.59598887248627241</v>
       </c>
       <c r="E11">
-        <v>0.47058032652713411</v>
+        <v>0.47088171102994458</v>
       </c>
       <c r="F11">
-        <v>0.59873100123725531</v>
+        <v>0.5987310012372552</v>
       </c>
       <c r="G11">
-        <v>0.2743367127789596</v>
+        <v>0.27433101628973899</v>
       </c>
       <c r="H11">
         <v>0.274162592601149</v>
@@ -1419,48 +1422,48 @@
     </row>
     <row r="12" spans="2:9">
       <c r="B12">
-        <v>0.66084425036390104</v>
+        <v>0.66059723233794609</v>
       </c>
       <c r="C12">
         <v>0.6723372781065089</v>
       </c>
       <c r="D12">
-        <v>0.64694835680751173</v>
+        <v>0.64755639097744366</v>
       </c>
       <c r="E12">
-        <v>0.66609783845278725</v>
+        <v>0.66590779738190098</v>
       </c>
       <c r="F12">
         <v>0.64195804195804196</v>
       </c>
       <c r="G12">
-        <v>0.65840378277690215</v>
+        <v>0.65840022935779818</v>
       </c>
       <c r="H12">
         <v>0.6585575271894677</v>
       </c>
       <c r="I12">
-        <v>0.72926019548172927</v>
+        <v>0.73606972985425867</v>
       </c>
     </row>
     <row r="13" spans="2:9">
       <c r="B13">
-        <v>1.9264793906698385E-2</v>
+        <v>1.942399743102876E-2</v>
       </c>
       <c r="C13">
-        <v>1.8898567915395067E-2</v>
+        <v>1.889856791539507E-2</v>
       </c>
       <c r="D13">
-        <v>2.4289475036466852E-2</v>
+        <v>2.4224528087916579E-2</v>
       </c>
       <c r="E13">
-        <v>1.6413508256461058E-2</v>
+        <v>1.6421808697529818E-2</v>
       </c>
       <c r="F13">
-        <v>1.6299242242827347E-2</v>
+        <v>1.629924224282735E-2</v>
       </c>
       <c r="G13">
-        <v>8.3829252867613068E-3</v>
+        <v>8.3918174033719081E-3</v>
       </c>
       <c r="H13">
         <v>8.3888552688200987E-3</v>
@@ -1474,22 +1477,22 @@
         <v>0.74738114423851731</v>
       </c>
       <c r="D14">
-        <v>0.80380333951762528</v>
+        <v>0.80371229698375868</v>
       </c>
       <c r="E14">
-        <v>0.77211874272409775</v>
+        <v>0.77205240174672485</v>
       </c>
       <c r="F14">
         <v>0.79305354558610708</v>
       </c>
       <c r="G14">
-        <v>0.77632264305379861</v>
+        <v>0.77628935030140656</v>
       </c>
       <c r="H14">
         <v>0.57324509220701958</v>
       </c>
       <c r="I14">
-        <v>0.50221520369769657</v>
+        <v>0.50326097085279187</v>
       </c>
     </row>
     <row r="15" spans="2:9">
@@ -1497,19 +1500,19 @@
         <v>1.9892859098745899E-2</v>
       </c>
       <c r="C15">
-        <v>2.5623636641152012E-2</v>
+        <v>2.5623636641152008E-2</v>
       </c>
       <c r="D15">
-        <v>2.3871935695980513E-2</v>
+        <v>2.3867007306229256E-2</v>
       </c>
       <c r="E15">
-        <v>2.3661163960051097E-2</v>
+        <v>2.3659037145027335E-2</v>
       </c>
       <c r="F15">
         <v>2.2444999654912107E-2</v>
       </c>
       <c r="G15">
-        <v>1.0492907532541668E-2</v>
+        <v>1.0492228006191808E-2</v>
       </c>
       <c r="H15">
         <v>9.4357020529609956E-3</v>
@@ -1523,10 +1526,10 @@
         <v>1855</v>
       </c>
       <c r="D16">
-        <v>1733</v>
+        <v>1732</v>
       </c>
       <c r="E16">
-        <v>2653</v>
+        <v>2652</v>
       </c>
       <c r="F16">
         <v>2192</v>
@@ -1541,7 +1544,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A2:I45"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A20" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
       <selection activeCell="A2" sqref="A2:I44"/>
     </sheetView>
   </sheetViews>
@@ -1934,7 +1937,7 @@
       </c>
       <c r="I15" s="15">
         <f>ROUND(SS_survey!I2,2)</f>
-        <v>0.42</v>
+        <v>0.41</v>
       </c>
     </row>
     <row r="16" spans="1:9">
@@ -2028,11 +2031,11 @@
       </c>
       <c r="B19" s="1">
         <f>ROUND(SS_survey!G6,0)</f>
-        <v>3069</v>
+        <v>3068</v>
       </c>
       <c r="D19" s="1">
         <f>ROUND(SS_survey!B6,0)</f>
-        <v>3152</v>
+        <v>3151</v>
       </c>
       <c r="E19" s="1">
         <f>ROUND(SS_survey!C6,0)</f>
@@ -2040,15 +2043,15 @@
       </c>
       <c r="F19" s="1">
         <f>ROUND(SS_survey!D6,0)</f>
-        <v>2988</v>
+        <v>2985</v>
       </c>
       <c r="G19" s="15">
         <f>ROUND(SS_survey!E6,0)</f>
-        <v>3115</v>
+        <v>3114</v>
       </c>
       <c r="H19" s="15">
         <f>ROUND(SS_survey!F6,0)</f>
-        <v>3080</v>
+        <v>3079</v>
       </c>
       <c r="I19" s="15">
         <f>ROUND(SS_survey!I6,2)</f>
@@ -2170,7 +2173,7 @@
       </c>
       <c r="I23" s="15">
         <f>ROUND(SS_survey!I10,2)</f>
-        <v>0.45</v>
+        <v>0.46</v>
       </c>
     </row>
     <row r="24" spans="1:9">
@@ -2229,7 +2232,7 @@
       </c>
       <c r="I25" s="15">
         <f>ROUND(SS_survey!I12,2)</f>
-        <v>0.73</v>
+        <v>0.74</v>
       </c>
     </row>
     <row r="26" spans="1:9">
@@ -2324,7 +2327,7 @@
       </c>
       <c r="B29" s="11">
         <f>SUM(D29:H29)</f>
-        <v>10433</v>
+        <v>10431</v>
       </c>
       <c r="C29" s="17"/>
       <c r="D29" s="11">
@@ -2337,11 +2340,11 @@
       </c>
       <c r="F29" s="11">
         <f>ROUND(SS_survey!D16,2)</f>
-        <v>1733</v>
+        <v>1732</v>
       </c>
       <c r="G29" s="13">
         <f>ROUND(SS_survey!E16,2)</f>
-        <v>2653</v>
+        <v>2652</v>
       </c>
       <c r="H29" s="13">
         <f>ROUND(SS_survey!F16,2)</f>
@@ -2368,7 +2371,7 @@
       </c>
       <c r="B31" s="15">
         <f>ROUND(SS_survey_uncond!H2,2)</f>
-        <v>0.75</v>
+        <v>0.74</v>
       </c>
       <c r="C31" s="1">
         <f>ROUND(SS_survey_uncond!G2,2)</f>
@@ -2376,11 +2379,11 @@
       </c>
       <c r="D31" s="1">
         <f>ROUND(SS_survey_uncond!B2,2)</f>
-        <v>0.81</v>
+        <v>0.76</v>
       </c>
       <c r="E31" s="1">
         <f>ROUND(SS_survey_uncond!C2,2)</f>
-        <v>0.75</v>
+        <v>0.72</v>
       </c>
       <c r="F31" s="1">
         <f>ROUND(SS_survey_uncond!D2,2)</f>
@@ -2388,15 +2391,15 @@
       </c>
       <c r="G31" s="14">
         <f>ROUND(SS_survey_uncond!E2,2)</f>
-        <v>0.69</v>
+        <v>0.72</v>
       </c>
       <c r="H31" s="14">
         <f>ROUND(SS_survey_uncond!F2,2)</f>
-        <v>0.71</v>
+        <v>0.74</v>
       </c>
       <c r="I31" s="15">
         <f>ROUND(SS_survey_uncond!J2,2)</f>
-        <v>0.27</v>
+        <v>0.32</v>
       </c>
     </row>
     <row r="32" spans="1:9">
@@ -2410,23 +2413,23 @@
       </c>
       <c r="D32" s="1" t="str">
         <f>CONCATENATE("(",ROUND(SS_survey_uncond!B3,2),")")</f>
-        <v>(0.03)</v>
+        <v>(0.02)</v>
       </c>
       <c r="E32" s="1" t="str">
         <f>CONCATENATE("(",ROUND(SS_survey_uncond!C3,2),")")</f>
-        <v>(0.04)</v>
+        <v>(0.02)</v>
       </c>
       <c r="F32" s="1" t="str">
         <f>CONCATENATE("(",ROUND(SS_survey_uncond!D3,2),")")</f>
-        <v>(0.05)</v>
+        <v>(0.02)</v>
       </c>
       <c r="G32" s="15" t="str">
         <f>CONCATENATE("(",ROUND(SS_survey_uncond!E3,2),")")</f>
-        <v>(0.05)</v>
+        <v>(0.02)</v>
       </c>
       <c r="H32" s="15" t="str">
         <f>CONCATENATE("(",ROUND(SS_survey_uncond!F3,2),")")</f>
-        <v>(0.04)</v>
+        <v>(0.01)</v>
       </c>
     </row>
     <row r="33" spans="1:9">
@@ -2435,41 +2438,41 @@
       </c>
       <c r="B33" s="15">
         <f>ROUND(SS_survey_uncond!H4,2)</f>
-        <v>43.31</v>
+        <v>43.24</v>
       </c>
       <c r="C33" s="1">
         <f>ROUND(SS_survey_uncond!G4,2)</f>
-        <v>43.05</v>
+        <v>43.06</v>
       </c>
       <c r="D33" s="1">
         <f>ROUND(SS_survey_uncond!B4,2)</f>
-        <v>42.75</v>
+        <v>43.2</v>
       </c>
       <c r="E33" s="1">
         <f>ROUND(SS_survey_uncond!C4,2)</f>
-        <v>45.67</v>
+        <v>43.21</v>
       </c>
       <c r="F33" s="1">
         <f>ROUND(SS_survey_uncond!D4,2)</f>
-        <v>45.42</v>
+        <v>43.01</v>
       </c>
       <c r="G33" s="15">
         <f>ROUND(SS_survey_uncond!E4,2)</f>
-        <v>45.31</v>
+        <v>44.07</v>
       </c>
       <c r="H33" s="15">
         <f>ROUND(SS_survey_uncond!F4,2)</f>
-        <v>44.65</v>
+        <v>43.07</v>
       </c>
       <c r="I33" s="15">
         <f>ROUND(SS_survey_uncond!J4,2)</f>
-        <v>0.11</v>
+        <v>0.79</v>
       </c>
     </row>
     <row r="34" spans="1:9">
       <c r="B34" s="15" t="str">
         <f>CONCATENATE("(",ROUND(SS_survey_uncond!H5,2),")")</f>
-        <v>(0.29)</v>
+        <v>(0.21)</v>
       </c>
       <c r="C34" s="1" t="str">
         <f>CONCATENATE("(",ROUND(SS_survey_uncond!G5,2),")")</f>
@@ -2477,23 +2480,23 @@
       </c>
       <c r="D34" s="1" t="str">
         <f>CONCATENATE("(",ROUND(SS_survey_uncond!B5,2),")")</f>
-        <v>(1.14)</v>
+        <v>(0.56)</v>
       </c>
       <c r="E34" s="1" t="str">
         <f>CONCATENATE("(",ROUND(SS_survey_uncond!C5,2),")")</f>
-        <v>(1.31)</v>
+        <v>(0.77)</v>
       </c>
       <c r="F34" s="1" t="str">
         <f>CONCATENATE("(",ROUND(SS_survey_uncond!D5,2),")")</f>
-        <v>(1.27)</v>
+        <v>(0.66)</v>
       </c>
       <c r="G34" s="15" t="str">
         <f>CONCATENATE("(",ROUND(SS_survey_uncond!E5,2),")")</f>
-        <v>(1.88)</v>
+        <v>(0.61)</v>
       </c>
       <c r="H34" s="15" t="str">
         <f>CONCATENATE("(",ROUND(SS_survey_uncond!F5,2),")")</f>
-        <v>(1.42)</v>
+        <v>(0.51)</v>
       </c>
     </row>
     <row r="35" spans="1:9">
@@ -2502,41 +2505,41 @@
       </c>
       <c r="B35" s="15">
         <f>ROUND(SS_survey_uncond!H6,0)</f>
-        <v>3198</v>
+        <v>3112</v>
       </c>
       <c r="C35" s="1">
         <f>ROUND(SS_survey_uncond!G6,0)</f>
-        <v>3195</v>
+        <v>3192</v>
       </c>
       <c r="D35" s="1">
         <f>ROUND(SS_survey_uncond!B6,0)</f>
-        <v>2682</v>
+        <v>3145</v>
       </c>
       <c r="E35" s="1">
         <f>ROUND(SS_survey_uncond!C6,0)</f>
-        <v>3336</v>
+        <v>2985</v>
       </c>
       <c r="F35" s="1">
         <f>ROUND(SS_survey_uncond!D6,0)</f>
-        <v>5200</v>
+        <v>3010</v>
       </c>
       <c r="G35" s="15">
         <f>ROUND(SS_survey_uncond!E6,0)</f>
-        <v>2926</v>
+        <v>3111</v>
       </c>
       <c r="H35" s="15">
         <f>ROUND(SS_survey_uncond!F6,0)</f>
-        <v>3473</v>
+        <v>3082</v>
       </c>
       <c r="I35" s="15">
         <f>ROUND(SS_survey_uncond!J6,2)</f>
-        <v>0.1</v>
+        <v>0.41</v>
       </c>
     </row>
     <row r="36" spans="1:9">
       <c r="B36" s="15" t="str">
         <f>CONCATENATE("(",ROUND(SS_survey_uncond!H7,0),")")</f>
-        <v>(74)</v>
+        <v>(36)</v>
       </c>
       <c r="C36" s="1" t="str">
         <f>CONCATENATE("(",ROUND(SS_survey_uncond!G7,0),")")</f>
@@ -2544,23 +2547,23 @@
       </c>
       <c r="D36" s="1" t="str">
         <f>CONCATENATE("(",ROUND(SS_survey_uncond!B7,0),")")</f>
-        <v>(336)</v>
+        <v>(68)</v>
       </c>
       <c r="E36" s="15" t="str">
         <f>CONCATENATE("(",ROUND(SS_survey_uncond!C7,0),")")</f>
-        <v>(379)</v>
+        <v>(88)</v>
       </c>
       <c r="F36" s="15" t="str">
         <f>CONCATENATE("(",ROUND(SS_survey_uncond!D7,0),")")</f>
-        <v>(822)</v>
+        <v>(76)</v>
       </c>
       <c r="G36" s="15" t="str">
         <f>CONCATENATE("(",ROUND(SS_survey_uncond!E7,0),")")</f>
-        <v>(666)</v>
+        <v>(84)</v>
       </c>
       <c r="H36" s="15" t="str">
         <f>CONCATENATE("(",ROUND(SS_survey_uncond!F7,0),")")</f>
-        <v>(784)</v>
+        <v>(99)</v>
       </c>
     </row>
     <row r="37" spans="1:9">
@@ -2577,27 +2580,27 @@
       </c>
       <c r="D37" s="1">
         <f>ROUND(SS_survey_uncond!B8,2)</f>
-        <v>0.88</v>
+        <v>0.89</v>
       </c>
       <c r="E37" s="1">
         <f>ROUND(SS_survey_uncond!C8,2)</f>
-        <v>0.93</v>
+        <v>0.9</v>
       </c>
       <c r="F37" s="1">
         <f>ROUND(SS_survey_uncond!D8,2)</f>
-        <v>0.93</v>
+        <v>0.89</v>
       </c>
       <c r="G37" s="15">
         <f>ROUND(SS_survey_uncond!E8,2)</f>
-        <v>0.97</v>
+        <v>0.91</v>
       </c>
       <c r="H37" s="15">
         <f>ROUND(SS_survey_uncond!F8,2)</f>
-        <v>0.93</v>
+        <v>0.89</v>
       </c>
       <c r="I37" s="15">
         <f>ROUND(SS_survey_uncond!J8,2)</f>
-        <v>0</v>
+        <v>0.56000000000000005</v>
       </c>
     </row>
     <row r="38" spans="1:9">
@@ -2611,15 +2614,15 @@
       </c>
       <c r="D38" s="1" t="str">
         <f>CONCATENATE("(",ROUND(SS_survey_uncond!B9,2),")")</f>
-        <v>(0.03)</v>
+        <v>(0.01)</v>
       </c>
       <c r="E38" s="1" t="str">
         <f>CONCATENATE("(",ROUND(SS_survey_uncond!C9,2),")")</f>
-        <v>(0.02)</v>
+        <v>(0.01)</v>
       </c>
       <c r="F38" s="1" t="str">
         <f>CONCATENATE("(",ROUND(SS_survey_uncond!D9,2),")")</f>
-        <v>(0.03)</v>
+        <v>(0.01)</v>
       </c>
       <c r="G38" s="15" t="str">
         <f>CONCATENATE("(",ROUND(SS_survey_uncond!E9,2),")")</f>
@@ -2627,7 +2630,7 @@
       </c>
       <c r="H38" s="15" t="str">
         <f>CONCATENATE("(",ROUND(SS_survey_uncond!F9,2),")")</f>
-        <v>(0.02)</v>
+        <v>(0.01)</v>
       </c>
     </row>
     <row r="39" spans="1:9">
@@ -2636,31 +2639,31 @@
       </c>
       <c r="B39" s="15">
         <f>ROUND(SS_survey_uncond!H10,2)</f>
-        <v>91.91</v>
+        <v>92.64</v>
       </c>
       <c r="C39" s="1">
         <f>ROUND(SS_survey_uncond!G10,2)</f>
-        <v>91.83</v>
+        <v>91.84</v>
       </c>
       <c r="D39" s="1">
         <f>ROUND(SS_survey_uncond!B10,2)</f>
-        <v>91.82</v>
+        <v>92.73</v>
       </c>
       <c r="E39" s="1">
         <f>ROUND(SS_survey_uncond!C10,2)</f>
-        <v>93.54</v>
+        <v>92.19</v>
       </c>
       <c r="F39" s="1">
         <f>ROUND(SS_survey_uncond!D10,2)</f>
-        <v>97.39</v>
+        <v>93.66</v>
       </c>
       <c r="G39" s="15">
         <f>ROUND(SS_survey_uncond!E10,2)</f>
-        <v>95.71</v>
+        <v>93.71</v>
       </c>
       <c r="H39" s="15">
         <f>ROUND(SS_survey_uncond!F10,2)</f>
-        <v>97.08</v>
+        <v>93.34</v>
       </c>
       <c r="I39" s="15">
         <f>ROUND(SS_survey_uncond!J10,2)</f>
@@ -2670,7 +2673,7 @@
     <row r="40" spans="1:9">
       <c r="B40" s="15" t="str">
         <f>CONCATENATE("(",ROUND(SS_survey_uncond!H11,2),")")</f>
-        <v>(0.3)</v>
+        <v>(0.2)</v>
       </c>
       <c r="C40" s="1" t="str">
         <f>CONCATENATE("(",ROUND(SS_survey_uncond!G11,2),")")</f>
@@ -2678,23 +2681,23 @@
       </c>
       <c r="D40" s="1" t="str">
         <f>CONCATENATE("(",ROUND(SS_survey_uncond!B11,2),")")</f>
-        <v>(3.15)</v>
+        <v>(0.54)</v>
       </c>
       <c r="E40" s="1" t="str">
         <f>CONCATENATE("(",ROUND(SS_survey_uncond!C11,2),")")</f>
-        <v>(2.11)</v>
+        <v>(0.84)</v>
       </c>
       <c r="F40" s="1" t="str">
         <f>CONCATENATE("(",ROUND(SS_survey_uncond!D11,2),")")</f>
-        <v>(1.89)</v>
+        <v>(0.59)</v>
       </c>
       <c r="G40" s="15" t="str">
         <f>CONCATENATE("(",ROUND(SS_survey_uncond!E11,2),")")</f>
-        <v>(1.92)</v>
+        <v>(0.46)</v>
       </c>
       <c r="H40" s="15" t="str">
         <f>CONCATENATE("(",ROUND(SS_survey_uncond!F11,2),")")</f>
-        <v>(2.05)</v>
+        <v>(0.59)</v>
       </c>
     </row>
     <row r="41" spans="1:9">
@@ -2703,7 +2706,7 @@
       </c>
       <c r="B41" s="15">
         <f>ROUND(SS_survey_uncond!H12,2)</f>
-        <v>0.6</v>
+        <v>0.63</v>
       </c>
       <c r="C41" s="1">
         <f>ROUND(SS_survey_uncond!G12,2)</f>
@@ -2711,27 +2714,27 @@
       </c>
       <c r="D41" s="1">
         <f>ROUND(SS_survey_uncond!B12,2)</f>
-        <v>0.68</v>
+        <v>0.66</v>
       </c>
       <c r="E41" s="1">
         <f>ROUND(SS_survey_uncond!C12,2)</f>
-        <v>0.64</v>
+        <v>0.67</v>
       </c>
       <c r="F41" s="1">
         <f>ROUND(SS_survey_uncond!D12,2)</f>
-        <v>0.82</v>
+        <v>0.65</v>
       </c>
       <c r="G41" s="15">
         <f>ROUND(SS_survey_uncond!E12,2)</f>
-        <v>0.59</v>
+        <v>0.66</v>
       </c>
       <c r="H41" s="15">
         <f>ROUND(SS_survey_uncond!F12,2)</f>
-        <v>0.56999999999999995</v>
+        <v>0.64</v>
       </c>
       <c r="I41" s="15">
         <f>ROUND(SS_survey_uncond!J12,2)</f>
-        <v>0</v>
+        <v>0.01</v>
       </c>
     </row>
     <row r="42" spans="1:9">
@@ -2745,23 +2748,23 @@
       </c>
       <c r="D42" s="1" t="str">
         <f>CONCATENATE("(",ROUND(SS_survey_uncond!B13,2),")")</f>
-        <v>(0.04)</v>
+        <v>(0.02)</v>
       </c>
       <c r="E42" s="1" t="str">
         <f>CONCATENATE("(",ROUND(SS_survey_uncond!C13,2),")")</f>
-        <v>(0.04)</v>
+        <v>(0.02)</v>
       </c>
       <c r="F42" s="1" t="str">
         <f>CONCATENATE("(",ROUND(SS_survey_uncond!D13,2),")")</f>
-        <v>(0.05)</v>
+        <v>(0.02)</v>
       </c>
       <c r="G42" s="15" t="str">
         <f>CONCATENATE("(",ROUND(SS_survey_uncond!E13,2),")")</f>
-        <v>(0.06)</v>
+        <v>(0.02)</v>
       </c>
       <c r="H42" s="15" t="str">
         <f>CONCATENATE("(",ROUND(SS_survey_uncond!F13,2),")")</f>
-        <v>(0.06)</v>
+        <v>(0.02)</v>
       </c>
     </row>
     <row r="43" spans="1:9">
@@ -2772,27 +2775,27 @@
       <c r="C43" s="1"/>
       <c r="D43" s="1">
         <f>ROUND(SS_survey_uncond!B14,2)</f>
-        <v>0</v>
+        <v>0.98</v>
       </c>
       <c r="E43" s="1">
         <f>ROUND(SS_survey_uncond!C14,2)</f>
-        <v>0</v>
+        <v>0.97</v>
       </c>
       <c r="F43" s="1">
         <f>ROUND(SS_survey_uncond!D14,2)</f>
-        <v>0</v>
+        <v>0.99</v>
       </c>
       <c r="G43" s="15">
         <f>ROUND(SS_survey_uncond!E14,2)</f>
-        <v>0</v>
+        <v>0.98</v>
       </c>
       <c r="H43" s="15">
         <f>ROUND(SS_survey_uncond!F14,2)</f>
-        <v>0</v>
+        <v>0.99</v>
       </c>
       <c r="I43" s="15">
         <f>ROUND(SS_survey_uncond!J14,2)</f>
-        <v>0</v>
+        <v>0.25</v>
       </c>
     </row>
     <row r="44" spans="1:9" ht="15" thickBot="1">
@@ -2801,31 +2804,31 @@
       </c>
       <c r="B44" s="11">
         <f>SUM(C44:H44)</f>
-        <v>7104</v>
+        <v>17546</v>
       </c>
       <c r="C44" s="17">
         <f>ROUND(SS_survey_uncond!G16,2)</f>
-        <v>6910</v>
+        <v>6919</v>
       </c>
       <c r="D44" s="11">
         <f>ROUND(SS_survey_uncond!B16,2)</f>
-        <v>35</v>
+        <v>2035</v>
       </c>
       <c r="E44" s="11">
         <f>ROUND(SS_survey_uncond!C16,2)</f>
-        <v>52</v>
+        <v>1907</v>
       </c>
       <c r="F44" s="11">
         <f>ROUND(SS_survey_uncond!D16,2)</f>
-        <v>23</v>
+        <v>1757</v>
       </c>
       <c r="G44" s="13">
         <f>ROUND(SS_survey_uncond!E16,2)</f>
-        <v>58</v>
+        <v>2710</v>
       </c>
       <c r="H44" s="13">
         <f>ROUND(SS_survey_uncond!F16,2)</f>
-        <v>26</v>
+        <v>2218</v>
       </c>
       <c r="I44" s="13"/>
     </row>

</xml_diff>

<commit_message>
review of the paper, major revisions
Former-commit-id: f0ba952ceba4dcebac4f60c80e3534421325c165
</commit_message>
<xml_diff>
--- a/Tables/SS.xlsx
+++ b/Tables/SS.xlsx
@@ -1,16 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22527"/>
   <workbookPr defaultThemeVersion="166925"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\xps-seira\Dropbox\Apps\ShareLaTeX\Donde2020\Tables\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A3C2CBA4-0CAB-489C-AF5A-38DFBE5118E1}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12600" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12600" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="SS_admin" sheetId="1" r:id="rId1"/>
@@ -18,17 +12,7 @@
     <sheet name="SS_survey" sheetId="2" r:id="rId3"/>
     <sheet name="SS" sheetId="3" r:id="rId4"/>
   </sheets>
-  <calcPr calcId="191029"/>
-  <extLst>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
-      </xcalcf:calcFeatures>
-    </ext>
-  </extLst>
+  <calcPr calcId="191029" fullCalcOnLoad="true"/>
 </workbook>
 </file>
 
@@ -116,7 +100,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <fonts count="1">
     <font>
       <sz val="11"/>
@@ -194,54 +178,54 @@
   </cellStyleXfs>
   <cellXfs count="21">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="true">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="true"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="true"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="true"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="true" applyAlignment="true">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="true" applyAlignment="true">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="true"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="true"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="true" applyAlignment="true">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="true" applyAlignment="true">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="true" applyAlignment="true">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="true" applyAlignment="true">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="true" applyAlignment="true">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="true" applyAlignment="true">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="true">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="true" applyAlignment="true">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="true" applyAlignment="true">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="true" applyAlignment="true">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="true" applyAlignment="true">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="true" applyAlignment="true">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -250,14 +234,6 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
-      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
-    </ext>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
-      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
-    </ext>
-  </extLst>
 </styleSheet>
 </file>
 
@@ -557,7 +533,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="B2:J10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -566,220 +542,220 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
   <sheetData>
-    <row r="2" spans="2:10">
-      <c r="B2">
+    <row r="2">
+      <c r="B2" s="0">
         <v>2301.0995770857362</v>
       </c>
-      <c r="C2">
+      <c r="C2" s="0">
         <v>2147.1437198067633</v>
       </c>
-      <c r="D2">
-        <v>2132.6205936920223</v>
-      </c>
-      <c r="E2">
-        <v>2180.996215429403</v>
-      </c>
-      <c r="F2">
-        <v>2089.3112798264642</v>
-      </c>
-      <c r="G2">
-        <v>2239.0573888091822</v>
-      </c>
-      <c r="H2">
-        <v>2197.3231220764928</v>
-      </c>
-      <c r="J2">
-        <v>0.32446131464480321</v>
-      </c>
-    </row>
-    <row r="3" spans="2:10">
-      <c r="B3">
-        <v>79.416968039721894</v>
-      </c>
-      <c r="C3">
+      <c r="D2" s="0">
+        <v>2132.9021789522485</v>
+      </c>
+      <c r="E2" s="0">
+        <v>2182.1076833527359</v>
+      </c>
+      <c r="F2" s="0">
+        <v>2089.2792630057802</v>
+      </c>
+      <c r="G2" s="0">
+        <v>2237.6690182948701</v>
+      </c>
+      <c r="H2" s="0">
+        <v>2196.9740932642485</v>
+      </c>
+      <c r="J2" s="0">
+        <v>0.32332390189094179</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="B3" s="0">
+        <v>79.416968039721866</v>
+      </c>
+      <c r="C3" s="0">
         <v>71.911953944693508</v>
       </c>
-      <c r="D3">
-        <v>74.033283407617645</v>
-      </c>
-      <c r="E3">
-        <v>65.120503781670294</v>
-      </c>
-      <c r="F3">
-        <v>64.583610998175828</v>
-      </c>
-      <c r="G3">
-        <v>39.337883620480333</v>
-      </c>
-      <c r="H3">
-        <v>24.754156479662203</v>
-      </c>
-    </row>
-    <row r="4" spans="2:10">
-      <c r="B4">
+      <c r="D3" s="0">
+        <v>73.985411575168996</v>
+      </c>
+      <c r="E3" s="0">
+        <v>64.994187260506536</v>
+      </c>
+      <c r="F3" s="0">
+        <v>64.541278696715779</v>
+      </c>
+      <c r="G3" s="0">
+        <v>39.321634665077902</v>
+      </c>
+      <c r="H3" s="0">
+        <v>24.73701848637311</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="B4" s="0">
         <v>0.18300653594771241</v>
       </c>
-      <c r="C4">
+      <c r="C4" s="0">
         <v>0.15660225442834139</v>
       </c>
-      <c r="D4">
-        <v>0.17115027829313545</v>
-      </c>
-      <c r="E4">
-        <v>0.18544395924308588</v>
-      </c>
-      <c r="F4">
-        <v>0.21294287780187998</v>
-      </c>
-      <c r="G4">
+      <c r="D4" s="0">
+        <v>0.17153453871117291</v>
+      </c>
+      <c r="E4" s="0">
+        <v>0.18538998835855647</v>
+      </c>
+      <c r="F4" s="0">
+        <v>0.21315028901734104</v>
+      </c>
+      <c r="G4" s="0">
         <v>0.16334633587251973</v>
       </c>
-      <c r="H4">
-        <v>0.17546567525263665</v>
-      </c>
-      <c r="J4">
-        <v>0.96119404460628477</v>
-      </c>
-    </row>
-    <row r="5" spans="2:10">
-      <c r="B5">
-        <v>4.6899158297364733E-2</v>
-      </c>
-      <c r="C5">
-        <v>5.0426323482161958E-2</v>
-      </c>
-      <c r="D5">
-        <v>6.2958909127783763E-2</v>
-      </c>
-      <c r="E5">
-        <v>5.52270251303826E-2</v>
-      </c>
-      <c r="F5">
-        <v>5.4525598840516186E-2</v>
-      </c>
-      <c r="G5">
-        <v>2.9307647529097775E-2</v>
-      </c>
-      <c r="H5">
-        <v>1.8761523488194442E-2</v>
-      </c>
-    </row>
-    <row r="6" spans="2:10">
-      <c r="B6">
+      <c r="H4" s="0">
+        <v>0.1755251900747066</v>
+      </c>
+      <c r="J4" s="0">
+        <v>0.96109250462689699</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="B5" s="0">
+        <v>0.046899158297364733</v>
+      </c>
+      <c r="C5" s="0">
+        <v>0.050426323482161958</v>
+      </c>
+      <c r="D5" s="0">
+        <v>0.063011562076970493</v>
+      </c>
+      <c r="E5" s="0">
+        <v>0.055217291625827412</v>
+      </c>
+      <c r="F5" s="0">
+        <v>0.054634146343476728</v>
+      </c>
+      <c r="G5" s="0">
+        <v>0.029307647529097775</v>
+      </c>
+      <c r="H5" s="0">
+        <v>0.018768813498507914</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="B6" s="0">
         <v>30.964285714285715</v>
       </c>
-      <c r="C6">
-        <v>31.05</v>
-      </c>
-      <c r="D6">
-        <v>31.705882352941178</v>
-      </c>
-      <c r="E6">
-        <v>36.935483870967744</v>
-      </c>
-      <c r="F6">
-        <v>33.731707317073173</v>
-      </c>
-      <c r="G6">
+      <c r="C6" s="0">
+        <v>31.050000000000001</v>
+      </c>
+      <c r="D6" s="0">
+        <v>31.720588235294116</v>
+      </c>
+      <c r="E6" s="0">
+        <v>36.946236559139784</v>
+      </c>
+      <c r="F6" s="0">
+        <v>33.756097560975611</v>
+      </c>
+      <c r="G6" s="0">
         <v>36.085999441146853</v>
       </c>
-      <c r="H6">
-        <v>33.965042418068883</v>
-      </c>
-      <c r="J6">
-        <v>0.38197353151189578</v>
-      </c>
-    </row>
-    <row r="7" spans="2:10">
-      <c r="B7">
+      <c r="H6" s="0">
+        <v>33.971856728119988</v>
+      </c>
+      <c r="J6" s="0">
+        <v>0.38016330251224012</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="B7" s="0">
         <v>2.2039217137676097</v>
       </c>
-      <c r="C7">
+      <c r="C7" s="0">
         <v>2.3481004981403775</v>
       </c>
-      <c r="D7">
-        <v>2.3776522848922048</v>
-      </c>
-      <c r="E7">
-        <v>2.6461403107335482</v>
-      </c>
-      <c r="F7">
-        <v>1.7583669968981817</v>
-      </c>
-      <c r="G7">
+      <c r="D7" s="0">
+        <v>2.378278716305112</v>
+      </c>
+      <c r="E7" s="0">
+        <v>2.6489461589498058</v>
+      </c>
+      <c r="F7" s="0">
+        <v>1.7656736463335312</v>
+      </c>
+      <c r="G7" s="0">
         <v>1.2515869857807669</v>
       </c>
-      <c r="H7">
-        <v>0.81557186601969811</v>
-      </c>
-    </row>
-    <row r="8" spans="2:10">
-      <c r="B8">
+      <c r="H7" s="0">
+        <v>0.81612819251442403</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="B8" s="0">
         <v>84</v>
       </c>
-      <c r="C8">
+      <c r="C8" s="0">
         <v>80</v>
       </c>
-      <c r="D8">
+      <c r="D8" s="0">
         <v>68</v>
       </c>
-      <c r="E8">
+      <c r="E8" s="0">
         <v>93</v>
       </c>
-      <c r="F8">
+      <c r="F8" s="0">
         <v>82</v>
       </c>
-      <c r="G8">
+      <c r="G8" s="0">
         <v>180</v>
       </c>
-      <c r="H8">
-        <v>119.95409941305942</v>
-      </c>
-    </row>
-    <row r="9" spans="2:10">
-      <c r="B9">
+      <c r="H8" s="0">
+        <v>119.94700165046763</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="B9" s="0">
         <v>0</v>
       </c>
-      <c r="C9">
+      <c r="C9" s="0">
         <v>0</v>
       </c>
-      <c r="D9">
+      <c r="D9" s="0">
         <v>0</v>
       </c>
-      <c r="E9">
+      <c r="E9" s="0">
         <v>0</v>
       </c>
-      <c r="F9">
+      <c r="F9" s="0">
         <v>0</v>
       </c>
-      <c r="G9">
+      <c r="G9" s="0">
         <v>0</v>
       </c>
-      <c r="H9">
-        <v>2.4106356641674171</v>
-      </c>
-    </row>
-    <row r="10" spans="2:10">
-      <c r="B10">
+      <c r="H9" s="0">
+        <v>2.4105929754037141</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="B10" s="0">
         <v>2601</v>
       </c>
-      <c r="C10">
+      <c r="C10" s="0">
         <v>2484</v>
       </c>
-      <c r="D10">
-        <v>2156</v>
-      </c>
-      <c r="E10">
-        <v>3435</v>
-      </c>
-      <c r="F10">
-        <v>2766</v>
-      </c>
-      <c r="G10">
+      <c r="D10" s="0">
+        <v>2157</v>
+      </c>
+      <c r="E10" s="0">
+        <v>3436</v>
+      </c>
+      <c r="F10" s="0">
+        <v>2768</v>
+      </c>
+      <c r="G10" s="0">
         <v>8366</v>
       </c>
-      <c r="H10">
-        <v>21808</v>
+      <c r="H10" s="0">
+        <v>21812</v>
       </c>
     </row>
   </sheetData>
@@ -788,7 +764,7 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="B2:J16"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -797,366 +773,366 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
   <sheetData>
-    <row r="2" spans="2:10">
-      <c r="B2">
-        <v>0.75564409030544488</v>
-      </c>
-      <c r="C2">
+    <row r="2">
+      <c r="B2" s="0">
+        <v>0.75514266755142667</v>
+      </c>
+      <c r="C2" s="0">
         <v>0.72237196765498657</v>
       </c>
-      <c r="D2">
-        <v>0.72575250836120397</v>
-      </c>
-      <c r="E2">
-        <v>0.71847070506454813</v>
-      </c>
-      <c r="F2">
-        <v>0.74042027194066751</v>
-      </c>
-      <c r="G2">
+      <c r="D2" s="0">
+        <v>0.72635983263598325</v>
+      </c>
+      <c r="E2" s="0">
+        <v>0.71811414392059558</v>
+      </c>
+      <c r="F2" s="0">
+        <v>0.74058060531192094</v>
+      </c>
+      <c r="G2" s="0">
         <v>0.74980252764612954</v>
       </c>
-      <c r="H2">
-        <v>0.73901568079490765</v>
-      </c>
-      <c r="J2">
-        <v>0.3199816408066643</v>
-      </c>
-    </row>
-    <row r="3" spans="2:10">
-      <c r="B3">
-        <v>1.644910941444085E-2</v>
-      </c>
-      <c r="C3">
-        <v>1.609110026524976E-2</v>
-      </c>
-      <c r="D3">
-        <v>2.0205125736203776E-2</v>
-      </c>
-      <c r="E3">
-        <v>1.5011614271560187E-2</v>
-      </c>
-      <c r="F3">
-        <v>1.2844826313395475E-2</v>
-      </c>
-      <c r="G3">
-        <v>9.0149695175873682E-3</v>
-      </c>
-      <c r="H3">
-        <v>5.6636661229594034E-3</v>
-      </c>
-    </row>
-    <row r="4" spans="2:10">
-      <c r="B4">
-        <v>43.197724039829303</v>
-      </c>
-      <c r="C4">
+      <c r="H2" s="0">
+        <v>0.73897857808134115</v>
+      </c>
+      <c r="J2" s="0">
+        <v>0.32676495649175458</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="B3" s="0">
+        <v>0.016425991245592322</v>
+      </c>
+      <c r="C3" s="0">
+        <v>0.01609110026524976</v>
+      </c>
+      <c r="D3" s="0">
+        <v>0.020324180320801289</v>
+      </c>
+      <c r="E3" s="0">
+        <v>0.015140443704992809</v>
+      </c>
+      <c r="F3" s="0">
+        <v>0.012828726752602795</v>
+      </c>
+      <c r="G3" s="0">
+        <v>0.0090149695175873682</v>
+      </c>
+      <c r="H3" s="0">
+        <v>0.0056750398759389089</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="B4" s="0">
+        <v>43.197583511016347</v>
+      </c>
+      <c r="C4" s="0">
         <v>43.214285714285715</v>
       </c>
-      <c r="D4">
-        <v>43.012808783165596</v>
-      </c>
-      <c r="E4">
-        <v>44.068702290076338</v>
-      </c>
-      <c r="F4">
-        <v>43.071663379355684</v>
-      </c>
-      <c r="G4">
+      <c r="D4" s="0">
+        <v>43.014652014652015</v>
+      </c>
+      <c r="E4" s="0">
+        <v>44.068119891008173</v>
+      </c>
+      <c r="F4" s="0">
+        <v>43.085413929040733</v>
+      </c>
+      <c r="G4" s="0">
         <v>43.05681818181818</v>
       </c>
-      <c r="H4">
-        <v>43.244162775183455</v>
-      </c>
-      <c r="J4">
-        <v>0.78677267826023056</v>
-      </c>
-    </row>
-    <row r="5" spans="2:10">
-      <c r="B5">
-        <v>0.56403599075095434</v>
-      </c>
-      <c r="C5">
-        <v>0.77069700997930002</v>
-      </c>
-      <c r="D5">
-        <v>0.65952524226845821</v>
-      </c>
-      <c r="E5">
-        <v>0.60510467478567853</v>
-      </c>
-      <c r="F5">
-        <v>0.51494995970101298</v>
-      </c>
-      <c r="G5">
-        <v>0.31582069920051548</v>
-      </c>
-      <c r="H5">
-        <v>0.21147020058714425</v>
-      </c>
-    </row>
-    <row r="6" spans="2:10">
-      <c r="B6">
-        <v>3144.9910089163509</v>
-      </c>
-      <c r="C6">
-        <v>2985.0461656208972</v>
-      </c>
-      <c r="D6">
-        <v>3010.0226498567731</v>
-      </c>
-      <c r="E6">
-        <v>3110.5951057232041</v>
-      </c>
-      <c r="F6">
-        <v>3082.4794570266222</v>
-      </c>
-      <c r="G6">
-        <v>3192.3475956420366</v>
-      </c>
-      <c r="H6">
-        <v>3111.5831964531485</v>
-      </c>
-      <c r="J6">
-        <v>0.40587608283675952</v>
-      </c>
-    </row>
-    <row r="7" spans="2:10">
-      <c r="B7">
-        <v>68.21540163415446</v>
-      </c>
-      <c r="C7">
-        <v>88.350791604799952</v>
-      </c>
-      <c r="D7">
-        <v>76.46623124498781</v>
-      </c>
-      <c r="E7">
-        <v>84.456979102137012</v>
-      </c>
-      <c r="F7">
-        <v>99.018458366442971</v>
-      </c>
-      <c r="G7">
-        <v>75.187904829259352</v>
-      </c>
-      <c r="H7">
-        <v>35.73867184340029</v>
-      </c>
-    </row>
-    <row r="8" spans="2:10">
-      <c r="B8">
-        <v>0.8904494382022472</v>
-      </c>
-      <c r="C8">
+      <c r="H4" s="0">
+        <v>43.246039686509924</v>
+      </c>
+      <c r="J4" s="0">
+        <v>0.78897874356254194</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="B5" s="0">
+        <v>0.56359423339355952</v>
+      </c>
+      <c r="C5" s="0">
+        <v>0.77069700997930024</v>
+      </c>
+      <c r="D5" s="0">
+        <v>0.66004082042892598</v>
+      </c>
+      <c r="E5" s="0">
+        <v>0.60465537492814869</v>
+      </c>
+      <c r="F5" s="0">
+        <v>0.51619884617405898</v>
+      </c>
+      <c r="G5" s="0">
+        <v>0.31582069920051536</v>
+      </c>
+      <c r="H5" s="0">
+        <v>0.21148102499151927</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="B6" s="0">
+        <v>3145.352544966549</v>
+      </c>
+      <c r="C6" s="0">
+        <v>2985.2732691622746</v>
+      </c>
+      <c r="D6" s="0">
+        <v>3010.3149184642348</v>
+      </c>
+      <c r="E6" s="0">
+        <v>3110.9508585695362</v>
+      </c>
+      <c r="F6" s="0">
+        <v>3082.6830472633487</v>
+      </c>
+      <c r="G6" s="0">
+        <v>3192.3481642889119</v>
+      </c>
+      <c r="H6" s="0">
+        <v>3111.7794650246028</v>
+      </c>
+      <c r="J6" s="0">
+        <v>0.40669071195869227</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="B7" s="0">
+        <v>68.222299405324407</v>
+      </c>
+      <c r="C7" s="0">
+        <v>88.361354683798055</v>
+      </c>
+      <c r="D7" s="0">
+        <v>76.470442299269308</v>
+      </c>
+      <c r="E7" s="0">
+        <v>84.469381845420926</v>
+      </c>
+      <c r="F7" s="0">
+        <v>99.031452584314096</v>
+      </c>
+      <c r="G7" s="0">
+        <v>75.187897820076472</v>
+      </c>
+      <c r="H7" s="0">
+        <v>35.740522483170373</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="B8" s="0">
+        <v>0.89052631578947372</v>
+      </c>
+      <c r="C8" s="0">
         <v>0.89978828510938602</v>
       </c>
-      <c r="D8">
-        <v>0.89142335766423353</v>
-      </c>
-      <c r="E8">
-        <v>0.91065662002152847</v>
-      </c>
-      <c r="F8">
-        <v>0.89407061958694201</v>
-      </c>
-      <c r="G8">
+      <c r="D8" s="0">
+        <v>0.89132420091324205</v>
+      </c>
+      <c r="E8" s="0">
+        <v>0.91070467993544912</v>
+      </c>
+      <c r="F8" s="0">
+        <v>0.89414114513981358</v>
+      </c>
+      <c r="G8" s="0">
         <v>0.88422131147540983</v>
       </c>
-      <c r="H8">
-        <v>0.89265768725361372</v>
-      </c>
-      <c r="J8">
-        <v>0.55584000072208539</v>
-      </c>
-    </row>
-    <row r="9" spans="2:10">
-      <c r="B9">
-        <v>1.1507748187866138E-2</v>
-      </c>
-      <c r="C9">
-        <v>1.057909469617015E-2</v>
-      </c>
-      <c r="D9">
-        <v>1.4552389380818403E-2</v>
-      </c>
-      <c r="E9">
-        <v>9.9277590884214503E-3</v>
-      </c>
-      <c r="F9">
-        <v>9.4668089479309457E-3</v>
-      </c>
-      <c r="G9">
-        <v>1.0533724370448033E-2</v>
-      </c>
-      <c r="H9">
-        <v>5.2053730841606369E-3</v>
-      </c>
-    </row>
-    <row r="10" spans="2:10">
-      <c r="B10">
+      <c r="H8" s="0">
+        <v>0.89267531614386597</v>
+      </c>
+      <c r="J8" s="0">
+        <v>0.55470049940501021</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="B9" s="0">
+        <v>0.011504362429475282</v>
+      </c>
+      <c r="C9" s="0">
+        <v>0.01057909469617015</v>
+      </c>
+      <c r="D9" s="0">
+        <v>0.014535413795478427</v>
+      </c>
+      <c r="E9" s="0">
+        <v>0.0099323761115656124</v>
+      </c>
+      <c r="F9" s="0">
+        <v>0.0094836902763061077</v>
+      </c>
+      <c r="G9" s="0">
+        <v>0.010533724370448033</v>
+      </c>
+      <c r="H9" s="0">
+        <v>0.0052054873450900745</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="B10" s="0">
         <v>92.725089422585597</v>
       </c>
-      <c r="C10">
+      <c r="C10" s="0">
         <v>92.193231441048042</v>
       </c>
-      <c r="D10">
-        <v>93.658892128279888</v>
-      </c>
-      <c r="E10">
-        <v>93.714012982054214</v>
-      </c>
-      <c r="F10">
+      <c r="D10" s="0">
+        <v>93.655192532088677</v>
+      </c>
+      <c r="E10" s="0">
+        <v>93.716412213740455</v>
+      </c>
+      <c r="F10" s="0">
         <v>93.339202965708992</v>
       </c>
-      <c r="G10">
+      <c r="G10" s="0">
         <v>91.835829749369722</v>
       </c>
-      <c r="H10">
+      <c r="H10" s="0">
         <v>92.639685150375939</v>
       </c>
-      <c r="J10">
-        <v>4.6684240622125997E-3</v>
-      </c>
-    </row>
-    <row r="11" spans="2:10">
-      <c r="B11">
+      <c r="J10" s="0">
+        <v>0.0046482646196749997</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="B11" s="0">
         <v>0.54084732630950216</v>
       </c>
-      <c r="C11">
+      <c r="C11" s="0">
         <v>0.83856879215694513</v>
       </c>
-      <c r="D11">
-        <v>0.59084286834349808</v>
-      </c>
-      <c r="E11">
-        <v>0.45528703025952877</v>
-      </c>
-      <c r="F11">
-        <v>0.5948733338915928</v>
-      </c>
-      <c r="G11">
+      <c r="D11" s="0">
+        <v>0.59030374500190863</v>
+      </c>
+      <c r="E11" s="0">
+        <v>0.45517920772459858</v>
+      </c>
+      <c r="F11" s="0">
+        <v>0.59487333389159291</v>
+      </c>
+      <c r="G11" s="0">
         <v>0.30818777366122263</v>
       </c>
-      <c r="H11">
-        <v>0.20479038611903611</v>
-      </c>
-    </row>
-    <row r="12" spans="2:10">
-      <c r="B12">
-        <v>0.65949820788530467</v>
-      </c>
-      <c r="C12">
+      <c r="H11" s="0">
+        <v>0.20476842319378327</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="B12" s="0">
+        <v>0.6597421203438395</v>
+      </c>
+      <c r="C12" s="0">
         <v>0.66884057971014488</v>
       </c>
-      <c r="D12">
-        <v>0.64749536178107603</v>
-      </c>
-      <c r="E12">
-        <v>0.66257668711656437</v>
-      </c>
-      <c r="F12">
-        <v>0.64335180055401664</v>
-      </c>
-      <c r="G12">
+      <c r="D12" s="0">
+        <v>0.64716805942432687</v>
+      </c>
+      <c r="E12" s="0">
+        <v>0.66276477146042367</v>
+      </c>
+      <c r="F12" s="0">
+        <v>0.643598615916955</v>
+      </c>
+      <c r="G12" s="0">
         <v>0.59694943585457583</v>
       </c>
-      <c r="H12">
-        <v>0.63278881778376561</v>
-      </c>
-      <c r="J12">
-        <v>6.6108847471301998E-3</v>
-      </c>
-    </row>
-    <row r="13" spans="2:10">
-      <c r="B13">
-        <v>1.9536506277868428E-2</v>
-      </c>
-      <c r="C13">
-        <v>1.9329841394817811E-2</v>
-      </c>
-      <c r="D13">
-        <v>2.4043222313478024E-2</v>
-      </c>
-      <c r="E13">
-        <v>1.6894823421726591E-2</v>
-      </c>
-      <c r="F13">
-        <v>1.6696589416796935E-2</v>
-      </c>
-      <c r="G13">
-        <v>1.2957951584969644E-2</v>
-      </c>
-      <c r="H13">
-        <v>7.4863193792611979E-3</v>
-      </c>
-    </row>
-    <row r="14" spans="2:10">
-      <c r="B14">
+      <c r="H12" s="0">
+        <v>0.63285064825728232</v>
+      </c>
+      <c r="J12" s="0">
+        <v>0.0063827033858757003</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="B13" s="0">
+        <v>0.01938204739007152</v>
+      </c>
+      <c r="C13" s="0">
+        <v>0.019329841394817807</v>
+      </c>
+      <c r="D13" s="0">
+        <v>0.024251483945742541</v>
+      </c>
+      <c r="E13" s="0">
+        <v>0.016843213086678365</v>
+      </c>
+      <c r="F13" s="0">
+        <v>0.016646508216829121</v>
+      </c>
+      <c r="G13" s="0">
+        <v>0.012957951584969644</v>
+      </c>
+      <c r="H13" s="0">
+        <v>0.0074824965608947022</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="B14" s="0">
         <v>0.98280098280098283</v>
       </c>
-      <c r="C14">
+      <c r="C14" s="0">
         <v>0.97273203985317247</v>
       </c>
-      <c r="D14">
-        <v>0.98577120091064319</v>
-      </c>
-      <c r="E14">
-        <v>0.97859778597785974</v>
-      </c>
-      <c r="F14">
-        <v>0.98827772768259692</v>
-      </c>
-      <c r="G14">
-        <v>1.3007660066483597E-3</v>
-      </c>
-      <c r="H14">
-        <v>0.59500740909609029</v>
-      </c>
-      <c r="J14">
-        <v>0.2454321833124756</v>
-      </c>
-    </row>
-    <row r="15" spans="2:10">
-      <c r="B15">
-        <v>4.0156175496241656E-3</v>
-      </c>
-      <c r="C15">
-        <v>7.3961905116490204E-3</v>
-      </c>
-      <c r="D15">
-        <v>3.380162850677099E-3</v>
-      </c>
-      <c r="E15">
-        <v>5.9663991659335853E-3</v>
-      </c>
-      <c r="F15">
-        <v>3.007259722267115E-3</v>
-      </c>
-      <c r="G15">
-        <v>7.2827849166321888E-4</v>
-      </c>
-      <c r="H15">
-        <v>2.0884546392501639E-2</v>
-      </c>
-    </row>
-    <row r="16" spans="2:10">
-      <c r="B16">
+      <c r="D14" s="0">
+        <v>0.9869020501138952</v>
+      </c>
+      <c r="E14" s="0">
+        <v>0.97860568056067876</v>
+      </c>
+      <c r="F14" s="0">
+        <v>0.9887285843101894</v>
+      </c>
+      <c r="G14" s="0">
+        <v>0.0013007660066483597</v>
+      </c>
+      <c r="H14" s="0">
+        <v>0.59517838823663516</v>
+      </c>
+      <c r="J14" s="0">
+        <v>0.18748172159766091</v>
+      </c>
+    </row>
+    <row r="15">
+      <c r="B15" s="0">
+        <v>0.0040156175496241656</v>
+      </c>
+      <c r="C15" s="0">
+        <v>0.0073961905116490204</v>
+      </c>
+      <c r="D15" s="0">
+        <v>0.0033401981602603041</v>
+      </c>
+      <c r="E15" s="0">
+        <v>0.005958008474724193</v>
+      </c>
+      <c r="F15" s="0">
+        <v>0.0029388029720992903</v>
+      </c>
+      <c r="G15" s="0">
+        <v>0.00072827849166321888</v>
+      </c>
+      <c r="H15" s="0">
+        <v>0.020893601789431546</v>
+      </c>
+    </row>
+    <row r="16">
+      <c r="B16" s="0">
         <v>2035</v>
       </c>
-      <c r="C16">
+      <c r="C16" s="0">
         <v>1907</v>
       </c>
-      <c r="D16">
-        <v>1757</v>
-      </c>
-      <c r="E16">
-        <v>2710</v>
-      </c>
-      <c r="F16">
+      <c r="D16" s="0">
+        <v>1756</v>
+      </c>
+      <c r="E16" s="0">
+        <v>2711</v>
+      </c>
+      <c r="F16" s="0">
         <v>2218</v>
       </c>
-      <c r="G16">
+      <c r="G16" s="0">
         <v>6919</v>
       </c>
     </row>
@@ -1166,7 +1142,7 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="B2:I16"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -1175,364 +1151,364 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
   <sheetData>
-    <row r="2" spans="2:9">
-      <c r="B2">
-        <v>0.75757575757575757</v>
-      </c>
-      <c r="C2">
+    <row r="2">
+      <c r="B2" s="0">
+        <v>0.75706594885598921</v>
+      </c>
+      <c r="C2" s="0">
         <v>0.72451790633608815</v>
       </c>
-      <c r="D2">
-        <v>0.72504230118443314</v>
-      </c>
-      <c r="E2">
-        <v>0.71811740890688258</v>
-      </c>
-      <c r="F2">
-        <v>0.74094881398252188</v>
-      </c>
-      <c r="G2">
-        <v>0.732753020657399</v>
+      <c r="D2" s="0">
+        <v>0.72527472527472525</v>
+      </c>
+      <c r="E2" s="0">
+        <v>0.71775417298937783</v>
+      </c>
+      <c r="F2" s="0">
+        <v>0.74111041796631316</v>
+      </c>
+      <c r="G2" s="0">
+        <v>0.73263212569796132</v>
       </c>
       <c r="H2">
         <v>0.73239071215462448</v>
       </c>
-      <c r="I2">
-        <v>0.41285083973109971</v>
-      </c>
-    </row>
-    <row r="3" spans="2:9">
-      <c r="B3">
-        <v>1.6353148457536527E-2</v>
-      </c>
-      <c r="C3">
-        <v>1.6037712453979815E-2</v>
-      </c>
-      <c r="D3">
-        <v>2.0714850878795654E-2</v>
-      </c>
-      <c r="E3">
-        <v>1.5694316621148546E-2</v>
-      </c>
-      <c r="F3">
-        <v>1.2961944419642095E-2</v>
-      </c>
-      <c r="G3">
-        <v>7.3610489260520747E-3</v>
+      <c r="I2" s="0">
+        <v>0.41991256838455371</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="B3" s="0">
+        <v>0.016329938660297399</v>
+      </c>
+      <c r="C3" s="0">
+        <v>0.016037712453979815</v>
+      </c>
+      <c r="D3" s="0">
+        <v>0.020704066804602267</v>
+      </c>
+      <c r="E3" s="0">
+        <v>0.015845064022229488</v>
+      </c>
+      <c r="F3" s="0">
+        <v>0.012945207155944546</v>
+      </c>
+      <c r="G3" s="0">
+        <v>0.0073798781164302616</v>
       </c>
       <c r="H3">
         <v>7.3732935414456838E-3</v>
       </c>
     </row>
-    <row r="4" spans="2:9">
-      <c r="B4">
-        <v>43.164985590778095</v>
-      </c>
-      <c r="C4">
+    <row r="4">
+      <c r="B4" s="0">
+        <v>43.164866810655148</v>
+      </c>
+      <c r="C4" s="0">
         <v>43.174778761061944</v>
       </c>
-      <c r="D4">
-        <v>42.961075069508802</v>
-      </c>
-      <c r="E4">
-        <v>43.956037840845852</v>
-      </c>
-      <c r="F4">
-        <v>43.058471760797339</v>
-      </c>
-      <c r="G4">
-        <v>43.312982456140354</v>
+      <c r="D4" s="0">
+        <v>42.960185185185182</v>
+      </c>
+      <c r="E4" s="0">
+        <v>43.95550611790879</v>
+      </c>
+      <c r="F4" s="0">
+        <v>43.072377158034527</v>
+      </c>
+      <c r="G4" s="0">
+        <v>43.315612287838405</v>
       </c>
       <c r="H4">
         <v>43.318341039652516</v>
       </c>
-      <c r="I4">
-        <v>0.78911299773387222</v>
-      </c>
-    </row>
-    <row r="5" spans="2:9">
-      <c r="B5">
-        <v>0.5734678785745746</v>
-      </c>
-      <c r="C5">
+      <c r="I4" s="0">
+        <v>0.79274632706051551</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="B5" s="0">
+        <v>0.57302039418728534</v>
+      </c>
+      <c r="C5" s="0">
         <v>0.78693411412047953</v>
       </c>
-      <c r="D5">
-        <v>0.65217105015255705</v>
-      </c>
-      <c r="E5">
-        <v>0.6123643223001326</v>
-      </c>
-      <c r="F5">
-        <v>0.51624441834800938</v>
-      </c>
-      <c r="G5">
-        <v>0.28324945753639863</v>
+      <c r="D5" s="0">
+        <v>0.65161383087213021</v>
+      </c>
+      <c r="E5" s="0">
+        <v>0.6120577121187506</v>
+      </c>
+      <c r="F5" s="0">
+        <v>0.51753954960280979</v>
+      </c>
+      <c r="G5" s="0">
+        <v>0.28318450221186076</v>
       </c>
       <c r="H5">
         <v>0.28291232956547702</v>
       </c>
     </row>
-    <row r="6" spans="2:9">
-      <c r="B6">
-        <v>3151.4645968486266</v>
-      </c>
-      <c r="C6">
-        <v>2977.5760595933448</v>
-      </c>
-      <c r="D6">
-        <v>2985.3601239472823</v>
-      </c>
-      <c r="E6">
-        <v>3114.4788654572976</v>
-      </c>
-      <c r="F6">
-        <v>3079.4527104367407</v>
-      </c>
-      <c r="G6">
-        <v>3068.4022871033972</v>
+    <row r="6">
+      <c r="B6" s="0">
+        <v>3151.8311879330831</v>
+      </c>
+      <c r="C6" s="0">
+        <v>2977.8080010068757</v>
+      </c>
+      <c r="D6" s="0">
+        <v>2987.6091755578368</v>
+      </c>
+      <c r="E6" s="0">
+        <v>3114.8420998012557</v>
+      </c>
+      <c r="F6" s="0">
+        <v>3080.6487658710303</v>
+      </c>
+      <c r="G6" s="0">
+        <v>3069.2245258990883</v>
       </c>
       <c r="H6">
         <v>3067.9203108635979</v>
       </c>
-      <c r="I6">
-        <v>0.40512608371464598</v>
-      </c>
-    </row>
-    <row r="7" spans="2:9">
-      <c r="B7">
-        <v>68.625662226643939</v>
-      </c>
-      <c r="C7">
-        <v>90.810127072547061</v>
-      </c>
-      <c r="D7">
-        <v>75.7749764033302</v>
-      </c>
-      <c r="E7">
-        <v>84.539006543944083</v>
-      </c>
-      <c r="F7">
-        <v>99.50770961838613</v>
-      </c>
-      <c r="G7">
-        <v>38.646858824752861</v>
+      <c r="I6" s="0">
+        <v>0.41290770426955908</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="B7" s="0">
+        <v>68.633705702668749</v>
+      </c>
+      <c r="C7" s="0">
+        <v>90.821567649747067</v>
+      </c>
+      <c r="D7" s="0">
+        <v>76.019238973365518</v>
+      </c>
+      <c r="E7" s="0">
+        <v>84.552913105159746</v>
+      </c>
+      <c r="F7" s="0">
+        <v>99.417675983085019</v>
+      </c>
+      <c r="G7" s="0">
+        <v>38.649480296696282</v>
       </c>
       <c r="H7">
         <v>38.640982667796216</v>
       </c>
     </row>
-    <row r="8" spans="2:9">
-      <c r="B8">
-        <v>0.89094796863863146</v>
-      </c>
-      <c r="C8">
+    <row r="8">
+      <c r="B8" s="0">
+        <v>0.89102564102564108</v>
+      </c>
+      <c r="C8" s="0">
         <v>0.89841498559077815</v>
       </c>
-      <c r="D8">
-        <v>0.89279112754158962</v>
-      </c>
-      <c r="E8">
-        <v>0.91058694459681844</v>
-      </c>
-      <c r="F8">
-        <v>0.89367429340511439</v>
-      </c>
-      <c r="G8">
-        <v>0.89821776663881925</v>
+      <c r="D8" s="0">
+        <v>0.89289012003693446</v>
+      </c>
+      <c r="E8" s="0">
+        <v>0.91063596491228072</v>
+      </c>
+      <c r="F8" s="0">
+        <v>0.89374579690652323</v>
+      </c>
+      <c r="G8" s="0">
+        <v>0.89827442248817146</v>
       </c>
       <c r="H8">
         <v>0.89838754517653596</v>
       </c>
-      <c r="I8">
-        <v>0.67936345560508071</v>
-      </c>
-    </row>
-    <row r="9" spans="2:9">
-      <c r="B9">
-        <v>1.1702510413535415E-2</v>
-      </c>
-      <c r="C9">
-        <v>1.0536449576402311E-2</v>
-      </c>
-      <c r="D9">
-        <v>1.441850449267084E-2</v>
-      </c>
-      <c r="E9">
-        <v>9.9874959754338993E-3</v>
-      </c>
-      <c r="F9">
-        <v>9.5208878346407667E-3</v>
-      </c>
-      <c r="G9">
-        <v>4.9467781608944564E-3</v>
+      <c r="I8" s="0">
+        <v>0.68102424610675305</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="B9" s="0">
+        <v>0.011699017063997981</v>
+      </c>
+      <c r="C9" s="0">
+        <v>0.010536449576402313</v>
+      </c>
+      <c r="D9" s="0">
+        <v>0.014414244480650894</v>
+      </c>
+      <c r="E9" s="0">
+        <v>0.0099893832545590328</v>
+      </c>
+      <c r="F9" s="0">
+        <v>0.0095382524633601719</v>
+      </c>
+      <c r="G9" s="0">
+        <v>0.0049480485445660988</v>
       </c>
       <c r="H9">
         <v>4.9392865548329125E-3</v>
       </c>
     </row>
-    <row r="10" spans="2:9">
-      <c r="B10">
+    <row r="10">
+      <c r="B10" s="0">
         <v>92.740644490644485</v>
       </c>
-      <c r="C10">
+      <c r="C10" s="0">
         <v>92.156950672645735</v>
       </c>
-      <c r="D10">
-        <v>93.600591715976336</v>
-      </c>
-      <c r="E10">
-        <v>93.670308232539995</v>
-      </c>
-      <c r="F10">
-        <v>93.297094657919402</v>
-      </c>
-      <c r="G10">
-        <v>93.135116394254581</v>
+      <c r="D10" s="0">
+        <v>93.604376108811351</v>
+      </c>
+      <c r="E10" s="0">
+        <v>93.67277691107644</v>
+      </c>
+      <c r="F10" s="0">
+        <v>93.290866510538635</v>
+      </c>
+      <c r="G10" s="0">
+        <v>93.135175282234101</v>
       </c>
       <c r="H10">
         <v>93.139930727362696</v>
       </c>
-      <c r="I10">
-        <v>0.45561209600109898</v>
-      </c>
-    </row>
-    <row r="11" spans="2:9">
-      <c r="B11">
-        <v>0.55282250572746683</v>
-      </c>
-      <c r="C11">
+      <c r="I10" s="0">
+        <v>0.45326860406694858</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="B11" s="0">
+        <v>0.55282250572746672</v>
+      </c>
+      <c r="C11" s="0">
         <v>0.85746436976065976</v>
       </c>
-      <c r="D11">
-        <v>0.59598887248627241</v>
-      </c>
-      <c r="E11">
-        <v>0.47088171102994458</v>
-      </c>
-      <c r="F11">
-        <v>0.5987310012372552</v>
-      </c>
-      <c r="G11">
-        <v>0.27433101628973899</v>
+      <c r="D11" s="0">
+        <v>0.59648670007090754</v>
+      </c>
+      <c r="E11" s="0">
+        <v>0.47058032652713411</v>
+      </c>
+      <c r="F11" s="0">
+        <v>0.59891547015170421</v>
+      </c>
+      <c r="G11" s="0">
+        <v>0.27435415453128736</v>
       </c>
       <c r="H11">
         <v>0.274162592601149</v>
       </c>
     </row>
-    <row r="12" spans="2:9">
-      <c r="B12">
-        <v>0.66059723233794609</v>
-      </c>
-      <c r="C12">
+    <row r="12">
+      <c r="B12" s="0">
+        <v>0.66084425036390104</v>
+      </c>
+      <c r="C12" s="0">
         <v>0.6723372781065089</v>
       </c>
-      <c r="D12">
-        <v>0.64755639097744366</v>
-      </c>
-      <c r="E12">
-        <v>0.66590779738190098</v>
-      </c>
-      <c r="F12">
-        <v>0.64195804195804196</v>
-      </c>
-      <c r="G12">
-        <v>0.65840022935779818</v>
+      <c r="D12" s="0">
+        <v>0.64694835680751173</v>
+      </c>
+      <c r="E12" s="0">
+        <v>0.66609783845278725</v>
+      </c>
+      <c r="F12" s="0">
+        <v>0.64220824598183091</v>
+      </c>
+      <c r="G12" s="0">
+        <v>0.65845272206303729</v>
       </c>
       <c r="H12">
         <v>0.6585575271894677</v>
       </c>
-      <c r="I12">
-        <v>0.73606972985425867</v>
-      </c>
-    </row>
-    <row r="13" spans="2:9">
-      <c r="B13">
-        <v>1.942399743102876E-2</v>
-      </c>
-      <c r="C13">
-        <v>1.889856791539507E-2</v>
-      </c>
-      <c r="D13">
-        <v>2.4224528087916579E-2</v>
-      </c>
-      <c r="E13">
-        <v>1.6421808697529818E-2</v>
-      </c>
-      <c r="F13">
-        <v>1.629924224282735E-2</v>
-      </c>
-      <c r="G13">
-        <v>8.3918174033719081E-3</v>
+      <c r="I12" s="0">
+        <v>0.7337161985642775</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="B13" s="0">
+        <v>0.019264793906698385</v>
+      </c>
+      <c r="C13" s="0">
+        <v>0.018898567915395067</v>
+      </c>
+      <c r="D13" s="0">
+        <v>0.024289475036466855</v>
+      </c>
+      <c r="E13" s="0">
+        <v>0.016413508256461058</v>
+      </c>
+      <c r="F13" s="0">
+        <v>0.016248832152705936</v>
+      </c>
+      <c r="G13" s="0">
+        <v>0.0083777184461360614</v>
       </c>
       <c r="H13">
         <v>8.3888552688200987E-3</v>
       </c>
     </row>
-    <row r="14" spans="2:9">
-      <c r="B14">
+    <row r="14">
+      <c r="B14" s="0">
         <v>0.76893502499038835</v>
       </c>
-      <c r="C14">
+      <c r="C14" s="0">
         <v>0.74738114423851731</v>
       </c>
-      <c r="D14">
-        <v>0.80371229698375868</v>
-      </c>
-      <c r="E14">
-        <v>0.77205240174672485</v>
-      </c>
-      <c r="F14">
-        <v>0.79305354558610708</v>
-      </c>
-      <c r="G14">
-        <v>0.77628935030140656</v>
+      <c r="D14" s="0">
+        <v>0.80380333951762528</v>
+      </c>
+      <c r="E14" s="0">
+        <v>0.77211874272409775</v>
+      </c>
+      <c r="F14" s="0">
+        <v>0.79284164859002171</v>
+      </c>
+      <c r="G14" s="0">
+        <v>0.77628152667212258</v>
       </c>
       <c r="H14">
         <v>0.57324509220701958</v>
       </c>
-      <c r="I14">
-        <v>0.50326097085279187</v>
-      </c>
-    </row>
-    <row r="15" spans="2:9">
-      <c r="B15">
-        <v>1.9892859098745899E-2</v>
-      </c>
-      <c r="C15">
-        <v>2.5623636641152008E-2</v>
-      </c>
-      <c r="D15">
-        <v>2.3867007306229256E-2</v>
-      </c>
-      <c r="E15">
-        <v>2.3659037145027335E-2</v>
-      </c>
-      <c r="F15">
-        <v>2.2444999654912107E-2</v>
-      </c>
-      <c r="G15">
-        <v>1.0492228006191808E-2</v>
+      <c r="I14" s="0">
+        <v>0.50444889849500241</v>
+      </c>
+    </row>
+    <row r="15">
+      <c r="B15" s="0">
+        <v>0.019892859098745903</v>
+      </c>
+      <c r="C15" s="0">
+        <v>0.025623636641152012</v>
+      </c>
+      <c r="D15" s="0">
+        <v>0.023871935695980506</v>
+      </c>
+      <c r="E15" s="0">
+        <v>0.02366116396005109</v>
+      </c>
+      <c r="F15" s="0">
+        <v>0.022472107685513332</v>
+      </c>
+      <c r="G15" s="0">
+        <v>0.010494345328496491</v>
       </c>
       <c r="H15">
         <v>9.4357020529609956E-3</v>
       </c>
     </row>
-    <row r="16" spans="2:9">
-      <c r="B16">
+    <row r="16">
+      <c r="B16" s="0">
         <v>2000</v>
       </c>
-      <c r="C16">
+      <c r="C16" s="0">
         <v>1855</v>
       </c>
-      <c r="D16">
-        <v>1732</v>
-      </c>
-      <c r="E16">
-        <v>2652</v>
-      </c>
-      <c r="F16">
-        <v>2192</v>
+      <c r="D16" s="0">
+        <v>1733</v>
+      </c>
+      <c r="E16" s="0">
+        <v>2653</v>
+      </c>
+      <c r="F16" s="0">
+        <v>2193</v>
       </c>
     </row>
   </sheetData>
@@ -1541,27 +1517,27 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A2:I45"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
+    <sheetView tabSelected="true" topLeftCell="A19" workbookViewId="0">
       <selection activeCell="A2" sqref="A2:I44"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="1" width="28.5546875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="16.109375" style="1" customWidth="1"/>
-    <col min="3" max="3" width="11.109375" style="15" customWidth="1"/>
+    <col min="1" max="1" width="28.5546875" bestFit="true" customWidth="true"/>
+    <col min="2" max="2" width="16.109375" style="1" customWidth="true"/>
+    <col min="3" max="3" width="11.109375" style="15" customWidth="true"/>
     <col min="4" max="4" width="8.88671875" style="1"/>
-    <col min="5" max="5" width="10.5546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="9.5546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="9.5546875" style="15" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="10.5546875" style="15" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="11.6640625" style="15" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="10.5546875" style="1" bestFit="true" customWidth="true"/>
+    <col min="6" max="6" width="9.5546875" style="1" bestFit="true" customWidth="true"/>
+    <col min="7" max="7" width="9.5546875" style="15" bestFit="true" customWidth="true"/>
+    <col min="8" max="8" width="10.5546875" style="15" bestFit="true" customWidth="true"/>
+    <col min="9" max="9" width="11.6640625" style="15" bestFit="true" customWidth="true"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:9">
+    <row r="2">
       <c r="A2" s="4"/>
       <c r="B2" s="10"/>
       <c r="C2" s="18"/>
@@ -1574,7 +1550,7 @@
       <c r="H2" s="20"/>
       <c r="I2" s="12"/>
     </row>
-    <row r="3" spans="1:9" ht="15" thickBot="1">
+    <row r="3" ht="15" thickBot="true">
       <c r="A3" s="2"/>
       <c r="B3" s="11"/>
       <c r="C3" s="17"/>
@@ -1589,7 +1565,7 @@
       <c r="H3" s="19"/>
       <c r="I3" s="13"/>
     </row>
-    <row r="4" spans="1:9" ht="15" thickTop="1">
+    <row r="4" ht="15" thickTop="true">
       <c r="B4" s="1" t="s">
         <v>18</v>
       </c>
@@ -1615,7 +1591,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="5" spans="1:9" ht="15" thickBot="1">
+    <row r="5" ht="15" thickBot="true">
       <c r="A5" s="2"/>
       <c r="B5" s="19" t="s">
         <v>4</v>
@@ -1628,7 +1604,7 @@
       <c r="H5" s="19"/>
       <c r="I5" s="19"/>
     </row>
-    <row r="6" spans="1:9" ht="15" thickTop="1">
+    <row r="6" ht="15" thickTop="true">
       <c r="A6" t="s">
         <v>13</v>
       </c>
@@ -1665,7 +1641,7 @@
         <v>0.32</v>
       </c>
     </row>
-    <row r="7" spans="1:9">
+    <row r="7">
       <c r="B7" s="15" t="str">
         <f>CONCATENATE("(",ROUND(SS_admin!H3,0),")")</f>
         <v>(25)</v>
@@ -1695,7 +1671,7 @@
         <v>(65)</v>
       </c>
     </row>
-    <row r="8" spans="1:9">
+    <row r="8">
       <c r="A8" t="s">
         <v>5</v>
       </c>
@@ -1732,7 +1708,7 @@
         <v>0.96</v>
       </c>
     </row>
-    <row r="9" spans="1:9">
+    <row r="9">
       <c r="B9" s="15" t="str">
         <f>CONCATENATE("(",ROUND(SS_admin!H5,2),")")</f>
         <v>(0.02)</v>
@@ -1762,7 +1738,7 @@
         <v>(0.05)</v>
       </c>
     </row>
-    <row r="10" spans="1:9">
+    <row r="10">
       <c r="A10" t="s">
         <v>21</v>
       </c>
@@ -1799,7 +1775,7 @@
         <v>0.38</v>
       </c>
     </row>
-    <row r="11" spans="1:9">
+    <row r="11">
       <c r="B11" s="15" t="str">
         <f>CONCATENATE("(",ROUND(SS_admin!H7,2),")")</f>
         <v>(0.82)</v>
@@ -1830,7 +1806,7 @@
       </c>
       <c r="I11" s="6"/>
     </row>
-    <row r="12" spans="1:9">
+    <row r="12">
       <c r="A12" s="8" t="s">
         <v>17</v>
       </c>
@@ -1860,7 +1836,7 @@
       </c>
       <c r="I12" s="9"/>
     </row>
-    <row r="13" spans="1:9">
+    <row r="13">
       <c r="A13" s="7" t="s">
         <v>10</v>
       </c>
@@ -1894,7 +1870,7 @@
       </c>
       <c r="I13" s="16"/>
     </row>
-    <row r="14" spans="1:9" ht="15" thickBot="1">
+    <row r="14" ht="15" thickBot="true">
       <c r="A14" s="2"/>
       <c r="B14" s="19" t="s">
         <v>23</v>
@@ -1907,7 +1883,7 @@
       <c r="H14" s="19"/>
       <c r="I14" s="19"/>
     </row>
-    <row r="15" spans="1:9" ht="15" thickTop="1">
+    <row r="15" ht="15" thickTop="true">
       <c r="A15" t="s">
         <v>6</v>
       </c>
@@ -1940,7 +1916,7 @@
         <v>0.41</v>
       </c>
     </row>
-    <row r="16" spans="1:9">
+    <row r="16">
       <c r="B16" s="1" t="str">
         <f>CONCATENATE("(",ROUND(SS_survey!G3,2),")")</f>
         <v>(0.01)</v>
@@ -1966,7 +1942,7 @@
         <v>(0.01)</v>
       </c>
     </row>
-    <row r="17" spans="1:9">
+    <row r="17">
       <c r="A17" t="s">
         <v>7</v>
       </c>
@@ -1999,7 +1975,7 @@
         <v>0.79</v>
       </c>
     </row>
-    <row r="18" spans="1:9">
+    <row r="18">
       <c r="B18" s="1" t="str">
         <f>CONCATENATE("(",ROUND(SS_survey!G5,2),")")</f>
         <v>(0.28)</v>
@@ -2025,7 +2001,7 @@
         <v>(0.52)</v>
       </c>
     </row>
-    <row r="19" spans="1:9">
+    <row r="19">
       <c r="A19" t="s">
         <v>14</v>
       </c>
@@ -2058,7 +2034,7 @@
         <v>0.41</v>
       </c>
     </row>
-    <row r="20" spans="1:9">
+    <row r="20">
       <c r="B20" s="1" t="str">
         <f>CONCATENATE("(",ROUND(SS_survey!G7,0),")")</f>
         <v>(39)</v>
@@ -2084,7 +2060,7 @@
         <v>(100)</v>
       </c>
     </row>
-    <row r="21" spans="1:9">
+    <row r="21">
       <c r="A21" t="s">
         <v>8</v>
       </c>
@@ -2117,7 +2093,7 @@
         <v>0.68</v>
       </c>
     </row>
-    <row r="22" spans="1:9">
+    <row r="22">
       <c r="B22" s="1" t="str">
         <f>CONCATENATE("(",ROUND(SS_survey!G9,2),")")</f>
         <v>(0)</v>
@@ -2143,7 +2119,7 @@
         <v>(0.01)</v>
       </c>
     </row>
-    <row r="23" spans="1:9">
+    <row r="23">
       <c r="A23" t="s">
         <v>15</v>
       </c>
@@ -2176,7 +2152,7 @@
         <v>0.46</v>
       </c>
     </row>
-    <row r="24" spans="1:9">
+    <row r="24">
       <c r="B24" s="1" t="str">
         <f>CONCATENATE("(",ROUND(SS_survey!G11,0),")")</f>
         <v>(0)</v>
@@ -2202,7 +2178,7 @@
         <v>(0.6)</v>
       </c>
     </row>
-    <row r="25" spans="1:9">
+    <row r="25">
       <c r="A25" s="3" t="s">
         <v>9</v>
       </c>
@@ -2235,7 +2211,7 @@
         <v>0.74</v>
       </c>
     </row>
-    <row r="26" spans="1:9">
+    <row r="26">
       <c r="B26" s="1" t="str">
         <f>CONCATENATE("(",ROUND(SS_survey!G13,2),")")</f>
         <v>(0.01)</v>
@@ -2261,7 +2237,7 @@
         <v>(0.02)</v>
       </c>
     </row>
-    <row r="27" spans="1:9">
+    <row r="27">
       <c r="A27" t="s">
         <v>25</v>
       </c>
@@ -2294,7 +2270,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="28" spans="1:9">
+    <row r="28">
       <c r="B28" s="1" t="str">
         <f>CONCATENATE("(",ROUND(SS_survey!G15,2),")")</f>
         <v>(0.01)</v>
@@ -2321,7 +2297,7 @@
       </c>
       <c r="I28" s="6"/>
     </row>
-    <row r="29" spans="1:9" ht="15" thickBot="1">
+    <row r="29" ht="15" thickBot="true">
       <c r="A29" s="2" t="s">
         <v>10</v>
       </c>
@@ -2352,7 +2328,7 @@
       </c>
       <c r="I29" s="13"/>
     </row>
-    <row r="30" spans="1:9" ht="15.6" thickTop="1" thickBot="1">
+    <row r="30" ht="15.6" thickTop="true" thickBot="true">
       <c r="A30" s="2"/>
       <c r="B30" s="19" t="s">
         <v>24</v>
@@ -2365,7 +2341,7 @@
       <c r="H30" s="19"/>
       <c r="I30" s="19"/>
     </row>
-    <row r="31" spans="1:9" ht="15" thickTop="1">
+    <row r="31" ht="15" thickTop="true">
       <c r="A31" t="s">
         <v>6</v>
       </c>
@@ -2402,7 +2378,7 @@
         <v>0.32</v>
       </c>
     </row>
-    <row r="32" spans="1:9">
+    <row r="32">
       <c r="B32" s="15" t="str">
         <f>CONCATENATE("(",ROUND(SS_survey_uncond!H3,2),")")</f>
         <v>(0.01)</v>
@@ -2432,7 +2408,7 @@
         <v>(0.01)</v>
       </c>
     </row>
-    <row r="33" spans="1:9">
+    <row r="33">
       <c r="A33" t="s">
         <v>7</v>
       </c>
@@ -2469,7 +2445,7 @@
         <v>0.79</v>
       </c>
     </row>
-    <row r="34" spans="1:9">
+    <row r="34">
       <c r="B34" s="15" t="str">
         <f>CONCATENATE("(",ROUND(SS_survey_uncond!H5,2),")")</f>
         <v>(0.21)</v>
@@ -2499,7 +2475,7 @@
         <v>(0.51)</v>
       </c>
     </row>
-    <row r="35" spans="1:9">
+    <row r="35">
       <c r="A35" t="s">
         <v>14</v>
       </c>
@@ -2536,7 +2512,7 @@
         <v>0.41</v>
       </c>
     </row>
-    <row r="36" spans="1:9">
+    <row r="36">
       <c r="B36" s="15" t="str">
         <f>CONCATENATE("(",ROUND(SS_survey_uncond!H7,0),")")</f>
         <v>(36)</v>
@@ -2566,7 +2542,7 @@
         <v>(99)</v>
       </c>
     </row>
-    <row r="37" spans="1:9">
+    <row r="37">
       <c r="A37" t="s">
         <v>8</v>
       </c>
@@ -2603,7 +2579,7 @@
         <v>0.56000000000000005</v>
       </c>
     </row>
-    <row r="38" spans="1:9">
+    <row r="38">
       <c r="B38" s="15" t="str">
         <f>CONCATENATE("(",ROUND(SS_survey_uncond!H9,2),")")</f>
         <v>(0.01)</v>
@@ -2633,7 +2609,7 @@
         <v>(0.01)</v>
       </c>
     </row>
-    <row r="39" spans="1:9">
+    <row r="39">
       <c r="A39" t="s">
         <v>15</v>
       </c>
@@ -2670,7 +2646,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="40" spans="1:9">
+    <row r="40">
       <c r="B40" s="15" t="str">
         <f>CONCATENATE("(",ROUND(SS_survey_uncond!H11,2),")")</f>
         <v>(0.2)</v>
@@ -2700,7 +2676,7 @@
         <v>(0.59)</v>
       </c>
     </row>
-    <row r="41" spans="1:9">
+    <row r="41">
       <c r="A41" t="s">
         <v>9</v>
       </c>
@@ -2737,7 +2713,7 @@
         <v>0.01</v>
       </c>
     </row>
-    <row r="42" spans="1:9">
+    <row r="42">
       <c r="B42" s="15" t="str">
         <f>CONCATENATE("(",ROUND(SS_survey_uncond!H13,2),")")</f>
         <v>(0.01)</v>
@@ -2767,7 +2743,7 @@
         <v>(0.02)</v>
       </c>
     </row>
-    <row r="43" spans="1:9">
+    <row r="43">
       <c r="A43" t="s">
         <v>22</v>
       </c>
@@ -2798,7 +2774,7 @@
         <v>0.25</v>
       </c>
     </row>
-    <row r="44" spans="1:9" ht="15" thickBot="1">
+    <row r="44" ht="15" thickBot="true">
       <c r="A44" s="2" t="s">
         <v>10</v>
       </c>
@@ -2832,7 +2808,7 @@
       </c>
       <c r="I44" s="13"/>
     </row>
-    <row r="45" spans="1:9" ht="15" thickTop="1"/>
+    <row r="45" ht="15" thickTop="true"/>
   </sheetData>
   <mergeCells count="6">
     <mergeCell ref="B30:I30"/>

</xml_diff>

<commit_message>
annualize apr and effects in std deviations
</commit_message>
<xml_diff>
--- a/Tables/SS.xlsx
+++ b/Tables/SS.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24729"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24827"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\isaac\Dropbox\Apps\ShareLaTeX\Donde2020\Tables\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FED9AAB8-5282-4045-819A-23CCF6D26ED1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0E64E179-18A2-43A0-9DA4-2410346A3E09}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-10695" windowWidth="29040" windowHeight="15720" firstSheet="1" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-28920" yWindow="-10695" windowWidth="29040" windowHeight="15720" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="SS_admin" sheetId="1" r:id="rId1"/>
@@ -29,6 +29,7 @@
         <xcalcf:feature name="microsoft.com:FV"/>
         <xcalcf:feature name="microsoft.com:CNMTM"/>
         <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -36,12 +37,9 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="22">
   <si>
     <t>Choice</t>
-  </si>
-  <si>
-    <t>Overall</t>
   </si>
   <si>
     <t>Control</t>
@@ -54,9 +52,6 @@
   </si>
   <si>
     <t xml:space="preserve">Loan amount </t>
-  </si>
-  <si>
-    <t>Monday</t>
   </si>
   <si>
     <t>Obs</t>
@@ -80,28 +75,10 @@
     <t>+High-school</t>
   </si>
   <si>
-    <t>Forced-fee</t>
-  </si>
-  <si>
-    <t>Promise arms</t>
-  </si>
-  <si>
-    <t>Fee arms</t>
-  </si>
-  <si>
     <t>Forced</t>
   </si>
   <si>
     <t xml:space="preserve">Choice </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Panel A : Admin Data </t>
-  </si>
-  <si>
-    <t>Panel B : Survey Data (unconditional)</t>
-  </si>
-  <si>
-    <t>Panel C : Survey Data (conditional on pawning)</t>
   </si>
   <si>
     <t>% ended up pawning</t>
@@ -113,16 +90,19 @@
     <t>Survey response rate</t>
   </si>
   <si>
-    <t>Number of branch-days</t>
+    <t>Weekday</t>
   </si>
   <si>
-    <t>-</t>
+    <t>Soft arms</t>
   </si>
   <si>
-    <t>Attrition Table</t>
+    <t>Commitment arms</t>
   </si>
   <si>
-    <t>Pre-exp</t>
+    <t>Panel C : Survey Data (conditional on pawning)</t>
+  </si>
+  <si>
+    <t>Panel B : Survey Data (unconditional)</t>
   </si>
 </sst>
 </file>
@@ -143,7 +123,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="7">
+  <borders count="8">
     <border>
       <left/>
       <right/>
@@ -213,11 +193,22 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="double">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="18">
+  <cellXfs count="19">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
@@ -248,16 +239,19 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -574,15 +568,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="B2:K6"/>
+  <dimension ref="B2:M6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="J6" sqref="J5:K6"/>
+      <selection activeCell="J5" sqref="J2:J5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData>
-    <row r="2" spans="2:11" x14ac:dyDescent="0.35">
+    <row r="2" spans="2:13" x14ac:dyDescent="0.35">
       <c r="B2">
         <v>2288.9361702127658</v>
       </c>
@@ -596,97 +590,103 @@
         <v>2179.709923664122</v>
       </c>
       <c r="F2">
-        <v>2089.8602540834845</v>
+        <v>2089.8928441699964</v>
       </c>
       <c r="G2">
-        <v>1956.8888888888889</v>
+        <v>2024.022346368715</v>
       </c>
       <c r="H2">
-        <v>2163.4174671198462</v>
-      </c>
-      <c r="J2">
-        <v>0.37524819828929151</v>
+        <v>2164.3383341955509</v>
       </c>
       <c r="K2">
-        <v>0.14781668620652361</v>
-      </c>
-    </row>
-    <row r="3" spans="2:11" x14ac:dyDescent="0.35">
+        <v>0.31380642461500552</v>
+      </c>
+      <c r="L2">
+        <v>0.32029811665546248</v>
+      </c>
+      <c r="M2">
+        <v>0.13737619175017129</v>
+      </c>
+    </row>
+    <row r="3" spans="2:13" x14ac:dyDescent="0.35">
       <c r="B3">
         <v>78.79053698585561</v>
       </c>
       <c r="C3">
-        <v>72.608792900438658</v>
+        <v>72.608792900438672</v>
       </c>
       <c r="D3">
-        <v>73.768907168664796</v>
+        <v>73.768907168664811</v>
       </c>
       <c r="E3">
         <v>66.211707129485063</v>
       </c>
       <c r="F3">
-        <v>64.845886968919075</v>
+        <v>64.891311599127775</v>
       </c>
       <c r="G3">
-        <v>141.12629526755791</v>
+        <v>137.64917255699254</v>
       </c>
       <c r="H3">
-        <v>31.583174346858844</v>
-      </c>
-    </row>
-    <row r="4" spans="2:11" x14ac:dyDescent="0.35">
+        <v>31.579556901935923</v>
+      </c>
+    </row>
+    <row r="4" spans="2:13" x14ac:dyDescent="0.35">
       <c r="B4">
-        <v>0.18143133462282399</v>
+        <v>0.87814313346228234</v>
       </c>
       <c r="C4">
-        <v>0.15618661257606492</v>
+        <v>0.8908722109533469</v>
       </c>
       <c r="D4">
-        <v>0.17172188520765283</v>
+        <v>0.88520765282314517</v>
       </c>
       <c r="E4">
-        <v>0.18408690546095127</v>
+        <v>0.8476218438050499</v>
       </c>
       <c r="F4">
-        <v>0.21125226860254084</v>
+        <v>0.82891391209589538</v>
       </c>
       <c r="G4">
-        <v>0.16666666335529751</v>
+        <v>0.83333331677648759</v>
       </c>
       <c r="H4">
-        <v>0.18183833304299937</v>
-      </c>
-      <c r="J4">
-        <v>0.96459481357959076</v>
+        <v>0.86328702313181849</v>
       </c>
       <c r="K4">
-        <v>0.69840875173302863</v>
-      </c>
-    </row>
-    <row r="5" spans="2:11" x14ac:dyDescent="0.35">
+        <v>0.51794407065163461</v>
+      </c>
+      <c r="L4">
+        <v>0.71839367357685091</v>
+      </c>
+      <c r="M4">
+        <v>0.62258453328249541</v>
+      </c>
+    </row>
+    <row r="5" spans="2:13" x14ac:dyDescent="0.35">
       <c r="B5">
-        <v>4.6478642296877162E-2</v>
+        <v>4.0033960932364658E-2</v>
       </c>
       <c r="C5">
-        <v>5.0274154878399223E-2</v>
+        <v>3.3821563907464283E-2</v>
       </c>
       <c r="D5">
-        <v>6.2992353579937002E-2</v>
+        <v>3.5723933418048991E-2</v>
       </c>
       <c r="E5">
-        <v>5.4533212144107591E-2</v>
+        <v>4.1755107742770553E-2</v>
       </c>
       <c r="F5">
-        <v>5.4240873797511281E-2</v>
+        <v>4.8523915015899789E-2</v>
       </c>
       <c r="G5">
-        <v>3.1515123504987114E-2</v>
+        <v>4.3154986380046355E-2</v>
       </c>
       <c r="H5">
-        <v>2.3844304999395653E-2</v>
-      </c>
-    </row>
-    <row r="6" spans="2:11" x14ac:dyDescent="0.35">
+        <v>1.8385912471474301E-2</v>
+      </c>
+    </row>
+    <row r="6" spans="2:13" x14ac:dyDescent="0.35">
       <c r="B6">
         <v>2585</v>
       </c>
@@ -700,13 +700,13 @@
         <v>3406</v>
       </c>
       <c r="F6">
-        <v>2755</v>
+        <v>2753</v>
       </c>
       <c r="G6">
         <v>180</v>
       </c>
       <c r="H6">
-        <v>13534</v>
+        <v>13532</v>
       </c>
     </row>
   </sheetData>
@@ -716,15 +716,15 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="B2:K11"/>
+  <dimension ref="B2:M11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="I30" sqref="I30"/>
+      <selection activeCell="J1" sqref="J1:J13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData>
-    <row r="2" spans="2:11" x14ac:dyDescent="0.35">
+    <row r="2" spans="2:13" x14ac:dyDescent="0.35">
       <c r="B2">
         <v>30.773809523809526</v>
       </c>
@@ -738,22 +738,25 @@
         <v>36.623655913978496</v>
       </c>
       <c r="F2">
-        <v>33.597560975609753</v>
+        <v>33.573170731707314</v>
       </c>
       <c r="G2">
         <v>36.085999441146853</v>
       </c>
       <c r="H2">
-        <v>33.815127596944521</v>
-      </c>
-      <c r="J2">
-        <v>0.37832004849353312</v>
+        <v>33.811720441918965</v>
       </c>
       <c r="K2">
-        <v>0.70675873767503816</v>
-      </c>
-    </row>
-    <row r="3" spans="2:11" x14ac:dyDescent="0.35">
+        <v>0.7062867593846045</v>
+      </c>
+      <c r="L2">
+        <v>0.1619408349718037</v>
+      </c>
+      <c r="M2">
+        <v>0.569666506831908</v>
+      </c>
+    </row>
+    <row r="3" spans="2:13" x14ac:dyDescent="0.35">
       <c r="B3">
         <v>2.191515427974172</v>
       </c>
@@ -767,16 +770,16 @@
         <v>2.6016462754055563</v>
       </c>
       <c r="F3">
-        <v>1.7495953639049344</v>
+        <v>1.7423667125082001</v>
       </c>
       <c r="G3">
         <v>1.2515869857807669</v>
       </c>
       <c r="H3">
-        <v>0.80825071336603993</v>
-      </c>
-    </row>
-    <row r="4" spans="2:11" x14ac:dyDescent="0.35">
+        <v>0.80795077985236741</v>
+      </c>
+    </row>
+    <row r="4" spans="2:13" x14ac:dyDescent="0.35">
       <c r="B4">
         <v>84</v>
       </c>
@@ -796,10 +799,10 @@
         <v>180</v>
       </c>
       <c r="H4">
-        <v>83.872617112457519</v>
-      </c>
-    </row>
-    <row r="5" spans="2:11" x14ac:dyDescent="0.35">
+        <v>83.872893881170555</v>
+      </c>
+    </row>
+    <row r="5" spans="2:13" x14ac:dyDescent="0.35">
       <c r="B5">
         <v>0</v>
       </c>
@@ -819,10 +822,10 @@
         <v>0</v>
       </c>
       <c r="H5">
-        <v>0.48131786912369195</v>
-      </c>
-    </row>
-    <row r="6" spans="2:11" x14ac:dyDescent="0.35">
+        <v>0.48138428798549088</v>
+      </c>
+    </row>
+    <row r="6" spans="2:13" x14ac:dyDescent="0.35">
       <c r="B6">
         <v>2585</v>
       </c>
@@ -836,16 +839,16 @@
         <v>3406</v>
       </c>
       <c r="F6">
-        <v>2755</v>
+        <v>2753</v>
       </c>
       <c r="G6">
         <v>180</v>
       </c>
       <c r="H6">
-        <v>13534</v>
-      </c>
-    </row>
-    <row r="8" spans="2:11" x14ac:dyDescent="0.35">
+        <v>13532</v>
+      </c>
+    </row>
+    <row r="8" spans="2:13" x14ac:dyDescent="0.35">
       <c r="B8">
         <v>0.97445972495088407</v>
       </c>
@@ -859,18 +862,21 @@
         <v>0.97195571955719562</v>
       </c>
       <c r="F8">
-        <v>0.98646209386281591</v>
+        <v>0.98601083032490977</v>
       </c>
       <c r="G8">
-        <v>0.97571993224167142</v>
-      </c>
-      <c r="J8">
-        <v>2.9149548766551899E-2</v>
-      </c>
-    </row>
-    <row r="9" spans="2:11" x14ac:dyDescent="0.35">
+        <v>0.9756258234519104</v>
+      </c>
+      <c r="L8">
+        <v>0.58825046706800044</v>
+      </c>
+      <c r="M8">
+        <v>0.11110410557859279</v>
+      </c>
+    </row>
+    <row r="9" spans="2:13" x14ac:dyDescent="0.35">
       <c r="B9">
-        <v>4.4833017561553548E-3</v>
+        <v>4.4833017561553556E-3</v>
       </c>
       <c r="C9">
         <v>8.2133083066849039E-3</v>
@@ -882,13 +888,13 @@
         <v>6.3019449093397522E-3</v>
       </c>
       <c r="F9">
-        <v>3.1384517284954731E-3</v>
+        <v>3.1940620474848742E-3</v>
       </c>
       <c r="G9">
-        <v>2.5459453489787131E-3</v>
-      </c>
-    </row>
-    <row r="10" spans="2:11" x14ac:dyDescent="0.35">
+        <v>2.5465995142291463E-3</v>
+      </c>
+    </row>
+    <row r="10" spans="2:13" x14ac:dyDescent="0.35">
       <c r="B10">
         <v>0.76750483558994198</v>
       </c>
@@ -902,16 +908,19 @@
         <v>0.77334116265413977</v>
       </c>
       <c r="F10">
-        <v>0.7940428623320015</v>
+        <v>0.79425663395129042</v>
       </c>
       <c r="G10">
-        <v>0.77668739231403106</v>
-      </c>
-      <c r="J10">
-        <v>0.4615032323086109</v>
-      </c>
-    </row>
-    <row r="11" spans="2:11" x14ac:dyDescent="0.35">
+        <v>0.77672885292575111</v>
+      </c>
+      <c r="L10">
+        <v>0.72661768802378535</v>
+      </c>
+      <c r="M10">
+        <v>0.44259059431665793</v>
+      </c>
+    </row>
+    <row r="11" spans="2:13" x14ac:dyDescent="0.35">
       <c r="B11">
         <v>2.0014887892783387E-2</v>
       </c>
@@ -919,16 +928,16 @@
         <v>2.5519225148308459E-2</v>
       </c>
       <c r="D11">
-        <v>2.3819765376005244E-2</v>
+        <v>2.3819765376005251E-2</v>
       </c>
       <c r="E11">
         <v>2.3224560628884606E-2</v>
       </c>
       <c r="F11">
-        <v>2.2198381032225181E-2</v>
+        <v>2.2172410929511183E-2</v>
       </c>
       <c r="G11">
-        <v>1.0398557985163693E-2</v>
+        <v>1.0397246226653783E-2</v>
       </c>
     </row>
   </sheetData>
@@ -938,15 +947,15 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
-  <dimension ref="B2:K16"/>
+  <dimension ref="B2:M16"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G12" sqref="G12"/>
+      <selection activeCell="J2" sqref="J2:J12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData>
-    <row r="2" spans="2:11" x14ac:dyDescent="0.35">
+    <row r="2" spans="2:13" x14ac:dyDescent="0.35">
       <c r="B2">
         <v>0.75433911882510019</v>
       </c>
@@ -960,22 +969,25 @@
         <v>0.71756487025948101</v>
       </c>
       <c r="F2">
-        <v>0.74023558586484806</v>
+        <v>0.74007444168734493</v>
       </c>
       <c r="G2">
         <v>0.74980252764612954</v>
       </c>
       <c r="H2">
-        <v>0.73863636363636365</v>
-      </c>
-      <c r="J2">
-        <v>0.44562045380002219</v>
+        <v>0.73861601930411769</v>
       </c>
       <c r="K2">
-        <v>0.11273018398748461</v>
-      </c>
-    </row>
-    <row r="3" spans="2:11" x14ac:dyDescent="0.35">
+        <v>0.11208209991636051</v>
+      </c>
+      <c r="L2">
+        <v>0.21626044184189269</v>
+      </c>
+      <c r="M2">
+        <v>0.52326338075561829</v>
+      </c>
+    </row>
+    <row r="3" spans="2:13" x14ac:dyDescent="0.35">
       <c r="B3">
         <v>1.6556851714845944E-2</v>
       </c>
@@ -986,19 +998,19 @@
         <v>2.0329367912066382E-2</v>
       </c>
       <c r="E3">
-        <v>1.5034947849718415E-2</v>
+        <v>1.5034947849718417E-2</v>
       </c>
       <c r="F3">
-        <v>1.2956526600607638E-2</v>
+        <v>1.2972552271708279E-2</v>
       </c>
       <c r="G3">
         <v>9.0149695175873682E-3</v>
       </c>
       <c r="H3">
-        <v>5.7018049226398486E-3</v>
-      </c>
-    </row>
-    <row r="4" spans="2:11" x14ac:dyDescent="0.35">
+        <v>5.7025026346927427E-3</v>
+      </c>
+    </row>
+    <row r="4" spans="2:13" x14ac:dyDescent="0.35">
       <c r="B4">
         <v>43.221586847748391</v>
       </c>
@@ -1012,27 +1024,30 @@
         <v>44.037746170678339</v>
       </c>
       <c r="F4">
-        <v>43.117182356813693</v>
+        <v>43.103425559947297</v>
       </c>
       <c r="G4">
         <v>43.05681818181818</v>
       </c>
       <c r="H4">
-        <v>43.244609727561425</v>
-      </c>
-      <c r="J4">
-        <v>0.83232729796463201</v>
+        <v>43.242875052235689</v>
       </c>
       <c r="K4">
-        <v>0.46096032999624409</v>
-      </c>
-    </row>
-    <row r="5" spans="2:11" x14ac:dyDescent="0.35">
+        <v>0.46505187451014002</v>
+      </c>
+      <c r="L4">
+        <v>0.55078041441066639</v>
+      </c>
+      <c r="M4">
+        <v>0.96669904994360278</v>
+      </c>
+    </row>
+    <row r="5" spans="2:13" x14ac:dyDescent="0.35">
       <c r="B5">
-        <v>0.56543539980823887</v>
+        <v>0.56543539980823898</v>
       </c>
       <c r="C5">
-        <v>0.76286676286261634</v>
+        <v>0.76286676286261612</v>
       </c>
       <c r="D5">
         <v>0.64748270122917573</v>
@@ -1041,16 +1056,16 @@
         <v>0.6071316707886486</v>
       </c>
       <c r="F5">
-        <v>0.52007372086135961</v>
+        <v>0.51886206376869348</v>
       </c>
       <c r="G5">
         <v>0.31582069920051542</v>
       </c>
       <c r="H5">
-        <v>0.21111281879575414</v>
-      </c>
-    </row>
-    <row r="6" spans="2:11" x14ac:dyDescent="0.35">
+        <v>0.21108025671162237</v>
+      </c>
+    </row>
+    <row r="6" spans="2:13" x14ac:dyDescent="0.35">
       <c r="B6">
         <v>3144.2258572273172</v>
       </c>
@@ -1072,16 +1087,19 @@
       <c r="H6">
         <v>3111.1842893999233</v>
       </c>
-      <c r="J6">
-        <v>0.42348542902362862</v>
-      </c>
       <c r="K6">
         <v>0.15227626931075919</v>
       </c>
-    </row>
-    <row r="7" spans="2:11" x14ac:dyDescent="0.35">
+      <c r="L6">
+        <v>0.30747604910588372</v>
+      </c>
+      <c r="M6">
+        <v>0.43244773970978462</v>
+      </c>
+    </row>
+    <row r="7" spans="2:13" x14ac:dyDescent="0.35">
       <c r="B7">
-        <v>68.001187760083482</v>
+        <v>68.001187760083468</v>
       </c>
       <c r="C7">
         <v>87.087553008590618</v>
@@ -1090,19 +1108,19 @@
         <v>76.712679194050935</v>
       </c>
       <c r="E7">
-        <v>84.619693541464585</v>
+        <v>84.619693541464599</v>
       </c>
       <c r="F7">
-        <v>99.097081529762733</v>
+        <v>99.097081529762747</v>
       </c>
       <c r="G7">
         <v>75.187908028614046</v>
       </c>
       <c r="H7">
-        <v>35.717284716677213</v>
-      </c>
-    </row>
-    <row r="8" spans="2:11" x14ac:dyDescent="0.35">
+        <v>35.717284716677206</v>
+      </c>
+    </row>
+    <row r="8" spans="2:13" x14ac:dyDescent="0.35">
       <c r="B8">
         <v>0.89210155148095904</v>
       </c>
@@ -1116,24 +1134,27 @@
         <v>0.91017316017316019</v>
       </c>
       <c r="F8">
-        <v>0.89459639759839893</v>
+        <v>0.89452603471295056</v>
       </c>
       <c r="G8">
         <v>0.88422131147540983</v>
       </c>
       <c r="H8">
-        <v>0.89282186368126437</v>
-      </c>
-      <c r="J8">
-        <v>0.74243815509172728</v>
+        <v>0.8928130402568536</v>
       </c>
       <c r="K8">
-        <v>0.21611770313985521</v>
-      </c>
-    </row>
-    <row r="9" spans="2:11" x14ac:dyDescent="0.35">
+        <v>0.2165470378557727</v>
+      </c>
+      <c r="L8">
+        <v>0.46842009181914179</v>
+      </c>
+      <c r="M8">
+        <v>0.98594182922713058</v>
+      </c>
+    </row>
+    <row r="9" spans="2:13" x14ac:dyDescent="0.35">
       <c r="B9">
-        <v>1.143781280019596E-2</v>
+        <v>1.1437812800195962E-2</v>
       </c>
       <c r="C9">
         <v>1.0521714206780004E-2</v>
@@ -1145,16 +1166,16 @@
         <v>9.955349958628441E-3</v>
       </c>
       <c r="F9">
-        <v>9.4612818679783769E-3</v>
+        <v>9.4444603824305161E-3</v>
       </c>
       <c r="G9">
         <v>1.0533724370448033E-2</v>
       </c>
       <c r="H9">
-        <v>5.2015714238519009E-3</v>
-      </c>
-    </row>
-    <row r="10" spans="2:11" x14ac:dyDescent="0.35">
+        <v>5.201314800898328E-3</v>
+      </c>
+    </row>
+    <row r="10" spans="2:13" x14ac:dyDescent="0.35">
       <c r="B10">
         <v>92.746680286006125</v>
       </c>
@@ -1176,16 +1197,19 @@
       <c r="H10">
         <v>92.642189978264696</v>
       </c>
-      <c r="J10">
-        <v>0.46460779492661669</v>
-      </c>
       <c r="K10">
-        <v>1.1531094878537E-3</v>
-      </c>
-    </row>
-    <row r="11" spans="2:11" x14ac:dyDescent="0.35">
+        <v>1.1531094878537999E-3</v>
+      </c>
+      <c r="L10">
+        <v>0.18126873036276731</v>
+      </c>
+      <c r="M10">
+        <v>0.5015072314659057</v>
+      </c>
+    </row>
+    <row r="11" spans="2:13" x14ac:dyDescent="0.35">
       <c r="B11">
-        <v>0.53706935836467429</v>
+        <v>0.53706935836467462</v>
       </c>
       <c r="C11">
         <v>0.83856879215694513</v>
@@ -1197,16 +1221,16 @@
         <v>0.45528703025952877</v>
       </c>
       <c r="F11">
-        <v>0.59572969114264707</v>
+        <v>0.59572969114264696</v>
       </c>
       <c r="G11">
-        <v>0.30818777366122263</v>
+        <v>0.30818777366122274</v>
       </c>
       <c r="H11">
         <v>0.20468275029985156</v>
       </c>
     </row>
-    <row r="12" spans="2:11" x14ac:dyDescent="0.35">
+    <row r="12" spans="2:13" x14ac:dyDescent="0.35">
       <c r="B12">
         <v>0.65825522710886808</v>
       </c>
@@ -1220,22 +1244,25 @@
         <v>0.66255605381165916</v>
       </c>
       <c r="F12">
-        <v>0.6428571428571429</v>
+        <v>0.6426092990978487</v>
       </c>
       <c r="G12">
         <v>0.59694943585457583</v>
       </c>
       <c r="H12">
-        <v>0.63253418875569811</v>
-      </c>
-      <c r="J12">
-        <v>0.72062082027172925</v>
+        <v>0.63250316589278177</v>
       </c>
       <c r="K12">
-        <v>1.2602705766639999E-4</v>
-      </c>
-    </row>
-    <row r="13" spans="2:11" x14ac:dyDescent="0.35">
+        <v>1.2796812933239999E-4</v>
+      </c>
+      <c r="L12">
+        <v>0.92123910783208673</v>
+      </c>
+      <c r="M12">
+        <v>0.82777141801359311</v>
+      </c>
+    </row>
+    <row r="13" spans="2:13" x14ac:dyDescent="0.35">
       <c r="B13">
         <v>1.9575506710528847E-2</v>
       </c>
@@ -1243,22 +1270,22 @@
         <v>1.9664178070939481E-2</v>
       </c>
       <c r="D13">
-        <v>2.3651650315642415E-2</v>
+        <v>2.3651650315642418E-2</v>
       </c>
       <c r="E13">
-        <v>1.6910104498970225E-2</v>
+        <v>1.6910104498970228E-2</v>
       </c>
       <c r="F13">
-        <v>1.6714497693811701E-2</v>
+        <v>1.6764309126234812E-2</v>
       </c>
       <c r="G13">
         <v>1.2957951584969644E-2</v>
       </c>
       <c r="H13">
-        <v>7.4947166879319026E-3</v>
-      </c>
-    </row>
-    <row r="14" spans="2:11" x14ac:dyDescent="0.35">
+        <v>7.4963906102697275E-3</v>
+      </c>
+    </row>
+    <row r="14" spans="2:13" x14ac:dyDescent="0.35">
       <c r="B14">
         <v>2637</v>
       </c>
@@ -1272,30 +1299,30 @@
         <v>3482</v>
       </c>
       <c r="F14">
-        <v>2783</v>
+        <v>2782</v>
       </c>
       <c r="G14">
         <v>6919</v>
       </c>
       <c r="H14">
-        <v>20526</v>
-      </c>
-    </row>
-    <row r="16" spans="2:11" x14ac:dyDescent="0.35">
+        <v>20525</v>
+      </c>
+    </row>
+    <row r="16" spans="2:13" x14ac:dyDescent="0.35">
       <c r="B16">
         <v>2036</v>
       </c>
       <c r="C16">
-        <v>1840</v>
+        <v>1907</v>
       </c>
       <c r="D16">
-        <v>1724</v>
+        <v>1757</v>
       </c>
       <c r="E16">
-        <v>2634</v>
+        <v>2710</v>
       </c>
       <c r="F16">
-        <v>2186</v>
+        <v>2216</v>
       </c>
       <c r="G16">
         <v>6919</v>
@@ -1308,15 +1335,15 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
-  <dimension ref="B2:J16"/>
+  <dimension ref="B2:K16"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="K14" sqref="K2:K14"/>
+      <selection activeCell="O6" sqref="O6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData>
-    <row r="2" spans="2:10" x14ac:dyDescent="0.35">
+    <row r="2" spans="2:11" x14ac:dyDescent="0.35">
       <c r="B2">
         <v>0.75578231292517006</v>
       </c>
@@ -1330,18 +1357,21 @@
         <v>0.7164790174002047</v>
       </c>
       <c r="F2">
-        <v>0.74043887147335419</v>
+        <v>0.740276035131744</v>
       </c>
       <c r="G2">
-        <v>0.73188310837373871</v>
+        <v>0.73184796854521628</v>
       </c>
       <c r="J2">
-        <v>0.44562045380002219</v>
-      </c>
-    </row>
-    <row r="3" spans="2:10" x14ac:dyDescent="0.35">
+        <v>0.19876896641301439</v>
+      </c>
+      <c r="K2">
+        <v>0.49195240167249149</v>
+      </c>
+    </row>
+    <row r="3" spans="2:11" x14ac:dyDescent="0.35">
       <c r="B3">
-        <v>1.6494973868034873E-2</v>
+        <v>1.6494973868034876E-2</v>
       </c>
       <c r="C3">
         <v>1.7691100137449553E-2</v>
@@ -1350,16 +1380,16 @@
         <v>2.0783334672938653E-2</v>
       </c>
       <c r="E3">
-        <v>1.5767935213445723E-2</v>
+        <v>1.576793521344572E-2</v>
       </c>
       <c r="F3">
-        <v>1.3112141500137104E-2</v>
+        <v>1.3130695539826494E-2</v>
       </c>
       <c r="G3">
-        <v>7.5274894891986738E-3</v>
-      </c>
-    </row>
-    <row r="4" spans="2:10" x14ac:dyDescent="0.35">
+        <v>7.5289195119028051E-3</v>
+      </c>
+    </row>
+    <row r="4" spans="2:11" x14ac:dyDescent="0.35">
       <c r="B4">
         <v>43.217612809315867</v>
       </c>
@@ -1373,21 +1403,24 @@
         <v>43.905829596412559</v>
       </c>
       <c r="F4">
-        <v>43.095269820119917</v>
+        <v>43.081333333333333</v>
       </c>
       <c r="G4">
-        <v>43.309204015269337</v>
+        <v>43.306278280542983</v>
       </c>
       <c r="J4">
-        <v>0.83232729796463167</v>
-      </c>
-    </row>
-    <row r="5" spans="2:10" x14ac:dyDescent="0.35">
+        <v>0.64268457005413904</v>
+      </c>
+      <c r="K4">
+        <v>0.95371567366848975</v>
+      </c>
+    </row>
+    <row r="5" spans="2:11" x14ac:dyDescent="0.35">
       <c r="B5">
         <v>0.57228204463326615</v>
       </c>
       <c r="C5">
-        <v>0.77802775203513097</v>
+        <v>0.77802775203513075</v>
       </c>
       <c r="D5">
         <v>0.63847586117189081</v>
@@ -1396,13 +1429,13 @@
         <v>0.61729446550591693</v>
       </c>
       <c r="F5">
-        <v>0.52009580821400614</v>
+        <v>0.51915566425229054</v>
       </c>
       <c r="G5">
-        <v>0.28251508807132936</v>
-      </c>
-    </row>
-    <row r="6" spans="2:10" x14ac:dyDescent="0.35">
+        <v>0.28248392615092249</v>
+      </c>
+    </row>
+    <row r="6" spans="2:11" x14ac:dyDescent="0.35">
       <c r="B6">
         <v>3141.2189276129911</v>
       </c>
@@ -1416,36 +1449,39 @@
         <v>3107.1898911642975</v>
       </c>
       <c r="F6">
-        <v>3078.6470657561767</v>
+        <v>3077.652576659777</v>
       </c>
       <c r="G6">
-        <v>3062.4216133308619</v>
+        <v>3062.2107548711087</v>
       </c>
       <c r="J6">
-        <v>0.42348542902362901</v>
-      </c>
-    </row>
-    <row r="7" spans="2:10" x14ac:dyDescent="0.35">
+        <v>0.29045103565750929</v>
+      </c>
+      <c r="K6">
+        <v>0.29728566162528908</v>
+      </c>
+    </row>
+    <row r="7" spans="2:11" x14ac:dyDescent="0.35">
       <c r="B7">
-        <v>68.414710468808906</v>
+        <v>68.41471046880892</v>
       </c>
       <c r="C7">
-        <v>88.438762370272073</v>
+        <v>88.438762370272087</v>
       </c>
       <c r="D7">
-        <v>76.543605627057033</v>
+        <v>76.543605627057048</v>
       </c>
       <c r="E7">
-        <v>84.797934069022133</v>
+        <v>84.797934069022119</v>
       </c>
       <c r="F7">
-        <v>98.844746917276694</v>
+        <v>98.948225748151543</v>
       </c>
       <c r="G7">
-        <v>38.465540458328547</v>
-      </c>
-    </row>
-    <row r="8" spans="2:10" x14ac:dyDescent="0.35">
+        <v>38.475753401046958</v>
+      </c>
+    </row>
+    <row r="8" spans="2:11" x14ac:dyDescent="0.35">
       <c r="B8">
         <v>0.89280575539568341</v>
       </c>
@@ -1459,16 +1495,19 @@
         <v>0.91004997223764572</v>
       </c>
       <c r="F8">
-        <v>0.89406207827260464</v>
+        <v>0.89399054692775148</v>
       </c>
       <c r="G8">
-        <v>0.89848357203032858</v>
+        <v>0.89846931610728831</v>
       </c>
       <c r="J8">
-        <v>0.74243815509172717</v>
-      </c>
-    </row>
-    <row r="9" spans="2:10" x14ac:dyDescent="0.35">
+        <v>0.47512184769960331</v>
+      </c>
+      <c r="K8">
+        <v>0.99580107322835887</v>
+      </c>
+    </row>
+    <row r="9" spans="2:11" x14ac:dyDescent="0.35">
       <c r="B9">
         <v>1.1622893010130052E-2</v>
       </c>
@@ -1476,19 +1515,19 @@
         <v>1.0580674917488611E-2</v>
       </c>
       <c r="D9">
-        <v>1.4180980099055E-2</v>
+        <v>1.4180980099054998E-2</v>
       </c>
       <c r="E9">
         <v>9.8185033789223025E-3</v>
       </c>
       <c r="F9">
-        <v>9.5071896230625886E-3</v>
+        <v>9.4902417155907914E-3</v>
       </c>
       <c r="G9">
-        <v>4.8997337885991485E-3</v>
-      </c>
-    </row>
-    <row r="10" spans="2:10" x14ac:dyDescent="0.35">
+        <v>4.8987197660100082E-3</v>
+      </c>
+    </row>
+    <row r="10" spans="2:11" x14ac:dyDescent="0.35">
       <c r="B10">
         <v>92.735987427972759</v>
       </c>
@@ -1502,16 +1541,19 @@
         <v>93.658029053788766</v>
       </c>
       <c r="F10">
-        <v>93.280545112781951</v>
+        <v>93.28678890456041</v>
       </c>
       <c r="G10">
-        <v>93.120167397369471</v>
+        <v>93.12147483806676</v>
       </c>
       <c r="J10">
-        <v>0.46460779492661708</v>
-      </c>
-    </row>
-    <row r="11" spans="2:10" x14ac:dyDescent="0.35">
+        <v>0.21307492896970701</v>
+      </c>
+      <c r="K10">
+        <v>0.57371335416765823</v>
+      </c>
+    </row>
+    <row r="11" spans="2:11" x14ac:dyDescent="0.35">
       <c r="B11">
         <v>0.55413475643748189</v>
       </c>
@@ -1522,16 +1564,16 @@
         <v>0.5964620025914954</v>
       </c>
       <c r="E11">
-        <v>0.47302089318136298</v>
+        <v>0.47302089318136314</v>
       </c>
       <c r="F11">
-        <v>0.60091306879226836</v>
+        <v>0.60073118278698534</v>
       </c>
       <c r="G11">
-        <v>0.27480569952290418</v>
-      </c>
-    </row>
-    <row r="12" spans="2:10" x14ac:dyDescent="0.35">
+        <v>0.27478835496977028</v>
+      </c>
+    </row>
+    <row r="12" spans="2:11" x14ac:dyDescent="0.35">
       <c r="B12">
         <v>0.6585724797645327</v>
       </c>
@@ -1545,21 +1587,24 @@
         <v>0.66493955094991364</v>
       </c>
       <c r="F12">
-        <v>0.64190609670637699</v>
+        <v>0.64165497896213186</v>
       </c>
       <c r="G12">
-        <v>0.65779962411450055</v>
+        <v>0.6577501445922499</v>
       </c>
       <c r="J12">
-        <v>0.72062082027172936</v>
-      </c>
-    </row>
-    <row r="13" spans="2:10" x14ac:dyDescent="0.35">
+        <v>0.85242462741585068</v>
+      </c>
+      <c r="K12">
+        <v>0.79637875222901477</v>
+      </c>
+    </row>
+    <row r="13" spans="2:11" x14ac:dyDescent="0.35">
       <c r="B13">
         <v>1.955606823859319E-2</v>
       </c>
       <c r="C13">
-        <v>1.984821638070523E-2</v>
+        <v>1.9848216380705226E-2</v>
       </c>
       <c r="D13">
         <v>2.3771097841722523E-2</v>
@@ -1568,13 +1613,13 @@
         <v>1.6558305389398693E-2</v>
       </c>
       <c r="F13">
-        <v>1.626709573106366E-2</v>
+        <v>1.6310835628075143E-2</v>
       </c>
       <c r="G13">
-        <v>8.4757570932599627E-3</v>
-      </c>
-    </row>
-    <row r="14" spans="2:10" x14ac:dyDescent="0.35">
+        <v>8.4804378847425609E-3</v>
+      </c>
+    </row>
+    <row r="14" spans="2:11" x14ac:dyDescent="0.35">
       <c r="B14">
         <v>2585</v>
       </c>
@@ -1588,13 +1633,13 @@
         <v>3406</v>
       </c>
       <c r="F14">
-        <v>2753</v>
+        <v>2751</v>
       </c>
       <c r="G14">
-        <v>13349</v>
-      </c>
-    </row>
-    <row r="16" spans="2:10" x14ac:dyDescent="0.35">
+        <v>13347</v>
+      </c>
+    </row>
+    <row r="16" spans="2:11" x14ac:dyDescent="0.35">
       <c r="B16">
         <v>1984</v>
       </c>
@@ -1608,7 +1653,7 @@
         <v>2634</v>
       </c>
       <c r="F16">
-        <v>2186</v>
+        <v>2185</v>
       </c>
     </row>
   </sheetData>
@@ -1618,1158 +1663,966 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3B054637-0760-4807-B01C-4419EACB0C14}">
-  <dimension ref="A2:J39"/>
+  <dimension ref="A2:H39"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:J38"/>
+    <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2:H38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="18.08984375" bestFit="1" customWidth="1"/>
-    <col min="2" max="3" width="7.6328125" style="3" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="7.36328125" style="3" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="7.1796875" style="3" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="10.54296875" style="3" customWidth="1"/>
-    <col min="7" max="7" width="7.6328125" style="3" bestFit="1" customWidth="1"/>
-    <col min="8" max="9" width="8.7265625" style="3"/>
-    <col min="10" max="10" width="7.1796875" style="3" customWidth="1"/>
+    <col min="1" max="1" width="18.1796875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="9.7265625" style="3" customWidth="1"/>
+    <col min="3" max="3" width="10.54296875" style="3" customWidth="1"/>
+    <col min="4" max="4" width="7.54296875" style="3" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="7.54296875" style="3" customWidth="1"/>
+    <col min="6" max="7" width="8.7265625" style="3"/>
+    <col min="8" max="8" width="9.7265625" style="3" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="2" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A2" s="10"/>
-      <c r="B2" s="16" t="s">
-        <v>19</v>
-      </c>
+      <c r="B2" s="16"/>
       <c r="C2" s="16"/>
       <c r="D2" s="16"/>
       <c r="E2" s="16"/>
       <c r="F2" s="16"/>
       <c r="G2" s="16"/>
       <c r="H2" s="16"/>
-      <c r="I2" s="16"/>
-      <c r="J2" s="16"/>
-    </row>
-    <row r="3" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    </row>
+    <row r="3" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A3" s="8"/>
       <c r="B3" s="9"/>
-      <c r="C3" s="9"/>
-      <c r="D3" s="9"/>
-      <c r="E3" s="9"/>
-      <c r="F3" s="15" t="s">
-        <v>16</v>
-      </c>
-      <c r="G3" s="15"/>
-      <c r="H3" s="15" t="s">
-        <v>15</v>
-      </c>
-      <c r="I3" s="15"/>
-      <c r="J3" s="9"/>
-    </row>
-    <row r="4" spans="1:10" s="6" customFormat="1" ht="15" thickTop="1" x14ac:dyDescent="0.35">
+      <c r="C3" s="18" t="s">
+        <v>19</v>
+      </c>
+      <c r="D3" s="18"/>
+      <c r="E3" s="18"/>
+      <c r="F3" s="18" t="s">
+        <v>18</v>
+      </c>
+      <c r="G3" s="18"/>
+      <c r="H3" s="18"/>
+    </row>
+    <row r="4" spans="1:8" s="6" customFormat="1" ht="15" thickTop="1" x14ac:dyDescent="0.35">
       <c r="B4" s="7" t="s">
         <v>1</v>
       </c>
       <c r="C4" s="7" t="s">
-        <v>28</v>
+        <v>12</v>
       </c>
       <c r="D4" s="7" t="s">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="E4" s="7" t="s">
         <v>2</v>
       </c>
       <c r="F4" s="7" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="G4" s="7" t="s">
-        <v>0</v>
+        <v>13</v>
       </c>
       <c r="H4" s="7" t="s">
-        <v>17</v>
-      </c>
-      <c r="I4" s="7" t="s">
-        <v>18</v>
-      </c>
-      <c r="J4" s="7" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A5" s="2"/>
+      <c r="B5" s="17" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="5" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A5" s="2"/>
-      <c r="B5" s="5"/>
-      <c r="C5" s="5"/>
-      <c r="D5" s="5"/>
-      <c r="E5" s="17" t="s">
-        <v>4</v>
-      </c>
+      <c r="C5" s="17"/>
+      <c r="D5" s="17"/>
+      <c r="E5" s="17"/>
       <c r="F5" s="17"/>
       <c r="G5" s="17"/>
       <c r="H5" s="17"/>
-      <c r="I5" s="17"/>
-      <c r="J5" s="17"/>
-    </row>
-    <row r="6" spans="1:10" ht="15" thickTop="1" x14ac:dyDescent="0.35">
+    </row>
+    <row r="6" spans="1:8" ht="15" thickTop="1" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B6" s="3">
-        <f>ROUND(SS_admin!H2,0)</f>
-        <v>2163</v>
-      </c>
-      <c r="C6" s="3">
-        <f>ROUND(SS_admin!G2,0)</f>
-        <v>1957</v>
-      </c>
-      <c r="D6" s="3">
-        <f>ROUND(SS_admin!K2,2)</f>
-        <v>0.15</v>
-      </c>
-      <c r="E6" s="3">
         <f>ROUND(SS_admin!B2,0)</f>
         <v>2289</v>
       </c>
-      <c r="F6" s="3">
+      <c r="C6" s="3">
         <f>ROUND(SS_admin!C2,0)</f>
         <v>2131</v>
       </c>
-      <c r="G6" s="3">
+      <c r="D6" s="3">
         <f>ROUND(SS_admin!E2,0)</f>
         <v>2180</v>
       </c>
-      <c r="H6" s="3">
+      <c r="E6" s="3">
+        <f>ROUND(SS_admin!L2,2)</f>
+        <v>0.32</v>
+      </c>
+      <c r="F6" s="3">
         <f>ROUND(SS_admin!D2,0)</f>
         <v>2136</v>
       </c>
-      <c r="I6" s="3">
+      <c r="G6" s="3">
         <f>ROUND(SS_admin!F2,0)</f>
         <v>2090</v>
       </c>
-      <c r="J6" s="3">
-        <f>ROUND(SS_admin!J2,2)</f>
-        <v>0.38</v>
-      </c>
-    </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="H6" s="3">
+        <f>ROUND(SS_admin!M2,2)</f>
+        <v>0.14000000000000001</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.35">
       <c r="B7" s="3" t="str">
-        <f>CONCATENATE("(",ROUND(SS_admin!H3,0),")")</f>
-        <v>(32)</v>
-      </c>
-      <c r="C7" s="3" t="str">
-        <f>CONCATENATE("(",ROUND(SS_admin!G3,0),")")</f>
-        <v>(141)</v>
-      </c>
-      <c r="E7" s="3" t="str">
         <f>CONCATENATE("(",ROUND(SS_admin!B3,0),")")</f>
         <v>(79)</v>
       </c>
-      <c r="F7" s="3" t="str">
+      <c r="C7" s="3" t="str">
         <f>CONCATENATE("(",ROUND(SS_admin!C3,0),")")</f>
         <v>(73)</v>
       </c>
-      <c r="G7" s="3" t="str">
+      <c r="D7" s="3" t="str">
         <f>CONCATENATE("(",ROUND(SS_admin!E3,0),")")</f>
         <v>(66)</v>
       </c>
-      <c r="H7" s="3" t="str">
+      <c r="F7" s="3" t="str">
         <f>CONCATENATE("(",ROUND(SS_admin!D3,0),")")</f>
         <v>(74)</v>
       </c>
-      <c r="I7" s="3" t="str">
+      <c r="G7" s="3" t="str">
         <f>CONCATENATE("(",ROUND(SS_admin!F3,0),")")</f>
         <v>(65)</v>
       </c>
     </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
-        <v>6</v>
+        <v>17</v>
       </c>
       <c r="B8" s="3">
-        <f>ROUND(SS_admin!H4,2)</f>
-        <v>0.18</v>
+        <f>ROUND(SS_admin!B4,2)</f>
+        <v>0.88</v>
       </c>
       <c r="C8" s="3">
-        <f>ROUND(SS_admin!G4,2)</f>
-        <v>0.17</v>
+        <f>ROUND(SS_admin!C4,2)</f>
+        <v>0.89</v>
       </c>
       <c r="D8" s="3">
-        <f>ROUND(SS_admin!K4,2)</f>
-        <v>0.7</v>
+        <f>ROUND(SS_admin!E4,2)</f>
+        <v>0.85</v>
       </c>
       <c r="E8" s="3">
-        <f>ROUND(SS_admin!B4,2)</f>
-        <v>0.18</v>
+        <f>ROUND(SS_admin!L4,2)</f>
+        <v>0.72</v>
       </c>
       <c r="F8" s="3">
-        <f>ROUND(SS_admin!C4,2)</f>
-        <v>0.16</v>
+        <f>ROUND(SS_admin!D4,2)</f>
+        <v>0.89</v>
       </c>
       <c r="G8" s="3">
-        <f>ROUND(SS_admin!E4,2)</f>
-        <v>0.18</v>
+        <f>ROUND(SS_admin!F4,2)</f>
+        <v>0.83</v>
       </c>
       <c r="H8" s="3">
-        <f>ROUND(SS_admin!D4,2)</f>
-        <v>0.17</v>
-      </c>
-      <c r="I8" s="3">
-        <f>ROUND(SS_admin!F4,2)</f>
-        <v>0.21</v>
-      </c>
-      <c r="J8" s="3">
-        <f>ROUND(SS_admin!J4,2)</f>
-        <v>0.96</v>
-      </c>
-    </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.35">
+        <f>ROUND(SS_admin!M4,2)</f>
+        <v>0.62</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.35">
       <c r="B9" s="3" t="str">
-        <f>CONCATENATE("(",ROUND(SS_admin!H5,3),")")</f>
-        <v>(0.024)</v>
+        <f>CONCATENATE("(",ROUND(SS_admin!B5,3),")")</f>
+        <v>(0.04)</v>
       </c>
       <c r="C9" s="3" t="str">
-        <f>CONCATENATE("(",ROUND(SS_admin!G5,3),")")</f>
-        <v>(0.032)</v>
-      </c>
-      <c r="E9" s="3" t="str">
-        <f>CONCATENATE("(",ROUND(SS_admin!B5,3),")")</f>
-        <v>(0.046)</v>
+        <f>CONCATENATE("(",ROUND(SS_admin!C5,3),")")</f>
+        <v>(0.034)</v>
+      </c>
+      <c r="D9" s="3" t="str">
+        <f>CONCATENATE("(",ROUND(SS_admin!E5,3),")")</f>
+        <v>(0.042)</v>
       </c>
       <c r="F9" s="3" t="str">
-        <f>CONCATENATE("(",ROUND(SS_admin!C5,3),")")</f>
-        <v>(0.05)</v>
+        <f>CONCATENATE("(",ROUND(SS_admin!D5,3),")")</f>
+        <v>(0.036)</v>
       </c>
       <c r="G9" s="3" t="str">
-        <f>CONCATENATE("(",ROUND(SS_admin!E5,3),")")</f>
-        <v>(0.055)</v>
-      </c>
-      <c r="H9" s="3" t="str">
-        <f>CONCATENATE("(",ROUND(SS_admin!D5,3),")")</f>
-        <v>(0.063)</v>
-      </c>
-      <c r="I9" s="3" t="str">
         <f>CONCATENATE("(",ROUND(SS_admin!F5,3),")")</f>
-        <v>(0.054)</v>
-      </c>
-    </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.35">
+        <v>(0.049)</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A10" s="1" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="B10" s="4">
-        <f>SS_admin!H6</f>
-        <v>13534</v>
-      </c>
-      <c r="C10" s="4">
-        <f>SS_admin!G6</f>
-        <v>180</v>
-      </c>
-      <c r="D10" s="4"/>
-      <c r="E10" s="4">
         <f>SS_admin!B6</f>
         <v>2585</v>
       </c>
-      <c r="F10" s="4">
+      <c r="C10" s="4">
         <f>SS_admin!C6</f>
         <v>2465</v>
       </c>
-      <c r="G10" s="4">
+      <c r="D10" s="4">
         <f>SS_admin!E6</f>
         <v>3406</v>
       </c>
-      <c r="H10" s="4">
+      <c r="E10" s="4"/>
+      <c r="F10" s="4">
         <f>SS_admin!D6</f>
         <v>2143</v>
       </c>
-      <c r="I10" s="4">
+      <c r="G10" s="4">
         <f>SS_admin!F6</f>
-        <v>2755</v>
-      </c>
-      <c r="J10" s="4"/>
-    </row>
-    <row r="11" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+        <v>2753</v>
+      </c>
+      <c r="H10" s="4"/>
+    </row>
+    <row r="11" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A11" s="10"/>
-      <c r="B11" s="16" t="s">
-        <v>20</v>
-      </c>
-      <c r="C11" s="16"/>
-      <c r="D11" s="16"/>
-      <c r="E11" s="16"/>
-      <c r="F11" s="16"/>
-      <c r="G11" s="16"/>
-      <c r="H11" s="16"/>
-      <c r="I11" s="16"/>
-      <c r="J11" s="16"/>
-    </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="B11" s="17" t="s">
+        <v>21</v>
+      </c>
+      <c r="C11" s="17"/>
+      <c r="D11" s="17"/>
+      <c r="E11" s="17"/>
+      <c r="F11" s="17"/>
+      <c r="G11" s="17"/>
+      <c r="H11" s="17"/>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="B12" s="3">
-        <f>ROUND(SS_survey_uncond!H2,2)</f>
-        <v>0.74</v>
-      </c>
-      <c r="C12" s="3">
-        <f>ROUND(SS_survey_uncond!G2,2)</f>
-        <v>0.75</v>
-      </c>
-      <c r="D12" s="3">
-        <f>ROUND(SS_survey_uncond!K2,2)</f>
-        <v>0.11</v>
-      </c>
-      <c r="E12" s="3">
         <f>ROUND(SS_survey_uncond!B2,2)</f>
         <v>0.75</v>
       </c>
-      <c r="F12" s="3">
+      <c r="C12" s="3">
         <f>ROUND(SS_survey_uncond!C2,2)</f>
         <v>0.72</v>
       </c>
-      <c r="G12" s="3">
+      <c r="D12" s="3">
         <f>ROUND(SS_survey_uncond!E2,2)</f>
         <v>0.72</v>
       </c>
-      <c r="H12" s="3">
+      <c r="E12" s="3">
+        <f>ROUND(SS_survey_uncond!L2,2)</f>
+        <v>0.22</v>
+      </c>
+      <c r="F12" s="3">
         <f>ROUND(SS_survey_uncond!D2,2)</f>
         <v>0.72</v>
       </c>
-      <c r="I12" s="3">
+      <c r="G12" s="3">
         <f>ROUND(SS_survey_uncond!F2,2)</f>
         <v>0.74</v>
       </c>
-      <c r="J12" s="3">
-        <f>ROUND(SS_survey_uncond!J2,2)</f>
-        <v>0.45</v>
-      </c>
-    </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="H12" s="3">
+        <f>ROUND(SS_survey_uncond!M2,2)</f>
+        <v>0.52</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.35">
       <c r="B13" s="3" t="str">
-        <f>CONCATENATE("(",ROUND(SS_survey_uncond!H3,3),")")</f>
-        <v>(0.006)</v>
-      </c>
-      <c r="C13" s="3" t="str">
-        <f>CONCATENATE("(",ROUND(SS_survey_uncond!G3,3),")")</f>
-        <v>(0.009)</v>
-      </c>
-      <c r="E13" s="3" t="str">
         <f>CONCATENATE("(",ROUND(SS_survey_uncond!B3,3),")")</f>
         <v>(0.017)</v>
       </c>
-      <c r="F13" s="3" t="str">
+      <c r="C13" s="3" t="str">
         <f>CONCATENATE("(",ROUND(SS_survey_uncond!C3,3),")")</f>
         <v>(0.017)</v>
       </c>
-      <c r="G13" s="3" t="str">
+      <c r="D13" s="3" t="str">
         <f>CONCATENATE("(",ROUND(SS_survey_uncond!E3,3),")")</f>
         <v>(0.015)</v>
       </c>
-      <c r="H13" s="3" t="str">
+      <c r="F13" s="3" t="str">
         <f>CONCATENATE("(",ROUND(SS_survey_uncond!D3,3),")")</f>
         <v>(0.02)</v>
       </c>
-      <c r="I13" s="3" t="str">
+      <c r="G13" s="3" t="str">
         <f>CONCATENATE("(",ROUND(SS_survey_uncond!F3,3),")")</f>
         <v>(0.013)</v>
       </c>
     </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="B14" s="3">
-        <f>ROUND(SS_survey_uncond!H4,2)</f>
-        <v>43.24</v>
-      </c>
-      <c r="C14" s="3">
-        <f>ROUND(SS_survey_uncond!G4,2)</f>
-        <v>43.06</v>
-      </c>
-      <c r="D14" s="3">
-        <f>ROUND(SS_survey_uncond!K4,2)</f>
-        <v>0.46</v>
-      </c>
-      <c r="E14" s="3">
         <f>ROUND(SS_survey_uncond!B4,2)</f>
         <v>43.22</v>
       </c>
-      <c r="F14" s="3">
+      <c r="C14" s="3">
         <f>ROUND(SS_survey_uncond!C4,2)</f>
         <v>43.2</v>
       </c>
-      <c r="G14" s="3">
+      <c r="D14" s="3">
         <f>ROUND(SS_survey_uncond!E4,2)</f>
         <v>44.04</v>
       </c>
-      <c r="H14" s="3">
+      <c r="E14" s="3">
+        <f>ROUND(SS_survey_uncond!L4,2)</f>
+        <v>0.55000000000000004</v>
+      </c>
+      <c r="F14" s="3">
         <f>ROUND(SS_survey_uncond!D4,2)</f>
         <v>43</v>
       </c>
-      <c r="I14" s="3">
+      <c r="G14" s="3">
         <f>ROUND(SS_survey_uncond!F4,2)</f>
-        <v>43.12</v>
-      </c>
-      <c r="J14" s="3">
-        <f>ROUND(SS_survey_uncond!J4,2)</f>
-        <v>0.83</v>
-      </c>
-    </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.35">
+        <v>43.1</v>
+      </c>
+      <c r="H14" s="3">
+        <f>ROUND(SS_survey_uncond!M4,2)</f>
+        <v>0.97</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.35">
       <c r="B15" s="3" t="str">
-        <f>CONCATENATE("(",ROUND(SS_survey_uncond!H5,3),")")</f>
-        <v>(0.211)</v>
-      </c>
-      <c r="C15" s="3" t="str">
-        <f>CONCATENATE("(",ROUND(SS_survey_uncond!G5,3),")")</f>
-        <v>(0.316)</v>
-      </c>
-      <c r="E15" s="3" t="str">
         <f>CONCATENATE("(",ROUND(SS_survey_uncond!B5,3),")")</f>
         <v>(0.565)</v>
       </c>
-      <c r="F15" s="3" t="str">
+      <c r="C15" s="3" t="str">
         <f>CONCATENATE("(",ROUND(SS_survey_uncond!C5,3),")")</f>
         <v>(0.763)</v>
       </c>
-      <c r="G15" s="3" t="str">
+      <c r="D15" s="3" t="str">
         <f>CONCATENATE("(",ROUND(SS_survey_uncond!E5,3),")")</f>
         <v>(0.607)</v>
       </c>
-      <c r="H15" s="3" t="str">
+      <c r="F15" s="3" t="str">
         <f>CONCATENATE("(",ROUND(SS_survey_uncond!D5,3),")")</f>
         <v>(0.647)</v>
       </c>
-      <c r="I15" s="3" t="str">
+      <c r="G15" s="3" t="str">
         <f>CONCATENATE("(",ROUND(SS_survey_uncond!F5,3),")")</f>
-        <v>(0.52)</v>
-      </c>
-    </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.35">
+        <v>(0.519)</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A16" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="B16" s="3">
-        <f>ROUND(SS_survey_uncond!H6,0)</f>
-        <v>3111</v>
-      </c>
-      <c r="C16" s="3">
-        <f>ROUND(SS_survey_uncond!G6,0)</f>
-        <v>3192</v>
-      </c>
-      <c r="D16" s="3">
-        <f>ROUND(SS_survey_uncond!K6,2)</f>
-        <v>0.15</v>
-      </c>
-      <c r="E16" s="3">
         <f>ROUND(SS_survey_uncond!B6,0)</f>
         <v>3144</v>
       </c>
-      <c r="F16" s="3">
+      <c r="C16" s="3">
         <f>ROUND(SS_survey_uncond!C6,0)</f>
         <v>2978</v>
       </c>
-      <c r="G16" s="3">
+      <c r="D16" s="3">
         <f>ROUND(SS_survey_uncond!E6,0)</f>
         <v>3112</v>
       </c>
-      <c r="H16" s="3">
+      <c r="E16" s="3">
+        <f>ROUND(SS_survey_uncond!L6,2)</f>
+        <v>0.31</v>
+      </c>
+      <c r="F16" s="3">
         <f>ROUND(SS_survey_uncond!D6,0)</f>
         <v>3012</v>
       </c>
-      <c r="I16" s="3">
+      <c r="G16" s="3">
         <f>ROUND(SS_survey_uncond!F6,0)</f>
         <v>3082</v>
       </c>
-      <c r="J16" s="3">
-        <f>ROUND(SS_survey_uncond!J6,2)</f>
-        <v>0.42</v>
-      </c>
-    </row>
-    <row r="17" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="H16" s="3">
+        <f>ROUND(SS_survey_uncond!M6,2)</f>
+        <v>0.43</v>
+      </c>
+    </row>
+    <row r="17" spans="1:8" x14ac:dyDescent="0.35">
       <c r="B17" s="3" t="str">
-        <f>CONCATENATE("(",ROUND(SS_survey_uncond!H7,0),")")</f>
-        <v>(36)</v>
-      </c>
-      <c r="C17" s="3" t="str">
-        <f>CONCATENATE("(",ROUND(SS_survey_uncond!G7,0),")")</f>
-        <v>(75)</v>
-      </c>
-      <c r="E17" s="3" t="str">
         <f>CONCATENATE("(",ROUND(SS_survey_uncond!B7,0),")")</f>
         <v>(68)</v>
       </c>
-      <c r="F17" s="3" t="str">
+      <c r="C17" s="3" t="str">
         <f>CONCATENATE("(",ROUND(SS_survey_uncond!C7,0),")")</f>
         <v>(87)</v>
       </c>
-      <c r="G17" s="3" t="str">
+      <c r="D17" s="3" t="str">
         <f>CONCATENATE("(",ROUND(SS_survey_uncond!E7,0),")")</f>
         <v>(85)</v>
       </c>
-      <c r="H17" s="3" t="str">
+      <c r="F17" s="3" t="str">
         <f>CONCATENATE("(",ROUND(SS_survey_uncond!D7,0),")")</f>
         <v>(77)</v>
       </c>
-      <c r="I17" s="3" t="str">
+      <c r="G17" s="3" t="str">
         <f>CONCATENATE("(",ROUND(SS_survey_uncond!F7,0),")")</f>
         <v>(99)</v>
       </c>
     </row>
-    <row r="18" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A18" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="B18" s="3">
-        <f>ROUND(SS_survey_uncond!H8,2)</f>
-        <v>0.89</v>
-      </c>
-      <c r="C18" s="3">
-        <f>ROUND(SS_survey_uncond!G8,2)</f>
-        <v>0.88</v>
-      </c>
-      <c r="D18" s="3">
-        <f>ROUND(SS_survey_uncond!K8,2)</f>
-        <v>0.22</v>
-      </c>
-      <c r="E18" s="3">
         <f>ROUND(SS_survey_uncond!B8,2)</f>
         <v>0.89</v>
       </c>
-      <c r="F18" s="3">
+      <c r="C18" s="3">
         <f>ROUND(SS_survey_uncond!C8,2)</f>
         <v>0.9</v>
       </c>
-      <c r="G18" s="3">
+      <c r="D18" s="3">
         <f>ROUND(SS_survey_uncond!E8,2)</f>
         <v>0.91</v>
       </c>
-      <c r="H18" s="3">
+      <c r="E18" s="3">
+        <f>ROUND(SS_survey_uncond!L8,2)</f>
+        <v>0.47</v>
+      </c>
+      <c r="F18" s="3">
         <f>ROUND(SS_survey_uncond!D8,2)</f>
         <v>0.89</v>
       </c>
-      <c r="I18" s="3">
+      <c r="G18" s="3">
         <f>ROUND(SS_survey_uncond!F8,2)</f>
         <v>0.89</v>
       </c>
-      <c r="J18" s="3">
-        <f>ROUND(SS_survey_uncond!J8,2)</f>
-        <v>0.74</v>
-      </c>
-    </row>
-    <row r="19" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="H18" s="3">
+        <f>ROUND(SS_survey_uncond!M8,2)</f>
+        <v>0.99</v>
+      </c>
+    </row>
+    <row r="19" spans="1:8" x14ac:dyDescent="0.35">
       <c r="B19" s="3" t="str">
-        <f>CONCATENATE("(",ROUND(SS_survey_uncond!H9,3),")")</f>
-        <v>(0.005)</v>
-      </c>
-      <c r="C19" s="3" t="str">
-        <f>CONCATENATE("(",ROUND(SS_survey_uncond!G9,3),")")</f>
-        <v>(0.011)</v>
-      </c>
-      <c r="E19" s="3" t="str">
         <f>CONCATENATE("(",ROUND(SS_survey_uncond!B9,3),")")</f>
         <v>(0.011)</v>
       </c>
-      <c r="F19" s="3" t="str">
+      <c r="C19" s="3" t="str">
         <f>CONCATENATE("(",ROUND(SS_survey_uncond!C9,3),")")</f>
         <v>(0.011)</v>
       </c>
-      <c r="G19" s="3" t="str">
+      <c r="D19" s="3" t="str">
         <f>CONCATENATE("(",ROUND(SS_survey_uncond!E9,3),")")</f>
         <v>(0.01)</v>
       </c>
-      <c r="H19" s="3" t="str">
+      <c r="F19" s="3" t="str">
         <f>CONCATENATE("(",ROUND(SS_survey_uncond!D9,3),")")</f>
         <v>(0.014)</v>
       </c>
-      <c r="I19" s="3" t="str">
+      <c r="G19" s="3" t="str">
         <f>CONCATENATE("(",ROUND(SS_survey_uncond!F9,3),")")</f>
         <v>(0.009)</v>
       </c>
     </row>
-    <row r="20" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A20" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="B20" s="3">
-        <f>ROUND(SS_survey_uncond!H10,2)</f>
-        <v>92.64</v>
-      </c>
-      <c r="C20" s="3">
-        <f>ROUND(SS_survey_uncond!G10,2)</f>
-        <v>91.84</v>
-      </c>
-      <c r="D20" s="3">
-        <f>ROUND(SS_survey_uncond!K10,3)</f>
-        <v>1E-3</v>
-      </c>
-      <c r="E20" s="3">
         <f>ROUND(SS_survey_uncond!B10,2)</f>
         <v>92.75</v>
       </c>
-      <c r="F20" s="3">
+      <c r="C20" s="3">
         <f>ROUND(SS_survey_uncond!C10,2)</f>
         <v>92.19</v>
       </c>
-      <c r="G20" s="3">
+      <c r="D20" s="3">
         <f>ROUND(SS_survey_uncond!E10,2)</f>
         <v>93.71</v>
       </c>
-      <c r="H20" s="3">
+      <c r="E20" s="3">
+        <f>ROUND(SS_survey_uncond!L10,2)</f>
+        <v>0.18</v>
+      </c>
+      <c r="F20" s="3">
         <f>ROUND(SS_survey_uncond!D10,2)</f>
         <v>93.66</v>
       </c>
-      <c r="I20" s="3">
+      <c r="G20" s="3">
         <f>ROUND(SS_survey_uncond!F10,2)</f>
         <v>93.34</v>
       </c>
-      <c r="J20" s="3">
-        <f>ROUND(SS_survey_uncond!J10,2)</f>
-        <v>0.46</v>
-      </c>
-    </row>
-    <row r="21" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="H20" s="3">
+        <f>ROUND(SS_survey_uncond!M10,2)</f>
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="21" spans="1:8" x14ac:dyDescent="0.35">
       <c r="B21" s="3" t="str">
-        <f>CONCATENATE("(",ROUND(SS_survey_uncond!H11,3),")")</f>
-        <v>(0.205)</v>
-      </c>
-      <c r="C21" s="3" t="str">
-        <f>CONCATENATE("(",ROUND(SS_survey_uncond!G11,3),")")</f>
-        <v>(0.308)</v>
-      </c>
-      <c r="E21" s="3" t="str">
         <f>CONCATENATE("(",ROUND(SS_survey_uncond!B11,3),")")</f>
         <v>(0.537)</v>
       </c>
-      <c r="F21" s="3" t="str">
+      <c r="C21" s="3" t="str">
         <f>CONCATENATE("(",ROUND(SS_survey_uncond!C11,3),")")</f>
         <v>(0.839)</v>
       </c>
-      <c r="G21" s="3" t="str">
+      <c r="D21" s="3" t="str">
         <f>CONCATENATE("(",ROUND(SS_survey_uncond!E11,3),")")</f>
         <v>(0.455)</v>
       </c>
-      <c r="H21" s="3" t="str">
+      <c r="F21" s="3" t="str">
         <f>CONCATENATE("(",ROUND(SS_survey_uncond!D11,3),")")</f>
         <v>(0.591)</v>
       </c>
-      <c r="I21" s="3" t="str">
+      <c r="G21" s="3" t="str">
         <f>CONCATENATE("(",ROUND(SS_survey_uncond!F11,3),")")</f>
         <v>(0.596)</v>
       </c>
     </row>
-    <row r="22" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A22" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="B22" s="3">
-        <f>ROUND(SS_survey_uncond!H12,2)</f>
-        <v>0.63</v>
-      </c>
-      <c r="C22" s="3">
-        <f>ROUND(SS_survey_uncond!G12,2)</f>
-        <v>0.6</v>
-      </c>
-      <c r="D22" s="3">
-        <f>ROUND(SS_survey_uncond!K12,3)</f>
-        <v>0</v>
-      </c>
-      <c r="E22" s="3">
         <f>ROUND(SS_survey_uncond!B12,2)</f>
         <v>0.66</v>
       </c>
-      <c r="F22" s="3">
+      <c r="C22" s="3">
         <f>ROUND(SS_survey_uncond!C12,2)</f>
         <v>0.67</v>
       </c>
-      <c r="G22" s="3">
+      <c r="D22" s="3">
         <f>ROUND(SS_survey_uncond!E12,2)</f>
         <v>0.66</v>
       </c>
-      <c r="H22" s="3">
+      <c r="E22" s="3">
+        <f>ROUND(SS_survey_uncond!L12,2)</f>
+        <v>0.92</v>
+      </c>
+      <c r="F22" s="3">
         <f>ROUND(SS_survey_uncond!D12,2)</f>
         <v>0.65</v>
       </c>
-      <c r="I22" s="3">
+      <c r="G22" s="3">
         <f>ROUND(SS_survey_uncond!F12,2)</f>
         <v>0.64</v>
       </c>
-      <c r="J22" s="3">
-        <f>ROUND(SS_survey_uncond!J12,2)</f>
-        <v>0.72</v>
-      </c>
-    </row>
-    <row r="23" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="H22" s="3">
+        <f>ROUND(SS_survey_uncond!M12,2)</f>
+        <v>0.83</v>
+      </c>
+    </row>
+    <row r="23" spans="1:8" x14ac:dyDescent="0.35">
       <c r="B23" s="3" t="str">
-        <f>CONCATENATE("(",ROUND(SS_survey_uncond!H13,3),")")</f>
-        <v>(0.007)</v>
-      </c>
-      <c r="C23" s="3" t="str">
-        <f>CONCATENATE("(",ROUND(SS_survey_uncond!G13,3),")")</f>
-        <v>(0.013)</v>
-      </c>
-      <c r="E23" s="3" t="str">
         <f>CONCATENATE("(",ROUND(SS_survey_uncond!B13,3),")")</f>
         <v>(0.02)</v>
       </c>
-      <c r="F23" s="3" t="str">
+      <c r="C23" s="3" t="str">
         <f>CONCATENATE("(",ROUND(SS_survey_uncond!C13,3),")")</f>
         <v>(0.02)</v>
       </c>
-      <c r="G23" s="3" t="str">
+      <c r="D23" s="3" t="str">
         <f>CONCATENATE("(",ROUND(SS_survey_uncond!E13,3),")")</f>
         <v>(0.017)</v>
       </c>
-      <c r="H23" s="3" t="str">
+      <c r="F23" s="3" t="str">
         <f>CONCATENATE("(",ROUND(SS_survey_uncond!D13,3),")")</f>
         <v>(0.024)</v>
       </c>
-      <c r="I23" s="3" t="str">
+      <c r="G23" s="3" t="str">
         <f>CONCATENATE("(",ROUND(SS_survey_uncond!F13,3),")")</f>
         <v>(0.017)</v>
       </c>
     </row>
-    <row r="24" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A24" s="11" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="B24" s="12">
-        <f>SUM(E24:J24)</f>
-        <v>10420</v>
-      </c>
-      <c r="C24" s="12">
-        <f>SS_survey_uncond!G16</f>
-        <v>6919</v>
-      </c>
-      <c r="D24" s="12"/>
-      <c r="E24" s="12">
         <f>SS_survey_uncond!B16</f>
         <v>2036</v>
       </c>
+      <c r="C24" s="12">
+        <f>SS_survey_uncond!C16</f>
+        <v>1907</v>
+      </c>
+      <c r="D24" s="12">
+        <f>SS_survey_uncond!E16</f>
+        <v>2710</v>
+      </c>
+      <c r="E24" s="12"/>
       <c r="F24" s="12">
-        <f>SS_survey_uncond!C16</f>
-        <v>1840</v>
+        <f>SS_survey_uncond!D16</f>
+        <v>1757</v>
       </c>
       <c r="G24" s="12">
-        <f>SS_survey_uncond!E16</f>
-        <v>2634</v>
-      </c>
-      <c r="H24" s="12">
-        <f>SS_survey_uncond!D16</f>
-        <v>1724</v>
-      </c>
-      <c r="I24" s="12">
         <f>SS_survey_uncond!F16</f>
-        <v>2186</v>
-      </c>
-      <c r="J24" s="12"/>
-    </row>
-    <row r="25" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+        <v>2216</v>
+      </c>
+      <c r="H24" s="12"/>
+    </row>
+    <row r="25" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A25" s="10"/>
-      <c r="B25" s="16" t="s">
-        <v>21</v>
-      </c>
-      <c r="C25" s="16"/>
-      <c r="D25" s="16"/>
-      <c r="E25" s="16"/>
-      <c r="F25" s="16"/>
-      <c r="G25" s="16"/>
-      <c r="H25" s="16"/>
-      <c r="I25" s="16"/>
-      <c r="J25" s="16"/>
-    </row>
-    <row r="26" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="B25" s="17" t="s">
+        <v>20</v>
+      </c>
+      <c r="C25" s="17"/>
+      <c r="D25" s="17"/>
+      <c r="E25" s="17"/>
+      <c r="F25" s="17"/>
+      <c r="G25" s="17"/>
+      <c r="H25" s="17"/>
+    </row>
+    <row r="26" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A26" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="B26" s="3">
-        <f>ROUND(SS_survey!G2,2)</f>
-        <v>0.73</v>
-      </c>
-      <c r="E26" s="3">
         <f>ROUND(SS_survey!B2,2)</f>
         <v>0.76</v>
       </c>
-      <c r="F26" s="3">
+      <c r="C26" s="3">
         <f>ROUND(SS_survey!C2,2)</f>
         <v>0.72</v>
       </c>
-      <c r="G26" s="3">
+      <c r="D26" s="3">
         <f>ROUND(SS_survey!E2,2)</f>
         <v>0.72</v>
       </c>
-      <c r="H26" s="3">
+      <c r="E26" s="3">
+        <f>ROUND(SS_survey!J2,2)</f>
+        <v>0.2</v>
+      </c>
+      <c r="F26" s="3">
         <f>ROUND(SS_survey!D2,2)</f>
         <v>0.72</v>
       </c>
-      <c r="I26" s="3">
+      <c r="G26" s="3">
         <f>ROUND(SS_survey!F2,2)</f>
         <v>0.74</v>
       </c>
-      <c r="J26" s="3">
-        <f>ROUND(SS_survey!J2,2)</f>
-        <v>0.45</v>
-      </c>
-    </row>
-    <row r="27" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="H26" s="3">
+        <f>ROUND(SS_survey!K2,2)</f>
+        <v>0.49</v>
+      </c>
+    </row>
+    <row r="27" spans="1:8" x14ac:dyDescent="0.35">
       <c r="B27" s="3" t="str">
-        <f>CONCATENATE("(",ROUND(SS_survey!G3,3),")")</f>
-        <v>(0.008)</v>
-      </c>
-      <c r="E27" s="3" t="str">
         <f>CONCATENATE("(",ROUND(SS_survey!B3,3),")")</f>
         <v>(0.016)</v>
       </c>
-      <c r="F27" s="3" t="str">
+      <c r="C27" s="3" t="str">
         <f>CONCATENATE("(",ROUND(SS_survey!C3,3),")")</f>
         <v>(0.018)</v>
       </c>
-      <c r="G27" s="3" t="str">
+      <c r="D27" s="3" t="str">
         <f>CONCATENATE("(",ROUND(SS_survey!E3,3),")")</f>
         <v>(0.016)</v>
       </c>
-      <c r="H27" s="3" t="str">
+      <c r="F27" s="3" t="str">
         <f>CONCATENATE("(",ROUND(SS_survey!D3,3),")")</f>
         <v>(0.021)</v>
       </c>
-      <c r="I27" s="3" t="str">
+      <c r="G27" s="3" t="str">
         <f>CONCATENATE("(",ROUND(SS_survey!F3,3),")")</f>
         <v>(0.013)</v>
       </c>
     </row>
-    <row r="28" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A28" t="s">
-        <v>9</v>
-      </c>
-      <c r="B28" s="3" t="str">
-        <f>CONCATENATE("(",ROUND(SS_survey!G4,3),")")</f>
-        <v>(43.309)</v>
-      </c>
-      <c r="E28" s="3">
+        <v>7</v>
+      </c>
+      <c r="B28" s="3">
         <f>ROUND(SS_survey!B4,2)</f>
         <v>43.22</v>
       </c>
-      <c r="F28" s="3" t="str">
+      <c r="C28" s="3" t="str">
         <f>CONCATENATE("(",ROUND(SS_survey!C4,3),")")</f>
         <v>(43.131)</v>
       </c>
-      <c r="G28" s="3" t="str">
+      <c r="D28" s="3" t="str">
         <f>CONCATENATE("(",ROUND(SS_survey!E4,3),")")</f>
         <v>(43.906)</v>
       </c>
-      <c r="H28" s="3" t="str">
+      <c r="E28" s="3">
+        <f>ROUND(SS_survey!J4,2)</f>
+        <v>0.64</v>
+      </c>
+      <c r="F28" s="3" t="str">
         <f>CONCATENATE("(",ROUND(SS_survey!D4,3),")")</f>
         <v>(42.956)</v>
       </c>
-      <c r="I28" s="3" t="str">
+      <c r="G28" s="3" t="str">
         <f>CONCATENATE("(",ROUND(SS_survey!F4,3),")")</f>
-        <v>(43.095)</v>
-      </c>
-      <c r="J28" s="3">
-        <f>ROUND(SS_survey!J4,2)</f>
-        <v>0.83</v>
-      </c>
-    </row>
-    <row r="29" spans="1:10" x14ac:dyDescent="0.35">
+        <v>(43.081)</v>
+      </c>
+      <c r="H28" s="3">
+        <f>ROUND(SS_survey!K4,2)</f>
+        <v>0.95</v>
+      </c>
+    </row>
+    <row r="29" spans="1:8" x14ac:dyDescent="0.35">
       <c r="B29" s="3" t="str">
-        <f>CONCATENATE("(",ROUND(SS_survey!G5,3),")")</f>
-        <v>(0.283)</v>
-      </c>
-      <c r="E29" s="3" t="str">
         <f>CONCATENATE("(",ROUND(SS_survey!B5,3),")")</f>
         <v>(0.572)</v>
       </c>
-      <c r="F29" s="3" t="str">
+      <c r="C29" s="3" t="str">
         <f>CONCATENATE("(",ROUND(SS_survey!C5,3),")")</f>
         <v>(0.778)</v>
       </c>
-      <c r="G29" s="3" t="str">
+      <c r="D29" s="3" t="str">
         <f>CONCATENATE("(",ROUND(SS_survey!E5,3),")")</f>
         <v>(0.617)</v>
       </c>
-      <c r="H29" s="3" t="str">
+      <c r="F29" s="3" t="str">
         <f>CONCATENATE("(",ROUND(SS_survey!D5,3),")")</f>
         <v>(0.638)</v>
       </c>
-      <c r="I29" s="3" t="str">
+      <c r="G29" s="3" t="str">
         <f>CONCATENATE("(",ROUND(SS_survey!F5,3),")")</f>
-        <v>(0.52)</v>
-      </c>
-    </row>
-    <row r="30" spans="1:10" x14ac:dyDescent="0.35">
+        <v>(0.519)</v>
+      </c>
+    </row>
+    <row r="30" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A30" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="B30" s="3">
-        <f>ROUND(SS_survey!G6,0)</f>
-        <v>3062</v>
-      </c>
-      <c r="E30" s="3">
         <f>ROUND(SS_survey!B6,0)</f>
         <v>3141</v>
       </c>
-      <c r="F30" s="3">
+      <c r="C30" s="3">
         <f>ROUND(SS_survey!C6,0)</f>
         <v>2969</v>
       </c>
-      <c r="G30" s="3">
+      <c r="D30" s="3">
         <f>ROUND(SS_survey!E6,0)</f>
         <v>3107</v>
       </c>
-      <c r="H30" s="3">
+      <c r="E30" s="3">
+        <f>ROUND(SS_survey!J6,2)</f>
+        <v>0.28999999999999998</v>
+      </c>
+      <c r="F30" s="3">
         <f>ROUND(SS_survey!D6,0)</f>
         <v>2982</v>
       </c>
-      <c r="I30" s="3">
+      <c r="G30" s="3">
         <f>ROUND(SS_survey!F6,0)</f>
-        <v>3079</v>
-      </c>
-      <c r="J30" s="3">
-        <f>ROUND(SS_survey!J6,2)</f>
-        <v>0.42</v>
-      </c>
-    </row>
-    <row r="31" spans="1:10" x14ac:dyDescent="0.35">
+        <v>3078</v>
+      </c>
+      <c r="H30" s="3">
+        <f>ROUND(SS_survey!K6,2)</f>
+        <v>0.3</v>
+      </c>
+    </row>
+    <row r="31" spans="1:8" x14ac:dyDescent="0.35">
       <c r="B31" s="3" t="str">
-        <f>CONCATENATE("(",ROUND(SS_survey!G7,0),")")</f>
-        <v>(38)</v>
-      </c>
-      <c r="E31" s="3" t="str">
         <f>CONCATENATE("(",ROUND(SS_survey!B7,0),")")</f>
         <v>(68)</v>
       </c>
-      <c r="F31" s="3" t="str">
+      <c r="C31" s="3" t="str">
         <f>CONCATENATE("(",ROUND(SS_survey!C7,0),")")</f>
         <v>(88)</v>
       </c>
-      <c r="G31" s="3" t="str">
+      <c r="D31" s="3" t="str">
         <f>CONCATENATE("(",ROUND(SS_survey!E7,0),")")</f>
         <v>(85)</v>
       </c>
-      <c r="H31" s="3" t="str">
+      <c r="F31" s="3" t="str">
         <f>CONCATENATE("(",ROUND(SS_survey!D7,0),")")</f>
         <v>(77)</v>
       </c>
-      <c r="I31" s="3" t="str">
+      <c r="G31" s="3" t="str">
         <f>CONCATENATE("(",ROUND(SS_survey!F7,0),")")</f>
         <v>(99)</v>
       </c>
     </row>
-    <row r="32" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A32" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="B32" s="3">
-        <f>ROUND(SS_survey!G8,2)</f>
-        <v>0.9</v>
-      </c>
-      <c r="E32" s="3">
         <f>ROUND(SS_survey!B8,2)</f>
         <v>0.89</v>
       </c>
-      <c r="F32" s="3">
+      <c r="C32" s="3">
         <f>ROUND(SS_survey!C8,2)</f>
         <v>0.9</v>
       </c>
-      <c r="G32" s="3">
+      <c r="D32" s="3">
         <f>ROUND(SS_survey!E8,2)</f>
         <v>0.91</v>
       </c>
-      <c r="H32" s="3">
+      <c r="E32" s="3">
+        <f>ROUND(SS_survey!J8,2)</f>
+        <v>0.48</v>
+      </c>
+      <c r="F32" s="3">
         <f>ROUND(SS_survey!D8,2)</f>
         <v>0.89</v>
       </c>
-      <c r="I32" s="3">
+      <c r="G32" s="3">
         <f>ROUND(SS_survey!F8,2)</f>
         <v>0.89</v>
       </c>
-      <c r="J32" s="3">
-        <f>ROUND(SS_survey!J8,2)</f>
-        <v>0.74</v>
-      </c>
-    </row>
-    <row r="33" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="H32" s="3">
+        <f>ROUND(SS_survey!K8,2)</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="33" spans="1:8" x14ac:dyDescent="0.35">
       <c r="B33" s="3" t="str">
-        <f>CONCATENATE("(",ROUND(SS_survey!G9,3),")")</f>
-        <v>(0.005)</v>
-      </c>
-      <c r="E33" s="3" t="str">
         <f>CONCATENATE("(",ROUND(SS_survey!B9,3),")")</f>
         <v>(0.012)</v>
       </c>
-      <c r="F33" s="3" t="str">
+      <c r="C33" s="3" t="str">
         <f>CONCATENATE("(",ROUND(SS_survey!C9,3),")")</f>
         <v>(0.011)</v>
       </c>
-      <c r="G33" s="3" t="str">
+      <c r="D33" s="3" t="str">
         <f>CONCATENATE("(",ROUND(SS_survey!E9,3),")")</f>
         <v>(0.01)</v>
       </c>
-      <c r="H33" s="3" t="str">
+      <c r="F33" s="3" t="str">
         <f>CONCATENATE("(",ROUND(SS_survey!D9,3),")")</f>
         <v>(0.014)</v>
       </c>
-      <c r="I33" s="3" t="str">
+      <c r="G33" s="3" t="str">
         <f>CONCATENATE("(",ROUND(SS_survey!F9,3),")")</f>
-        <v>(0.01)</v>
-      </c>
-    </row>
-    <row r="34" spans="1:10" x14ac:dyDescent="0.35">
+        <v>(0.009)</v>
+      </c>
+    </row>
+    <row r="34" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A34" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="B34" s="3">
-        <f>ROUND(SS_survey!G10,2)</f>
-        <v>93.12</v>
-      </c>
-      <c r="E34" s="3">
         <f>ROUND(SS_survey!B10,2)</f>
         <v>92.74</v>
       </c>
-      <c r="F34" s="3">
+      <c r="C34" s="3">
         <f>ROUND(SS_survey!C10,2)</f>
         <v>92.14</v>
       </c>
-      <c r="G34" s="3">
+      <c r="D34" s="3">
         <f>ROUND(SS_survey!E10,2)</f>
         <v>93.66</v>
       </c>
-      <c r="H34" s="3">
+      <c r="E34" s="3">
+        <f>ROUND(SS_survey!J10,2)</f>
+        <v>0.21</v>
+      </c>
+      <c r="F34" s="3">
         <f>ROUND(SS_survey!D10,2)</f>
         <v>93.57</v>
       </c>
-      <c r="I34" s="3">
+      <c r="G34" s="3">
         <f>ROUND(SS_survey!F10,2)</f>
-        <v>93.28</v>
-      </c>
-      <c r="J34" s="3">
-        <f>ROUND(SS_survey!J10,2)</f>
-        <v>0.46</v>
-      </c>
-    </row>
-    <row r="35" spans="1:10" x14ac:dyDescent="0.35">
+        <v>93.29</v>
+      </c>
+      <c r="H34" s="3">
+        <f>ROUND(SS_survey!K10,2)</f>
+        <v>0.56999999999999995</v>
+      </c>
+    </row>
+    <row r="35" spans="1:8" x14ac:dyDescent="0.35">
       <c r="B35" s="3" t="str">
-        <f>CONCATENATE("(",ROUND(SS_survey!G11,3),")")</f>
-        <v>(0.275)</v>
-      </c>
-      <c r="E35" s="3" t="str">
         <f>CONCATENATE("(",ROUND(SS_survey!B11,3),")")</f>
         <v>(0.554)</v>
       </c>
-      <c r="F35" s="3" t="str">
+      <c r="C35" s="3" t="str">
         <f>CONCATENATE("(",ROUND(SS_survey!C11,3),")")</f>
         <v>(0.857)</v>
       </c>
-      <c r="G35" s="3" t="str">
+      <c r="D35" s="3" t="str">
         <f>CONCATENATE("(",ROUND(SS_survey!E11,3),")")</f>
         <v>(0.473)</v>
       </c>
-      <c r="H35" s="3" t="str">
+      <c r="F35" s="3" t="str">
         <f>CONCATENATE("(",ROUND(SS_survey!D11,3),")")</f>
         <v>(0.596)</v>
       </c>
-      <c r="I35" s="3" t="str">
+      <c r="G35" s="3" t="str">
         <f>CONCATENATE("(",ROUND(SS_survey!F11,3),")")</f>
         <v>(0.601)</v>
       </c>
     </row>
-    <row r="36" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="36" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A36" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="B36" s="3">
-        <f>ROUND(SS_survey!G12,2)</f>
-        <v>0.66</v>
-      </c>
-      <c r="E36" s="3">
         <f>ROUND(SS_survey!B12,2)</f>
         <v>0.66</v>
       </c>
-      <c r="F36" s="3">
+      <c r="C36" s="3">
         <f>ROUND(SS_survey!C12,2)</f>
         <v>0.67</v>
       </c>
-      <c r="G36" s="3">
+      <c r="D36" s="3">
         <f>ROUND(SS_survey!E12,2)</f>
         <v>0.66</v>
       </c>
-      <c r="H36" s="3">
+      <c r="E36" s="3">
+        <f>ROUND(SS_survey!J12,2)</f>
+        <v>0.85</v>
+      </c>
+      <c r="F36" s="3">
         <f>ROUND(SS_survey!D12,2)</f>
         <v>0.65</v>
       </c>
-      <c r="I36" s="3">
+      <c r="G36" s="3">
         <f>ROUND(SS_survey!F12,2)</f>
         <v>0.64</v>
       </c>
-      <c r="J36" s="3">
-        <f>ROUND(SS_survey!J12,2)</f>
-        <v>0.72</v>
-      </c>
-    </row>
-    <row r="37" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="H36" s="3">
+        <f>ROUND(SS_survey!K12,2)</f>
+        <v>0.8</v>
+      </c>
+    </row>
+    <row r="37" spans="1:8" x14ac:dyDescent="0.35">
       <c r="B37" s="3" t="str">
-        <f>CONCATENATE("(",ROUND(SS_survey!G13,3),")")</f>
-        <v>(0.008)</v>
-      </c>
-      <c r="E37" s="3" t="str">
         <f>CONCATENATE("(",ROUND(SS_survey!B13,3),")")</f>
         <v>(0.02)</v>
       </c>
-      <c r="F37" s="3" t="str">
+      <c r="C37" s="3" t="str">
         <f>CONCATENATE("(",ROUND(SS_survey!C13,3),")")</f>
         <v>(0.02)</v>
       </c>
-      <c r="G37" s="3" t="str">
+      <c r="D37" s="3" t="str">
         <f>CONCATENATE("(",ROUND(SS_survey!E13,3),")")</f>
         <v>(0.017)</v>
       </c>
-      <c r="H37" s="3" t="str">
+      <c r="F37" s="3" t="str">
         <f>CONCATENATE("(",ROUND(SS_survey!D13,3),")")</f>
         <v>(0.024)</v>
       </c>
-      <c r="I37" s="3" t="str">
+      <c r="G37" s="3" t="str">
         <f>CONCATENATE("(",ROUND(SS_survey!F13,3),")")</f>
         <v>(0.016)</v>
       </c>
     </row>
-    <row r="38" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="38" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A38" s="2" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="B38" s="5">
-        <f>SUM(E38:I38)</f>
-        <v>10368</v>
-      </c>
-      <c r="C38" s="5"/>
-      <c r="D38" s="5"/>
-      <c r="E38" s="5">
         <f>SS_survey!B16</f>
         <v>1984</v>
       </c>
-      <c r="F38" s="5">
+      <c r="C38" s="5">
         <f>SS_survey!C16</f>
         <v>1840</v>
       </c>
-      <c r="G38" s="5">
+      <c r="D38" s="5">
         <f>SS_survey!E16</f>
         <v>2634</v>
       </c>
-      <c r="H38" s="5">
+      <c r="E38" s="14"/>
+      <c r="F38" s="5">
         <f>SS_survey!D16</f>
         <v>1724</v>
       </c>
-      <c r="I38" s="5">
+      <c r="G38" s="5">
         <f>SS_survey!F16</f>
-        <v>2186</v>
-      </c>
-      <c r="J38" s="5"/>
-    </row>
-    <row r="39" spans="1:10" ht="15" thickTop="1" x14ac:dyDescent="0.35"/>
+        <v>2185</v>
+      </c>
+      <c r="H38" s="5"/>
+    </row>
+    <row r="39" spans="1:8" ht="15" thickTop="1" x14ac:dyDescent="0.35"/>
   </sheetData>
   <mergeCells count="6">
-    <mergeCell ref="F3:G3"/>
-    <mergeCell ref="H3:I3"/>
-    <mergeCell ref="B2:J2"/>
-    <mergeCell ref="B11:J11"/>
-    <mergeCell ref="B25:J25"/>
-    <mergeCell ref="E5:J5"/>
+    <mergeCell ref="B2:H2"/>
+    <mergeCell ref="B11:H11"/>
+    <mergeCell ref="B25:H25"/>
+    <mergeCell ref="B5:H5"/>
+    <mergeCell ref="C3:E3"/>
+    <mergeCell ref="F3:H3"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -2777,346 +2630,270 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{754403B8-1DA5-4CBA-B8B6-94BFF0A849DB}">
-  <dimension ref="A3:J14"/>
+  <dimension ref="A3:H13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A3" sqref="A3:J13"/>
+      <selection activeCell="A3" sqref="A3:H12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="26.26953125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="8.7265625" style="3"/>
-    <col min="3" max="3" width="7.6328125" style="3" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="7.36328125" style="3" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="7.1796875" style="3" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="10.1796875" style="3" bestFit="1" customWidth="1"/>
-    <col min="7" max="9" width="6.6328125" style="3" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="7.36328125" style="3" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="7.1796875" style="3" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10.1796875" style="3" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="6.54296875" style="3" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="6.54296875" style="3" customWidth="1"/>
+    <col min="6" max="6" width="7" style="3" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="7.453125" style="3" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="7.7265625" style="3" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="3" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A3" s="10"/>
-      <c r="B3" s="16" t="s">
-        <v>27</v>
-      </c>
+      <c r="B3" s="16"/>
       <c r="C3" s="16"/>
       <c r="D3" s="16"/>
       <c r="E3" s="16"/>
       <c r="F3" s="16"/>
       <c r="G3" s="16"/>
       <c r="H3" s="16"/>
-      <c r="I3" s="16"/>
-      <c r="J3" s="16"/>
-    </row>
-    <row r="4" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    </row>
+    <row r="4" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A4" s="8"/>
       <c r="B4" s="9"/>
-      <c r="C4" s="9"/>
-      <c r="D4" s="9"/>
-      <c r="E4" s="9"/>
-      <c r="F4" s="15" t="s">
-        <v>16</v>
-      </c>
-      <c r="G4" s="15"/>
-      <c r="H4" s="15" t="s">
+      <c r="C4" s="18" t="s">
+        <v>19</v>
+      </c>
+      <c r="D4" s="18"/>
+      <c r="E4" s="18"/>
+      <c r="F4" s="18" t="s">
+        <v>18</v>
+      </c>
+      <c r="G4" s="18"/>
+      <c r="H4" s="18"/>
+    </row>
+    <row r="5" spans="1:8" ht="16.5" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A5" s="13"/>
+      <c r="B5" s="15" t="s">
+        <v>1</v>
+      </c>
+      <c r="C5" s="15" t="s">
+        <v>12</v>
+      </c>
+      <c r="D5" s="15" t="s">
+        <v>0</v>
+      </c>
+      <c r="E5" s="15" t="s">
+        <v>2</v>
+      </c>
+      <c r="F5" s="15" t="s">
+        <v>12</v>
+      </c>
+      <c r="G5" s="15" t="s">
+        <v>13</v>
+      </c>
+      <c r="H5" s="15" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" ht="15" thickTop="1" x14ac:dyDescent="0.35">
+      <c r="A6" t="s">
         <v>15</v>
       </c>
-      <c r="I4" s="15"/>
-      <c r="J4" s="9"/>
-    </row>
-    <row r="5" spans="1:10" ht="15.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A5" s="13"/>
-      <c r="B5" s="14" t="s">
-        <v>1</v>
-      </c>
-      <c r="C5" s="14" t="s">
-        <v>28</v>
-      </c>
-      <c r="D5" s="14" t="s">
-        <v>3</v>
-      </c>
-      <c r="E5" s="14" t="s">
-        <v>2</v>
-      </c>
-      <c r="F5" s="14" t="s">
-        <v>14</v>
-      </c>
-      <c r="G5" s="14" t="s">
-        <v>0</v>
-      </c>
-      <c r="H5" s="14" t="s">
-        <v>17</v>
-      </c>
-      <c r="I5" s="14" t="s">
-        <v>18</v>
-      </c>
-      <c r="J5" s="14" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="6" spans="1:10" ht="15" thickTop="1" x14ac:dyDescent="0.35">
-      <c r="A6" t="s">
-        <v>23</v>
-      </c>
       <c r="B6" s="3">
-        <f>ROUND(SS_att!H2,0)</f>
-        <v>34</v>
-      </c>
-      <c r="C6" s="3">
-        <f>ROUND(SS_att!G2,0)</f>
-        <v>36</v>
-      </c>
-      <c r="D6" s="3">
-        <f>ROUND(SS_att!K2,2)</f>
-        <v>0.71</v>
-      </c>
-      <c r="E6" s="3">
         <f>ROUND(SS_att!B2,0)</f>
         <v>31</v>
       </c>
-      <c r="F6" s="3">
+      <c r="C6" s="3">
         <f>ROUND(SS_att!C2,0)</f>
         <v>31</v>
       </c>
-      <c r="G6" s="3">
+      <c r="D6" s="3">
         <f>ROUND(SS_att!E2,0)</f>
         <v>37</v>
       </c>
-      <c r="H6" s="3">
+      <c r="E6" s="3">
+        <f>ROUND(SS_att!L2,2)</f>
+        <v>0.16</v>
+      </c>
+      <c r="F6" s="3">
         <f>ROUND(SS_att!D2,0)</f>
         <v>32</v>
       </c>
-      <c r="I6" s="3">
+      <c r="G6" s="3">
         <f>ROUND(SS_att!F2,0)</f>
         <v>34</v>
       </c>
-      <c r="J6" s="3">
-        <f>ROUND(SS_att!J2,2)</f>
-        <v>0.38</v>
-      </c>
-    </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="H6" s="3">
+        <f>ROUND(SS_att!M2,2)</f>
+        <v>0.56999999999999995</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.35">
       <c r="B7" s="3" t="str">
-        <f>CONCATENATE("(",ROUND(SS_att!H3,1),")")</f>
-        <v>(0.8)</v>
-      </c>
-      <c r="C7" s="3" t="str">
-        <f>CONCATENATE("(",ROUND(SS_att!G3,1),")")</f>
-        <v>(1.3)</v>
-      </c>
-      <c r="E7" s="3" t="str">
         <f>CONCATENATE("(",ROUND(SS_att!B3,1),")")</f>
         <v>(2.2)</v>
       </c>
-      <c r="F7" s="3" t="str">
+      <c r="C7" s="3" t="str">
         <f>CONCATENATE("(",ROUND(SS_att!C3,1),")")</f>
         <v>(2.3)</v>
       </c>
-      <c r="G7" s="3" t="str">
+      <c r="D7" s="3" t="str">
         <f>CONCATENATE("(",ROUND(SS_att!E3,1),")")</f>
         <v>(2.6)</v>
       </c>
-      <c r="H7" s="3" t="str">
+      <c r="F7" s="3" t="str">
         <f>CONCATENATE("(",ROUND(SS_att!D3,1),")")</f>
         <v>(2.4)</v>
       </c>
-      <c r="I7" s="3" t="str">
+      <c r="G7" s="3" t="str">
         <f>CONCATENATE("(",ROUND(SS_att!F3,1),")")</f>
         <v>(1.7)</v>
       </c>
     </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
-        <v>24</v>
-      </c>
-      <c r="C8" s="3">
-        <f>ROUND(SS_att!G10,2)</f>
-        <v>0.78</v>
-      </c>
-      <c r="E8" s="3">
+        <v>16</v>
+      </c>
+      <c r="B8" s="3">
         <f>ROUND(SS_att!B10,2)</f>
         <v>0.77</v>
       </c>
-      <c r="F8" s="3">
+      <c r="C8" s="3">
         <f>ROUND(SS_att!C10,2)</f>
         <v>0.75</v>
       </c>
-      <c r="G8" s="3">
+      <c r="D8" s="3">
         <f>ROUND(SS_att!E10,2)</f>
         <v>0.77</v>
       </c>
-      <c r="H8" s="3">
+      <c r="E8" s="3">
+        <f>ROUND(SS_att!L10,2)</f>
+        <v>0.73</v>
+      </c>
+      <c r="F8" s="3">
         <f>ROUND(SS_att!D10,2)</f>
         <v>0.8</v>
       </c>
-      <c r="I8" s="3">
+      <c r="G8" s="3">
         <f>ROUND(SS_att!F10,2)</f>
         <v>0.79</v>
       </c>
-      <c r="J8" s="3">
-        <f>ROUND(SS_att!J10,2)</f>
-        <v>0.46</v>
-      </c>
-    </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="C9" s="3" t="str">
-        <f>CONCATENATE("(",ROUND(SS_att!G11,2),")")</f>
-        <v>(0.01)</v>
-      </c>
-      <c r="E9" s="3" t="str">
+      <c r="H8" s="3">
+        <f>ROUND(SS_att!M10,2)</f>
+        <v>0.44</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="B9" s="3" t="str">
         <f>CONCATENATE("(",ROUND(SS_att!B11,2),")")</f>
         <v>(0.02)</v>
       </c>
-      <c r="F9" s="3" t="str">
+      <c r="C9" s="3" t="str">
         <f>CONCATENATE("(",ROUND(SS_att!C11,2),")")</f>
         <v>(0.03)</v>
       </c>
-      <c r="G9" s="3" t="str">
+      <c r="D9" s="3" t="str">
         <f>CONCATENATE("(",ROUND(SS_att!E11,2),")")</f>
         <v>(0.02)</v>
       </c>
-      <c r="H9" s="3" t="str">
+      <c r="F9" s="3" t="str">
         <f>CONCATENATE("(",ROUND(SS_att!D11,2),")")</f>
         <v>(0.02)</v>
       </c>
-      <c r="I9" s="3" t="str">
+      <c r="G9" s="3" t="str">
         <f>CONCATENATE("(",ROUND(SS_att!F11,2),")")</f>
         <v>(0.02)</v>
       </c>
     </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
-        <v>22</v>
-      </c>
-      <c r="C10" s="3">
-        <f>ROUND(SS_att!G8,2)</f>
-        <v>0.98</v>
-      </c>
-      <c r="E10" s="3">
+        <v>14</v>
+      </c>
+      <c r="B10" s="3">
         <f>ROUND(SS_att!B8,2)</f>
         <v>0.97</v>
       </c>
-      <c r="F10" s="3">
+      <c r="C10" s="3">
         <f>ROUND(SS_att!C8,2)</f>
         <v>0.96</v>
       </c>
-      <c r="G10" s="3">
+      <c r="D10" s="3">
         <f>ROUND(SS_att!E8,2)</f>
         <v>0.97</v>
       </c>
-      <c r="H10" s="3">
+      <c r="E10" s="3">
+        <f>ROUND(SS_att!L8,2)</f>
+        <v>0.59</v>
+      </c>
+      <c r="F10" s="3">
         <f>ROUND(SS_att!D8,2)</f>
         <v>0.98</v>
       </c>
-      <c r="I10" s="3">
+      <c r="G10" s="3">
         <f>ROUND(SS_att!F8,2)</f>
         <v>0.99</v>
       </c>
-      <c r="J10" s="3">
-        <f>ROUND(SS_att!J8,2)</f>
-        <v>0.03</v>
-      </c>
-    </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="C11" s="3" t="str">
-        <f>CONCATENATE("(",ROUND(SS_att!G9,3),")")</f>
-        <v>(0.003)</v>
-      </c>
-      <c r="E11" s="3" t="str">
+      <c r="H10" s="3">
+        <f>ROUND(SS_att!M8,2)</f>
+        <v>0.11</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="B11" s="3" t="str">
         <f>CONCATENATE("(",ROUND(SS_att!B9,3),")")</f>
         <v>(0.004)</v>
       </c>
-      <c r="F11" s="3" t="str">
+      <c r="C11" s="3" t="str">
         <f>CONCATENATE("(",ROUND(SS_att!C9,3),")")</f>
         <v>(0.008)</v>
       </c>
-      <c r="G11" s="3" t="str">
+      <c r="D11" s="3" t="str">
         <f>CONCATENATE("(",ROUND(SS_att!E9,3),")")</f>
         <v>(0.006)</v>
       </c>
-      <c r="H11" s="3" t="str">
+      <c r="F11" s="3" t="str">
         <f>CONCATENATE("(",ROUND(SS_att!D9,3),")")</f>
         <v>(0.004)</v>
       </c>
-      <c r="I11" s="3" t="str">
+      <c r="G11" s="3" t="str">
         <f>CONCATENATE("(",ROUND(SS_att!F9,3),")")</f>
         <v>(0.003)</v>
       </c>
     </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A12" t="s">
-        <v>25</v>
-      </c>
-      <c r="B12" s="3" t="s">
-        <v>26</v>
-      </c>
-      <c r="C12" s="3">
-        <f>SS_att!G4</f>
-        <v>180</v>
-      </c>
-      <c r="E12" s="3">
-        <f>SS_att!B4</f>
-        <v>84</v>
-      </c>
-      <c r="F12" s="3">
-        <f>SS_att!C4</f>
-        <v>80</v>
-      </c>
-      <c r="G12" s="3">
-        <f>SS_att!E4</f>
-        <v>93</v>
-      </c>
-      <c r="H12" s="3">
-        <f>SS_att!D4</f>
-        <v>68</v>
-      </c>
-      <c r="I12" s="3">
-        <f>SS_att!F4</f>
-        <v>82</v>
-      </c>
-    </row>
-    <row r="13" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A13" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="B13" s="5">
-        <f>SS_att!H6</f>
-        <v>13534</v>
-      </c>
-      <c r="C13" s="5">
-        <f>SS_att!G6</f>
-        <v>180</v>
-      </c>
-      <c r="D13" s="5"/>
-      <c r="E13" s="5">
+    <row r="12" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A12" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="B12" s="5">
         <f>SS_att!B6</f>
         <v>2585</v>
       </c>
-      <c r="F13" s="5">
+      <c r="C12" s="5">
         <f>SS_att!C6</f>
         <v>2465</v>
       </c>
-      <c r="G13" s="5">
+      <c r="D12" s="5">
         <f>SS_att!E6</f>
         <v>3406</v>
       </c>
-      <c r="H13" s="5">
+      <c r="E12" s="14"/>
+      <c r="F12" s="5">
         <f>SS_att!D6</f>
         <v>2143</v>
       </c>
-      <c r="I13" s="5">
+      <c r="G12" s="5">
         <f>SS_att!F6</f>
-        <v>2755</v>
-      </c>
-      <c r="J13" s="5"/>
-    </row>
-    <row r="14" spans="1:10" ht="15" thickTop="1" x14ac:dyDescent="0.35"/>
+        <v>2753</v>
+      </c>
+      <c r="H12" s="5"/>
+    </row>
+    <row r="13" spans="1:8" ht="15" thickTop="1" x14ac:dyDescent="0.35"/>
   </sheetData>
   <mergeCells count="3">
-    <mergeCell ref="B3:J3"/>
-    <mergeCell ref="F4:G4"/>
-    <mergeCell ref="H4:I4"/>
+    <mergeCell ref="B3:H3"/>
+    <mergeCell ref="F4:H4"/>
+    <mergeCell ref="C4:E4"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
description of experiment figs
</commit_message>
<xml_diff>
--- a/Tables/SS.xlsx
+++ b/Tables/SS.xlsx
@@ -1,6 +1,6 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24827"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\isaac\Dropbox\Apps\ShareLaTeX\Donde2020\Tables\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0E64E179-18A2-43A0-9DA4-2410346A3E09}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{655C151C-D549-491D-AE82-3E2710791C28}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-10695" windowWidth="29040" windowHeight="15720" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-28365" yWindow="-9315" windowWidth="12915" windowHeight="7470" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="SS_admin" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
     <sheet name="SS" sheetId="5" r:id="rId5"/>
     <sheet name="Attrition" sheetId="6" r:id="rId6"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="191029" fullCalcOnLoad="true"/>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
@@ -123,7 +123,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="8">
+  <borders count="6">
     <border>
       <left/>
       <right/>
@@ -156,17 +156,6 @@
     <border>
       <left/>
       <right/>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="medium">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
       <top/>
       <bottom style="double">
         <color indexed="64"/>
@@ -176,19 +165,8 @@
     <border>
       <left/>
       <right/>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="double">
-        <color indexed="64"/>
-      </top>
-      <bottom style="double">
+      <top/>
+      <bottom style="thin">
         <color indexed="64"/>
       </bottom>
       <diagonal/>
@@ -196,10 +174,8 @@
     <border>
       <left/>
       <right/>
-      <top style="medium">
-        <color indexed="64"/>
-      </top>
-      <bottom style="double">
+      <top/>
+      <bottom style="medium">
         <color indexed="64"/>
       </bottom>
       <diagonal/>
@@ -210,48 +186,50 @@
   </cellStyleXfs>
   <cellXfs count="19">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="true"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="true"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="true">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="true" applyAlignment="true">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="true" applyAlignment="true">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment wrapText="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="true">
+      <alignment wrapText="true"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="true" applyAlignment="true">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="true" applyAlignment="true">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="true" applyAlignment="true">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="true" applyAlignment="true">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="true"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="true" applyAlignment="true">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="true" applyAlignment="true">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="true" applyAlignment="true">
+      <alignment horizontal="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="true" applyAlignment="true">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="true" applyAlignment="true">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="true"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="true" applyAlignment="true">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -576,137 +554,137 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData>
-    <row r="2" spans="2:13" x14ac:dyDescent="0.35">
+    <row r="2" x14ac:dyDescent="0.35">
       <c r="B2">
-        <v>2288.9361702127658</v>
+        <v>2301.0995770857362</v>
       </c>
       <c r="C2">
-        <v>2130.5496957403652</v>
+        <v>2147.1437198067633</v>
       </c>
       <c r="D2">
-        <v>2135.8329444703686</v>
+        <v>2132.9021789522485</v>
       </c>
       <c r="E2">
-        <v>2179.709923664122</v>
+        <v>2182.1076833527359</v>
       </c>
       <c r="F2">
-        <v>2089.8928441699964</v>
+        <v>2089.2792630057802</v>
       </c>
       <c r="G2">
-        <v>2024.022346368715</v>
+        <v>2161.6666666666665</v>
       </c>
       <c r="H2">
-        <v>2164.3383341955509</v>
+        <v>2171.5310435931306</v>
       </c>
       <c r="K2">
-        <v>0.31380642461500552</v>
+        <v>0.9541119628933088</v>
       </c>
       <c r="L2">
-        <v>0.32029811665546248</v>
+        <v>0.32512302780150443</v>
       </c>
       <c r="M2">
-        <v>0.13737619175017129</v>
-      </c>
-    </row>
-    <row r="3" spans="2:13" x14ac:dyDescent="0.35">
+        <v>0.1049606267091812</v>
+      </c>
+    </row>
+    <row r="3" x14ac:dyDescent="0.35">
       <c r="B3">
-        <v>78.79053698585561</v>
+        <v>79.41696803972188</v>
       </c>
       <c r="C3">
-        <v>72.608792900438672</v>
+        <v>71.911953944693522</v>
       </c>
       <c r="D3">
-        <v>73.768907168664811</v>
+        <v>73.985411575168982</v>
       </c>
       <c r="E3">
-        <v>66.211707129485063</v>
+        <v>64.994187260506564</v>
       </c>
       <c r="F3">
-        <v>64.891311599127775</v>
+        <v>64.541278696715779</v>
       </c>
       <c r="G3">
-        <v>137.64917255699254</v>
+        <v>171.03256538840651</v>
       </c>
       <c r="H3">
-        <v>31.579556901935923</v>
-      </c>
-    </row>
-    <row r="4" spans="2:13" x14ac:dyDescent="0.35">
+        <v>31.454802670595651</v>
+      </c>
+    </row>
+    <row r="4" x14ac:dyDescent="0.35">
       <c r="B4">
-        <v>0.87814313346228234</v>
+        <v>0.87812379853902345</v>
       </c>
       <c r="C4">
-        <v>0.8908722109533469</v>
+        <v>0.89130434782608692</v>
       </c>
       <c r="D4">
-        <v>0.88520765282314517</v>
+        <v>0.88317107093184977</v>
       </c>
       <c r="E4">
-        <v>0.8476218438050499</v>
+        <v>0.84662398137369033</v>
       </c>
       <c r="F4">
-        <v>0.82891391209589538</v>
+        <v>0.82947976878612717</v>
       </c>
       <c r="G4">
         <v>0.83333331677648759</v>
       </c>
       <c r="H4">
-        <v>0.86328702313181849</v>
+        <v>0.86290914406427177</v>
       </c>
       <c r="K4">
-        <v>0.51794407065163461</v>
+        <v>0.52347675751961098</v>
       </c>
       <c r="L4">
-        <v>0.71839367357685091</v>
+        <v>0.70540311975926762</v>
       </c>
       <c r="M4">
-        <v>0.62258453328249541</v>
-      </c>
-    </row>
-    <row r="5" spans="2:13" x14ac:dyDescent="0.35">
+        <v>0.64425763902730926</v>
+      </c>
+    </row>
+    <row r="5" x14ac:dyDescent="0.35">
       <c r="B5">
-        <v>4.0033960932364658E-2</v>
+        <v>0.039962138649154974</v>
       </c>
       <c r="C5">
-        <v>3.3821563907464283E-2</v>
+        <v>0.033776765366283587</v>
       </c>
       <c r="D5">
-        <v>3.5723933418048991E-2</v>
+        <v>0.036353445955306977</v>
       </c>
       <c r="E5">
-        <v>4.1755107742770553E-2</v>
+        <v>0.042138188314307712</v>
       </c>
       <c r="F5">
-        <v>4.8523915015899789E-2</v>
+        <v>0.04836901048168215</v>
       </c>
       <c r="G5">
-        <v>4.3154986380046355E-2</v>
+        <v>0.043154986380046355</v>
       </c>
       <c r="H5">
-        <v>1.8385912471474301E-2</v>
-      </c>
-    </row>
-    <row r="6" spans="2:13" x14ac:dyDescent="0.35">
+        <v>0.018444101393584482</v>
+      </c>
+    </row>
+    <row r="6" x14ac:dyDescent="0.35">
       <c r="B6">
-        <v>2585</v>
+        <v>2601</v>
       </c>
       <c r="C6">
-        <v>2465</v>
+        <v>2484</v>
       </c>
       <c r="D6">
-        <v>2143</v>
+        <v>2157</v>
       </c>
       <c r="E6">
-        <v>3406</v>
+        <v>3436</v>
       </c>
       <c r="F6">
-        <v>2753</v>
+        <v>2768</v>
       </c>
       <c r="G6">
         <v>180</v>
       </c>
       <c r="H6">
-        <v>13532</v>
+        <v>13626</v>
       </c>
     </row>
   </sheetData>
@@ -718,68 +696,68 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="B2:M11"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="true" workbookViewId="0">
       <selection activeCell="J1" sqref="J1:J13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData>
-    <row r="2" spans="2:13" x14ac:dyDescent="0.35">
+    <row r="2" x14ac:dyDescent="0.35">
       <c r="B2">
-        <v>30.773809523809526</v>
+        <v>30.892857142857142</v>
       </c>
       <c r="C2">
-        <v>30.8125</v>
+        <v>31</v>
       </c>
       <c r="D2">
-        <v>31.514705882352942</v>
+        <v>31.691176470588236</v>
       </c>
       <c r="E2">
-        <v>36.623655913978496</v>
+        <v>36.892473118279568</v>
       </c>
       <c r="F2">
-        <v>33.573170731707314</v>
+        <v>33.731707317073173</v>
       </c>
       <c r="G2">
-        <v>36.085999441146853</v>
+        <v>36.021871704525417</v>
       </c>
       <c r="H2">
-        <v>33.811720441918965</v>
+        <v>33.919824372767593</v>
       </c>
       <c r="K2">
-        <v>0.7062867593846045</v>
+        <v>0.72947061051374762</v>
       </c>
       <c r="L2">
-        <v>0.1619408349718037</v>
+        <v>0.15905141841818249</v>
       </c>
       <c r="M2">
-        <v>0.569666506831908</v>
-      </c>
-    </row>
-    <row r="3" spans="2:13" x14ac:dyDescent="0.35">
+        <v>0.56873437132818427</v>
+      </c>
+    </row>
+    <row r="3" x14ac:dyDescent="0.35">
       <c r="B3">
-        <v>2.191515427974172</v>
+        <v>2.1952210296988395</v>
       </c>
       <c r="C3">
-        <v>2.3014231803523866</v>
+        <v>2.3418320211300112</v>
       </c>
       <c r="D3">
-        <v>2.3664961566181195</v>
+        <v>2.3739752054504661</v>
       </c>
       <c r="E3">
-        <v>2.6016462754055563</v>
+        <v>2.6475381476904647</v>
       </c>
       <c r="F3">
-        <v>1.7423667125082001</v>
+        <v>1.7640090781652411</v>
       </c>
       <c r="G3">
-        <v>1.2515869857807669</v>
+        <v>1.2524285128627448</v>
       </c>
       <c r="H3">
-        <v>0.80795077985236741</v>
-      </c>
-    </row>
-    <row r="4" spans="2:13" x14ac:dyDescent="0.35">
+        <v>0.81507699640653886</v>
+      </c>
+    </row>
+    <row r="4" x14ac:dyDescent="0.35">
       <c r="B4">
         <v>84</v>
       </c>
@@ -799,10 +777,10 @@
         <v>180</v>
       </c>
       <c r="H4">
-        <v>83.872893881170555</v>
-      </c>
-    </row>
-    <row r="5" spans="2:13" x14ac:dyDescent="0.35">
+        <v>83.86936738587994</v>
+      </c>
+    </row>
+    <row r="5" x14ac:dyDescent="0.35">
       <c r="B5">
         <v>0</v>
       </c>
@@ -822,122 +800,122 @@
         <v>0</v>
       </c>
       <c r="H5">
-        <v>0.48138428798549088</v>
-      </c>
-    </row>
-    <row r="6" spans="2:13" x14ac:dyDescent="0.35">
+        <v>0.48193515492329214</v>
+      </c>
+    </row>
+    <row r="6" x14ac:dyDescent="0.35">
       <c r="B6">
-        <v>2585</v>
+        <v>2601</v>
       </c>
       <c r="C6">
-        <v>2465</v>
+        <v>2484</v>
       </c>
       <c r="D6">
-        <v>2143</v>
+        <v>2157</v>
       </c>
       <c r="E6">
-        <v>3406</v>
+        <v>3436</v>
       </c>
       <c r="F6">
-        <v>2753</v>
+        <v>2768</v>
       </c>
       <c r="G6">
         <v>180</v>
       </c>
       <c r="H6">
-        <v>13532</v>
-      </c>
-    </row>
-    <row r="8" spans="2:13" x14ac:dyDescent="0.35">
+        <v>13626</v>
+      </c>
+    </row>
+    <row r="8" x14ac:dyDescent="0.35">
       <c r="B8">
-        <v>0.97445972495088407</v>
+        <v>0.98280098280098283</v>
       </c>
       <c r="C8">
-        <v>0.96486628211851078</v>
+        <v>0.97273203985317247</v>
       </c>
       <c r="D8">
-        <v>0.98121798520204895</v>
+        <v>0.9869020501138952</v>
       </c>
       <c r="E8">
-        <v>0.97195571955719562</v>
+        <v>0.97860568056067876</v>
       </c>
       <c r="F8">
-        <v>0.98601083032490977</v>
+        <v>0.9887285843101894</v>
       </c>
       <c r="G8">
-        <v>0.9756258234519104</v>
+        <v>0.98183871271290113</v>
       </c>
       <c r="L8">
-        <v>0.58825046706800044</v>
+        <v>0.4682775695018524</v>
       </c>
       <c r="M8">
-        <v>0.11110410557859279</v>
-      </c>
-    </row>
-    <row r="9" spans="2:13" x14ac:dyDescent="0.35">
+        <v>0.48848582659027617</v>
+      </c>
+    </row>
+    <row r="9" x14ac:dyDescent="0.35">
       <c r="B9">
-        <v>4.4833017561553556E-3</v>
+        <v>0.0040156175496241656</v>
       </c>
       <c r="C9">
-        <v>8.2133083066849039E-3</v>
+        <v>0.0073961905116490204</v>
       </c>
       <c r="D9">
-        <v>3.8746463630254615E-3</v>
+        <v>0.0033401981602603041</v>
       </c>
       <c r="E9">
-        <v>6.3019449093397522E-3</v>
+        <v>0.0059580084747241947</v>
       </c>
       <c r="F9">
-        <v>3.1940620474848742E-3</v>
+        <v>0.0029388029720992899</v>
       </c>
       <c r="G9">
-        <v>2.5465995142291463E-3</v>
-      </c>
-    </row>
-    <row r="10" spans="2:13" x14ac:dyDescent="0.35">
+        <v>0.0023277574303601015</v>
+      </c>
+    </row>
+    <row r="10" x14ac:dyDescent="0.35">
       <c r="B10">
-        <v>0.76750483558994198</v>
+        <v>0.76893502499038835</v>
       </c>
       <c r="C10">
-        <v>0.74705643524157528</v>
+        <v>0.74738114423851731</v>
       </c>
       <c r="D10">
-        <v>0.80485527544351076</v>
+        <v>0.80380333951762528</v>
       </c>
       <c r="E10">
-        <v>0.77334116265413977</v>
+        <v>0.77211874272409775</v>
       </c>
       <c r="F10">
-        <v>0.79425663395129042</v>
+        <v>0.79284164859002171</v>
       </c>
       <c r="G10">
-        <v>0.77672885292575111</v>
+        <v>0.77628152667212258</v>
       </c>
       <c r="L10">
-        <v>0.72661768802378535</v>
+        <v>0.73908202673193557</v>
       </c>
       <c r="M10">
-        <v>0.44259059431665793</v>
-      </c>
-    </row>
-    <row r="11" spans="2:13" x14ac:dyDescent="0.35">
+        <v>0.49749765961667392</v>
+      </c>
+    </row>
+    <row r="11" x14ac:dyDescent="0.35">
       <c r="B11">
-        <v>2.0014887892783387E-2</v>
+        <v>0.019892859098745899</v>
       </c>
       <c r="C11">
-        <v>2.5519225148308459E-2</v>
+        <v>0.025623636641152012</v>
       </c>
       <c r="D11">
-        <v>2.3819765376005251E-2</v>
+        <v>0.023871935695980506</v>
       </c>
       <c r="E11">
-        <v>2.3224560628884606E-2</v>
+        <v>0.023661163960051093</v>
       </c>
       <c r="F11">
-        <v>2.2172410929511183E-2</v>
+        <v>0.022472107685513335</v>
       </c>
       <c r="G11">
-        <v>1.0397246226653783E-2</v>
+        <v>0.010494345328496491</v>
       </c>
     </row>
   </sheetData>
@@ -955,374 +933,374 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData>
-    <row r="2" spans="2:13" x14ac:dyDescent="0.35">
+    <row r="2" x14ac:dyDescent="0.35">
       <c r="B2">
-        <v>0.75433911882510019</v>
+        <v>0.75514266755142667</v>
       </c>
       <c r="C2">
-        <v>0.72241029113067023</v>
+        <v>0.72237196765498657</v>
       </c>
       <c r="D2">
-        <v>0.72483221476510062</v>
+        <v>0.72635983263598325</v>
       </c>
       <c r="E2">
-        <v>0.71756487025948101</v>
+        <v>0.71811414392059558</v>
       </c>
       <c r="F2">
-        <v>0.74007444168734493</v>
+        <v>0.74058060531192094</v>
       </c>
       <c r="G2">
         <v>0.74980252764612954</v>
       </c>
       <c r="H2">
-        <v>0.73861601930411769</v>
+        <v>0.73897857808134115</v>
       </c>
       <c r="K2">
-        <v>0.11208209991636051</v>
+        <v>0.12370990152692971</v>
       </c>
       <c r="L2">
-        <v>0.21626044184189269</v>
+        <v>0.20316365915662879</v>
       </c>
       <c r="M2">
-        <v>0.52326338075561829</v>
-      </c>
-    </row>
-    <row r="3" spans="2:13" x14ac:dyDescent="0.35">
+        <v>0.53421473315735057</v>
+      </c>
+    </row>
+    <row r="3" x14ac:dyDescent="0.35">
       <c r="B3">
-        <v>1.6556851714845944E-2</v>
+        <v>0.016425991245592318</v>
       </c>
       <c r="C3">
-        <v>1.6718261868105887E-2</v>
+        <v>0.016091100265249764</v>
       </c>
       <c r="D3">
-        <v>2.0329367912066382E-2</v>
+        <v>0.020324180320801286</v>
       </c>
       <c r="E3">
-        <v>1.5034947849718417E-2</v>
+        <v>0.015140443704992809</v>
       </c>
       <c r="F3">
-        <v>1.2972552271708279E-2</v>
+        <v>0.012828726752602795</v>
       </c>
       <c r="G3">
-        <v>9.0149695175873682E-3</v>
+        <v>0.0090149695175873699</v>
       </c>
       <c r="H3">
-        <v>5.7025026346927427E-3</v>
-      </c>
-    </row>
-    <row r="4" spans="2:13" x14ac:dyDescent="0.35">
+        <v>0.0056750398759389097</v>
+      </c>
+    </row>
+    <row r="4" x14ac:dyDescent="0.35">
       <c r="B4">
-        <v>43.221586847748391</v>
+        <v>43.197583511016347</v>
       </c>
       <c r="C4">
-        <v>43.196519216823788</v>
+        <v>43.214285714285715</v>
       </c>
       <c r="D4">
-        <v>43.000918273645546</v>
+        <v>43.014652014652015</v>
       </c>
       <c r="E4">
-        <v>44.037746170678339</v>
+        <v>44.068119891008173</v>
       </c>
       <c r="F4">
-        <v>43.103425559947297</v>
+        <v>43.085413929040733</v>
       </c>
       <c r="G4">
         <v>43.05681818181818</v>
       </c>
       <c r="H4">
-        <v>43.242875052235689</v>
+        <v>43.246039686509924</v>
       </c>
       <c r="K4">
-        <v>0.46505187451014002</v>
+        <v>0.45869706596643639</v>
       </c>
       <c r="L4">
-        <v>0.55078041441066639</v>
+        <v>0.51811943398266236</v>
       </c>
       <c r="M4">
-        <v>0.96669904994360278</v>
-      </c>
-    </row>
-    <row r="5" spans="2:13" x14ac:dyDescent="0.35">
+        <v>0.97646568723149629</v>
+      </c>
+    </row>
+    <row r="5" x14ac:dyDescent="0.35">
       <c r="B5">
-        <v>0.56543539980823898</v>
+        <v>0.56359423339355974</v>
       </c>
       <c r="C5">
-        <v>0.76286676286261612</v>
+        <v>0.77069700997930024</v>
       </c>
       <c r="D5">
-        <v>0.64748270122917573</v>
+        <v>0.66004082042892598</v>
       </c>
       <c r="E5">
-        <v>0.6071316707886486</v>
+        <v>0.60465537492814869</v>
       </c>
       <c r="F5">
-        <v>0.51886206376869348</v>
+        <v>0.51619884617405898</v>
       </c>
       <c r="G5">
         <v>0.31582069920051542</v>
       </c>
       <c r="H5">
-        <v>0.21108025671162237</v>
-      </c>
-    </row>
-    <row r="6" spans="2:13" x14ac:dyDescent="0.35">
+        <v>0.21148102499151927</v>
+      </c>
+    </row>
+    <row r="6" x14ac:dyDescent="0.35">
       <c r="B6">
-        <v>3144.2258572273172</v>
+        <v>3145.352544966549</v>
       </c>
       <c r="C6">
-        <v>2978.4851423284058</v>
+        <v>2985.2732691622746</v>
       </c>
       <c r="D6">
-        <v>3012.0756539184413</v>
+        <v>3010.3149184642348</v>
       </c>
       <c r="E6">
-        <v>3111.984225240552</v>
+        <v>3110.9508585695362</v>
       </c>
       <c r="F6">
-        <v>3082.3294608440233</v>
+        <v>3082.6830472633487</v>
       </c>
       <c r="G6">
-        <v>3192.3473313966551</v>
+        <v>3192.3481642889119</v>
       </c>
       <c r="H6">
-        <v>3111.1842893999233</v>
+        <v>3111.7794650246028</v>
       </c>
       <c r="K6">
-        <v>0.15227626931075919</v>
+        <v>0.15568188813603681</v>
       </c>
       <c r="L6">
-        <v>0.30747604910588372</v>
+        <v>0.34382243121919293</v>
       </c>
       <c r="M6">
-        <v>0.43244773970978462</v>
-      </c>
-    </row>
-    <row r="7" spans="2:13" x14ac:dyDescent="0.35">
+        <v>0.41658257300111001</v>
+      </c>
+    </row>
+    <row r="7" x14ac:dyDescent="0.35">
       <c r="B7">
-        <v>68.001187760083468</v>
+        <v>68.222299405324407</v>
       </c>
       <c r="C7">
-        <v>87.087553008590618</v>
+        <v>88.361354683798069</v>
       </c>
       <c r="D7">
-        <v>76.712679194050935</v>
+        <v>76.470442299269308</v>
       </c>
       <c r="E7">
-        <v>84.619693541464599</v>
+        <v>84.469381845420969</v>
       </c>
       <c r="F7">
-        <v>99.097081529762747</v>
+        <v>99.031452584314096</v>
       </c>
       <c r="G7">
-        <v>75.187908028614046</v>
+        <v>75.187897820076458</v>
       </c>
       <c r="H7">
-        <v>35.717284716677206</v>
-      </c>
-    </row>
-    <row r="8" spans="2:13" x14ac:dyDescent="0.35">
+        <v>35.740522483170373</v>
+      </c>
+    </row>
+    <row r="8" x14ac:dyDescent="0.35">
       <c r="B8">
-        <v>0.89210155148095904</v>
+        <v>0.89052631578947372</v>
       </c>
       <c r="C8">
-        <v>0.89858156028368796</v>
+        <v>0.89978828510938602</v>
       </c>
       <c r="D8">
-        <v>0.89295516925892038</v>
+        <v>0.89132420091324205</v>
       </c>
       <c r="E8">
-        <v>0.91017316017316019</v>
+        <v>0.91070467993544912</v>
       </c>
       <c r="F8">
-        <v>0.89452603471295056</v>
+        <v>0.89414114513981358</v>
       </c>
       <c r="G8">
         <v>0.88422131147540983</v>
       </c>
       <c r="H8">
-        <v>0.8928130402568536</v>
+        <v>0.89267531614386597</v>
       </c>
       <c r="K8">
-        <v>0.2165470378557727</v>
+        <v>0.225273760595539</v>
       </c>
       <c r="L8">
-        <v>0.46842009181914179</v>
+        <v>0.40550231444286611</v>
       </c>
       <c r="M8">
-        <v>0.98594182922713058</v>
-      </c>
-    </row>
-    <row r="9" spans="2:13" x14ac:dyDescent="0.35">
+        <v>0.96738092930936548</v>
+      </c>
+    </row>
+    <row r="9" x14ac:dyDescent="0.35">
       <c r="B9">
-        <v>1.1437812800195962E-2</v>
+        <v>0.011504362429475282</v>
       </c>
       <c r="C9">
-        <v>1.0521714206780004E-2</v>
+        <v>0.010579094696170152</v>
       </c>
       <c r="D9">
-        <v>1.4321027388666783E-2</v>
+        <v>0.014535413795478428</v>
       </c>
       <c r="E9">
-        <v>9.955349958628441E-3</v>
+        <v>0.0099323761115656124</v>
       </c>
       <c r="F9">
-        <v>9.4444603824305161E-3</v>
+        <v>0.0094836902763061059</v>
       </c>
       <c r="G9">
-        <v>1.0533724370448033E-2</v>
+        <v>0.010533724370448033</v>
       </c>
       <c r="H9">
-        <v>5.201314800898328E-3</v>
-      </c>
-    </row>
-    <row r="10" spans="2:13" x14ac:dyDescent="0.35">
+        <v>0.0052054873450900745</v>
+      </c>
+    </row>
+    <row r="10" x14ac:dyDescent="0.35">
       <c r="B10">
-        <v>92.746680286006125</v>
+        <v>92.725089422585597</v>
       </c>
       <c r="C10">
         <v>92.193231441048042</v>
       </c>
       <c r="D10">
-        <v>93.658892128279888</v>
+        <v>93.655192532088677</v>
       </c>
       <c r="E10">
-        <v>93.714012982054214</v>
+        <v>93.716412213740455</v>
       </c>
       <c r="F10">
-        <v>93.339981447124302</v>
+        <v>93.339202965708992</v>
       </c>
       <c r="G10">
         <v>91.835829749369722</v>
       </c>
       <c r="H10">
-        <v>92.642189978264696</v>
+        <v>92.639685150375939</v>
       </c>
       <c r="K10">
-        <v>1.1531094878537999E-3</v>
+        <v>0.0011989512452381999</v>
       </c>
       <c r="L10">
-        <v>0.18126873036276731</v>
+        <v>0.1753183756276937</v>
       </c>
       <c r="M10">
-        <v>0.5015072314659057</v>
-      </c>
-    </row>
-    <row r="11" spans="2:13" x14ac:dyDescent="0.35">
+        <v>0.48869910509747372</v>
+      </c>
+    </row>
+    <row r="11" x14ac:dyDescent="0.35">
       <c r="B11">
-        <v>0.53706935836467462</v>
+        <v>0.54084732630950216</v>
       </c>
       <c r="C11">
-        <v>0.83856879215694513</v>
+        <v>0.83856879215694502</v>
       </c>
       <c r="D11">
-        <v>0.59084286834349808</v>
+        <v>0.59030374500190863</v>
       </c>
       <c r="E11">
-        <v>0.45528703025952877</v>
+        <v>0.45517920772459858</v>
       </c>
       <c r="F11">
-        <v>0.59572969114264696</v>
+        <v>0.59487333389159291</v>
       </c>
       <c r="G11">
         <v>0.30818777366122274</v>
       </c>
       <c r="H11">
-        <v>0.20468275029985156</v>
-      </c>
-    </row>
-    <row r="12" spans="2:13" x14ac:dyDescent="0.35">
+        <v>0.20476842319378324</v>
+      </c>
+    </row>
+    <row r="12" x14ac:dyDescent="0.35">
       <c r="B12">
-        <v>0.65825522710886808</v>
+        <v>0.6597421203438395</v>
       </c>
       <c r="C12">
-        <v>0.66933721777130373</v>
+        <v>0.66884057971014488</v>
       </c>
       <c r="D12">
-        <v>0.64711359404096835</v>
+        <v>0.64716805942432687</v>
       </c>
       <c r="E12">
-        <v>0.66255605381165916</v>
+        <v>0.66276477146042367</v>
       </c>
       <c r="F12">
-        <v>0.6426092990978487</v>
+        <v>0.643598615916955</v>
       </c>
       <c r="G12">
         <v>0.59694943585457583</v>
       </c>
       <c r="H12">
-        <v>0.63250316589278177</v>
+        <v>0.63285064825728232</v>
       </c>
       <c r="K12">
-        <v>1.2796812933239999E-4</v>
+        <v>0.0001115253817344</v>
       </c>
       <c r="L12">
-        <v>0.92123910783208673</v>
+        <v>0.94338858432257511</v>
       </c>
       <c r="M12">
-        <v>0.82777141801359311</v>
-      </c>
-    </row>
-    <row r="13" spans="2:13" x14ac:dyDescent="0.35">
+        <v>0.81166552956809135</v>
+      </c>
+    </row>
+    <row r="13" x14ac:dyDescent="0.35">
       <c r="B13">
-        <v>1.9575506710528847E-2</v>
+        <v>0.019382047390071523</v>
       </c>
       <c r="C13">
-        <v>1.9664178070939481E-2</v>
+        <v>0.019329841394817811</v>
       </c>
       <c r="D13">
-        <v>2.3651650315642418E-2</v>
+        <v>0.024251483945742537</v>
       </c>
       <c r="E13">
-        <v>1.6910104498970228E-2</v>
+        <v>0.016843213086678365</v>
       </c>
       <c r="F13">
-        <v>1.6764309126234812E-2</v>
+        <v>0.016646508216829125</v>
       </c>
       <c r="G13">
-        <v>1.2957951584969644E-2</v>
+        <v>0.012957951584969644</v>
       </c>
       <c r="H13">
-        <v>7.4963906102697275E-3</v>
-      </c>
-    </row>
-    <row r="14" spans="2:13" x14ac:dyDescent="0.35">
+        <v>0.0074824965608947022</v>
+      </c>
+    </row>
+    <row r="14" x14ac:dyDescent="0.35">
       <c r="B14">
-        <v>2637</v>
+        <v>2636</v>
       </c>
       <c r="C14">
-        <v>2530</v>
+        <v>2534</v>
       </c>
       <c r="D14">
-        <v>2175</v>
+        <v>2179</v>
       </c>
       <c r="E14">
-        <v>3482</v>
+        <v>3494</v>
       </c>
       <c r="F14">
-        <v>2782</v>
+        <v>2791</v>
       </c>
       <c r="G14">
         <v>6919</v>
       </c>
       <c r="H14">
-        <v>20525</v>
-      </c>
-    </row>
-    <row r="16" spans="2:13" x14ac:dyDescent="0.35">
+        <v>20553</v>
+      </c>
+    </row>
+    <row r="16" x14ac:dyDescent="0.35">
       <c r="B16">
-        <v>2036</v>
+        <v>2035</v>
       </c>
       <c r="C16">
         <v>1907</v>
       </c>
       <c r="D16">
-        <v>1757</v>
+        <v>1756</v>
       </c>
       <c r="E16">
-        <v>2710</v>
+        <v>2711</v>
       </c>
       <c r="F16">
-        <v>2216</v>
+        <v>2218</v>
       </c>
       <c r="G16">
         <v>6919</v>
@@ -1343,317 +1321,317 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData>
-    <row r="2" spans="2:11" x14ac:dyDescent="0.35">
+    <row r="2" x14ac:dyDescent="0.35">
       <c r="B2">
-        <v>0.75578231292517006</v>
+        <v>0.75706594885598921</v>
       </c>
       <c r="C2">
-        <v>0.72473867595818819</v>
+        <v>0.72451790633608815</v>
       </c>
       <c r="D2">
-        <v>0.72472387425658458</v>
+        <v>0.72527472527472525</v>
       </c>
       <c r="E2">
-        <v>0.7164790174002047</v>
+        <v>0.71775417298937783</v>
       </c>
       <c r="F2">
-        <v>0.740276035131744</v>
+        <v>0.74111041796631316</v>
       </c>
       <c r="G2">
-        <v>0.73184796854521628</v>
+        <v>0.73263212569796132</v>
       </c>
       <c r="J2">
-        <v>0.19876896641301439</v>
+        <v>0.1834112165576095</v>
       </c>
       <c r="K2">
-        <v>0.49195240167249149</v>
-      </c>
-    </row>
-    <row r="3" spans="2:11" x14ac:dyDescent="0.35">
+        <v>0.47018825520502039</v>
+      </c>
+    </row>
+    <row r="3" x14ac:dyDescent="0.35">
       <c r="B3">
-        <v>1.6494973868034876E-2</v>
+        <v>0.016329938660297399</v>
       </c>
       <c r="C3">
-        <v>1.7691100137449553E-2</v>
+        <v>0.016037712453979815</v>
       </c>
       <c r="D3">
-        <v>2.0783334672938653E-2</v>
+        <v>0.020704066804602263</v>
       </c>
       <c r="E3">
-        <v>1.576793521344572E-2</v>
+        <v>0.015845064022229488</v>
       </c>
       <c r="F3">
-        <v>1.3130695539826494E-2</v>
+        <v>0.012945207155944546</v>
       </c>
       <c r="G3">
-        <v>7.5289195119028051E-3</v>
-      </c>
-    </row>
-    <row r="4" spans="2:11" x14ac:dyDescent="0.35">
+        <v>0.0073798781164302616</v>
+      </c>
+    </row>
+    <row r="4" x14ac:dyDescent="0.35">
       <c r="B4">
-        <v>43.217612809315867</v>
+        <v>43.164866810655148</v>
       </c>
       <c r="C4">
-        <v>43.13134328358209</v>
+        <v>43.174778761061944</v>
       </c>
       <c r="D4">
-        <v>42.956238361266294</v>
+        <v>42.960185185185182</v>
       </c>
       <c r="E4">
-        <v>43.905829596412559</v>
+        <v>43.95550611790879</v>
       </c>
       <c r="F4">
-        <v>43.081333333333333</v>
+        <v>43.072377158034527</v>
       </c>
       <c r="G4">
-        <v>43.306278280542983</v>
+        <v>43.315612287838405</v>
       </c>
       <c r="J4">
-        <v>0.64268457005413904</v>
+        <v>0.58878257193305883</v>
       </c>
       <c r="K4">
-        <v>0.95371567366848975</v>
-      </c>
-    </row>
-    <row r="5" spans="2:11" x14ac:dyDescent="0.35">
+        <v>0.97226330514763726</v>
+      </c>
+    </row>
+    <row r="5" x14ac:dyDescent="0.35">
       <c r="B5">
-        <v>0.57228204463326615</v>
+        <v>0.57302039418728534</v>
       </c>
       <c r="C5">
-        <v>0.77802775203513075</v>
+        <v>0.7869341141204792</v>
       </c>
       <c r="D5">
-        <v>0.63847586117189081</v>
+        <v>0.6516138308721301</v>
       </c>
       <c r="E5">
-        <v>0.61729446550591693</v>
+        <v>0.61205771211875037</v>
       </c>
       <c r="F5">
-        <v>0.51915566425229054</v>
+        <v>0.5175395496028099</v>
       </c>
       <c r="G5">
-        <v>0.28248392615092249</v>
-      </c>
-    </row>
-    <row r="6" spans="2:11" x14ac:dyDescent="0.35">
+        <v>0.2831845022118607</v>
+      </c>
+    </row>
+    <row r="6" x14ac:dyDescent="0.35">
       <c r="B6">
-        <v>3141.2189276129911</v>
+        <v>3151.8311879330831</v>
       </c>
       <c r="C6">
-        <v>2969.2540664157987</v>
+        <v>2977.8080010068757</v>
       </c>
       <c r="D6">
-        <v>2982.0820526759658</v>
+        <v>2987.6091755578368</v>
       </c>
       <c r="E6">
-        <v>3107.1898911642975</v>
+        <v>3114.8420998012557</v>
       </c>
       <c r="F6">
-        <v>3077.652576659777</v>
+        <v>3080.6487658710303</v>
       </c>
       <c r="G6">
-        <v>3062.2107548711087</v>
+        <v>3069.2245258990883</v>
       </c>
       <c r="J6">
-        <v>0.29045103565750929</v>
+        <v>0.29805537908350171</v>
       </c>
       <c r="K6">
-        <v>0.29728566162528908</v>
-      </c>
-    </row>
-    <row r="7" spans="2:11" x14ac:dyDescent="0.35">
+        <v>0.27369802702174151</v>
+      </c>
+    </row>
+    <row r="7" x14ac:dyDescent="0.35">
       <c r="B7">
-        <v>68.41471046880892</v>
+        <v>68.633705702668735</v>
       </c>
       <c r="C7">
-        <v>88.438762370272087</v>
+        <v>90.821567649747067</v>
       </c>
       <c r="D7">
-        <v>76.543605627057048</v>
+        <v>76.019238973365503</v>
       </c>
       <c r="E7">
-        <v>84.797934069022119</v>
+        <v>84.552913105159746</v>
       </c>
       <c r="F7">
-        <v>98.948225748151543</v>
+        <v>99.417675983085019</v>
       </c>
       <c r="G7">
-        <v>38.475753401046958</v>
-      </c>
-    </row>
-    <row r="8" spans="2:11" x14ac:dyDescent="0.35">
+        <v>38.649480296696282</v>
+      </c>
+    </row>
+    <row r="8" x14ac:dyDescent="0.35">
       <c r="B8">
-        <v>0.89280575539568341</v>
+        <v>0.89102564102564108</v>
       </c>
       <c r="C8">
-        <v>0.89715536105032823</v>
+        <v>0.89841498559077815</v>
       </c>
       <c r="D8">
-        <v>0.89424860853432286</v>
+        <v>0.89289012003693446</v>
       </c>
       <c r="E8">
-        <v>0.91004997223764572</v>
+        <v>0.91063596491228072</v>
       </c>
       <c r="F8">
-        <v>0.89399054692775148</v>
+        <v>0.89374579690652323</v>
       </c>
       <c r="G8">
-        <v>0.89846931610728831</v>
+        <v>0.89827442248817146</v>
       </c>
       <c r="J8">
-        <v>0.47512184769960331</v>
+        <v>0.42137792268207369</v>
       </c>
       <c r="K8">
-        <v>0.99580107322835887</v>
-      </c>
-    </row>
-    <row r="9" spans="2:11" x14ac:dyDescent="0.35">
+        <v>0.98364695237340527</v>
+      </c>
+    </row>
+    <row r="9" x14ac:dyDescent="0.35">
       <c r="B9">
-        <v>1.1622893010130052E-2</v>
+        <v>0.011699017063997981</v>
       </c>
       <c r="C9">
-        <v>1.0580674917488611E-2</v>
+        <v>0.010536449576402311</v>
       </c>
       <c r="D9">
-        <v>1.4180980099054998E-2</v>
+        <v>0.014414244480650894</v>
       </c>
       <c r="E9">
-        <v>9.8185033789223025E-3</v>
+        <v>0.0099893832545590311</v>
       </c>
       <c r="F9">
-        <v>9.4902417155907914E-3</v>
+        <v>0.0095382524633601719</v>
       </c>
       <c r="G9">
-        <v>4.8987197660100082E-3</v>
-      </c>
-    </row>
-    <row r="10" spans="2:11" x14ac:dyDescent="0.35">
+        <v>0.0049480485445660988</v>
+      </c>
+    </row>
+    <row r="10" x14ac:dyDescent="0.35">
       <c r="B10">
-        <v>92.735987427972759</v>
+        <v>92.740644490644485</v>
       </c>
       <c r="C10">
-        <v>92.140112994350289</v>
+        <v>92.156950672645735</v>
       </c>
       <c r="D10">
-        <v>93.570154577883471</v>
+        <v>93.604376108811351</v>
       </c>
       <c r="E10">
-        <v>93.658029053788766</v>
+        <v>93.67277691107644</v>
       </c>
       <c r="F10">
-        <v>93.28678890456041</v>
+        <v>93.290866510538635</v>
       </c>
       <c r="G10">
-        <v>93.12147483806676</v>
+        <v>93.135175282234101</v>
       </c>
       <c r="J10">
-        <v>0.21307492896970701</v>
+        <v>0.20933519826952979</v>
       </c>
       <c r="K10">
-        <v>0.57371335416765823</v>
-      </c>
-    </row>
-    <row r="11" spans="2:11" x14ac:dyDescent="0.35">
+        <v>0.55369820684746696</v>
+      </c>
+    </row>
+    <row r="11" x14ac:dyDescent="0.35">
       <c r="B11">
-        <v>0.55413475643748189</v>
+        <v>0.55282250572746683</v>
       </c>
       <c r="C11">
-        <v>0.85744345549059264</v>
+        <v>0.85746436976065976</v>
       </c>
       <c r="D11">
-        <v>0.5964620025914954</v>
+        <v>0.59648670007090754</v>
       </c>
       <c r="E11">
-        <v>0.47302089318136314</v>
+        <v>0.47058032652713411</v>
       </c>
       <c r="F11">
-        <v>0.60073118278698534</v>
+        <v>0.59891547015170421</v>
       </c>
       <c r="G11">
-        <v>0.27478835496977028</v>
-      </c>
-    </row>
-    <row r="12" spans="2:11" x14ac:dyDescent="0.35">
+        <v>0.27435415453128742</v>
+      </c>
+    </row>
+    <row r="12" x14ac:dyDescent="0.35">
       <c r="B12">
-        <v>0.6585724797645327</v>
+        <v>0.66084425036390104</v>
       </c>
       <c r="C12">
-        <v>0.6741573033707865</v>
+        <v>0.6723372781065089</v>
       </c>
       <c r="D12">
-        <v>0.6458923512747875</v>
+        <v>0.64694835680751173</v>
       </c>
       <c r="E12">
-        <v>0.66493955094991364</v>
+        <v>0.66609783845278725</v>
       </c>
       <c r="F12">
-        <v>0.64165497896213186</v>
+        <v>0.64220824598183091</v>
       </c>
       <c r="G12">
-        <v>0.6577501445922499</v>
+        <v>0.65845272206303729</v>
       </c>
       <c r="J12">
-        <v>0.85242462741585068</v>
+        <v>0.91217898619646376</v>
       </c>
       <c r="K12">
-        <v>0.79637875222901477</v>
-      </c>
-    </row>
-    <row r="13" spans="2:11" x14ac:dyDescent="0.35">
+        <v>0.75438827879433412</v>
+      </c>
+    </row>
+    <row r="13" x14ac:dyDescent="0.35">
       <c r="B13">
-        <v>1.955606823859319E-2</v>
+        <v>0.019264793906698385</v>
       </c>
       <c r="C13">
-        <v>1.9848216380705226E-2</v>
+        <v>0.018898567915395067</v>
       </c>
       <c r="D13">
-        <v>2.3771097841722523E-2</v>
+        <v>0.024289475036466852</v>
       </c>
       <c r="E13">
-        <v>1.6558305389398693E-2</v>
+        <v>0.016413508256461058</v>
       </c>
       <c r="F13">
-        <v>1.6310835628075143E-2</v>
+        <v>0.016248832152705936</v>
       </c>
       <c r="G13">
-        <v>8.4804378847425609E-3</v>
-      </c>
-    </row>
-    <row r="14" spans="2:11" x14ac:dyDescent="0.35">
+        <v>0.0083777184461360614</v>
+      </c>
+    </row>
+    <row r="14" x14ac:dyDescent="0.35">
       <c r="B14">
-        <v>2585</v>
+        <v>2601</v>
       </c>
       <c r="C14">
-        <v>2463</v>
+        <v>2482</v>
       </c>
       <c r="D14">
-        <v>2142</v>
+        <v>2156</v>
       </c>
       <c r="E14">
-        <v>3406</v>
+        <v>3436</v>
       </c>
       <c r="F14">
-        <v>2751</v>
+        <v>2766</v>
       </c>
       <c r="G14">
-        <v>13347</v>
-      </c>
-    </row>
-    <row r="16" spans="2:11" x14ac:dyDescent="0.35">
+        <v>13441</v>
+      </c>
+    </row>
+    <row r="16" x14ac:dyDescent="0.35">
       <c r="B16">
-        <v>1984</v>
+        <v>2000</v>
       </c>
       <c r="C16">
-        <v>1840</v>
+        <v>1855</v>
       </c>
       <c r="D16">
-        <v>1724</v>
+        <v>1733</v>
       </c>
       <c r="E16">
-        <v>2634</v>
+        <v>2653</v>
       </c>
       <c r="F16">
-        <v>2185</v>
+        <v>2193</v>
       </c>
     </row>
   </sheetData>
@@ -1663,193 +1641,209 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3B054637-0760-4807-B01C-4419EACB0C14}">
-  <dimension ref="A2:H39"/>
+  <dimension ref="A2:I39"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:H38"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A3" sqref="A3:I38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="18.1796875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="9.7265625" style="3" customWidth="1"/>
-    <col min="3" max="3" width="10.54296875" style="3" customWidth="1"/>
-    <col min="4" max="4" width="7.54296875" style="3" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="7.54296875" style="3" customWidth="1"/>
-    <col min="6" max="7" width="8.7265625" style="3"/>
-    <col min="8" max="8" width="9.7265625" style="3" customWidth="1"/>
+    <col min="1" max="1" width="18.1796875" bestFit="true" customWidth="true"/>
+    <col min="2" max="2" width="9.7265625" style="3" customWidth="true"/>
+    <col min="3" max="3" width="10.54296875" style="3" customWidth="true"/>
+    <col min="4" max="4" width="7.54296875" style="3" bestFit="true" customWidth="true"/>
+    <col min="5" max="5" width="7.54296875" style="3" customWidth="true"/>
+    <col min="6" max="6" width="1.36328125" style="3" customWidth="true"/>
+    <col min="7" max="8" width="8.7265625" style="3"/>
+    <col min="9" max="9" width="9.7265625" style="3" customWidth="true"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A2" s="10"/>
-      <c r="B2" s="16"/>
-      <c r="C2" s="16"/>
-      <c r="D2" s="16"/>
-      <c r="E2" s="16"/>
-      <c r="F2" s="16"/>
-      <c r="G2" s="16"/>
-      <c r="H2" s="16"/>
-    </row>
-    <row r="3" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A3" s="8"/>
-      <c r="B3" s="9"/>
-      <c r="C3" s="18" t="s">
+    <row r="2" s="11" customFormat="true" ht="15" thickBot="true" x14ac:dyDescent="0.4">
+      <c r="A2" s="17"/>
+      <c r="B2" s="18"/>
+      <c r="C2" s="18"/>
+      <c r="D2" s="18"/>
+      <c r="E2" s="18"/>
+      <c r="F2" s="18"/>
+      <c r="G2" s="18"/>
+      <c r="H2" s="18"/>
+      <c r="I2" s="18"/>
+    </row>
+    <row r="3" x14ac:dyDescent="0.35">
+      <c r="A3" s="11"/>
+      <c r="B3" s="12"/>
+      <c r="C3" s="15" t="s">
         <v>19</v>
       </c>
-      <c r="D3" s="18"/>
-      <c r="E3" s="18"/>
-      <c r="F3" s="18" t="s">
+      <c r="D3" s="15"/>
+      <c r="E3" s="15"/>
+      <c r="F3" s="12"/>
+      <c r="G3" s="15" t="s">
         <v>18</v>
       </c>
-      <c r="G3" s="18"/>
-      <c r="H3" s="18"/>
-    </row>
-    <row r="4" spans="1:8" s="6" customFormat="1" ht="15" thickTop="1" x14ac:dyDescent="0.35">
-      <c r="B4" s="7" t="s">
+      <c r="H3" s="15"/>
+      <c r="I3" s="15"/>
+    </row>
+    <row r="4" s="6" customFormat="true" x14ac:dyDescent="0.35">
+      <c r="A4" s="13"/>
+      <c r="B4" s="14" t="s">
         <v>1</v>
       </c>
-      <c r="C4" s="7" t="s">
+      <c r="C4" s="14" t="s">
         <v>12</v>
       </c>
-      <c r="D4" s="7" t="s">
+      <c r="D4" s="14" t="s">
         <v>0</v>
       </c>
-      <c r="E4" s="7" t="s">
+      <c r="E4" s="14" t="s">
         <v>2</v>
       </c>
-      <c r="F4" s="7" t="s">
+      <c r="F4" s="14"/>
+      <c r="G4" s="14" t="s">
         <v>12</v>
       </c>
-      <c r="G4" s="7" t="s">
+      <c r="H4" s="14" t="s">
         <v>13</v>
       </c>
-      <c r="H4" s="7" t="s">
+      <c r="I4" s="14" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="5" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="5" ht="15" thickBot="true" x14ac:dyDescent="0.4">
       <c r="A5" s="2"/>
-      <c r="B5" s="17" t="s">
+      <c r="B5" s="10" t="s">
         <v>3</v>
       </c>
-      <c r="C5" s="17"/>
-      <c r="D5" s="17"/>
-      <c r="E5" s="17"/>
-      <c r="F5" s="17"/>
-      <c r="G5" s="17"/>
-      <c r="H5" s="17"/>
-    </row>
-    <row r="6" spans="1:8" ht="15" thickTop="1" x14ac:dyDescent="0.35">
-      <c r="A6" t="s">
+      <c r="C5" s="10"/>
+      <c r="D5" s="10"/>
+      <c r="E5" s="10"/>
+      <c r="F5" s="10"/>
+      <c r="G5" s="10"/>
+      <c r="H5" s="10"/>
+      <c r="I5" s="10"/>
+    </row>
+    <row r="6" ht="15" thickTop="true" x14ac:dyDescent="0.35">
+      <c r="A6" s="11" t="s">
         <v>4</v>
       </c>
-      <c r="B6" s="3">
+      <c r="B6" s="12">
         <f>ROUND(SS_admin!B2,0)</f>
         <v>2289</v>
       </c>
-      <c r="C6" s="3">
+      <c r="C6" s="12">
         <f>ROUND(SS_admin!C2,0)</f>
         <v>2131</v>
       </c>
-      <c r="D6" s="3">
+      <c r="D6" s="12">
         <f>ROUND(SS_admin!E2,0)</f>
         <v>2180</v>
       </c>
-      <c r="E6" s="3">
+      <c r="E6" s="12">
         <f>ROUND(SS_admin!L2,2)</f>
         <v>0.32</v>
       </c>
-      <c r="F6" s="3">
+      <c r="F6" s="12"/>
+      <c r="G6" s="12">
         <f>ROUND(SS_admin!D2,0)</f>
         <v>2136</v>
       </c>
-      <c r="G6" s="3">
+      <c r="H6" s="12">
         <f>ROUND(SS_admin!F2,0)</f>
         <v>2090</v>
       </c>
-      <c r="H6" s="3">
+      <c r="I6" s="12">
         <f>ROUND(SS_admin!M2,2)</f>
         <v>0.14000000000000001</v>
       </c>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="B7" s="3" t="str">
+    <row r="7" x14ac:dyDescent="0.35">
+      <c r="A7" s="11"/>
+      <c r="B7" s="12" t="str">
         <f>CONCATENATE("(",ROUND(SS_admin!B3,0),")")</f>
         <v>(79)</v>
       </c>
-      <c r="C7" s="3" t="str">
+      <c r="C7" s="12" t="str">
         <f>CONCATENATE("(",ROUND(SS_admin!C3,0),")")</f>
         <v>(73)</v>
       </c>
-      <c r="D7" s="3" t="str">
+      <c r="D7" s="12" t="str">
         <f>CONCATENATE("(",ROUND(SS_admin!E3,0),")")</f>
         <v>(66)</v>
       </c>
-      <c r="F7" s="3" t="str">
+      <c r="E7" s="12"/>
+      <c r="F7" s="12"/>
+      <c r="G7" s="12" t="str">
         <f>CONCATENATE("(",ROUND(SS_admin!D3,0),")")</f>
         <v>(74)</v>
       </c>
-      <c r="G7" s="3" t="str">
+      <c r="H7" s="12" t="str">
         <f>CONCATENATE("(",ROUND(SS_admin!F3,0),")")</f>
         <v>(65)</v>
       </c>
-    </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A8" t="s">
+      <c r="I7" s="12"/>
+    </row>
+    <row r="8" x14ac:dyDescent="0.35">
+      <c r="A8" s="11" t="s">
         <v>17</v>
       </c>
-      <c r="B8" s="3">
+      <c r="B8" s="12">
         <f>ROUND(SS_admin!B4,2)</f>
         <v>0.88</v>
       </c>
-      <c r="C8" s="3">
+      <c r="C8" s="12">
         <f>ROUND(SS_admin!C4,2)</f>
         <v>0.89</v>
       </c>
-      <c r="D8" s="3">
+      <c r="D8" s="12">
         <f>ROUND(SS_admin!E4,2)</f>
         <v>0.85</v>
       </c>
-      <c r="E8" s="3">
+      <c r="E8" s="12">
         <f>ROUND(SS_admin!L4,2)</f>
         <v>0.72</v>
       </c>
-      <c r="F8" s="3">
+      <c r="F8" s="12"/>
+      <c r="G8" s="12">
         <f>ROUND(SS_admin!D4,2)</f>
         <v>0.89</v>
       </c>
-      <c r="G8" s="3">
+      <c r="H8" s="12">
         <f>ROUND(SS_admin!F4,2)</f>
         <v>0.83</v>
       </c>
-      <c r="H8" s="3">
+      <c r="I8" s="12">
         <f>ROUND(SS_admin!M4,2)</f>
         <v>0.62</v>
       </c>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="B9" s="3" t="str">
+    <row r="9" x14ac:dyDescent="0.35">
+      <c r="A9" s="11"/>
+      <c r="B9" s="12" t="str">
         <f>CONCATENATE("(",ROUND(SS_admin!B5,3),")")</f>
         <v>(0.04)</v>
       </c>
-      <c r="C9" s="3" t="str">
+      <c r="C9" s="12" t="str">
         <f>CONCATENATE("(",ROUND(SS_admin!C5,3),")")</f>
         <v>(0.034)</v>
       </c>
-      <c r="D9" s="3" t="str">
+      <c r="D9" s="12" t="str">
         <f>CONCATENATE("(",ROUND(SS_admin!E5,3),")")</f>
         <v>(0.042)</v>
       </c>
-      <c r="F9" s="3" t="str">
+      <c r="E9" s="12"/>
+      <c r="F9" s="12"/>
+      <c r="G9" s="12" t="str">
         <f>CONCATENATE("(",ROUND(SS_admin!D5,3),")")</f>
         <v>(0.036)</v>
       </c>
-      <c r="G9" s="3" t="str">
+      <c r="H9" s="12" t="str">
         <f>CONCATENATE("(",ROUND(SS_admin!F5,3),")")</f>
         <v>(0.049)</v>
       </c>
-    </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="I9" s="12"/>
+    </row>
+    <row r="10" x14ac:dyDescent="0.35">
       <c r="A10" s="1" t="s">
         <v>5</v>
       </c>
@@ -1866,763 +1860,828 @@
         <v>3406</v>
       </c>
       <c r="E10" s="4"/>
-      <c r="F10" s="4">
+      <c r="F10" s="4"/>
+      <c r="G10" s="4">
         <f>SS_admin!D6</f>
         <v>2143</v>
       </c>
-      <c r="G10" s="4">
+      <c r="H10" s="4">
         <f>SS_admin!F6</f>
         <v>2753</v>
       </c>
-      <c r="H10" s="4"/>
-    </row>
-    <row r="11" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A11" s="10"/>
-      <c r="B11" s="17" t="s">
+      <c r="I10" s="4"/>
+    </row>
+    <row r="11" ht="15" thickBot="true" x14ac:dyDescent="0.4">
+      <c r="A11" s="2"/>
+      <c r="B11" s="10" t="s">
         <v>21</v>
       </c>
-      <c r="C11" s="17"/>
-      <c r="D11" s="17"/>
-      <c r="E11" s="17"/>
-      <c r="F11" s="17"/>
-      <c r="G11" s="17"/>
-      <c r="H11" s="17"/>
-    </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A12" t="s">
+      <c r="C11" s="10"/>
+      <c r="D11" s="10"/>
+      <c r="E11" s="10"/>
+      <c r="F11" s="10"/>
+      <c r="G11" s="10"/>
+      <c r="H11" s="10"/>
+      <c r="I11" s="10"/>
+    </row>
+    <row r="12" ht="15" thickTop="true" x14ac:dyDescent="0.35">
+      <c r="A12" s="11" t="s">
         <v>6</v>
       </c>
-      <c r="B12" s="3">
+      <c r="B12" s="12">
         <f>ROUND(SS_survey_uncond!B2,2)</f>
         <v>0.75</v>
       </c>
-      <c r="C12" s="3">
+      <c r="C12" s="12">
         <f>ROUND(SS_survey_uncond!C2,2)</f>
         <v>0.72</v>
       </c>
-      <c r="D12" s="3">
+      <c r="D12" s="12">
         <f>ROUND(SS_survey_uncond!E2,2)</f>
         <v>0.72</v>
       </c>
-      <c r="E12" s="3">
+      <c r="E12" s="12">
         <f>ROUND(SS_survey_uncond!L2,2)</f>
         <v>0.22</v>
       </c>
-      <c r="F12" s="3">
+      <c r="F12" s="12"/>
+      <c r="G12" s="12">
         <f>ROUND(SS_survey_uncond!D2,2)</f>
         <v>0.72</v>
       </c>
-      <c r="G12" s="3">
+      <c r="H12" s="12">
         <f>ROUND(SS_survey_uncond!F2,2)</f>
         <v>0.74</v>
       </c>
-      <c r="H12" s="3">
+      <c r="I12" s="12">
         <f>ROUND(SS_survey_uncond!M2,2)</f>
         <v>0.52</v>
       </c>
     </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="B13" s="3" t="str">
+    <row r="13" x14ac:dyDescent="0.35">
+      <c r="A13" s="11"/>
+      <c r="B13" s="12" t="str">
         <f>CONCATENATE("(",ROUND(SS_survey_uncond!B3,3),")")</f>
         <v>(0.017)</v>
       </c>
-      <c r="C13" s="3" t="str">
+      <c r="C13" s="12" t="str">
         <f>CONCATENATE("(",ROUND(SS_survey_uncond!C3,3),")")</f>
         <v>(0.017)</v>
       </c>
-      <c r="D13" s="3" t="str">
+      <c r="D13" s="12" t="str">
         <f>CONCATENATE("(",ROUND(SS_survey_uncond!E3,3),")")</f>
         <v>(0.015)</v>
       </c>
-      <c r="F13" s="3" t="str">
+      <c r="E13" s="12"/>
+      <c r="F13" s="12"/>
+      <c r="G13" s="12" t="str">
         <f>CONCATENATE("(",ROUND(SS_survey_uncond!D3,3),")")</f>
         <v>(0.02)</v>
       </c>
-      <c r="G13" s="3" t="str">
+      <c r="H13" s="12" t="str">
         <f>CONCATENATE("(",ROUND(SS_survey_uncond!F3,3),")")</f>
         <v>(0.013)</v>
       </c>
-    </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A14" t="s">
+      <c r="I13" s="12"/>
+    </row>
+    <row r="14" x14ac:dyDescent="0.35">
+      <c r="A14" s="11" t="s">
         <v>7</v>
       </c>
-      <c r="B14" s="3">
+      <c r="B14" s="12">
         <f>ROUND(SS_survey_uncond!B4,2)</f>
         <v>43.22</v>
       </c>
-      <c r="C14" s="3">
+      <c r="C14" s="12">
         <f>ROUND(SS_survey_uncond!C4,2)</f>
         <v>43.2</v>
       </c>
-      <c r="D14" s="3">
+      <c r="D14" s="12">
         <f>ROUND(SS_survey_uncond!E4,2)</f>
         <v>44.04</v>
       </c>
-      <c r="E14" s="3">
+      <c r="E14" s="12">
         <f>ROUND(SS_survey_uncond!L4,2)</f>
         <v>0.55000000000000004</v>
       </c>
-      <c r="F14" s="3">
+      <c r="F14" s="12"/>
+      <c r="G14" s="12">
         <f>ROUND(SS_survey_uncond!D4,2)</f>
         <v>43</v>
       </c>
-      <c r="G14" s="3">
+      <c r="H14" s="12">
         <f>ROUND(SS_survey_uncond!F4,2)</f>
         <v>43.1</v>
       </c>
-      <c r="H14" s="3">
+      <c r="I14" s="12">
         <f>ROUND(SS_survey_uncond!M4,2)</f>
         <v>0.97</v>
       </c>
     </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="B15" s="3" t="str">
+    <row r="15" x14ac:dyDescent="0.35">
+      <c r="A15" s="11"/>
+      <c r="B15" s="12" t="str">
         <f>CONCATENATE("(",ROUND(SS_survey_uncond!B5,3),")")</f>
         <v>(0.565)</v>
       </c>
-      <c r="C15" s="3" t="str">
+      <c r="C15" s="12" t="str">
         <f>CONCATENATE("(",ROUND(SS_survey_uncond!C5,3),")")</f>
         <v>(0.763)</v>
       </c>
-      <c r="D15" s="3" t="str">
+      <c r="D15" s="12" t="str">
         <f>CONCATENATE("(",ROUND(SS_survey_uncond!E5,3),")")</f>
         <v>(0.607)</v>
       </c>
-      <c r="F15" s="3" t="str">
+      <c r="E15" s="12"/>
+      <c r="F15" s="12"/>
+      <c r="G15" s="12" t="str">
         <f>CONCATENATE("(",ROUND(SS_survey_uncond!D5,3),")")</f>
         <v>(0.647)</v>
       </c>
-      <c r="G15" s="3" t="str">
+      <c r="H15" s="12" t="str">
         <f>CONCATENATE("(",ROUND(SS_survey_uncond!F5,3),")")</f>
         <v>(0.519)</v>
       </c>
-    </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A16" t="s">
+      <c r="I15" s="12"/>
+    </row>
+    <row r="16" x14ac:dyDescent="0.35">
+      <c r="A16" s="11" t="s">
         <v>8</v>
       </c>
-      <c r="B16" s="3">
+      <c r="B16" s="12">
         <f>ROUND(SS_survey_uncond!B6,0)</f>
         <v>3144</v>
       </c>
-      <c r="C16" s="3">
+      <c r="C16" s="12">
         <f>ROUND(SS_survey_uncond!C6,0)</f>
         <v>2978</v>
       </c>
-      <c r="D16" s="3">
+      <c r="D16" s="12">
         <f>ROUND(SS_survey_uncond!E6,0)</f>
         <v>3112</v>
       </c>
-      <c r="E16" s="3">
+      <c r="E16" s="12">
         <f>ROUND(SS_survey_uncond!L6,2)</f>
         <v>0.31</v>
       </c>
-      <c r="F16" s="3">
+      <c r="F16" s="12"/>
+      <c r="G16" s="12">
         <f>ROUND(SS_survey_uncond!D6,0)</f>
         <v>3012</v>
       </c>
-      <c r="G16" s="3">
+      <c r="H16" s="12">
         <f>ROUND(SS_survey_uncond!F6,0)</f>
         <v>3082</v>
       </c>
-      <c r="H16" s="3">
+      <c r="I16" s="12">
         <f>ROUND(SS_survey_uncond!M6,2)</f>
         <v>0.43</v>
       </c>
     </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="B17" s="3" t="str">
+    <row r="17" x14ac:dyDescent="0.35">
+      <c r="A17" s="11"/>
+      <c r="B17" s="12" t="str">
         <f>CONCATENATE("(",ROUND(SS_survey_uncond!B7,0),")")</f>
         <v>(68)</v>
       </c>
-      <c r="C17" s="3" t="str">
+      <c r="C17" s="12" t="str">
         <f>CONCATENATE("(",ROUND(SS_survey_uncond!C7,0),")")</f>
         <v>(87)</v>
       </c>
-      <c r="D17" s="3" t="str">
+      <c r="D17" s="12" t="str">
         <f>CONCATENATE("(",ROUND(SS_survey_uncond!E7,0),")")</f>
         <v>(85)</v>
       </c>
-      <c r="F17" s="3" t="str">
+      <c r="E17" s="12"/>
+      <c r="F17" s="12"/>
+      <c r="G17" s="12" t="str">
         <f>CONCATENATE("(",ROUND(SS_survey_uncond!D7,0),")")</f>
         <v>(77)</v>
       </c>
-      <c r="G17" s="3" t="str">
+      <c r="H17" s="12" t="str">
         <f>CONCATENATE("(",ROUND(SS_survey_uncond!F7,0),")")</f>
         <v>(99)</v>
       </c>
-    </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A18" t="s">
+      <c r="I17" s="12"/>
+    </row>
+    <row r="18" x14ac:dyDescent="0.35">
+      <c r="A18" s="11" t="s">
         <v>9</v>
       </c>
-      <c r="B18" s="3">
+      <c r="B18" s="12">
         <f>ROUND(SS_survey_uncond!B8,2)</f>
         <v>0.89</v>
       </c>
-      <c r="C18" s="3">
+      <c r="C18" s="12">
         <f>ROUND(SS_survey_uncond!C8,2)</f>
         <v>0.9</v>
       </c>
-      <c r="D18" s="3">
+      <c r="D18" s="12">
         <f>ROUND(SS_survey_uncond!E8,2)</f>
         <v>0.91</v>
       </c>
-      <c r="E18" s="3">
+      <c r="E18" s="12">
         <f>ROUND(SS_survey_uncond!L8,2)</f>
         <v>0.47</v>
       </c>
-      <c r="F18" s="3">
+      <c r="F18" s="12"/>
+      <c r="G18" s="12">
         <f>ROUND(SS_survey_uncond!D8,2)</f>
         <v>0.89</v>
       </c>
-      <c r="G18" s="3">
+      <c r="H18" s="12">
         <f>ROUND(SS_survey_uncond!F8,2)</f>
         <v>0.89</v>
       </c>
-      <c r="H18" s="3">
+      <c r="I18" s="12">
         <f>ROUND(SS_survey_uncond!M8,2)</f>
         <v>0.99</v>
       </c>
     </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="B19" s="3" t="str">
+    <row r="19" x14ac:dyDescent="0.35">
+      <c r="A19" s="11"/>
+      <c r="B19" s="12" t="str">
         <f>CONCATENATE("(",ROUND(SS_survey_uncond!B9,3),")")</f>
         <v>(0.011)</v>
       </c>
-      <c r="C19" s="3" t="str">
+      <c r="C19" s="12" t="str">
         <f>CONCATENATE("(",ROUND(SS_survey_uncond!C9,3),")")</f>
         <v>(0.011)</v>
       </c>
-      <c r="D19" s="3" t="str">
+      <c r="D19" s="12" t="str">
         <f>CONCATENATE("(",ROUND(SS_survey_uncond!E9,3),")")</f>
         <v>(0.01)</v>
       </c>
-      <c r="F19" s="3" t="str">
+      <c r="E19" s="12"/>
+      <c r="F19" s="12"/>
+      <c r="G19" s="12" t="str">
         <f>CONCATENATE("(",ROUND(SS_survey_uncond!D9,3),")")</f>
         <v>(0.014)</v>
       </c>
-      <c r="G19" s="3" t="str">
+      <c r="H19" s="12" t="str">
         <f>CONCATENATE("(",ROUND(SS_survey_uncond!F9,3),")")</f>
         <v>(0.009)</v>
       </c>
-    </row>
-    <row r="20" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A20" t="s">
+      <c r="I19" s="12"/>
+    </row>
+    <row r="20" x14ac:dyDescent="0.35">
+      <c r="A20" s="11" t="s">
         <v>10</v>
       </c>
-      <c r="B20" s="3">
+      <c r="B20" s="12">
         <f>ROUND(SS_survey_uncond!B10,2)</f>
         <v>92.75</v>
       </c>
-      <c r="C20" s="3">
+      <c r="C20" s="12">
         <f>ROUND(SS_survey_uncond!C10,2)</f>
         <v>92.19</v>
       </c>
-      <c r="D20" s="3">
+      <c r="D20" s="12">
         <f>ROUND(SS_survey_uncond!E10,2)</f>
         <v>93.71</v>
       </c>
-      <c r="E20" s="3">
+      <c r="E20" s="12">
         <f>ROUND(SS_survey_uncond!L10,2)</f>
         <v>0.18</v>
       </c>
-      <c r="F20" s="3">
+      <c r="F20" s="12"/>
+      <c r="G20" s="12">
         <f>ROUND(SS_survey_uncond!D10,2)</f>
         <v>93.66</v>
       </c>
-      <c r="G20" s="3">
+      <c r="H20" s="12">
         <f>ROUND(SS_survey_uncond!F10,2)</f>
         <v>93.34</v>
       </c>
-      <c r="H20" s="3">
+      <c r="I20" s="12">
         <f>ROUND(SS_survey_uncond!M10,2)</f>
         <v>0.5</v>
       </c>
     </row>
-    <row r="21" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="B21" s="3" t="str">
+    <row r="21" x14ac:dyDescent="0.35">
+      <c r="A21" s="11"/>
+      <c r="B21" s="12" t="str">
         <f>CONCATENATE("(",ROUND(SS_survey_uncond!B11,3),")")</f>
         <v>(0.537)</v>
       </c>
-      <c r="C21" s="3" t="str">
+      <c r="C21" s="12" t="str">
         <f>CONCATENATE("(",ROUND(SS_survey_uncond!C11,3),")")</f>
         <v>(0.839)</v>
       </c>
-      <c r="D21" s="3" t="str">
+      <c r="D21" s="12" t="str">
         <f>CONCATENATE("(",ROUND(SS_survey_uncond!E11,3),")")</f>
         <v>(0.455)</v>
       </c>
-      <c r="F21" s="3" t="str">
+      <c r="E21" s="12"/>
+      <c r="F21" s="12"/>
+      <c r="G21" s="12" t="str">
         <f>CONCATENATE("(",ROUND(SS_survey_uncond!D11,3),")")</f>
         <v>(0.591)</v>
       </c>
-      <c r="G21" s="3" t="str">
+      <c r="H21" s="12" t="str">
         <f>CONCATENATE("(",ROUND(SS_survey_uncond!F11,3),")")</f>
         <v>(0.596)</v>
       </c>
-    </row>
-    <row r="22" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A22" t="s">
+      <c r="I21" s="12"/>
+    </row>
+    <row r="22" x14ac:dyDescent="0.35">
+      <c r="A22" s="11" t="s">
         <v>11</v>
       </c>
-      <c r="B22" s="3">
+      <c r="B22" s="12">
         <f>ROUND(SS_survey_uncond!B12,2)</f>
         <v>0.66</v>
       </c>
-      <c r="C22" s="3">
+      <c r="C22" s="12">
         <f>ROUND(SS_survey_uncond!C12,2)</f>
         <v>0.67</v>
       </c>
-      <c r="D22" s="3">
+      <c r="D22" s="12">
         <f>ROUND(SS_survey_uncond!E12,2)</f>
         <v>0.66</v>
       </c>
-      <c r="E22" s="3">
+      <c r="E22" s="12">
         <f>ROUND(SS_survey_uncond!L12,2)</f>
         <v>0.92</v>
       </c>
-      <c r="F22" s="3">
+      <c r="F22" s="12"/>
+      <c r="G22" s="12">
         <f>ROUND(SS_survey_uncond!D12,2)</f>
         <v>0.65</v>
       </c>
-      <c r="G22" s="3">
+      <c r="H22" s="12">
         <f>ROUND(SS_survey_uncond!F12,2)</f>
         <v>0.64</v>
       </c>
-      <c r="H22" s="3">
+      <c r="I22" s="12">
         <f>ROUND(SS_survey_uncond!M12,2)</f>
         <v>0.83</v>
       </c>
     </row>
-    <row r="23" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="B23" s="3" t="str">
+    <row r="23" x14ac:dyDescent="0.35">
+      <c r="A23" s="11"/>
+      <c r="B23" s="12" t="str">
         <f>CONCATENATE("(",ROUND(SS_survey_uncond!B13,3),")")</f>
         <v>(0.02)</v>
       </c>
-      <c r="C23" s="3" t="str">
+      <c r="C23" s="12" t="str">
         <f>CONCATENATE("(",ROUND(SS_survey_uncond!C13,3),")")</f>
         <v>(0.02)</v>
       </c>
-      <c r="D23" s="3" t="str">
+      <c r="D23" s="12" t="str">
         <f>CONCATENATE("(",ROUND(SS_survey_uncond!E13,3),")")</f>
         <v>(0.017)</v>
       </c>
-      <c r="F23" s="3" t="str">
+      <c r="E23" s="12"/>
+      <c r="F23" s="12"/>
+      <c r="G23" s="12" t="str">
         <f>CONCATENATE("(",ROUND(SS_survey_uncond!D13,3),")")</f>
         <v>(0.024)</v>
       </c>
-      <c r="G23" s="3" t="str">
+      <c r="H23" s="12" t="str">
         <f>CONCATENATE("(",ROUND(SS_survey_uncond!F13,3),")")</f>
         <v>(0.017)</v>
       </c>
-    </row>
-    <row r="24" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A24" s="11" t="s">
+      <c r="I23" s="12"/>
+    </row>
+    <row r="24" x14ac:dyDescent="0.35">
+      <c r="A24" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="B24" s="12">
+      <c r="B24" s="4">
         <f>SS_survey_uncond!B16</f>
         <v>2036</v>
       </c>
-      <c r="C24" s="12">
+      <c r="C24" s="4">
         <f>SS_survey_uncond!C16</f>
         <v>1907</v>
       </c>
-      <c r="D24" s="12">
+      <c r="D24" s="4">
         <f>SS_survey_uncond!E16</f>
         <v>2710</v>
       </c>
-      <c r="E24" s="12"/>
-      <c r="F24" s="12">
+      <c r="E24" s="4"/>
+      <c r="F24" s="4"/>
+      <c r="G24" s="4">
         <f>SS_survey_uncond!D16</f>
         <v>1757</v>
       </c>
-      <c r="G24" s="12">
+      <c r="H24" s="4">
         <f>SS_survey_uncond!F16</f>
         <v>2216</v>
       </c>
-      <c r="H24" s="12"/>
-    </row>
-    <row r="25" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A25" s="10"/>
-      <c r="B25" s="17" t="s">
+      <c r="I24" s="4"/>
+    </row>
+    <row r="25" ht="15" thickBot="true" x14ac:dyDescent="0.4">
+      <c r="A25" s="2"/>
+      <c r="B25" s="10" t="s">
         <v>20</v>
       </c>
-      <c r="C25" s="17"/>
-      <c r="D25" s="17"/>
-      <c r="E25" s="17"/>
-      <c r="F25" s="17"/>
-      <c r="G25" s="17"/>
-      <c r="H25" s="17"/>
-    </row>
-    <row r="26" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A26" t="s">
+      <c r="C25" s="10"/>
+      <c r="D25" s="10"/>
+      <c r="E25" s="10"/>
+      <c r="F25" s="10"/>
+      <c r="G25" s="10"/>
+      <c r="H25" s="10"/>
+      <c r="I25" s="10"/>
+    </row>
+    <row r="26" ht="15" thickTop="true" x14ac:dyDescent="0.35">
+      <c r="A26" s="11" t="s">
         <v>6</v>
       </c>
-      <c r="B26" s="3">
+      <c r="B26" s="12">
         <f>ROUND(SS_survey!B2,2)</f>
         <v>0.76</v>
       </c>
-      <c r="C26" s="3">
+      <c r="C26" s="12">
         <f>ROUND(SS_survey!C2,2)</f>
         <v>0.72</v>
       </c>
-      <c r="D26" s="3">
+      <c r="D26" s="12">
         <f>ROUND(SS_survey!E2,2)</f>
         <v>0.72</v>
       </c>
-      <c r="E26" s="3">
+      <c r="E26" s="12">
         <f>ROUND(SS_survey!J2,2)</f>
         <v>0.2</v>
       </c>
-      <c r="F26" s="3">
+      <c r="F26" s="12"/>
+      <c r="G26" s="12">
         <f>ROUND(SS_survey!D2,2)</f>
         <v>0.72</v>
       </c>
-      <c r="G26" s="3">
+      <c r="H26" s="12">
         <f>ROUND(SS_survey!F2,2)</f>
         <v>0.74</v>
       </c>
-      <c r="H26" s="3">
+      <c r="I26" s="12">
         <f>ROUND(SS_survey!K2,2)</f>
         <v>0.49</v>
       </c>
     </row>
-    <row r="27" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="B27" s="3" t="str">
+    <row r="27" x14ac:dyDescent="0.35">
+      <c r="A27" s="11"/>
+      <c r="B27" s="12" t="str">
         <f>CONCATENATE("(",ROUND(SS_survey!B3,3),")")</f>
         <v>(0.016)</v>
       </c>
-      <c r="C27" s="3" t="str">
+      <c r="C27" s="12" t="str">
         <f>CONCATENATE("(",ROUND(SS_survey!C3,3),")")</f>
         <v>(0.018)</v>
       </c>
-      <c r="D27" s="3" t="str">
+      <c r="D27" s="12" t="str">
         <f>CONCATENATE("(",ROUND(SS_survey!E3,3),")")</f>
         <v>(0.016)</v>
       </c>
-      <c r="F27" s="3" t="str">
+      <c r="E27" s="12"/>
+      <c r="F27" s="12"/>
+      <c r="G27" s="12" t="str">
         <f>CONCATENATE("(",ROUND(SS_survey!D3,3),")")</f>
         <v>(0.021)</v>
       </c>
-      <c r="G27" s="3" t="str">
+      <c r="H27" s="12" t="str">
         <f>CONCATENATE("(",ROUND(SS_survey!F3,3),")")</f>
         <v>(0.013)</v>
       </c>
-    </row>
-    <row r="28" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A28" t="s">
+      <c r="I27" s="12"/>
+    </row>
+    <row r="28" x14ac:dyDescent="0.35">
+      <c r="A28" s="11" t="s">
         <v>7</v>
       </c>
-      <c r="B28" s="3">
+      <c r="B28" s="12">
         <f>ROUND(SS_survey!B4,2)</f>
         <v>43.22</v>
       </c>
-      <c r="C28" s="3" t="str">
+      <c r="C28" s="12" t="str">
         <f>CONCATENATE("(",ROUND(SS_survey!C4,3),")")</f>
         <v>(43.131)</v>
       </c>
-      <c r="D28" s="3" t="str">
+      <c r="D28" s="12" t="str">
         <f>CONCATENATE("(",ROUND(SS_survey!E4,3),")")</f>
         <v>(43.906)</v>
       </c>
-      <c r="E28" s="3">
+      <c r="E28" s="12">
         <f>ROUND(SS_survey!J4,2)</f>
         <v>0.64</v>
       </c>
-      <c r="F28" s="3" t="str">
+      <c r="F28" s="12"/>
+      <c r="G28" s="12" t="str">
         <f>CONCATENATE("(",ROUND(SS_survey!D4,3),")")</f>
         <v>(42.956)</v>
       </c>
-      <c r="G28" s="3" t="str">
+      <c r="H28" s="12" t="str">
         <f>CONCATENATE("(",ROUND(SS_survey!F4,3),")")</f>
         <v>(43.081)</v>
       </c>
-      <c r="H28" s="3">
+      <c r="I28" s="12">
         <f>ROUND(SS_survey!K4,2)</f>
         <v>0.95</v>
       </c>
     </row>
-    <row r="29" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="B29" s="3" t="str">
+    <row r="29" x14ac:dyDescent="0.35">
+      <c r="A29" s="11"/>
+      <c r="B29" s="12" t="str">
         <f>CONCATENATE("(",ROUND(SS_survey!B5,3),")")</f>
         <v>(0.572)</v>
       </c>
-      <c r="C29" s="3" t="str">
+      <c r="C29" s="12" t="str">
         <f>CONCATENATE("(",ROUND(SS_survey!C5,3),")")</f>
         <v>(0.778)</v>
       </c>
-      <c r="D29" s="3" t="str">
+      <c r="D29" s="12" t="str">
         <f>CONCATENATE("(",ROUND(SS_survey!E5,3),")")</f>
         <v>(0.617)</v>
       </c>
-      <c r="F29" s="3" t="str">
+      <c r="E29" s="12"/>
+      <c r="F29" s="12"/>
+      <c r="G29" s="12" t="str">
         <f>CONCATENATE("(",ROUND(SS_survey!D5,3),")")</f>
         <v>(0.638)</v>
       </c>
-      <c r="G29" s="3" t="str">
+      <c r="H29" s="12" t="str">
         <f>CONCATENATE("(",ROUND(SS_survey!F5,3),")")</f>
         <v>(0.519)</v>
       </c>
-    </row>
-    <row r="30" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A30" t="s">
+      <c r="I29" s="12"/>
+    </row>
+    <row r="30" x14ac:dyDescent="0.35">
+      <c r="A30" s="11" t="s">
         <v>8</v>
       </c>
-      <c r="B30" s="3">
+      <c r="B30" s="12">
         <f>ROUND(SS_survey!B6,0)</f>
         <v>3141</v>
       </c>
-      <c r="C30" s="3">
+      <c r="C30" s="12">
         <f>ROUND(SS_survey!C6,0)</f>
         <v>2969</v>
       </c>
-      <c r="D30" s="3">
+      <c r="D30" s="12">
         <f>ROUND(SS_survey!E6,0)</f>
         <v>3107</v>
       </c>
-      <c r="E30" s="3">
+      <c r="E30" s="12">
         <f>ROUND(SS_survey!J6,2)</f>
         <v>0.28999999999999998</v>
       </c>
-      <c r="F30" s="3">
+      <c r="F30" s="12"/>
+      <c r="G30" s="12">
         <f>ROUND(SS_survey!D6,0)</f>
         <v>2982</v>
       </c>
-      <c r="G30" s="3">
+      <c r="H30" s="12">
         <f>ROUND(SS_survey!F6,0)</f>
         <v>3078</v>
       </c>
-      <c r="H30" s="3">
+      <c r="I30" s="12">
         <f>ROUND(SS_survey!K6,2)</f>
         <v>0.3</v>
       </c>
     </row>
-    <row r="31" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="B31" s="3" t="str">
+    <row r="31" x14ac:dyDescent="0.35">
+      <c r="A31" s="11"/>
+      <c r="B31" s="12" t="str">
         <f>CONCATENATE("(",ROUND(SS_survey!B7,0),")")</f>
         <v>(68)</v>
       </c>
-      <c r="C31" s="3" t="str">
+      <c r="C31" s="12" t="str">
         <f>CONCATENATE("(",ROUND(SS_survey!C7,0),")")</f>
         <v>(88)</v>
       </c>
-      <c r="D31" s="3" t="str">
+      <c r="D31" s="12" t="str">
         <f>CONCATENATE("(",ROUND(SS_survey!E7,0),")")</f>
         <v>(85)</v>
       </c>
-      <c r="F31" s="3" t="str">
+      <c r="E31" s="12"/>
+      <c r="F31" s="12"/>
+      <c r="G31" s="12" t="str">
         <f>CONCATENATE("(",ROUND(SS_survey!D7,0),")")</f>
         <v>(77)</v>
       </c>
-      <c r="G31" s="3" t="str">
+      <c r="H31" s="12" t="str">
         <f>CONCATENATE("(",ROUND(SS_survey!F7,0),")")</f>
         <v>(99)</v>
       </c>
-    </row>
-    <row r="32" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A32" t="s">
+      <c r="I31" s="12"/>
+    </row>
+    <row r="32" x14ac:dyDescent="0.35">
+      <c r="A32" s="11" t="s">
         <v>9</v>
       </c>
-      <c r="B32" s="3">
+      <c r="B32" s="12">
         <f>ROUND(SS_survey!B8,2)</f>
         <v>0.89</v>
       </c>
-      <c r="C32" s="3">
+      <c r="C32" s="12">
         <f>ROUND(SS_survey!C8,2)</f>
         <v>0.9</v>
       </c>
-      <c r="D32" s="3">
+      <c r="D32" s="12">
         <f>ROUND(SS_survey!E8,2)</f>
         <v>0.91</v>
       </c>
-      <c r="E32" s="3">
+      <c r="E32" s="12">
         <f>ROUND(SS_survey!J8,2)</f>
         <v>0.48</v>
       </c>
-      <c r="F32" s="3">
+      <c r="F32" s="12"/>
+      <c r="G32" s="12">
         <f>ROUND(SS_survey!D8,2)</f>
         <v>0.89</v>
       </c>
-      <c r="G32" s="3">
+      <c r="H32" s="12">
         <f>ROUND(SS_survey!F8,2)</f>
         <v>0.89</v>
       </c>
-      <c r="H32" s="3">
+      <c r="I32" s="12">
         <f>ROUND(SS_survey!K8,2)</f>
         <v>1</v>
       </c>
     </row>
-    <row r="33" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="B33" s="3" t="str">
+    <row r="33" x14ac:dyDescent="0.35">
+      <c r="A33" s="11"/>
+      <c r="B33" s="12" t="str">
         <f>CONCATENATE("(",ROUND(SS_survey!B9,3),")")</f>
         <v>(0.012)</v>
       </c>
-      <c r="C33" s="3" t="str">
+      <c r="C33" s="12" t="str">
         <f>CONCATENATE("(",ROUND(SS_survey!C9,3),")")</f>
         <v>(0.011)</v>
       </c>
-      <c r="D33" s="3" t="str">
+      <c r="D33" s="12" t="str">
         <f>CONCATENATE("(",ROUND(SS_survey!E9,3),")")</f>
         <v>(0.01)</v>
       </c>
-      <c r="F33" s="3" t="str">
+      <c r="E33" s="12"/>
+      <c r="F33" s="12"/>
+      <c r="G33" s="12" t="str">
         <f>CONCATENATE("(",ROUND(SS_survey!D9,3),")")</f>
         <v>(0.014)</v>
       </c>
-      <c r="G33" s="3" t="str">
+      <c r="H33" s="12" t="str">
         <f>CONCATENATE("(",ROUND(SS_survey!F9,3),")")</f>
         <v>(0.009)</v>
       </c>
-    </row>
-    <row r="34" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A34" t="s">
+      <c r="I33" s="12"/>
+    </row>
+    <row r="34" x14ac:dyDescent="0.35">
+      <c r="A34" s="11" t="s">
         <v>10</v>
       </c>
-      <c r="B34" s="3">
+      <c r="B34" s="12">
         <f>ROUND(SS_survey!B10,2)</f>
         <v>92.74</v>
       </c>
-      <c r="C34" s="3">
+      <c r="C34" s="12">
         <f>ROUND(SS_survey!C10,2)</f>
         <v>92.14</v>
       </c>
-      <c r="D34" s="3">
+      <c r="D34" s="12">
         <f>ROUND(SS_survey!E10,2)</f>
         <v>93.66</v>
       </c>
-      <c r="E34" s="3">
+      <c r="E34" s="12">
         <f>ROUND(SS_survey!J10,2)</f>
         <v>0.21</v>
       </c>
-      <c r="F34" s="3">
+      <c r="F34" s="12"/>
+      <c r="G34" s="12">
         <f>ROUND(SS_survey!D10,2)</f>
         <v>93.57</v>
       </c>
-      <c r="G34" s="3">
+      <c r="H34" s="12">
         <f>ROUND(SS_survey!F10,2)</f>
         <v>93.29</v>
       </c>
-      <c r="H34" s="3">
+      <c r="I34" s="12">
         <f>ROUND(SS_survey!K10,2)</f>
         <v>0.56999999999999995</v>
       </c>
     </row>
-    <row r="35" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="B35" s="3" t="str">
+    <row r="35" x14ac:dyDescent="0.35">
+      <c r="A35" s="11"/>
+      <c r="B35" s="12" t="str">
         <f>CONCATENATE("(",ROUND(SS_survey!B11,3),")")</f>
         <v>(0.554)</v>
       </c>
-      <c r="C35" s="3" t="str">
+      <c r="C35" s="12" t="str">
         <f>CONCATENATE("(",ROUND(SS_survey!C11,3),")")</f>
         <v>(0.857)</v>
       </c>
-      <c r="D35" s="3" t="str">
+      <c r="D35" s="12" t="str">
         <f>CONCATENATE("(",ROUND(SS_survey!E11,3),")")</f>
         <v>(0.473)</v>
       </c>
-      <c r="F35" s="3" t="str">
+      <c r="E35" s="12"/>
+      <c r="F35" s="12"/>
+      <c r="G35" s="12" t="str">
         <f>CONCATENATE("(",ROUND(SS_survey!D11,3),")")</f>
         <v>(0.596)</v>
       </c>
-      <c r="G35" s="3" t="str">
+      <c r="H35" s="12" t="str">
         <f>CONCATENATE("(",ROUND(SS_survey!F11,3),")")</f>
         <v>(0.601)</v>
       </c>
-    </row>
-    <row r="36" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A36" t="s">
+      <c r="I35" s="12"/>
+    </row>
+    <row r="36" x14ac:dyDescent="0.35">
+      <c r="A36" s="11" t="s">
         <v>11</v>
       </c>
-      <c r="B36" s="3">
+      <c r="B36" s="12">
         <f>ROUND(SS_survey!B12,2)</f>
         <v>0.66</v>
       </c>
-      <c r="C36" s="3">
+      <c r="C36" s="12">
         <f>ROUND(SS_survey!C12,2)</f>
         <v>0.67</v>
       </c>
-      <c r="D36" s="3">
+      <c r="D36" s="12">
         <f>ROUND(SS_survey!E12,2)</f>
         <v>0.66</v>
       </c>
-      <c r="E36" s="3">
+      <c r="E36" s="12">
         <f>ROUND(SS_survey!J12,2)</f>
         <v>0.85</v>
       </c>
-      <c r="F36" s="3">
+      <c r="F36" s="12"/>
+      <c r="G36" s="12">
         <f>ROUND(SS_survey!D12,2)</f>
         <v>0.65</v>
       </c>
-      <c r="G36" s="3">
+      <c r="H36" s="12">
         <f>ROUND(SS_survey!F12,2)</f>
         <v>0.64</v>
       </c>
-      <c r="H36" s="3">
+      <c r="I36" s="12">
         <f>ROUND(SS_survey!K12,2)</f>
         <v>0.8</v>
       </c>
     </row>
-    <row r="37" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="B37" s="3" t="str">
+    <row r="37" x14ac:dyDescent="0.35">
+      <c r="A37" s="11"/>
+      <c r="B37" s="12" t="str">
         <f>CONCATENATE("(",ROUND(SS_survey!B13,3),")")</f>
         <v>(0.02)</v>
       </c>
-      <c r="C37" s="3" t="str">
+      <c r="C37" s="12" t="str">
         <f>CONCATENATE("(",ROUND(SS_survey!C13,3),")")</f>
         <v>(0.02)</v>
       </c>
-      <c r="D37" s="3" t="str">
+      <c r="D37" s="12" t="str">
         <f>CONCATENATE("(",ROUND(SS_survey!E13,3),")")</f>
         <v>(0.017)</v>
       </c>
-      <c r="F37" s="3" t="str">
+      <c r="E37" s="12"/>
+      <c r="F37" s="12"/>
+      <c r="G37" s="12" t="str">
         <f>CONCATENATE("(",ROUND(SS_survey!D13,3),")")</f>
         <v>(0.024)</v>
       </c>
-      <c r="G37" s="3" t="str">
+      <c r="H37" s="12" t="str">
         <f>CONCATENATE("(",ROUND(SS_survey!F13,3),")")</f>
         <v>(0.016)</v>
       </c>
-    </row>
-    <row r="38" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="I37" s="12"/>
+    </row>
+    <row r="38" ht="15" thickBot="true" x14ac:dyDescent="0.4">
       <c r="A38" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="B38" s="5">
+      <c r="B38" s="9">
         <f>SS_survey!B16</f>
         <v>1984</v>
       </c>
-      <c r="C38" s="5">
+      <c r="C38" s="9">
         <f>SS_survey!C16</f>
         <v>1840</v>
       </c>
-      <c r="D38" s="5">
+      <c r="D38" s="9">
         <f>SS_survey!E16</f>
         <v>2634</v>
       </c>
-      <c r="E38" s="14"/>
-      <c r="F38" s="5">
+      <c r="E38" s="9"/>
+      <c r="F38" s="9"/>
+      <c r="G38" s="9">
         <f>SS_survey!D16</f>
         <v>1724</v>
       </c>
-      <c r="G38" s="5">
+      <c r="H38" s="9">
         <f>SS_survey!F16</f>
         <v>2185</v>
       </c>
-      <c r="H38" s="5"/>
-    </row>
-    <row r="39" spans="1:8" ht="15" thickTop="1" x14ac:dyDescent="0.35"/>
+      <c r="I38" s="9"/>
+    </row>
+    <row r="39" ht="15" thickTop="true" x14ac:dyDescent="0.35"/>
   </sheetData>
   <mergeCells count="6">
-    <mergeCell ref="B2:H2"/>
-    <mergeCell ref="B11:H11"/>
-    <mergeCell ref="B25:H25"/>
-    <mergeCell ref="B5:H5"/>
+    <mergeCell ref="B2:I2"/>
+    <mergeCell ref="B11:I11"/>
+    <mergeCell ref="B25:I25"/>
+    <mergeCell ref="B5:I5"/>
     <mergeCell ref="C3:E3"/>
-    <mergeCell ref="F3:H3"/>
+    <mergeCell ref="G3:I3"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -2630,128 +2689,173 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{754403B8-1DA5-4CBA-B8B6-94BFF0A849DB}">
-  <dimension ref="A3:H13"/>
+  <dimension ref="A1:K13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A3" sqref="A3:H12"/>
+      <selection activeCell="A4" sqref="A4:I12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="26.26953125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="7.1796875" style="3" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="10.1796875" style="3" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="6.54296875" style="3" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="6.54296875" style="3" customWidth="1"/>
-    <col min="6" max="6" width="7" style="3" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="7.453125" style="3" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="7.7265625" style="3" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="26.26953125" bestFit="true" customWidth="true"/>
+    <col min="2" max="2" width="7.1796875" style="3" bestFit="true" customWidth="true"/>
+    <col min="3" max="3" width="10.1796875" style="3" bestFit="true" customWidth="true"/>
+    <col min="4" max="4" width="6.54296875" style="3" bestFit="true" customWidth="true"/>
+    <col min="5" max="5" width="6.54296875" style="3" customWidth="true"/>
+    <col min="6" max="6" width="1.7265625" style="3" customWidth="true"/>
+    <col min="7" max="7" width="7" style="3" bestFit="true" customWidth="true"/>
+    <col min="8" max="8" width="7.453125" style="3" bestFit="true" customWidth="true"/>
+    <col min="9" max="9" width="7.7265625" style="3" bestFit="true" customWidth="true"/>
   </cols>
   <sheetData>
-    <row r="3" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A3" s="10"/>
-      <c r="B3" s="16"/>
-      <c r="C3" s="16"/>
-      <c r="D3" s="16"/>
-      <c r="E3" s="16"/>
-      <c r="F3" s="16"/>
-      <c r="G3" s="16"/>
-      <c r="H3" s="16"/>
-    </row>
-    <row r="4" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A4" s="8"/>
-      <c r="B4" s="9"/>
-      <c r="C4" s="18" t="s">
+    <row r="1" x14ac:dyDescent="0.35">
+      <c r="A1" s="11"/>
+      <c r="B1" s="12"/>
+      <c r="C1" s="12"/>
+      <c r="D1" s="12"/>
+      <c r="E1" s="12"/>
+      <c r="F1" s="12"/>
+      <c r="G1" s="12"/>
+      <c r="H1" s="12"/>
+      <c r="I1" s="12"/>
+      <c r="J1" s="11"/>
+      <c r="K1" s="11"/>
+    </row>
+    <row r="2" x14ac:dyDescent="0.35">
+      <c r="A2" s="11"/>
+      <c r="B2" s="12"/>
+      <c r="C2" s="12"/>
+      <c r="D2" s="12"/>
+      <c r="E2" s="12"/>
+      <c r="F2" s="12"/>
+      <c r="G2" s="12"/>
+      <c r="H2" s="12"/>
+      <c r="I2" s="12"/>
+      <c r="J2" s="11"/>
+      <c r="K2" s="11"/>
+    </row>
+    <row r="3" ht="15" thickBot="true" x14ac:dyDescent="0.4">
+      <c r="A3" s="17"/>
+      <c r="B3" s="18"/>
+      <c r="C3" s="18"/>
+      <c r="D3" s="18"/>
+      <c r="E3" s="18"/>
+      <c r="F3" s="18"/>
+      <c r="G3" s="18"/>
+      <c r="H3" s="18"/>
+      <c r="I3" s="18"/>
+      <c r="J3" s="11"/>
+      <c r="K3" s="11"/>
+    </row>
+    <row r="4" x14ac:dyDescent="0.35">
+      <c r="A4" s="11"/>
+      <c r="B4" s="12"/>
+      <c r="C4" s="15" t="s">
         <v>19</v>
       </c>
-      <c r="D4" s="18"/>
-      <c r="E4" s="18"/>
-      <c r="F4" s="18" t="s">
+      <c r="D4" s="15"/>
+      <c r="E4" s="15"/>
+      <c r="F4" s="12"/>
+      <c r="G4" s="15" t="s">
         <v>18</v>
       </c>
-      <c r="G4" s="18"/>
-      <c r="H4" s="18"/>
-    </row>
-    <row r="5" spans="1:8" ht="16.5" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A5" s="13"/>
-      <c r="B5" s="15" t="s">
+      <c r="H4" s="15"/>
+      <c r="I4" s="15"/>
+      <c r="J4" s="11"/>
+      <c r="K4" s="11"/>
+    </row>
+    <row r="5" ht="16.5" customHeight="true" thickBot="true" x14ac:dyDescent="0.4">
+      <c r="A5" s="16"/>
+      <c r="B5" s="7" t="s">
         <v>1</v>
       </c>
-      <c r="C5" s="15" t="s">
+      <c r="C5" s="7" t="s">
         <v>12</v>
       </c>
-      <c r="D5" s="15" t="s">
+      <c r="D5" s="7" t="s">
         <v>0</v>
       </c>
-      <c r="E5" s="15" t="s">
+      <c r="E5" s="7" t="s">
         <v>2</v>
       </c>
-      <c r="F5" s="15" t="s">
+      <c r="F5" s="7"/>
+      <c r="G5" s="7" t="s">
         <v>12</v>
       </c>
-      <c r="G5" s="15" t="s">
+      <c r="H5" s="7" t="s">
         <v>13</v>
       </c>
-      <c r="H5" s="15" t="s">
+      <c r="I5" s="7" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="6" spans="1:8" ht="15" thickTop="1" x14ac:dyDescent="0.35">
-      <c r="A6" t="s">
+      <c r="J5" s="11"/>
+      <c r="K5" s="11"/>
+    </row>
+    <row r="6" ht="15" thickTop="true" x14ac:dyDescent="0.35">
+      <c r="A6" s="11" t="s">
         <v>15</v>
       </c>
-      <c r="B6" s="3">
+      <c r="B6" s="12">
         <f>ROUND(SS_att!B2,0)</f>
         <v>31</v>
       </c>
-      <c r="C6" s="3">
+      <c r="C6" s="12">
         <f>ROUND(SS_att!C2,0)</f>
         <v>31</v>
       </c>
-      <c r="D6" s="3">
+      <c r="D6" s="12">
         <f>ROUND(SS_att!E2,0)</f>
         <v>37</v>
       </c>
-      <c r="E6" s="3">
+      <c r="E6" s="12">
         <f>ROUND(SS_att!L2,2)</f>
         <v>0.16</v>
       </c>
-      <c r="F6" s="3">
+      <c r="F6" s="12"/>
+      <c r="G6" s="12">
         <f>ROUND(SS_att!D2,0)</f>
         <v>32</v>
       </c>
-      <c r="G6" s="3">
+      <c r="H6" s="12">
         <f>ROUND(SS_att!F2,0)</f>
         <v>34</v>
       </c>
-      <c r="H6" s="3">
+      <c r="I6" s="12">
         <f>ROUND(SS_att!M2,2)</f>
         <v>0.56999999999999995</v>
       </c>
-    </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="B7" s="3" t="str">
+      <c r="J6" s="11"/>
+      <c r="K6" s="11"/>
+    </row>
+    <row r="7" x14ac:dyDescent="0.35">
+      <c r="A7" s="11"/>
+      <c r="B7" s="12" t="str">
         <f>CONCATENATE("(",ROUND(SS_att!B3,1),")")</f>
         <v>(2.2)</v>
       </c>
-      <c r="C7" s="3" t="str">
+      <c r="C7" s="12" t="str">
         <f>CONCATENATE("(",ROUND(SS_att!C3,1),")")</f>
         <v>(2.3)</v>
       </c>
-      <c r="D7" s="3" t="str">
+      <c r="D7" s="12" t="str">
         <f>CONCATENATE("(",ROUND(SS_att!E3,1),")")</f>
         <v>(2.6)</v>
       </c>
-      <c r="F7" s="3" t="str">
+      <c r="E7" s="12"/>
+      <c r="F7" s="12"/>
+      <c r="G7" s="12" t="str">
         <f>CONCATENATE("(",ROUND(SS_att!D3,1),")")</f>
         <v>(2.4)</v>
       </c>
-      <c r="G7" s="3" t="str">
+      <c r="H7" s="12" t="str">
         <f>CONCATENATE("(",ROUND(SS_att!F3,1),")")</f>
         <v>(1.7)</v>
       </c>
-    </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="I7" s="12"/>
+      <c r="J7" s="11"/>
+      <c r="K7" s="11"/>
+    </row>
+    <row r="8" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
         <v>16</v>
       </c>
@@ -2771,20 +2875,20 @@
         <f>ROUND(SS_att!L10,2)</f>
         <v>0.73</v>
       </c>
-      <c r="F8" s="3">
+      <c r="G8" s="3">
         <f>ROUND(SS_att!D10,2)</f>
         <v>0.8</v>
       </c>
-      <c r="G8" s="3">
+      <c r="H8" s="3">
         <f>ROUND(SS_att!F10,2)</f>
         <v>0.79</v>
       </c>
-      <c r="H8" s="3">
+      <c r="I8" s="3">
         <f>ROUND(SS_att!M10,2)</f>
         <v>0.44</v>
       </c>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="9" x14ac:dyDescent="0.35">
       <c r="B9" s="3" t="str">
         <f>CONCATENATE("(",ROUND(SS_att!B11,2),")")</f>
         <v>(0.02)</v>
@@ -2797,16 +2901,16 @@
         <f>CONCATENATE("(",ROUND(SS_att!E11,2),")")</f>
         <v>(0.02)</v>
       </c>
-      <c r="F9" s="3" t="str">
+      <c r="G9" s="3" t="str">
         <f>CONCATENATE("(",ROUND(SS_att!D11,2),")")</f>
         <v>(0.02)</v>
       </c>
-      <c r="G9" s="3" t="str">
+      <c r="H9" s="3" t="str">
         <f>CONCATENATE("(",ROUND(SS_att!F11,2),")")</f>
         <v>(0.02)</v>
       </c>
     </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="10" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
         <v>14</v>
       </c>
@@ -2826,20 +2930,20 @@
         <f>ROUND(SS_att!L8,2)</f>
         <v>0.59</v>
       </c>
-      <c r="F10" s="3">
+      <c r="G10" s="3">
         <f>ROUND(SS_att!D8,2)</f>
         <v>0.98</v>
       </c>
-      <c r="G10" s="3">
+      <c r="H10" s="3">
         <f>ROUND(SS_att!F8,2)</f>
         <v>0.99</v>
       </c>
-      <c r="H10" s="3">
+      <c r="I10" s="3">
         <f>ROUND(SS_att!M8,2)</f>
         <v>0.11</v>
       </c>
     </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="11" x14ac:dyDescent="0.35">
       <c r="B11" s="3" t="str">
         <f>CONCATENATE("(",ROUND(SS_att!B9,3),")")</f>
         <v>(0.004)</v>
@@ -2852,16 +2956,16 @@
         <f>CONCATENATE("(",ROUND(SS_att!E9,3),")")</f>
         <v>(0.006)</v>
       </c>
-      <c r="F11" s="3" t="str">
+      <c r="G11" s="3" t="str">
         <f>CONCATENATE("(",ROUND(SS_att!D9,3),")")</f>
         <v>(0.004)</v>
       </c>
-      <c r="G11" s="3" t="str">
+      <c r="H11" s="3" t="str">
         <f>CONCATENATE("(",ROUND(SS_att!F9,3),")")</f>
         <v>(0.003)</v>
       </c>
     </row>
-    <row r="12" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="12" ht="15" thickBot="true" x14ac:dyDescent="0.4">
       <c r="A12" s="2" t="s">
         <v>5</v>
       </c>
@@ -2877,22 +2981,23 @@
         <f>SS_att!E6</f>
         <v>3406</v>
       </c>
-      <c r="E12" s="14"/>
-      <c r="F12" s="5">
+      <c r="E12" s="8"/>
+      <c r="F12" s="9"/>
+      <c r="G12" s="5">
         <f>SS_att!D6</f>
         <v>2143</v>
       </c>
-      <c r="G12" s="5">
+      <c r="H12" s="5">
         <f>SS_att!F6</f>
         <v>2753</v>
       </c>
-      <c r="H12" s="5"/>
-    </row>
-    <row r="13" spans="1:8" ht="15" thickTop="1" x14ac:dyDescent="0.35"/>
+      <c r="I12" s="5"/>
+    </row>
+    <row r="13" ht="15" thickTop="true" x14ac:dyDescent="0.35"/>
   </sheetData>
   <mergeCells count="3">
-    <mergeCell ref="B3:H3"/>
-    <mergeCell ref="F4:H4"/>
+    <mergeCell ref="B3:I3"/>
+    <mergeCell ref="G4:I4"/>
     <mergeCell ref="C4:E4"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
apr update and tot_tut analysis
</commit_message>
<xml_diff>
--- a/Tables/SS.xlsx
+++ b/Tables/SS.xlsx
@@ -1,6 +1,6 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24827"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\isaac\Dropbox\Apps\ShareLaTeX\Donde2020\Tables\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{655C151C-D549-491D-AE82-3E2710791C28}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5137F4EA-E541-4770-B5C6-9B9358049491}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28365" yWindow="-9315" windowWidth="12915" windowHeight="7470" activeTab="1"/>
+    <workbookView xWindow="-28920" yWindow="-10695" windowWidth="29040" windowHeight="15720" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="SS_admin" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
     <sheet name="SS" sheetId="5" r:id="rId5"/>
     <sheet name="Attrition" sheetId="6" r:id="rId6"/>
   </sheets>
-  <calcPr calcId="191029" fullCalcOnLoad="true"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
@@ -186,50 +186,50 @@
   </cellStyleXfs>
   <cellXfs count="19">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="true"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="true"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="true">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="true" applyAlignment="true">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="true" applyAlignment="true">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="true">
-      <alignment wrapText="true"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="true" applyAlignment="true">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="true" applyAlignment="true">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="true" applyAlignment="true">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="true" applyAlignment="true">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="true"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="true" applyAlignment="true">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="true" applyAlignment="true">
-      <alignment wrapText="true"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="true" applyAlignment="true">
-      <alignment horizontal="center" wrapText="true"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="true" applyAlignment="true">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="true" applyAlignment="true">
-      <alignment wrapText="true"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="true"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="true" applyAlignment="true">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -554,9 +554,9 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData>
-    <row r="2" x14ac:dyDescent="0.35">
+    <row r="2" spans="2:13" x14ac:dyDescent="0.35">
       <c r="B2">
-        <v>2301.0995770857362</v>
+        <v>2279.9653846153847</v>
       </c>
       <c r="C2">
         <v>2147.1437198067633</v>
@@ -565,53 +565,53 @@
         <v>2132.9021789522485</v>
       </c>
       <c r="E2">
-        <v>2182.1076833527359</v>
+        <v>2164.8011644832604</v>
       </c>
       <c r="F2">
         <v>2089.2792630057802</v>
       </c>
       <c r="G2">
-        <v>2161.6666666666665</v>
+        <v>2057.1111111111113</v>
       </c>
       <c r="H2">
-        <v>2171.5310435931306</v>
+        <v>2161.7426600117442</v>
       </c>
       <c r="K2">
-        <v>0.9541119628933088</v>
+        <v>0.46124979356012857</v>
       </c>
       <c r="L2">
-        <v>0.32512302780150443</v>
+        <v>0.37612637612186028</v>
       </c>
       <c r="M2">
-        <v>0.1049606267091812</v>
-      </c>
-    </row>
-    <row r="3" x14ac:dyDescent="0.35">
+        <v>0.14718551370824021</v>
+      </c>
+    </row>
+    <row r="3" spans="2:13" x14ac:dyDescent="0.35">
       <c r="B3">
-        <v>79.41696803972188</v>
+        <v>76.146605585818605</v>
       </c>
       <c r="C3">
-        <v>71.911953944693522</v>
+        <v>71.911953944693479</v>
       </c>
       <c r="D3">
         <v>73.985411575168982</v>
       </c>
       <c r="E3">
-        <v>64.994187260506564</v>
+        <v>57.575004627999661</v>
       </c>
       <c r="F3">
         <v>64.541278696715779</v>
       </c>
       <c r="G3">
-        <v>171.03256538840651</v>
+        <v>140.8140183528381</v>
       </c>
       <c r="H3">
-        <v>31.454802670595651</v>
-      </c>
-    </row>
-    <row r="4" x14ac:dyDescent="0.35">
+        <v>30.154263574554555</v>
+      </c>
+    </row>
+    <row r="4" spans="2:13" x14ac:dyDescent="0.35">
       <c r="B4">
-        <v>0.87812379853902345</v>
+        <v>0.87807692307692309</v>
       </c>
       <c r="C4">
         <v>0.89130434782608692</v>
@@ -620,7 +620,7 @@
         <v>0.88317107093184977</v>
       </c>
       <c r="E4">
-        <v>0.84662398137369033</v>
+        <v>0.84657933042212519</v>
       </c>
       <c r="F4">
         <v>0.82947976878612717</v>
@@ -629,44 +629,44 @@
         <v>0.83333331677648759</v>
       </c>
       <c r="H4">
-        <v>0.86290914406427177</v>
+        <v>0.86288901915882033</v>
       </c>
       <c r="K4">
-        <v>0.52347675751961098</v>
+        <v>0.52376627821867361</v>
       </c>
       <c r="L4">
-        <v>0.70540311975926762</v>
+        <v>0.70502590236959217</v>
       </c>
       <c r="M4">
-        <v>0.64425763902730926</v>
-      </c>
-    </row>
-    <row r="5" x14ac:dyDescent="0.35">
+        <v>0.64444779531836671</v>
+      </c>
+    </row>
+    <row r="5" spans="2:13" x14ac:dyDescent="0.35">
       <c r="B5">
-        <v>0.039962138649154974</v>
+        <v>3.9975841310504141E-2</v>
       </c>
       <c r="C5">
-        <v>0.033776765366283587</v>
+        <v>3.3776765366283587E-2</v>
       </c>
       <c r="D5">
-        <v>0.036353445955306977</v>
+        <v>3.6353445955306977E-2</v>
       </c>
       <c r="E5">
-        <v>0.042138188314307712</v>
+        <v>4.2147068344393836E-2</v>
       </c>
       <c r="F5">
-        <v>0.04836901048168215</v>
+        <v>4.836901048168215E-2</v>
       </c>
       <c r="G5">
-        <v>0.043154986380046355</v>
+        <v>4.3154986380046355E-2</v>
       </c>
       <c r="H5">
-        <v>0.018444101393584482</v>
-      </c>
-    </row>
-    <row r="6" x14ac:dyDescent="0.35">
+        <v>1.8446251080789934E-2</v>
+      </c>
+    </row>
+    <row r="6" spans="2:13" x14ac:dyDescent="0.35">
       <c r="B6">
-        <v>2601</v>
+        <v>2600</v>
       </c>
       <c r="C6">
         <v>2484</v>
@@ -675,7 +675,7 @@
         <v>2157</v>
       </c>
       <c r="E6">
-        <v>3436</v>
+        <v>3435</v>
       </c>
       <c r="F6">
         <v>2768</v>
@@ -684,7 +684,7 @@
         <v>180</v>
       </c>
       <c r="H6">
-        <v>13626</v>
+        <v>13624</v>
       </c>
     </row>
   </sheetData>
@@ -696,13 +696,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="B2:M11"/>
   <sheetViews>
-    <sheetView tabSelected="true" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="J1" sqref="J1:J13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData>
-    <row r="2" x14ac:dyDescent="0.35">
+    <row r="2" spans="2:13" x14ac:dyDescent="0.35">
       <c r="B2">
         <v>30.892857142857142</v>
       </c>
@@ -734,7 +734,7 @@
         <v>0.56873437132818427</v>
       </c>
     </row>
-    <row r="3" x14ac:dyDescent="0.35">
+    <row r="3" spans="2:13" x14ac:dyDescent="0.35">
       <c r="B3">
         <v>2.1952210296988395</v>
       </c>
@@ -757,7 +757,7 @@
         <v>0.81507699640653886</v>
       </c>
     </row>
-    <row r="4" x14ac:dyDescent="0.35">
+    <row r="4" spans="2:13" x14ac:dyDescent="0.35">
       <c r="B4">
         <v>84</v>
       </c>
@@ -777,10 +777,10 @@
         <v>180</v>
       </c>
       <c r="H4">
-        <v>83.86936738587994</v>
-      </c>
-    </row>
-    <row r="5" x14ac:dyDescent="0.35">
+        <v>83.868687610099826</v>
+      </c>
+    </row>
+    <row r="5" spans="2:13" x14ac:dyDescent="0.35">
       <c r="B5">
         <v>0</v>
       </c>
@@ -800,12 +800,12 @@
         <v>0</v>
       </c>
       <c r="H5">
-        <v>0.48193515492329214</v>
-      </c>
-    </row>
-    <row r="6" x14ac:dyDescent="0.35">
+        <v>0.48192768037495048</v>
+      </c>
+    </row>
+    <row r="6" spans="2:13" x14ac:dyDescent="0.35">
       <c r="B6">
-        <v>2601</v>
+        <v>2600</v>
       </c>
       <c r="C6">
         <v>2484</v>
@@ -814,7 +814,7 @@
         <v>2157</v>
       </c>
       <c r="E6">
-        <v>3436</v>
+        <v>3435</v>
       </c>
       <c r="F6">
         <v>2768</v>
@@ -823,58 +823,58 @@
         <v>180</v>
       </c>
       <c r="H6">
-        <v>13626</v>
-      </c>
-    </row>
-    <row r="8" x14ac:dyDescent="0.35">
+        <v>13624</v>
+      </c>
+    </row>
+    <row r="8" spans="2:13" x14ac:dyDescent="0.35">
       <c r="B8">
         <v>0.98280098280098283</v>
       </c>
       <c r="C8">
-        <v>0.97273203985317247</v>
+        <v>0.97222222222222221</v>
       </c>
       <c r="D8">
         <v>0.9869020501138952</v>
       </c>
       <c r="E8">
-        <v>0.97860568056067876</v>
+        <v>0.97823681298413867</v>
       </c>
       <c r="F8">
         <v>0.9887285843101894</v>
       </c>
       <c r="G8">
-        <v>0.98183871271290113</v>
+        <v>0.98165223936770796</v>
       </c>
       <c r="L8">
-        <v>0.4682775695018524</v>
+        <v>0.42791260083165938</v>
       </c>
       <c r="M8">
-        <v>0.48848582659027617</v>
-      </c>
-    </row>
-    <row r="9" x14ac:dyDescent="0.35">
+        <v>0.48848581421085902</v>
+      </c>
+    </row>
+    <row r="9" spans="2:13" x14ac:dyDescent="0.35">
       <c r="B9">
-        <v>0.0040156175496241656</v>
+        <v>4.0156175496241656E-3</v>
       </c>
       <c r="C9">
-        <v>0.0073961905116490204</v>
+        <v>7.3612074334708771E-3</v>
       </c>
       <c r="D9">
-        <v>0.0033401981602603041</v>
+        <v>3.3401981602603032E-3</v>
       </c>
       <c r="E9">
-        <v>0.0059580084747241947</v>
+        <v>5.982955141978775E-3</v>
       </c>
       <c r="F9">
-        <v>0.0029388029720992899</v>
+        <v>2.9388029720992899E-3</v>
       </c>
       <c r="G9">
-        <v>0.0023277574303601015</v>
-      </c>
-    </row>
-    <row r="10" x14ac:dyDescent="0.35">
+        <v>2.3323583385866185E-3</v>
+      </c>
+    </row>
+    <row r="10" spans="2:13" x14ac:dyDescent="0.35">
       <c r="B10">
-        <v>0.76893502499038835</v>
+        <v>0.76923076923076927</v>
       </c>
       <c r="C10">
         <v>0.74738114423851731</v>
@@ -883,39 +883,39 @@
         <v>0.80380333951762528</v>
       </c>
       <c r="E10">
-        <v>0.77211874272409775</v>
+        <v>0.77205240174672485</v>
       </c>
       <c r="F10">
         <v>0.79284164859002171</v>
       </c>
       <c r="G10">
-        <v>0.77628152667212258</v>
+        <v>0.77632264305379861</v>
       </c>
       <c r="L10">
-        <v>0.73908202673193557</v>
+        <v>0.73706312919069306</v>
       </c>
       <c r="M10">
-        <v>0.49749765961667392</v>
-      </c>
-    </row>
-    <row r="11" x14ac:dyDescent="0.35">
+        <v>0.50303070678483697</v>
+      </c>
+    </row>
+    <row r="11" spans="2:13" x14ac:dyDescent="0.35">
       <c r="B11">
-        <v>0.019892859098745899</v>
+        <v>1.9842184742342475E-2</v>
       </c>
       <c r="C11">
-        <v>0.025623636641152012</v>
+        <v>2.5623636641152012E-2</v>
       </c>
       <c r="D11">
-        <v>0.023871935695980506</v>
+        <v>2.3871935695980506E-2</v>
       </c>
       <c r="E11">
-        <v>0.023661163960051093</v>
+        <v>2.3676825836405423E-2</v>
       </c>
       <c r="F11">
-        <v>0.022472107685513335</v>
+        <v>2.2472107685513335E-2</v>
       </c>
       <c r="G11">
-        <v>0.010494345328496491</v>
+        <v>1.0493470680901324E-2</v>
       </c>
     </row>
   </sheetData>
@@ -933,7 +933,7 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData>
-    <row r="2" x14ac:dyDescent="0.35">
+    <row r="2" spans="2:13" x14ac:dyDescent="0.35">
       <c r="B2">
         <v>0.75514266755142667</v>
       </c>
@@ -956,39 +956,39 @@
         <v>0.73897857808134115</v>
       </c>
       <c r="K2">
-        <v>0.12370990152692971</v>
+        <v>0.1237099015269276</v>
       </c>
       <c r="L2">
-        <v>0.20316365915662879</v>
+        <v>0.20316365915662801</v>
       </c>
       <c r="M2">
-        <v>0.53421473315735057</v>
-      </c>
-    </row>
-    <row r="3" x14ac:dyDescent="0.35">
+        <v>0.53421473315735013</v>
+      </c>
+    </row>
+    <row r="3" spans="2:13" x14ac:dyDescent="0.35">
       <c r="B3">
-        <v>0.016425991245592318</v>
+        <v>1.6425991245592318E-2</v>
       </c>
       <c r="C3">
-        <v>0.016091100265249764</v>
+        <v>1.6091100265249757E-2</v>
       </c>
       <c r="D3">
-        <v>0.020324180320801286</v>
+        <v>2.0324180320801292E-2</v>
       </c>
       <c r="E3">
-        <v>0.015140443704992809</v>
+        <v>1.5140443704992812E-2</v>
       </c>
       <c r="F3">
-        <v>0.012828726752602795</v>
+        <v>1.2828726752602795E-2</v>
       </c>
       <c r="G3">
-        <v>0.0090149695175873699</v>
+        <v>9.0149695175873682E-3</v>
       </c>
       <c r="H3">
-        <v>0.0056750398759389097</v>
-      </c>
-    </row>
-    <row r="4" x14ac:dyDescent="0.35">
+        <v>5.6750398759389097E-3</v>
+      </c>
+    </row>
+    <row r="4" spans="2:13" x14ac:dyDescent="0.35">
       <c r="B4">
         <v>43.197583511016347</v>
       </c>
@@ -1011,44 +1011,44 @@
         <v>43.246039686509924</v>
       </c>
       <c r="K4">
-        <v>0.45869706596643639</v>
+        <v>0.45869706596643522</v>
       </c>
       <c r="L4">
-        <v>0.51811943398266236</v>
+        <v>0.51811943398266214</v>
       </c>
       <c r="M4">
-        <v>0.97646568723149629</v>
-      </c>
-    </row>
-    <row r="5" x14ac:dyDescent="0.35">
+        <v>0.97646568723149618</v>
+      </c>
+    </row>
+    <row r="5" spans="2:13" x14ac:dyDescent="0.35">
       <c r="B5">
-        <v>0.56359423339355974</v>
+        <v>0.56359423339355952</v>
       </c>
       <c r="C5">
-        <v>0.77069700997930024</v>
+        <v>0.77069700997930013</v>
       </c>
       <c r="D5">
-        <v>0.66004082042892598</v>
+        <v>0.66004082042892609</v>
       </c>
       <c r="E5">
-        <v>0.60465537492814869</v>
+        <v>0.6046553749281488</v>
       </c>
       <c r="F5">
         <v>0.51619884617405898</v>
       </c>
       <c r="G5">
-        <v>0.31582069920051542</v>
+        <v>0.31582069920051548</v>
       </c>
       <c r="H5">
         <v>0.21148102499151927</v>
       </c>
     </row>
-    <row r="6" x14ac:dyDescent="0.35">
+    <row r="6" spans="2:13" x14ac:dyDescent="0.35">
       <c r="B6">
         <v>3145.352544966549</v>
       </c>
       <c r="C6">
-        <v>2985.2732691622746</v>
+        <v>2984.9842439870736</v>
       </c>
       <c r="D6">
         <v>3010.3149184642348</v>
@@ -1063,42 +1063,42 @@
         <v>3192.3481642889119</v>
       </c>
       <c r="H6">
-        <v>3111.7794650246028</v>
+        <v>3111.7356224371706</v>
       </c>
       <c r="K6">
-        <v>0.15568188813603681</v>
+        <v>0.15545089802205039</v>
       </c>
       <c r="L6">
-        <v>0.34382243121919293</v>
+        <v>0.34170888107806208</v>
       </c>
       <c r="M6">
-        <v>0.41658257300111001</v>
-      </c>
-    </row>
-    <row r="7" x14ac:dyDescent="0.35">
+        <v>0.41658255644769909</v>
+      </c>
+    </row>
+    <row r="7" spans="2:13" x14ac:dyDescent="0.35">
       <c r="B7">
         <v>68.222299405324407</v>
       </c>
       <c r="C7">
-        <v>88.361354683798069</v>
+        <v>88.234047660960769</v>
       </c>
       <c r="D7">
-        <v>76.470442299269308</v>
+        <v>76.470442299269322</v>
       </c>
       <c r="E7">
-        <v>84.469381845420969</v>
+        <v>84.469381845420926</v>
       </c>
       <c r="F7">
-        <v>99.031452584314096</v>
+        <v>99.031452584314081</v>
       </c>
       <c r="G7">
-        <v>75.187897820076458</v>
+        <v>75.187897820076472</v>
       </c>
       <c r="H7">
-        <v>35.740522483170373</v>
-      </c>
-    </row>
-    <row r="8" x14ac:dyDescent="0.35">
+        <v>35.735445672018784</v>
+      </c>
+    </row>
+    <row r="8" spans="2:13" x14ac:dyDescent="0.35">
       <c r="B8">
         <v>0.89052631578947372</v>
       </c>
@@ -1124,41 +1124,41 @@
         <v>0.225273760595539</v>
       </c>
       <c r="L8">
-        <v>0.40550231444286611</v>
+        <v>0.40550231444286589</v>
       </c>
       <c r="M8">
-        <v>0.96738092930936548</v>
-      </c>
-    </row>
-    <row r="9" x14ac:dyDescent="0.35">
+        <v>0.96738092930936537</v>
+      </c>
+    </row>
+    <row r="9" spans="2:13" x14ac:dyDescent="0.35">
       <c r="B9">
-        <v>0.011504362429475282</v>
+        <v>1.1504362429475282E-2</v>
       </c>
       <c r="C9">
-        <v>0.010579094696170152</v>
+        <v>1.057909469617015E-2</v>
       </c>
       <c r="D9">
-        <v>0.014535413795478428</v>
+        <v>1.4535413795478427E-2</v>
       </c>
       <c r="E9">
-        <v>0.0099323761115656124</v>
+        <v>9.9323761115656124E-3</v>
       </c>
       <c r="F9">
-        <v>0.0094836902763061059</v>
+        <v>9.4836902763061059E-3</v>
       </c>
       <c r="G9">
-        <v>0.010533724370448033</v>
+        <v>1.0533724370448033E-2</v>
       </c>
       <c r="H9">
-        <v>0.0052054873450900745</v>
-      </c>
-    </row>
-    <row r="10" x14ac:dyDescent="0.35">
+        <v>5.2054873450900745E-3</v>
+      </c>
+    </row>
+    <row r="10" spans="2:13" x14ac:dyDescent="0.35">
       <c r="B10">
         <v>92.725089422585597</v>
       </c>
       <c r="C10">
-        <v>92.193231441048042</v>
+        <v>92.197490452809603</v>
       </c>
       <c r="D10">
         <v>93.655192532088677</v>
@@ -1173,24 +1173,24 @@
         <v>91.835829749369722</v>
       </c>
       <c r="H10">
-        <v>92.639685150375939</v>
+        <v>92.6401174743025</v>
       </c>
       <c r="K10">
-        <v>0.0011989512452381999</v>
+        <v>1.1912823211479E-3</v>
       </c>
       <c r="L10">
-        <v>0.1753183756276937</v>
+        <v>0.17622289997028059</v>
       </c>
       <c r="M10">
-        <v>0.48869910509747372</v>
-      </c>
-    </row>
-    <row r="11" x14ac:dyDescent="0.35">
+        <v>0.48869909187268379</v>
+      </c>
+    </row>
+    <row r="11" spans="2:13" x14ac:dyDescent="0.35">
       <c r="B11">
         <v>0.54084732630950216</v>
       </c>
       <c r="C11">
-        <v>0.83856879215694502</v>
+        <v>0.8381790132481084</v>
       </c>
       <c r="D11">
         <v>0.59030374500190863</v>
@@ -1202,13 +1202,13 @@
         <v>0.59487333389159291</v>
       </c>
       <c r="G11">
-        <v>0.30818777366122274</v>
+        <v>0.30818777366122263</v>
       </c>
       <c r="H11">
-        <v>0.20476842319378324</v>
-      </c>
-    </row>
-    <row r="12" x14ac:dyDescent="0.35">
+        <v>0.20475253752404457</v>
+      </c>
+    </row>
+    <row r="12" spans="2:13" x14ac:dyDescent="0.35">
       <c r="B12">
         <v>0.6597421203438395</v>
       </c>
@@ -1231,44 +1231,44 @@
         <v>0.63285064825728232</v>
       </c>
       <c r="K12">
-        <v>0.0001115253817344</v>
+        <v>1.115253817344E-4</v>
       </c>
       <c r="L12">
-        <v>0.94338858432257511</v>
+        <v>0.94338858432257489</v>
       </c>
       <c r="M12">
-        <v>0.81166552956809135</v>
-      </c>
-    </row>
-    <row r="13" x14ac:dyDescent="0.35">
+        <v>0.81166552956809146</v>
+      </c>
+    </row>
+    <row r="13" spans="2:13" x14ac:dyDescent="0.35">
       <c r="B13">
-        <v>0.019382047390071523</v>
+        <v>1.938204739007152E-2</v>
       </c>
       <c r="C13">
-        <v>0.019329841394817811</v>
+        <v>1.9329841394817811E-2</v>
       </c>
       <c r="D13">
-        <v>0.024251483945742537</v>
+        <v>2.4251483945742537E-2</v>
       </c>
       <c r="E13">
-        <v>0.016843213086678365</v>
+        <v>1.6843213086678365E-2</v>
       </c>
       <c r="F13">
-        <v>0.016646508216829125</v>
+        <v>1.6646508216829121E-2</v>
       </c>
       <c r="G13">
-        <v>0.012957951584969644</v>
+        <v>1.2957951584969644E-2</v>
       </c>
       <c r="H13">
-        <v>0.0074824965608947022</v>
-      </c>
-    </row>
-    <row r="14" x14ac:dyDescent="0.35">
+        <v>7.4824965608947022E-3</v>
+      </c>
+    </row>
+    <row r="14" spans="2:13" x14ac:dyDescent="0.35">
       <c r="B14">
-        <v>2636</v>
+        <v>2635</v>
       </c>
       <c r="C14">
-        <v>2534</v>
+        <v>2535</v>
       </c>
       <c r="D14">
         <v>2179</v>
@@ -1286,12 +1286,12 @@
         <v>20553</v>
       </c>
     </row>
-    <row r="16" x14ac:dyDescent="0.35">
+    <row r="16" spans="2:13" x14ac:dyDescent="0.35">
       <c r="B16">
         <v>2035</v>
       </c>
       <c r="C16">
-        <v>1907</v>
+        <v>1908</v>
       </c>
       <c r="D16">
         <v>1756</v>
@@ -1321,7 +1321,7 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData>
-    <row r="2" x14ac:dyDescent="0.35">
+    <row r="2" spans="2:11" x14ac:dyDescent="0.35">
       <c r="B2">
         <v>0.75706594885598921</v>
       </c>
@@ -1332,42 +1332,42 @@
         <v>0.72527472527472525</v>
       </c>
       <c r="E2">
-        <v>0.71775417298937783</v>
+        <v>0.71761133603238869</v>
       </c>
       <c r="F2">
         <v>0.74111041796631316</v>
       </c>
       <c r="G2">
-        <v>0.73263212569796132</v>
+        <v>0.73259740259740258</v>
       </c>
       <c r="J2">
-        <v>0.1834112165576095</v>
+        <v>0.18200741924100611</v>
       </c>
       <c r="K2">
-        <v>0.47018825520502039</v>
-      </c>
-    </row>
-    <row r="3" x14ac:dyDescent="0.35">
+        <v>0.47018827911332062</v>
+      </c>
+    </row>
+    <row r="3" spans="2:11" x14ac:dyDescent="0.35">
       <c r="B3">
-        <v>0.016329938660297399</v>
+        <v>1.6329938660297399E-2</v>
       </c>
       <c r="C3">
-        <v>0.016037712453979815</v>
+        <v>1.6037712453979818E-2</v>
       </c>
       <c r="D3">
-        <v>0.020704066804602263</v>
+        <v>2.0704066804602263E-2</v>
       </c>
       <c r="E3">
-        <v>0.015845064022229488</v>
+        <v>1.5859952936583335E-2</v>
       </c>
       <c r="F3">
-        <v>0.012945207155944546</v>
+        <v>1.2945207155944547E-2</v>
       </c>
       <c r="G3">
-        <v>0.0073798781164302616</v>
-      </c>
-    </row>
-    <row r="4" x14ac:dyDescent="0.35">
+        <v>7.382530362813145E-3</v>
+      </c>
+    </row>
+    <row r="4" spans="2:11" x14ac:dyDescent="0.35">
       <c r="B4">
         <v>43.164866810655148</v>
       </c>
@@ -1378,22 +1378,22 @@
         <v>42.960185185185182</v>
       </c>
       <c r="E4">
-        <v>43.95550611790879</v>
+        <v>43.963272120200337</v>
       </c>
       <c r="F4">
         <v>43.072377158034527</v>
       </c>
       <c r="G4">
-        <v>43.315612287838405</v>
+        <v>43.317480359147027</v>
       </c>
       <c r="J4">
-        <v>0.58878257193305883</v>
+        <v>0.58299404675484134</v>
       </c>
       <c r="K4">
-        <v>0.97226330514763726</v>
-      </c>
-    </row>
-    <row r="5" x14ac:dyDescent="0.35">
+        <v>0.97226330730205768</v>
+      </c>
+    </row>
+    <row r="5" spans="2:11" x14ac:dyDescent="0.35">
       <c r="B5">
         <v>0.57302039418728534</v>
       </c>
@@ -1401,19 +1401,19 @@
         <v>0.7869341141204792</v>
       </c>
       <c r="D5">
-        <v>0.6516138308721301</v>
+        <v>0.65161383087213032</v>
       </c>
       <c r="E5">
-        <v>0.61205771211875037</v>
+        <v>0.61260005153338226</v>
       </c>
       <c r="F5">
         <v>0.5175395496028099</v>
       </c>
       <c r="G5">
-        <v>0.2831845022118607</v>
-      </c>
-    </row>
-    <row r="6" x14ac:dyDescent="0.35">
+        <v>0.28326816453393761</v>
+      </c>
+    </row>
+    <row r="6" spans="2:11" x14ac:dyDescent="0.35">
       <c r="B6">
         <v>3151.8311879330831</v>
       </c>
@@ -1433,24 +1433,24 @@
         <v>3069.2245258990883</v>
       </c>
       <c r="J6">
-        <v>0.29805537908350171</v>
+        <v>0.29805537908350199</v>
       </c>
       <c r="K6">
         <v>0.27369802702174151</v>
       </c>
     </row>
-    <row r="7" x14ac:dyDescent="0.35">
+    <row r="7" spans="2:11" x14ac:dyDescent="0.35">
       <c r="B7">
-        <v>68.633705702668735</v>
+        <v>68.633705702668763</v>
       </c>
       <c r="C7">
         <v>90.821567649747067</v>
       </c>
       <c r="D7">
-        <v>76.019238973365503</v>
+        <v>76.019238973365518</v>
       </c>
       <c r="E7">
-        <v>84.552913105159746</v>
+        <v>84.55291310515976</v>
       </c>
       <c r="F7">
         <v>99.417675983085019</v>
@@ -1459,7 +1459,7 @@
         <v>38.649480296696282</v>
       </c>
     </row>
-    <row r="8" x14ac:dyDescent="0.35">
+    <row r="8" spans="2:11" x14ac:dyDescent="0.35">
       <c r="B8">
         <v>0.89102564102564108</v>
       </c>
@@ -1470,42 +1470,42 @@
         <v>0.89289012003693446</v>
       </c>
       <c r="E8">
-        <v>0.91063596491228072</v>
+        <v>0.91058694459681844</v>
       </c>
       <c r="F8">
         <v>0.89374579690652323</v>
       </c>
       <c r="G8">
-        <v>0.89827442248817146</v>
+        <v>0.89826026443980511</v>
       </c>
       <c r="J8">
-        <v>0.42137792268207369</v>
+        <v>0.42375394960748619</v>
       </c>
       <c r="K8">
-        <v>0.98364695237340527</v>
-      </c>
-    </row>
-    <row r="9" x14ac:dyDescent="0.35">
+        <v>0.98364695363089938</v>
+      </c>
+    </row>
+    <row r="9" spans="2:11" x14ac:dyDescent="0.35">
       <c r="B9">
-        <v>0.011699017063997981</v>
+        <v>1.1699017063997981E-2</v>
       </c>
       <c r="C9">
-        <v>0.010536449576402311</v>
+        <v>1.0536449576402311E-2</v>
       </c>
       <c r="D9">
-        <v>0.014414244480650894</v>
+        <v>1.4414244480650894E-2</v>
       </c>
       <c r="E9">
-        <v>0.0099893832545590311</v>
+        <v>9.9989344362034476E-3</v>
       </c>
       <c r="F9">
-        <v>0.0095382524633601719</v>
+        <v>9.5382524633601719E-3</v>
       </c>
       <c r="G9">
-        <v>0.0049480485445660988</v>
-      </c>
-    </row>
-    <row r="10" x14ac:dyDescent="0.35">
+        <v>4.9491419759811308E-3</v>
+      </c>
+    </row>
+    <row r="10" spans="2:11" x14ac:dyDescent="0.35">
       <c r="B10">
         <v>92.740644490644485</v>
       </c>
@@ -1516,24 +1516,24 @@
         <v>93.604376108811351</v>
       </c>
       <c r="E10">
-        <v>93.67277691107644</v>
+        <v>93.670308232539995</v>
       </c>
       <c r="F10">
         <v>93.290866510538635</v>
       </c>
       <c r="G10">
-        <v>93.135175282234101</v>
+        <v>93.134495394671688</v>
       </c>
       <c r="J10">
-        <v>0.20933519826952979</v>
+        <v>0.21062078261948161</v>
       </c>
       <c r="K10">
-        <v>0.55369820684746696</v>
-      </c>
-    </row>
-    <row r="11" x14ac:dyDescent="0.35">
+        <v>0.55369821967704347</v>
+      </c>
+    </row>
+    <row r="11" spans="2:11" x14ac:dyDescent="0.35">
       <c r="B11">
-        <v>0.55282250572746683</v>
+        <v>0.55282250572746661</v>
       </c>
       <c r="C11">
         <v>0.85746436976065976</v>
@@ -1542,16 +1542,16 @@
         <v>0.59648670007090754</v>
       </c>
       <c r="E11">
-        <v>0.47058032652713411</v>
+        <v>0.47054474058339091</v>
       </c>
       <c r="F11">
-        <v>0.59891547015170421</v>
+        <v>0.59891547015170432</v>
       </c>
       <c r="G11">
-        <v>0.27435415453128742</v>
-      </c>
-    </row>
-    <row r="12" x14ac:dyDescent="0.35">
+        <v>0.27434924538180411</v>
+      </c>
+    </row>
+    <row r="12" spans="2:11" x14ac:dyDescent="0.35">
       <c r="B12">
         <v>0.66084425036390104</v>
       </c>
@@ -1562,44 +1562,44 @@
         <v>0.64694835680751173</v>
       </c>
       <c r="E12">
-        <v>0.66609783845278725</v>
+        <v>0.66590779738190098</v>
       </c>
       <c r="F12">
         <v>0.64220824598183091</v>
       </c>
       <c r="G12">
-        <v>0.65845272206303729</v>
+        <v>0.65840378277690215</v>
       </c>
       <c r="J12">
-        <v>0.91217898619646376</v>
+        <v>0.91190770005625166</v>
       </c>
       <c r="K12">
-        <v>0.75438827879433412</v>
-      </c>
-    </row>
-    <row r="13" x14ac:dyDescent="0.35">
+        <v>0.75438829625622084</v>
+      </c>
+    </row>
+    <row r="13" spans="2:11" x14ac:dyDescent="0.35">
       <c r="B13">
-        <v>0.019264793906698385</v>
+        <v>1.9264793906698385E-2</v>
       </c>
       <c r="C13">
-        <v>0.018898567915395067</v>
+        <v>1.8898567915395067E-2</v>
       </c>
       <c r="D13">
-        <v>0.024289475036466852</v>
+        <v>2.4289475036466852E-2</v>
       </c>
       <c r="E13">
-        <v>0.016413508256461058</v>
+        <v>1.6402036310363216E-2</v>
       </c>
       <c r="F13">
-        <v>0.016248832152705936</v>
+        <v>1.6248832152705936E-2</v>
       </c>
       <c r="G13">
-        <v>0.0083777184461360614</v>
-      </c>
-    </row>
-    <row r="14" x14ac:dyDescent="0.35">
+        <v>8.3758892114355592E-3</v>
+      </c>
+    </row>
+    <row r="14" spans="2:11" x14ac:dyDescent="0.35">
       <c r="B14">
-        <v>2601</v>
+        <v>2600</v>
       </c>
       <c r="C14">
         <v>2482</v>
@@ -1608,16 +1608,16 @@
         <v>2156</v>
       </c>
       <c r="E14">
-        <v>3436</v>
+        <v>3435</v>
       </c>
       <c r="F14">
         <v>2766</v>
       </c>
       <c r="G14">
-        <v>13441</v>
-      </c>
-    </row>
-    <row r="16" x14ac:dyDescent="0.35">
+        <v>13439</v>
+      </c>
+    </row>
+    <row r="16" spans="2:11" x14ac:dyDescent="0.35">
       <c r="B16">
         <v>2000</v>
       </c>
@@ -1628,7 +1628,7 @@
         <v>1733</v>
       </c>
       <c r="E16">
-        <v>2653</v>
+        <v>2652</v>
       </c>
       <c r="F16">
         <v>2193</v>
@@ -1643,1037 +1643,1037 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3B054637-0760-4807-B01C-4419EACB0C14}">
   <dimension ref="A2:I39"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="A3" sqref="A3:I38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="18.1796875" bestFit="true" customWidth="true"/>
-    <col min="2" max="2" width="9.7265625" style="3" customWidth="true"/>
-    <col min="3" max="3" width="10.54296875" style="3" customWidth="true"/>
-    <col min="4" max="4" width="7.54296875" style="3" bestFit="true" customWidth="true"/>
-    <col min="5" max="5" width="7.54296875" style="3" customWidth="true"/>
-    <col min="6" max="6" width="1.36328125" style="3" customWidth="true"/>
+    <col min="1" max="1" width="18.1796875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="9.7265625" style="3" customWidth="1"/>
+    <col min="3" max="3" width="10.54296875" style="3" customWidth="1"/>
+    <col min="4" max="4" width="7.54296875" style="3" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="7.54296875" style="3" customWidth="1"/>
+    <col min="6" max="6" width="1.36328125" style="3" customWidth="1"/>
     <col min="7" max="8" width="8.7265625" style="3"/>
-    <col min="9" max="9" width="9.7265625" style="3" customWidth="true"/>
+    <col min="9" max="9" width="9.7265625" style="3" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" s="11" customFormat="true" ht="15" thickBot="true" x14ac:dyDescent="0.4">
-      <c r="A2" s="17"/>
-      <c r="B2" s="18"/>
-      <c r="C2" s="18"/>
-      <c r="D2" s="18"/>
-      <c r="E2" s="18"/>
-      <c r="F2" s="18"/>
-      <c r="G2" s="18"/>
-      <c r="H2" s="18"/>
-      <c r="I2" s="18"/>
-    </row>
-    <row r="3" x14ac:dyDescent="0.35">
-      <c r="A3" s="11"/>
-      <c r="B3" s="12"/>
-      <c r="C3" s="15" t="s">
+    <row r="2" spans="1:9" s="10" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A2" s="15"/>
+      <c r="B2" s="16"/>
+      <c r="C2" s="16"/>
+      <c r="D2" s="16"/>
+      <c r="E2" s="16"/>
+      <c r="F2" s="16"/>
+      <c r="G2" s="16"/>
+      <c r="H2" s="16"/>
+      <c r="I2" s="16"/>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A3" s="10"/>
+      <c r="B3" s="11"/>
+      <c r="C3" s="18" t="s">
         <v>19</v>
       </c>
-      <c r="D3" s="15"/>
-      <c r="E3" s="15"/>
-      <c r="F3" s="12"/>
-      <c r="G3" s="15" t="s">
+      <c r="D3" s="18"/>
+      <c r="E3" s="18"/>
+      <c r="F3" s="11"/>
+      <c r="G3" s="18" t="s">
         <v>18</v>
       </c>
-      <c r="H3" s="15"/>
-      <c r="I3" s="15"/>
-    </row>
-    <row r="4" s="6" customFormat="true" x14ac:dyDescent="0.35">
-      <c r="A4" s="13"/>
-      <c r="B4" s="14" t="s">
+      <c r="H3" s="18"/>
+      <c r="I3" s="18"/>
+    </row>
+    <row r="4" spans="1:9" s="6" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A4" s="12"/>
+      <c r="B4" s="13" t="s">
         <v>1</v>
       </c>
-      <c r="C4" s="14" t="s">
+      <c r="C4" s="13" t="s">
         <v>12</v>
       </c>
-      <c r="D4" s="14" t="s">
+      <c r="D4" s="13" t="s">
         <v>0</v>
       </c>
-      <c r="E4" s="14" t="s">
+      <c r="E4" s="13" t="s">
         <v>2</v>
       </c>
-      <c r="F4" s="14"/>
-      <c r="G4" s="14" t="s">
+      <c r="F4" s="13"/>
+      <c r="G4" s="13" t="s">
         <v>12</v>
       </c>
-      <c r="H4" s="14" t="s">
+      <c r="H4" s="13" t="s">
         <v>13</v>
       </c>
-      <c r="I4" s="14" t="s">
+      <c r="I4" s="13" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="5" ht="15" thickBot="true" x14ac:dyDescent="0.4">
+    <row r="5" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A5" s="2"/>
-      <c r="B5" s="10" t="s">
+      <c r="B5" s="17" t="s">
         <v>3</v>
       </c>
-      <c r="C5" s="10"/>
-      <c r="D5" s="10"/>
-      <c r="E5" s="10"/>
-      <c r="F5" s="10"/>
-      <c r="G5" s="10"/>
-      <c r="H5" s="10"/>
-      <c r="I5" s="10"/>
-    </row>
-    <row r="6" ht="15" thickTop="true" x14ac:dyDescent="0.35">
-      <c r="A6" s="11" t="s">
+      <c r="C5" s="17"/>
+      <c r="D5" s="17"/>
+      <c r="E5" s="17"/>
+      <c r="F5" s="17"/>
+      <c r="G5" s="17"/>
+      <c r="H5" s="17"/>
+      <c r="I5" s="17"/>
+    </row>
+    <row r="6" spans="1:9" ht="15" thickTop="1" x14ac:dyDescent="0.35">
+      <c r="A6" s="10" t="s">
         <v>4</v>
       </c>
-      <c r="B6" s="12">
+      <c r="B6" s="11">
         <f>ROUND(SS_admin!B2,0)</f>
-        <v>2289</v>
-      </c>
-      <c r="C6" s="12">
+        <v>2280</v>
+      </c>
+      <c r="C6" s="11">
         <f>ROUND(SS_admin!C2,0)</f>
-        <v>2131</v>
-      </c>
-      <c r="D6" s="12">
+        <v>2147</v>
+      </c>
+      <c r="D6" s="11">
         <f>ROUND(SS_admin!E2,0)</f>
-        <v>2180</v>
-      </c>
-      <c r="E6" s="12">
+        <v>2165</v>
+      </c>
+      <c r="E6" s="11">
         <f>ROUND(SS_admin!L2,2)</f>
-        <v>0.32</v>
-      </c>
-      <c r="F6" s="12"/>
-      <c r="G6" s="12">
+        <v>0.38</v>
+      </c>
+      <c r="F6" s="11"/>
+      <c r="G6" s="11">
         <f>ROUND(SS_admin!D2,0)</f>
-        <v>2136</v>
-      </c>
-      <c r="H6" s="12">
+        <v>2133</v>
+      </c>
+      <c r="H6" s="11">
         <f>ROUND(SS_admin!F2,0)</f>
-        <v>2090</v>
-      </c>
-      <c r="I6" s="12">
+        <v>2089</v>
+      </c>
+      <c r="I6" s="11">
         <f>ROUND(SS_admin!M2,2)</f>
-        <v>0.14000000000000001</v>
-      </c>
-    </row>
-    <row r="7" x14ac:dyDescent="0.35">
-      <c r="A7" s="11"/>
-      <c r="B7" s="12" t="str">
+        <v>0.15</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A7" s="10"/>
+      <c r="B7" s="11" t="str">
         <f>CONCATENATE("(",ROUND(SS_admin!B3,0),")")</f>
-        <v>(79)</v>
-      </c>
-      <c r="C7" s="12" t="str">
+        <v>(76)</v>
+      </c>
+      <c r="C7" s="11" t="str">
         <f>CONCATENATE("(",ROUND(SS_admin!C3,0),")")</f>
-        <v>(73)</v>
-      </c>
-      <c r="D7" s="12" t="str">
+        <v>(72)</v>
+      </c>
+      <c r="D7" s="11" t="str">
         <f>CONCATENATE("(",ROUND(SS_admin!E3,0),")")</f>
-        <v>(66)</v>
-      </c>
-      <c r="E7" s="12"/>
-      <c r="F7" s="12"/>
-      <c r="G7" s="12" t="str">
+        <v>(58)</v>
+      </c>
+      <c r="E7" s="11"/>
+      <c r="F7" s="11"/>
+      <c r="G7" s="11" t="str">
         <f>CONCATENATE("(",ROUND(SS_admin!D3,0),")")</f>
         <v>(74)</v>
       </c>
-      <c r="H7" s="12" t="str">
+      <c r="H7" s="11" t="str">
         <f>CONCATENATE("(",ROUND(SS_admin!F3,0),")")</f>
         <v>(65)</v>
       </c>
-      <c r="I7" s="12"/>
-    </row>
-    <row r="8" x14ac:dyDescent="0.35">
-      <c r="A8" s="11" t="s">
+      <c r="I7" s="11"/>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A8" s="10" t="s">
         <v>17</v>
       </c>
-      <c r="B8" s="12">
+      <c r="B8" s="11">
         <f>ROUND(SS_admin!B4,2)</f>
         <v>0.88</v>
       </c>
-      <c r="C8" s="12">
+      <c r="C8" s="11">
         <f>ROUND(SS_admin!C4,2)</f>
         <v>0.89</v>
       </c>
-      <c r="D8" s="12">
+      <c r="D8" s="11">
         <f>ROUND(SS_admin!E4,2)</f>
         <v>0.85</v>
       </c>
-      <c r="E8" s="12">
+      <c r="E8" s="11">
         <f>ROUND(SS_admin!L4,2)</f>
-        <v>0.72</v>
-      </c>
-      <c r="F8" s="12"/>
-      <c r="G8" s="12">
+        <v>0.71</v>
+      </c>
+      <c r="F8" s="11"/>
+      <c r="G8" s="11">
         <f>ROUND(SS_admin!D4,2)</f>
-        <v>0.89</v>
-      </c>
-      <c r="H8" s="12">
+        <v>0.88</v>
+      </c>
+      <c r="H8" s="11">
         <f>ROUND(SS_admin!F4,2)</f>
         <v>0.83</v>
       </c>
-      <c r="I8" s="12">
+      <c r="I8" s="11">
         <f>ROUND(SS_admin!M4,2)</f>
-        <v>0.62</v>
-      </c>
-    </row>
-    <row r="9" x14ac:dyDescent="0.35">
-      <c r="A9" s="11"/>
-      <c r="B9" s="12" t="str">
+        <v>0.64</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A9" s="10"/>
+      <c r="B9" s="11" t="str">
         <f>CONCATENATE("(",ROUND(SS_admin!B5,3),")")</f>
         <v>(0.04)</v>
       </c>
-      <c r="C9" s="12" t="str">
+      <c r="C9" s="11" t="str">
         <f>CONCATENATE("(",ROUND(SS_admin!C5,3),")")</f>
         <v>(0.034)</v>
       </c>
-      <c r="D9" s="12" t="str">
+      <c r="D9" s="11" t="str">
         <f>CONCATENATE("(",ROUND(SS_admin!E5,3),")")</f>
         <v>(0.042)</v>
       </c>
-      <c r="E9" s="12"/>
-      <c r="F9" s="12"/>
-      <c r="G9" s="12" t="str">
+      <c r="E9" s="11"/>
+      <c r="F9" s="11"/>
+      <c r="G9" s="11" t="str">
         <f>CONCATENATE("(",ROUND(SS_admin!D5,3),")")</f>
         <v>(0.036)</v>
       </c>
-      <c r="H9" s="12" t="str">
+      <c r="H9" s="11" t="str">
         <f>CONCATENATE("(",ROUND(SS_admin!F5,3),")")</f>
-        <v>(0.049)</v>
-      </c>
-      <c r="I9" s="12"/>
-    </row>
-    <row r="10" x14ac:dyDescent="0.35">
+        <v>(0.048)</v>
+      </c>
+      <c r="I9" s="11"/>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A10" s="1" t="s">
         <v>5</v>
       </c>
       <c r="B10" s="4">
         <f>SS_admin!B6</f>
-        <v>2585</v>
+        <v>2600</v>
       </c>
       <c r="C10" s="4">
         <f>SS_admin!C6</f>
-        <v>2465</v>
+        <v>2484</v>
       </c>
       <c r="D10" s="4">
         <f>SS_admin!E6</f>
-        <v>3406</v>
+        <v>3435</v>
       </c>
       <c r="E10" s="4"/>
       <c r="F10" s="4"/>
       <c r="G10" s="4">
         <f>SS_admin!D6</f>
-        <v>2143</v>
+        <v>2157</v>
       </c>
       <c r="H10" s="4">
         <f>SS_admin!F6</f>
-        <v>2753</v>
+        <v>2768</v>
       </c>
       <c r="I10" s="4"/>
     </row>
-    <row r="11" ht="15" thickBot="true" x14ac:dyDescent="0.4">
+    <row r="11" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A11" s="2"/>
-      <c r="B11" s="10" t="s">
+      <c r="B11" s="17" t="s">
         <v>21</v>
       </c>
-      <c r="C11" s="10"/>
-      <c r="D11" s="10"/>
-      <c r="E11" s="10"/>
-      <c r="F11" s="10"/>
-      <c r="G11" s="10"/>
-      <c r="H11" s="10"/>
-      <c r="I11" s="10"/>
-    </row>
-    <row r="12" ht="15" thickTop="true" x14ac:dyDescent="0.35">
-      <c r="A12" s="11" t="s">
+      <c r="C11" s="17"/>
+      <c r="D11" s="17"/>
+      <c r="E11" s="17"/>
+      <c r="F11" s="17"/>
+      <c r="G11" s="17"/>
+      <c r="H11" s="17"/>
+      <c r="I11" s="17"/>
+    </row>
+    <row r="12" spans="1:9" ht="15" thickTop="1" x14ac:dyDescent="0.35">
+      <c r="A12" s="10" t="s">
         <v>6</v>
       </c>
-      <c r="B12" s="12">
+      <c r="B12" s="11">
         <f>ROUND(SS_survey_uncond!B2,2)</f>
-        <v>0.75</v>
-      </c>
-      <c r="C12" s="12">
+        <v>0.76</v>
+      </c>
+      <c r="C12" s="11">
         <f>ROUND(SS_survey_uncond!C2,2)</f>
         <v>0.72</v>
       </c>
-      <c r="D12" s="12">
+      <c r="D12" s="11">
         <f>ROUND(SS_survey_uncond!E2,2)</f>
         <v>0.72</v>
       </c>
-      <c r="E12" s="12">
+      <c r="E12" s="11">
         <f>ROUND(SS_survey_uncond!L2,2)</f>
-        <v>0.22</v>
-      </c>
-      <c r="F12" s="12"/>
-      <c r="G12" s="12">
+        <v>0.2</v>
+      </c>
+      <c r="F12" s="11"/>
+      <c r="G12" s="11">
         <f>ROUND(SS_survey_uncond!D2,2)</f>
-        <v>0.72</v>
-      </c>
-      <c r="H12" s="12">
+        <v>0.73</v>
+      </c>
+      <c r="H12" s="11">
         <f>ROUND(SS_survey_uncond!F2,2)</f>
         <v>0.74</v>
       </c>
-      <c r="I12" s="12">
+      <c r="I12" s="11">
         <f>ROUND(SS_survey_uncond!M2,2)</f>
-        <v>0.52</v>
-      </c>
-    </row>
-    <row r="13" x14ac:dyDescent="0.35">
-      <c r="A13" s="11"/>
-      <c r="B13" s="12" t="str">
+        <v>0.53</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A13" s="10"/>
+      <c r="B13" s="11" t="str">
         <f>CONCATENATE("(",ROUND(SS_survey_uncond!B3,3),")")</f>
-        <v>(0.017)</v>
-      </c>
-      <c r="C13" s="12" t="str">
+        <v>(0.016)</v>
+      </c>
+      <c r="C13" s="11" t="str">
         <f>CONCATENATE("(",ROUND(SS_survey_uncond!C3,3),")")</f>
-        <v>(0.017)</v>
-      </c>
-      <c r="D13" s="12" t="str">
+        <v>(0.016)</v>
+      </c>
+      <c r="D13" s="11" t="str">
         <f>CONCATENATE("(",ROUND(SS_survey_uncond!E3,3),")")</f>
         <v>(0.015)</v>
       </c>
-      <c r="E13" s="12"/>
-      <c r="F13" s="12"/>
-      <c r="G13" s="12" t="str">
+      <c r="E13" s="11"/>
+      <c r="F13" s="11"/>
+      <c r="G13" s="11" t="str">
         <f>CONCATENATE("(",ROUND(SS_survey_uncond!D3,3),")")</f>
         <v>(0.02)</v>
       </c>
-      <c r="H13" s="12" t="str">
+      <c r="H13" s="11" t="str">
         <f>CONCATENATE("(",ROUND(SS_survey_uncond!F3,3),")")</f>
         <v>(0.013)</v>
       </c>
-      <c r="I13" s="12"/>
-    </row>
-    <row r="14" x14ac:dyDescent="0.35">
-      <c r="A14" s="11" t="s">
+      <c r="I13" s="11"/>
+    </row>
+    <row r="14" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A14" s="10" t="s">
         <v>7</v>
       </c>
-      <c r="B14" s="12">
+      <c r="B14" s="11">
         <f>ROUND(SS_survey_uncond!B4,2)</f>
-        <v>43.22</v>
-      </c>
-      <c r="C14" s="12">
+        <v>43.2</v>
+      </c>
+      <c r="C14" s="11">
         <f>ROUND(SS_survey_uncond!C4,2)</f>
-        <v>43.2</v>
-      </c>
-      <c r="D14" s="12">
+        <v>43.21</v>
+      </c>
+      <c r="D14" s="11">
         <f>ROUND(SS_survey_uncond!E4,2)</f>
-        <v>44.04</v>
-      </c>
-      <c r="E14" s="12">
+        <v>44.07</v>
+      </c>
+      <c r="E14" s="11">
         <f>ROUND(SS_survey_uncond!L4,2)</f>
-        <v>0.55000000000000004</v>
-      </c>
-      <c r="F14" s="12"/>
-      <c r="G14" s="12">
+        <v>0.52</v>
+      </c>
+      <c r="F14" s="11"/>
+      <c r="G14" s="11">
         <f>ROUND(SS_survey_uncond!D4,2)</f>
-        <v>43</v>
-      </c>
-      <c r="H14" s="12">
+        <v>43.01</v>
+      </c>
+      <c r="H14" s="11">
         <f>ROUND(SS_survey_uncond!F4,2)</f>
-        <v>43.1</v>
-      </c>
-      <c r="I14" s="12">
+        <v>43.09</v>
+      </c>
+      <c r="I14" s="11">
         <f>ROUND(SS_survey_uncond!M4,2)</f>
-        <v>0.97</v>
-      </c>
-    </row>
-    <row r="15" x14ac:dyDescent="0.35">
-      <c r="A15" s="11"/>
-      <c r="B15" s="12" t="str">
+        <v>0.98</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A15" s="10"/>
+      <c r="B15" s="11" t="str">
         <f>CONCATENATE("(",ROUND(SS_survey_uncond!B5,3),")")</f>
-        <v>(0.565)</v>
-      </c>
-      <c r="C15" s="12" t="str">
+        <v>(0.564)</v>
+      </c>
+      <c r="C15" s="11" t="str">
         <f>CONCATENATE("(",ROUND(SS_survey_uncond!C5,3),")")</f>
-        <v>(0.763)</v>
-      </c>
-      <c r="D15" s="12" t="str">
+        <v>(0.771)</v>
+      </c>
+      <c r="D15" s="11" t="str">
         <f>CONCATENATE("(",ROUND(SS_survey_uncond!E5,3),")")</f>
-        <v>(0.607)</v>
-      </c>
-      <c r="E15" s="12"/>
-      <c r="F15" s="12"/>
-      <c r="G15" s="12" t="str">
+        <v>(0.605)</v>
+      </c>
+      <c r="E15" s="11"/>
+      <c r="F15" s="11"/>
+      <c r="G15" s="11" t="str">
         <f>CONCATENATE("(",ROUND(SS_survey_uncond!D5,3),")")</f>
-        <v>(0.647)</v>
-      </c>
-      <c r="H15" s="12" t="str">
+        <v>(0.66)</v>
+      </c>
+      <c r="H15" s="11" t="str">
         <f>CONCATENATE("(",ROUND(SS_survey_uncond!F5,3),")")</f>
-        <v>(0.519)</v>
-      </c>
-      <c r="I15" s="12"/>
-    </row>
-    <row r="16" x14ac:dyDescent="0.35">
-      <c r="A16" s="11" t="s">
+        <v>(0.516)</v>
+      </c>
+      <c r="I15" s="11"/>
+    </row>
+    <row r="16" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A16" s="10" t="s">
         <v>8</v>
       </c>
-      <c r="B16" s="12">
+      <c r="B16" s="11">
         <f>ROUND(SS_survey_uncond!B6,0)</f>
-        <v>3144</v>
-      </c>
-      <c r="C16" s="12">
+        <v>3145</v>
+      </c>
+      <c r="C16" s="11">
         <f>ROUND(SS_survey_uncond!C6,0)</f>
-        <v>2978</v>
-      </c>
-      <c r="D16" s="12">
+        <v>2985</v>
+      </c>
+      <c r="D16" s="11">
         <f>ROUND(SS_survey_uncond!E6,0)</f>
-        <v>3112</v>
-      </c>
-      <c r="E16" s="12">
+        <v>3111</v>
+      </c>
+      <c r="E16" s="11">
         <f>ROUND(SS_survey_uncond!L6,2)</f>
-        <v>0.31</v>
-      </c>
-      <c r="F16" s="12"/>
-      <c r="G16" s="12">
+        <v>0.34</v>
+      </c>
+      <c r="F16" s="11"/>
+      <c r="G16" s="11">
         <f>ROUND(SS_survey_uncond!D6,0)</f>
-        <v>3012</v>
-      </c>
-      <c r="H16" s="12">
+        <v>3010</v>
+      </c>
+      <c r="H16" s="11">
         <f>ROUND(SS_survey_uncond!F6,0)</f>
-        <v>3082</v>
-      </c>
-      <c r="I16" s="12">
+        <v>3083</v>
+      </c>
+      <c r="I16" s="11">
         <f>ROUND(SS_survey_uncond!M6,2)</f>
-        <v>0.43</v>
-      </c>
-    </row>
-    <row r="17" x14ac:dyDescent="0.35">
-      <c r="A17" s="11"/>
-      <c r="B17" s="12" t="str">
+        <v>0.42</v>
+      </c>
+    </row>
+    <row r="17" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A17" s="10"/>
+      <c r="B17" s="11" t="str">
         <f>CONCATENATE("(",ROUND(SS_survey_uncond!B7,0),")")</f>
         <v>(68)</v>
       </c>
-      <c r="C17" s="12" t="str">
+      <c r="C17" s="11" t="str">
         <f>CONCATENATE("(",ROUND(SS_survey_uncond!C7,0),")")</f>
-        <v>(87)</v>
-      </c>
-      <c r="D17" s="12" t="str">
+        <v>(88)</v>
+      </c>
+      <c r="D17" s="11" t="str">
         <f>CONCATENATE("(",ROUND(SS_survey_uncond!E7,0),")")</f>
-        <v>(85)</v>
-      </c>
-      <c r="E17" s="12"/>
-      <c r="F17" s="12"/>
-      <c r="G17" s="12" t="str">
+        <v>(84)</v>
+      </c>
+      <c r="E17" s="11"/>
+      <c r="F17" s="11"/>
+      <c r="G17" s="11" t="str">
         <f>CONCATENATE("(",ROUND(SS_survey_uncond!D7,0),")")</f>
-        <v>(77)</v>
-      </c>
-      <c r="H17" s="12" t="str">
+        <v>(76)</v>
+      </c>
+      <c r="H17" s="11" t="str">
         <f>CONCATENATE("(",ROUND(SS_survey_uncond!F7,0),")")</f>
         <v>(99)</v>
       </c>
-      <c r="I17" s="12"/>
-    </row>
-    <row r="18" x14ac:dyDescent="0.35">
-      <c r="A18" s="11" t="s">
+      <c r="I17" s="11"/>
+    </row>
+    <row r="18" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A18" s="10" t="s">
         <v>9</v>
       </c>
-      <c r="B18" s="12">
+      <c r="B18" s="11">
         <f>ROUND(SS_survey_uncond!B8,2)</f>
         <v>0.89</v>
       </c>
-      <c r="C18" s="12">
+      <c r="C18" s="11">
         <f>ROUND(SS_survey_uncond!C8,2)</f>
         <v>0.9</v>
       </c>
-      <c r="D18" s="12">
+      <c r="D18" s="11">
         <f>ROUND(SS_survey_uncond!E8,2)</f>
         <v>0.91</v>
       </c>
-      <c r="E18" s="12">
+      <c r="E18" s="11">
         <f>ROUND(SS_survey_uncond!L8,2)</f>
-        <v>0.47</v>
-      </c>
-      <c r="F18" s="12"/>
-      <c r="G18" s="12">
+        <v>0.41</v>
+      </c>
+      <c r="F18" s="11"/>
+      <c r="G18" s="11">
         <f>ROUND(SS_survey_uncond!D8,2)</f>
         <v>0.89</v>
       </c>
-      <c r="H18" s="12">
+      <c r="H18" s="11">
         <f>ROUND(SS_survey_uncond!F8,2)</f>
         <v>0.89</v>
       </c>
-      <c r="I18" s="12">
+      <c r="I18" s="11">
         <f>ROUND(SS_survey_uncond!M8,2)</f>
-        <v>0.99</v>
-      </c>
-    </row>
-    <row r="19" x14ac:dyDescent="0.35">
-      <c r="A19" s="11"/>
-      <c r="B19" s="12" t="str">
+        <v>0.97</v>
+      </c>
+    </row>
+    <row r="19" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A19" s="10"/>
+      <c r="B19" s="11" t="str">
         <f>CONCATENATE("(",ROUND(SS_survey_uncond!B9,3),")")</f>
-        <v>(0.011)</v>
-      </c>
-      <c r="C19" s="12" t="str">
+        <v>(0.012)</v>
+      </c>
+      <c r="C19" s="11" t="str">
         <f>CONCATENATE("(",ROUND(SS_survey_uncond!C9,3),")")</f>
         <v>(0.011)</v>
       </c>
-      <c r="D19" s="12" t="str">
+      <c r="D19" s="11" t="str">
         <f>CONCATENATE("(",ROUND(SS_survey_uncond!E9,3),")")</f>
         <v>(0.01)</v>
       </c>
-      <c r="E19" s="12"/>
-      <c r="F19" s="12"/>
-      <c r="G19" s="12" t="str">
+      <c r="E19" s="11"/>
+      <c r="F19" s="11"/>
+      <c r="G19" s="11" t="str">
         <f>CONCATENATE("(",ROUND(SS_survey_uncond!D9,3),")")</f>
-        <v>(0.014)</v>
-      </c>
-      <c r="H19" s="12" t="str">
+        <v>(0.015)</v>
+      </c>
+      <c r="H19" s="11" t="str">
         <f>CONCATENATE("(",ROUND(SS_survey_uncond!F9,3),")")</f>
         <v>(0.009)</v>
       </c>
-      <c r="I19" s="12"/>
-    </row>
-    <row r="20" x14ac:dyDescent="0.35">
-      <c r="A20" s="11" t="s">
+      <c r="I19" s="11"/>
+    </row>
+    <row r="20" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A20" s="10" t="s">
         <v>10</v>
       </c>
-      <c r="B20" s="12">
+      <c r="B20" s="11">
         <f>ROUND(SS_survey_uncond!B10,2)</f>
-        <v>92.75</v>
-      </c>
-      <c r="C20" s="12">
+        <v>92.73</v>
+      </c>
+      <c r="C20" s="11">
         <f>ROUND(SS_survey_uncond!C10,2)</f>
-        <v>92.19</v>
-      </c>
-      <c r="D20" s="12">
+        <v>92.2</v>
+      </c>
+      <c r="D20" s="11">
         <f>ROUND(SS_survey_uncond!E10,2)</f>
-        <v>93.71</v>
-      </c>
-      <c r="E20" s="12">
+        <v>93.72</v>
+      </c>
+      <c r="E20" s="11">
         <f>ROUND(SS_survey_uncond!L10,2)</f>
         <v>0.18</v>
       </c>
-      <c r="F20" s="12"/>
-      <c r="G20" s="12">
+      <c r="F20" s="11"/>
+      <c r="G20" s="11">
         <f>ROUND(SS_survey_uncond!D10,2)</f>
         <v>93.66</v>
       </c>
-      <c r="H20" s="12">
+      <c r="H20" s="11">
         <f>ROUND(SS_survey_uncond!F10,2)</f>
         <v>93.34</v>
       </c>
-      <c r="I20" s="12">
+      <c r="I20" s="11">
         <f>ROUND(SS_survey_uncond!M10,2)</f>
-        <v>0.5</v>
-      </c>
-    </row>
-    <row r="21" x14ac:dyDescent="0.35">
-      <c r="A21" s="11"/>
-      <c r="B21" s="12" t="str">
+        <v>0.49</v>
+      </c>
+    </row>
+    <row r="21" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A21" s="10"/>
+      <c r="B21" s="11" t="str">
         <f>CONCATENATE("(",ROUND(SS_survey_uncond!B11,3),")")</f>
-        <v>(0.537)</v>
-      </c>
-      <c r="C21" s="12" t="str">
+        <v>(0.541)</v>
+      </c>
+      <c r="C21" s="11" t="str">
         <f>CONCATENATE("(",ROUND(SS_survey_uncond!C11,3),")")</f>
-        <v>(0.839)</v>
-      </c>
-      <c r="D21" s="12" t="str">
+        <v>(0.838)</v>
+      </c>
+      <c r="D21" s="11" t="str">
         <f>CONCATENATE("(",ROUND(SS_survey_uncond!E11,3),")")</f>
         <v>(0.455)</v>
       </c>
-      <c r="E21" s="12"/>
-      <c r="F21" s="12"/>
-      <c r="G21" s="12" t="str">
+      <c r="E21" s="11"/>
+      <c r="F21" s="11"/>
+      <c r="G21" s="11" t="str">
         <f>CONCATENATE("(",ROUND(SS_survey_uncond!D11,3),")")</f>
-        <v>(0.591)</v>
-      </c>
-      <c r="H21" s="12" t="str">
+        <v>(0.59)</v>
+      </c>
+      <c r="H21" s="11" t="str">
         <f>CONCATENATE("(",ROUND(SS_survey_uncond!F11,3),")")</f>
-        <v>(0.596)</v>
-      </c>
-      <c r="I21" s="12"/>
-    </row>
-    <row r="22" x14ac:dyDescent="0.35">
-      <c r="A22" s="11" t="s">
+        <v>(0.595)</v>
+      </c>
+      <c r="I21" s="11"/>
+    </row>
+    <row r="22" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A22" s="10" t="s">
         <v>11</v>
       </c>
-      <c r="B22" s="12">
+      <c r="B22" s="11">
         <f>ROUND(SS_survey_uncond!B12,2)</f>
         <v>0.66</v>
       </c>
-      <c r="C22" s="12">
+      <c r="C22" s="11">
         <f>ROUND(SS_survey_uncond!C12,2)</f>
         <v>0.67</v>
       </c>
-      <c r="D22" s="12">
+      <c r="D22" s="11">
         <f>ROUND(SS_survey_uncond!E12,2)</f>
         <v>0.66</v>
       </c>
-      <c r="E22" s="12">
+      <c r="E22" s="11">
         <f>ROUND(SS_survey_uncond!L12,2)</f>
-        <v>0.92</v>
-      </c>
-      <c r="F22" s="12"/>
-      <c r="G22" s="12">
+        <v>0.94</v>
+      </c>
+      <c r="F22" s="11"/>
+      <c r="G22" s="11">
         <f>ROUND(SS_survey_uncond!D12,2)</f>
         <v>0.65</v>
       </c>
-      <c r="H22" s="12">
+      <c r="H22" s="11">
         <f>ROUND(SS_survey_uncond!F12,2)</f>
         <v>0.64</v>
       </c>
-      <c r="I22" s="12">
+      <c r="I22" s="11">
         <f>ROUND(SS_survey_uncond!M12,2)</f>
-        <v>0.83</v>
-      </c>
-    </row>
-    <row r="23" x14ac:dyDescent="0.35">
-      <c r="A23" s="11"/>
-      <c r="B23" s="12" t="str">
+        <v>0.81</v>
+      </c>
+    </row>
+    <row r="23" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A23" s="10"/>
+      <c r="B23" s="11" t="str">
         <f>CONCATENATE("(",ROUND(SS_survey_uncond!B13,3),")")</f>
-        <v>(0.02)</v>
-      </c>
-      <c r="C23" s="12" t="str">
+        <v>(0.019)</v>
+      </c>
+      <c r="C23" s="11" t="str">
         <f>CONCATENATE("(",ROUND(SS_survey_uncond!C13,3),")")</f>
-        <v>(0.02)</v>
-      </c>
-      <c r="D23" s="12" t="str">
+        <v>(0.019)</v>
+      </c>
+      <c r="D23" s="11" t="str">
         <f>CONCATENATE("(",ROUND(SS_survey_uncond!E13,3),")")</f>
         <v>(0.017)</v>
       </c>
-      <c r="E23" s="12"/>
-      <c r="F23" s="12"/>
-      <c r="G23" s="12" t="str">
+      <c r="E23" s="11"/>
+      <c r="F23" s="11"/>
+      <c r="G23" s="11" t="str">
         <f>CONCATENATE("(",ROUND(SS_survey_uncond!D13,3),")")</f>
         <v>(0.024)</v>
       </c>
-      <c r="H23" s="12" t="str">
+      <c r="H23" s="11" t="str">
         <f>CONCATENATE("(",ROUND(SS_survey_uncond!F13,3),")")</f>
         <v>(0.017)</v>
       </c>
-      <c r="I23" s="12"/>
-    </row>
-    <row r="24" x14ac:dyDescent="0.35">
+      <c r="I23" s="11"/>
+    </row>
+    <row r="24" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A24" s="1" t="s">
         <v>5</v>
       </c>
       <c r="B24" s="4">
         <f>SS_survey_uncond!B16</f>
-        <v>2036</v>
+        <v>2035</v>
       </c>
       <c r="C24" s="4">
         <f>SS_survey_uncond!C16</f>
-        <v>1907</v>
+        <v>1908</v>
       </c>
       <c r="D24" s="4">
         <f>SS_survey_uncond!E16</f>
-        <v>2710</v>
+        <v>2711</v>
       </c>
       <c r="E24" s="4"/>
       <c r="F24" s="4"/>
       <c r="G24" s="4">
         <f>SS_survey_uncond!D16</f>
-        <v>1757</v>
+        <v>1756</v>
       </c>
       <c r="H24" s="4">
         <f>SS_survey_uncond!F16</f>
-        <v>2216</v>
+        <v>2218</v>
       </c>
       <c r="I24" s="4"/>
     </row>
-    <row r="25" ht="15" thickBot="true" x14ac:dyDescent="0.4">
+    <row r="25" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A25" s="2"/>
-      <c r="B25" s="10" t="s">
+      <c r="B25" s="17" t="s">
         <v>20</v>
       </c>
-      <c r="C25" s="10"/>
-      <c r="D25" s="10"/>
-      <c r="E25" s="10"/>
-      <c r="F25" s="10"/>
-      <c r="G25" s="10"/>
-      <c r="H25" s="10"/>
-      <c r="I25" s="10"/>
-    </row>
-    <row r="26" ht="15" thickTop="true" x14ac:dyDescent="0.35">
-      <c r="A26" s="11" t="s">
+      <c r="C25" s="17"/>
+      <c r="D25" s="17"/>
+      <c r="E25" s="17"/>
+      <c r="F25" s="17"/>
+      <c r="G25" s="17"/>
+      <c r="H25" s="17"/>
+      <c r="I25" s="17"/>
+    </row>
+    <row r="26" spans="1:9" ht="15" thickTop="1" x14ac:dyDescent="0.35">
+      <c r="A26" s="10" t="s">
         <v>6</v>
       </c>
-      <c r="B26" s="12">
+      <c r="B26" s="11">
         <f>ROUND(SS_survey!B2,2)</f>
         <v>0.76</v>
       </c>
-      <c r="C26" s="12">
+      <c r="C26" s="11">
         <f>ROUND(SS_survey!C2,2)</f>
         <v>0.72</v>
       </c>
-      <c r="D26" s="12">
+      <c r="D26" s="11">
         <f>ROUND(SS_survey!E2,2)</f>
         <v>0.72</v>
       </c>
-      <c r="E26" s="12">
+      <c r="E26" s="11">
         <f>ROUND(SS_survey!J2,2)</f>
-        <v>0.2</v>
-      </c>
-      <c r="F26" s="12"/>
-      <c r="G26" s="12">
+        <v>0.18</v>
+      </c>
+      <c r="F26" s="11"/>
+      <c r="G26" s="11">
         <f>ROUND(SS_survey!D2,2)</f>
-        <v>0.72</v>
-      </c>
-      <c r="H26" s="12">
+        <v>0.73</v>
+      </c>
+      <c r="H26" s="11">
         <f>ROUND(SS_survey!F2,2)</f>
         <v>0.74</v>
       </c>
-      <c r="I26" s="12">
+      <c r="I26" s="11">
         <f>ROUND(SS_survey!K2,2)</f>
-        <v>0.49</v>
-      </c>
-    </row>
-    <row r="27" x14ac:dyDescent="0.35">
-      <c r="A27" s="11"/>
-      <c r="B27" s="12" t="str">
+        <v>0.47</v>
+      </c>
+    </row>
+    <row r="27" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A27" s="10"/>
+      <c r="B27" s="11" t="str">
         <f>CONCATENATE("(",ROUND(SS_survey!B3,3),")")</f>
         <v>(0.016)</v>
       </c>
-      <c r="C27" s="12" t="str">
+      <c r="C27" s="11" t="str">
         <f>CONCATENATE("(",ROUND(SS_survey!C3,3),")")</f>
-        <v>(0.018)</v>
-      </c>
-      <c r="D27" s="12" t="str">
+        <v>(0.016)</v>
+      </c>
+      <c r="D27" s="11" t="str">
         <f>CONCATENATE("(",ROUND(SS_survey!E3,3),")")</f>
         <v>(0.016)</v>
       </c>
-      <c r="E27" s="12"/>
-      <c r="F27" s="12"/>
-      <c r="G27" s="12" t="str">
+      <c r="E27" s="11"/>
+      <c r="F27" s="11"/>
+      <c r="G27" s="11" t="str">
         <f>CONCATENATE("(",ROUND(SS_survey!D3,3),")")</f>
         <v>(0.021)</v>
       </c>
-      <c r="H27" s="12" t="str">
+      <c r="H27" s="11" t="str">
         <f>CONCATENATE("(",ROUND(SS_survey!F3,3),")")</f>
         <v>(0.013)</v>
       </c>
-      <c r="I27" s="12"/>
-    </row>
-    <row r="28" x14ac:dyDescent="0.35">
-      <c r="A28" s="11" t="s">
+      <c r="I27" s="11"/>
+    </row>
+    <row r="28" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A28" s="10" t="s">
         <v>7</v>
       </c>
-      <c r="B28" s="12">
+      <c r="B28" s="11">
         <f>ROUND(SS_survey!B4,2)</f>
-        <v>43.22</v>
-      </c>
-      <c r="C28" s="12" t="str">
+        <v>43.16</v>
+      </c>
+      <c r="C28" s="11" t="str">
         <f>CONCATENATE("(",ROUND(SS_survey!C4,3),")")</f>
-        <v>(43.131)</v>
-      </c>
-      <c r="D28" s="12" t="str">
+        <v>(43.175)</v>
+      </c>
+      <c r="D28" s="11" t="str">
         <f>CONCATENATE("(",ROUND(SS_survey!E4,3),")")</f>
-        <v>(43.906)</v>
-      </c>
-      <c r="E28" s="12">
+        <v>(43.963)</v>
+      </c>
+      <c r="E28" s="11">
         <f>ROUND(SS_survey!J4,2)</f>
-        <v>0.64</v>
-      </c>
-      <c r="F28" s="12"/>
-      <c r="G28" s="12" t="str">
+        <v>0.57999999999999996</v>
+      </c>
+      <c r="F28" s="11"/>
+      <c r="G28" s="11" t="str">
         <f>CONCATENATE("(",ROUND(SS_survey!D4,3),")")</f>
-        <v>(42.956)</v>
-      </c>
-      <c r="H28" s="12" t="str">
+        <v>(42.96)</v>
+      </c>
+      <c r="H28" s="11" t="str">
         <f>CONCATENATE("(",ROUND(SS_survey!F4,3),")")</f>
-        <v>(43.081)</v>
-      </c>
-      <c r="I28" s="12">
+        <v>(43.072)</v>
+      </c>
+      <c r="I28" s="11">
         <f>ROUND(SS_survey!K4,2)</f>
-        <v>0.95</v>
-      </c>
-    </row>
-    <row r="29" x14ac:dyDescent="0.35">
-      <c r="A29" s="11"/>
-      <c r="B29" s="12" t="str">
+        <v>0.97</v>
+      </c>
+    </row>
+    <row r="29" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A29" s="10"/>
+      <c r="B29" s="11" t="str">
         <f>CONCATENATE("(",ROUND(SS_survey!B5,3),")")</f>
-        <v>(0.572)</v>
-      </c>
-      <c r="C29" s="12" t="str">
+        <v>(0.573)</v>
+      </c>
+      <c r="C29" s="11" t="str">
         <f>CONCATENATE("(",ROUND(SS_survey!C5,3),")")</f>
-        <v>(0.778)</v>
-      </c>
-      <c r="D29" s="12" t="str">
+        <v>(0.787)</v>
+      </c>
+      <c r="D29" s="11" t="str">
         <f>CONCATENATE("(",ROUND(SS_survey!E5,3),")")</f>
-        <v>(0.617)</v>
-      </c>
-      <c r="E29" s="12"/>
-      <c r="F29" s="12"/>
-      <c r="G29" s="12" t="str">
+        <v>(0.613)</v>
+      </c>
+      <c r="E29" s="11"/>
+      <c r="F29" s="11"/>
+      <c r="G29" s="11" t="str">
         <f>CONCATENATE("(",ROUND(SS_survey!D5,3),")")</f>
-        <v>(0.638)</v>
-      </c>
-      <c r="H29" s="12" t="str">
+        <v>(0.652)</v>
+      </c>
+      <c r="H29" s="11" t="str">
         <f>CONCATENATE("(",ROUND(SS_survey!F5,3),")")</f>
-        <v>(0.519)</v>
-      </c>
-      <c r="I29" s="12"/>
-    </row>
-    <row r="30" x14ac:dyDescent="0.35">
-      <c r="A30" s="11" t="s">
+        <v>(0.518)</v>
+      </c>
+      <c r="I29" s="11"/>
+    </row>
+    <row r="30" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A30" s="10" t="s">
         <v>8</v>
       </c>
-      <c r="B30" s="12">
+      <c r="B30" s="11">
         <f>ROUND(SS_survey!B6,0)</f>
-        <v>3141</v>
-      </c>
-      <c r="C30" s="12">
+        <v>3152</v>
+      </c>
+      <c r="C30" s="11">
         <f>ROUND(SS_survey!C6,0)</f>
-        <v>2969</v>
-      </c>
-      <c r="D30" s="12">
+        <v>2978</v>
+      </c>
+      <c r="D30" s="11">
         <f>ROUND(SS_survey!E6,0)</f>
-        <v>3107</v>
-      </c>
-      <c r="E30" s="12">
+        <v>3115</v>
+      </c>
+      <c r="E30" s="11">
         <f>ROUND(SS_survey!J6,2)</f>
-        <v>0.28999999999999998</v>
-      </c>
-      <c r="F30" s="12"/>
-      <c r="G30" s="12">
+        <v>0.3</v>
+      </c>
+      <c r="F30" s="11"/>
+      <c r="G30" s="11">
         <f>ROUND(SS_survey!D6,0)</f>
-        <v>2982</v>
-      </c>
-      <c r="H30" s="12">
+        <v>2988</v>
+      </c>
+      <c r="H30" s="11">
         <f>ROUND(SS_survey!F6,0)</f>
-        <v>3078</v>
-      </c>
-      <c r="I30" s="12">
+        <v>3081</v>
+      </c>
+      <c r="I30" s="11">
         <f>ROUND(SS_survey!K6,2)</f>
-        <v>0.3</v>
-      </c>
-    </row>
-    <row r="31" x14ac:dyDescent="0.35">
-      <c r="A31" s="11"/>
-      <c r="B31" s="12" t="str">
+        <v>0.27</v>
+      </c>
+    </row>
+    <row r="31" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A31" s="10"/>
+      <c r="B31" s="11" t="str">
         <f>CONCATENATE("(",ROUND(SS_survey!B7,0),")")</f>
-        <v>(68)</v>
-      </c>
-      <c r="C31" s="12" t="str">
+        <v>(69)</v>
+      </c>
+      <c r="C31" s="11" t="str">
         <f>CONCATENATE("(",ROUND(SS_survey!C7,0),")")</f>
-        <v>(88)</v>
-      </c>
-      <c r="D31" s="12" t="str">
+        <v>(91)</v>
+      </c>
+      <c r="D31" s="11" t="str">
         <f>CONCATENATE("(",ROUND(SS_survey!E7,0),")")</f>
         <v>(85)</v>
       </c>
-      <c r="E31" s="12"/>
-      <c r="F31" s="12"/>
-      <c r="G31" s="12" t="str">
+      <c r="E31" s="11"/>
+      <c r="F31" s="11"/>
+      <c r="G31" s="11" t="str">
         <f>CONCATENATE("(",ROUND(SS_survey!D7,0),")")</f>
-        <v>(77)</v>
-      </c>
-      <c r="H31" s="12" t="str">
+        <v>(76)</v>
+      </c>
+      <c r="H31" s="11" t="str">
         <f>CONCATENATE("(",ROUND(SS_survey!F7,0),")")</f>
         <v>(99)</v>
       </c>
-      <c r="I31" s="12"/>
-    </row>
-    <row r="32" x14ac:dyDescent="0.35">
-      <c r="A32" s="11" t="s">
+      <c r="I31" s="11"/>
+    </row>
+    <row r="32" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A32" s="10" t="s">
         <v>9</v>
       </c>
-      <c r="B32" s="12">
+      <c r="B32" s="11">
         <f>ROUND(SS_survey!B8,2)</f>
         <v>0.89</v>
       </c>
-      <c r="C32" s="12">
+      <c r="C32" s="11">
         <f>ROUND(SS_survey!C8,2)</f>
         <v>0.9</v>
       </c>
-      <c r="D32" s="12">
+      <c r="D32" s="11">
         <f>ROUND(SS_survey!E8,2)</f>
         <v>0.91</v>
       </c>
-      <c r="E32" s="12">
+      <c r="E32" s="11">
         <f>ROUND(SS_survey!J8,2)</f>
-        <v>0.48</v>
-      </c>
-      <c r="F32" s="12"/>
-      <c r="G32" s="12">
+        <v>0.42</v>
+      </c>
+      <c r="F32" s="11"/>
+      <c r="G32" s="11">
         <f>ROUND(SS_survey!D8,2)</f>
         <v>0.89</v>
       </c>
-      <c r="H32" s="12">
+      <c r="H32" s="11">
         <f>ROUND(SS_survey!F8,2)</f>
         <v>0.89</v>
       </c>
-      <c r="I32" s="12">
+      <c r="I32" s="11">
         <f>ROUND(SS_survey!K8,2)</f>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="33" x14ac:dyDescent="0.35">
-      <c r="A33" s="11"/>
-      <c r="B33" s="12" t="str">
+        <v>0.98</v>
+      </c>
+    </row>
+    <row r="33" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A33" s="10"/>
+      <c r="B33" s="11" t="str">
         <f>CONCATENATE("(",ROUND(SS_survey!B9,3),")")</f>
         <v>(0.012)</v>
       </c>
-      <c r="C33" s="12" t="str">
+      <c r="C33" s="11" t="str">
         <f>CONCATENATE("(",ROUND(SS_survey!C9,3),")")</f>
         <v>(0.011)</v>
       </c>
-      <c r="D33" s="12" t="str">
+      <c r="D33" s="11" t="str">
         <f>CONCATENATE("(",ROUND(SS_survey!E9,3),")")</f>
         <v>(0.01)</v>
       </c>
-      <c r="E33" s="12"/>
-      <c r="F33" s="12"/>
-      <c r="G33" s="12" t="str">
+      <c r="E33" s="11"/>
+      <c r="F33" s="11"/>
+      <c r="G33" s="11" t="str">
         <f>CONCATENATE("(",ROUND(SS_survey!D9,3),")")</f>
         <v>(0.014)</v>
       </c>
-      <c r="H33" s="12" t="str">
+      <c r="H33" s="11" t="str">
         <f>CONCATENATE("(",ROUND(SS_survey!F9,3),")")</f>
-        <v>(0.009)</v>
-      </c>
-      <c r="I33" s="12"/>
-    </row>
-    <row r="34" x14ac:dyDescent="0.35">
-      <c r="A34" s="11" t="s">
+        <v>(0.01)</v>
+      </c>
+      <c r="I33" s="11"/>
+    </row>
+    <row r="34" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A34" s="10" t="s">
         <v>10</v>
       </c>
-      <c r="B34" s="12">
+      <c r="B34" s="11">
         <f>ROUND(SS_survey!B10,2)</f>
         <v>92.74</v>
       </c>
-      <c r="C34" s="12">
+      <c r="C34" s="11">
         <f>ROUND(SS_survey!C10,2)</f>
-        <v>92.14</v>
-      </c>
-      <c r="D34" s="12">
+        <v>92.16</v>
+      </c>
+      <c r="D34" s="11">
         <f>ROUND(SS_survey!E10,2)</f>
-        <v>93.66</v>
-      </c>
-      <c r="E34" s="12">
+        <v>93.67</v>
+      </c>
+      <c r="E34" s="11">
         <f>ROUND(SS_survey!J10,2)</f>
         <v>0.21</v>
       </c>
-      <c r="F34" s="12"/>
-      <c r="G34" s="12">
+      <c r="F34" s="11"/>
+      <c r="G34" s="11">
         <f>ROUND(SS_survey!D10,2)</f>
-        <v>93.57</v>
-      </c>
-      <c r="H34" s="12">
+        <v>93.6</v>
+      </c>
+      <c r="H34" s="11">
         <f>ROUND(SS_survey!F10,2)</f>
         <v>93.29</v>
       </c>
-      <c r="I34" s="12">
+      <c r="I34" s="11">
         <f>ROUND(SS_survey!K10,2)</f>
-        <v>0.56999999999999995</v>
-      </c>
-    </row>
-    <row r="35" x14ac:dyDescent="0.35">
-      <c r="A35" s="11"/>
-      <c r="B35" s="12" t="str">
+        <v>0.55000000000000004</v>
+      </c>
+    </row>
+    <row r="35" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A35" s="10"/>
+      <c r="B35" s="11" t="str">
         <f>CONCATENATE("(",ROUND(SS_survey!B11,3),")")</f>
-        <v>(0.554)</v>
-      </c>
-      <c r="C35" s="12" t="str">
+        <v>(0.553)</v>
+      </c>
+      <c r="C35" s="11" t="str">
         <f>CONCATENATE("(",ROUND(SS_survey!C11,3),")")</f>
         <v>(0.857)</v>
       </c>
-      <c r="D35" s="12" t="str">
+      <c r="D35" s="11" t="str">
         <f>CONCATENATE("(",ROUND(SS_survey!E11,3),")")</f>
-        <v>(0.473)</v>
-      </c>
-      <c r="E35" s="12"/>
-      <c r="F35" s="12"/>
-      <c r="G35" s="12" t="str">
+        <v>(0.471)</v>
+      </c>
+      <c r="E35" s="11"/>
+      <c r="F35" s="11"/>
+      <c r="G35" s="11" t="str">
         <f>CONCATENATE("(",ROUND(SS_survey!D11,3),")")</f>
         <v>(0.596)</v>
       </c>
-      <c r="H35" s="12" t="str">
+      <c r="H35" s="11" t="str">
         <f>CONCATENATE("(",ROUND(SS_survey!F11,3),")")</f>
-        <v>(0.601)</v>
-      </c>
-      <c r="I35" s="12"/>
-    </row>
-    <row r="36" x14ac:dyDescent="0.35">
-      <c r="A36" s="11" t="s">
+        <v>(0.599)</v>
+      </c>
+      <c r="I35" s="11"/>
+    </row>
+    <row r="36" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A36" s="10" t="s">
         <v>11</v>
       </c>
-      <c r="B36" s="12">
+      <c r="B36" s="11">
         <f>ROUND(SS_survey!B12,2)</f>
         <v>0.66</v>
       </c>
-      <c r="C36" s="12">
+      <c r="C36" s="11">
         <f>ROUND(SS_survey!C12,2)</f>
         <v>0.67</v>
       </c>
-      <c r="D36" s="12">
+      <c r="D36" s="11">
         <f>ROUND(SS_survey!E12,2)</f>
-        <v>0.66</v>
-      </c>
-      <c r="E36" s="12">
+        <v>0.67</v>
+      </c>
+      <c r="E36" s="11">
         <f>ROUND(SS_survey!J12,2)</f>
-        <v>0.85</v>
-      </c>
-      <c r="F36" s="12"/>
-      <c r="G36" s="12">
+        <v>0.91</v>
+      </c>
+      <c r="F36" s="11"/>
+      <c r="G36" s="11">
         <f>ROUND(SS_survey!D12,2)</f>
         <v>0.65</v>
       </c>
-      <c r="H36" s="12">
+      <c r="H36" s="11">
         <f>ROUND(SS_survey!F12,2)</f>
         <v>0.64</v>
       </c>
-      <c r="I36" s="12">
+      <c r="I36" s="11">
         <f>ROUND(SS_survey!K12,2)</f>
-        <v>0.8</v>
-      </c>
-    </row>
-    <row r="37" x14ac:dyDescent="0.35">
-      <c r="A37" s="11"/>
-      <c r="B37" s="12" t="str">
+        <v>0.75</v>
+      </c>
+    </row>
+    <row r="37" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A37" s="10"/>
+      <c r="B37" s="11" t="str">
         <f>CONCATENATE("(",ROUND(SS_survey!B13,3),")")</f>
-        <v>(0.02)</v>
-      </c>
-      <c r="C37" s="12" t="str">
+        <v>(0.019)</v>
+      </c>
+      <c r="C37" s="11" t="str">
         <f>CONCATENATE("(",ROUND(SS_survey!C13,3),")")</f>
-        <v>(0.02)</v>
-      </c>
-      <c r="D37" s="12" t="str">
+        <v>(0.019)</v>
+      </c>
+      <c r="D37" s="11" t="str">
         <f>CONCATENATE("(",ROUND(SS_survey!E13,3),")")</f>
-        <v>(0.017)</v>
-      </c>
-      <c r="E37" s="12"/>
-      <c r="F37" s="12"/>
-      <c r="G37" s="12" t="str">
+        <v>(0.016)</v>
+      </c>
+      <c r="E37" s="11"/>
+      <c r="F37" s="11"/>
+      <c r="G37" s="11" t="str">
         <f>CONCATENATE("(",ROUND(SS_survey!D13,3),")")</f>
         <v>(0.024)</v>
       </c>
-      <c r="H37" s="12" t="str">
+      <c r="H37" s="11" t="str">
         <f>CONCATENATE("(",ROUND(SS_survey!F13,3),")")</f>
         <v>(0.016)</v>
       </c>
-      <c r="I37" s="12"/>
-    </row>
-    <row r="38" ht="15" thickBot="true" x14ac:dyDescent="0.4">
+      <c r="I37" s="11"/>
+    </row>
+    <row r="38" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A38" s="2" t="s">
         <v>5</v>
       </c>
       <c r="B38" s="9">
         <f>SS_survey!B16</f>
-        <v>1984</v>
+        <v>2000</v>
       </c>
       <c r="C38" s="9">
         <f>SS_survey!C16</f>
-        <v>1840</v>
+        <v>1855</v>
       </c>
       <c r="D38" s="9">
         <f>SS_survey!E16</f>
-        <v>2634</v>
+        <v>2652</v>
       </c>
       <c r="E38" s="9"/>
       <c r="F38" s="9"/>
       <c r="G38" s="9">
         <f>SS_survey!D16</f>
-        <v>1724</v>
+        <v>1733</v>
       </c>
       <c r="H38" s="9">
         <f>SS_survey!F16</f>
-        <v>2185</v>
+        <v>2193</v>
       </c>
       <c r="I38" s="9"/>
     </row>
-    <row r="39" ht="15" thickTop="true" x14ac:dyDescent="0.35"/>
+    <row r="39" spans="1:9" ht="15" thickTop="1" x14ac:dyDescent="0.35"/>
   </sheetData>
   <mergeCells count="6">
     <mergeCell ref="B2:I2"/>
@@ -2697,75 +2697,75 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="26.26953125" bestFit="true" customWidth="true"/>
-    <col min="2" max="2" width="7.1796875" style="3" bestFit="true" customWidth="true"/>
-    <col min="3" max="3" width="10.1796875" style="3" bestFit="true" customWidth="true"/>
-    <col min="4" max="4" width="6.54296875" style="3" bestFit="true" customWidth="true"/>
-    <col min="5" max="5" width="6.54296875" style="3" customWidth="true"/>
-    <col min="6" max="6" width="1.7265625" style="3" customWidth="true"/>
-    <col min="7" max="7" width="7" style="3" bestFit="true" customWidth="true"/>
-    <col min="8" max="8" width="7.453125" style="3" bestFit="true" customWidth="true"/>
-    <col min="9" max="9" width="7.7265625" style="3" bestFit="true" customWidth="true"/>
+    <col min="1" max="1" width="26.26953125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="7.1796875" style="3" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10.1796875" style="3" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="6.54296875" style="3" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="6.54296875" style="3" customWidth="1"/>
+    <col min="6" max="6" width="1.7265625" style="3" customWidth="1"/>
+    <col min="7" max="7" width="7" style="3" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="7.453125" style="3" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="7.7265625" style="3" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="11"/>
-      <c r="B1" s="12"/>
-      <c r="C1" s="12"/>
-      <c r="D1" s="12"/>
-      <c r="E1" s="12"/>
-      <c r="F1" s="12"/>
-      <c r="G1" s="12"/>
-      <c r="H1" s="12"/>
-      <c r="I1" s="12"/>
-      <c r="J1" s="11"/>
-      <c r="K1" s="11"/>
-    </row>
-    <row r="2" x14ac:dyDescent="0.35">
-      <c r="A2" s="11"/>
-      <c r="B2" s="12"/>
-      <c r="C2" s="12"/>
-      <c r="D2" s="12"/>
-      <c r="E2" s="12"/>
-      <c r="F2" s="12"/>
-      <c r="G2" s="12"/>
-      <c r="H2" s="12"/>
-      <c r="I2" s="12"/>
-      <c r="J2" s="11"/>
-      <c r="K2" s="11"/>
-    </row>
-    <row r="3" ht="15" thickBot="true" x14ac:dyDescent="0.4">
-      <c r="A3" s="17"/>
-      <c r="B3" s="18"/>
-      <c r="C3" s="18"/>
-      <c r="D3" s="18"/>
-      <c r="E3" s="18"/>
-      <c r="F3" s="18"/>
-      <c r="G3" s="18"/>
-      <c r="H3" s="18"/>
-      <c r="I3" s="18"/>
-      <c r="J3" s="11"/>
-      <c r="K3" s="11"/>
-    </row>
-    <row r="4" x14ac:dyDescent="0.35">
-      <c r="A4" s="11"/>
-      <c r="B4" s="12"/>
-      <c r="C4" s="15" t="s">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A1" s="10"/>
+      <c r="B1" s="11"/>
+      <c r="C1" s="11"/>
+      <c r="D1" s="11"/>
+      <c r="E1" s="11"/>
+      <c r="F1" s="11"/>
+      <c r="G1" s="11"/>
+      <c r="H1" s="11"/>
+      <c r="I1" s="11"/>
+      <c r="J1" s="10"/>
+      <c r="K1" s="10"/>
+    </row>
+    <row r="2" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A2" s="10"/>
+      <c r="B2" s="11"/>
+      <c r="C2" s="11"/>
+      <c r="D2" s="11"/>
+      <c r="E2" s="11"/>
+      <c r="F2" s="11"/>
+      <c r="G2" s="11"/>
+      <c r="H2" s="11"/>
+      <c r="I2" s="11"/>
+      <c r="J2" s="10"/>
+      <c r="K2" s="10"/>
+    </row>
+    <row r="3" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A3" s="15"/>
+      <c r="B3" s="16"/>
+      <c r="C3" s="16"/>
+      <c r="D3" s="16"/>
+      <c r="E3" s="16"/>
+      <c r="F3" s="16"/>
+      <c r="G3" s="16"/>
+      <c r="H3" s="16"/>
+      <c r="I3" s="16"/>
+      <c r="J3" s="10"/>
+      <c r="K3" s="10"/>
+    </row>
+    <row r="4" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A4" s="10"/>
+      <c r="B4" s="11"/>
+      <c r="C4" s="18" t="s">
         <v>19</v>
       </c>
-      <c r="D4" s="15"/>
-      <c r="E4" s="15"/>
-      <c r="F4" s="12"/>
-      <c r="G4" s="15" t="s">
+      <c r="D4" s="18"/>
+      <c r="E4" s="18"/>
+      <c r="F4" s="11"/>
+      <c r="G4" s="18" t="s">
         <v>18</v>
       </c>
-      <c r="H4" s="15"/>
-      <c r="I4" s="15"/>
-      <c r="J4" s="11"/>
-      <c r="K4" s="11"/>
-    </row>
-    <row r="5" ht="16.5" customHeight="true" thickBot="true" x14ac:dyDescent="0.4">
-      <c r="A5" s="16"/>
+      <c r="H4" s="18"/>
+      <c r="I4" s="18"/>
+      <c r="J4" s="10"/>
+      <c r="K4" s="10"/>
+    </row>
+    <row r="5" spans="1:11" ht="16.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A5" s="14"/>
       <c r="B5" s="7" t="s">
         <v>1</v>
       </c>
@@ -2788,74 +2788,74 @@
       <c r="I5" s="7" t="s">
         <v>2</v>
       </c>
-      <c r="J5" s="11"/>
-      <c r="K5" s="11"/>
-    </row>
-    <row r="6" ht="15" thickTop="true" x14ac:dyDescent="0.35">
-      <c r="A6" s="11" t="s">
+      <c r="J5" s="10"/>
+      <c r="K5" s="10"/>
+    </row>
+    <row r="6" spans="1:11" ht="15" thickTop="1" x14ac:dyDescent="0.35">
+      <c r="A6" s="10" t="s">
         <v>15</v>
       </c>
-      <c r="B6" s="12">
+      <c r="B6" s="11">
         <f>ROUND(SS_att!B2,0)</f>
         <v>31</v>
       </c>
-      <c r="C6" s="12">
+      <c r="C6" s="11">
         <f>ROUND(SS_att!C2,0)</f>
         <v>31</v>
       </c>
-      <c r="D6" s="12">
+      <c r="D6" s="11">
         <f>ROUND(SS_att!E2,0)</f>
         <v>37</v>
       </c>
-      <c r="E6" s="12">
+      <c r="E6" s="11">
         <f>ROUND(SS_att!L2,2)</f>
         <v>0.16</v>
       </c>
-      <c r="F6" s="12"/>
-      <c r="G6" s="12">
+      <c r="F6" s="11"/>
+      <c r="G6" s="11">
         <f>ROUND(SS_att!D2,0)</f>
         <v>32</v>
       </c>
-      <c r="H6" s="12">
+      <c r="H6" s="11">
         <f>ROUND(SS_att!F2,0)</f>
         <v>34</v>
       </c>
-      <c r="I6" s="12">
+      <c r="I6" s="11">
         <f>ROUND(SS_att!M2,2)</f>
         <v>0.56999999999999995</v>
       </c>
-      <c r="J6" s="11"/>
-      <c r="K6" s="11"/>
-    </row>
-    <row r="7" x14ac:dyDescent="0.35">
-      <c r="A7" s="11"/>
-      <c r="B7" s="12" t="str">
+      <c r="J6" s="10"/>
+      <c r="K6" s="10"/>
+    </row>
+    <row r="7" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A7" s="10"/>
+      <c r="B7" s="11" t="str">
         <f>CONCATENATE("(",ROUND(SS_att!B3,1),")")</f>
         <v>(2.2)</v>
       </c>
-      <c r="C7" s="12" t="str">
+      <c r="C7" s="11" t="str">
         <f>CONCATENATE("(",ROUND(SS_att!C3,1),")")</f>
         <v>(2.3)</v>
       </c>
-      <c r="D7" s="12" t="str">
+      <c r="D7" s="11" t="str">
         <f>CONCATENATE("(",ROUND(SS_att!E3,1),")")</f>
         <v>(2.6)</v>
       </c>
-      <c r="E7" s="12"/>
-      <c r="F7" s="12"/>
-      <c r="G7" s="12" t="str">
+      <c r="E7" s="11"/>
+      <c r="F7" s="11"/>
+      <c r="G7" s="11" t="str">
         <f>CONCATENATE("(",ROUND(SS_att!D3,1),")")</f>
         <v>(2.4)</v>
       </c>
-      <c r="H7" s="12" t="str">
+      <c r="H7" s="11" t="str">
         <f>CONCATENATE("(",ROUND(SS_att!F3,1),")")</f>
-        <v>(1.7)</v>
-      </c>
-      <c r="I7" s="12"/>
-      <c r="J7" s="11"/>
-      <c r="K7" s="11"/>
-    </row>
-    <row r="8" x14ac:dyDescent="0.35">
+        <v>(1.8)</v>
+      </c>
+      <c r="I7" s="11"/>
+      <c r="J7" s="10"/>
+      <c r="K7" s="10"/>
+    </row>
+    <row r="8" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
         <v>16</v>
       </c>
@@ -2873,7 +2873,7 @@
       </c>
       <c r="E8" s="3">
         <f>ROUND(SS_att!L10,2)</f>
-        <v>0.73</v>
+        <v>0.74</v>
       </c>
       <c r="G8" s="3">
         <f>ROUND(SS_att!D10,2)</f>
@@ -2885,10 +2885,10 @@
       </c>
       <c r="I8" s="3">
         <f>ROUND(SS_att!M10,2)</f>
-        <v>0.44</v>
-      </c>
-    </row>
-    <row r="9" x14ac:dyDescent="0.35">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="9" spans="1:11" x14ac:dyDescent="0.35">
       <c r="B9" s="3" t="str">
         <f>CONCATENATE("(",ROUND(SS_att!B11,2),")")</f>
         <v>(0.02)</v>
@@ -2910,29 +2910,29 @@
         <v>(0.02)</v>
       </c>
     </row>
-    <row r="10" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
         <v>14</v>
       </c>
       <c r="B10" s="3">
         <f>ROUND(SS_att!B8,2)</f>
-        <v>0.97</v>
+        <v>0.98</v>
       </c>
       <c r="C10" s="3">
         <f>ROUND(SS_att!C8,2)</f>
-        <v>0.96</v>
+        <v>0.97</v>
       </c>
       <c r="D10" s="3">
         <f>ROUND(SS_att!E8,2)</f>
-        <v>0.97</v>
+        <v>0.98</v>
       </c>
       <c r="E10" s="3">
         <f>ROUND(SS_att!L8,2)</f>
-        <v>0.59</v>
+        <v>0.43</v>
       </c>
       <c r="G10" s="3">
         <f>ROUND(SS_att!D8,2)</f>
-        <v>0.98</v>
+        <v>0.99</v>
       </c>
       <c r="H10" s="3">
         <f>ROUND(SS_att!F8,2)</f>
@@ -2940,17 +2940,17 @@
       </c>
       <c r="I10" s="3">
         <f>ROUND(SS_att!M8,2)</f>
-        <v>0.11</v>
-      </c>
-    </row>
-    <row r="11" x14ac:dyDescent="0.35">
+        <v>0.49</v>
+      </c>
+    </row>
+    <row r="11" spans="1:11" x14ac:dyDescent="0.35">
       <c r="B11" s="3" t="str">
         <f>CONCATENATE("(",ROUND(SS_att!B9,3),")")</f>
         <v>(0.004)</v>
       </c>
       <c r="C11" s="3" t="str">
         <f>CONCATENATE("(",ROUND(SS_att!C9,3),")")</f>
-        <v>(0.008)</v>
+        <v>(0.007)</v>
       </c>
       <c r="D11" s="3" t="str">
         <f>CONCATENATE("(",ROUND(SS_att!E9,3),")")</f>
@@ -2958,42 +2958,42 @@
       </c>
       <c r="G11" s="3" t="str">
         <f>CONCATENATE("(",ROUND(SS_att!D9,3),")")</f>
-        <v>(0.004)</v>
+        <v>(0.003)</v>
       </c>
       <c r="H11" s="3" t="str">
         <f>CONCATENATE("(",ROUND(SS_att!F9,3),")")</f>
         <v>(0.003)</v>
       </c>
     </row>
-    <row r="12" ht="15" thickBot="true" x14ac:dyDescent="0.4">
+    <row r="12" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A12" s="2" t="s">
         <v>5</v>
       </c>
       <c r="B12" s="5">
         <f>SS_att!B6</f>
-        <v>2585</v>
+        <v>2600</v>
       </c>
       <c r="C12" s="5">
         <f>SS_att!C6</f>
-        <v>2465</v>
+        <v>2484</v>
       </c>
       <c r="D12" s="5">
         <f>SS_att!E6</f>
-        <v>3406</v>
+        <v>3435</v>
       </c>
       <c r="E12" s="8"/>
       <c r="F12" s="9"/>
       <c r="G12" s="5">
         <f>SS_att!D6</f>
-        <v>2143</v>
+        <v>2157</v>
       </c>
       <c r="H12" s="5">
         <f>SS_att!F6</f>
-        <v>2753</v>
+        <v>2768</v>
       </c>
       <c r="I12" s="5"/>
     </row>
-    <row r="13" ht="15" thickTop="true" x14ac:dyDescent="0.35"/>
+    <row r="13" spans="1:11" ht="15" thickTop="1" x14ac:dyDescent="0.35"/>
   </sheetData>
   <mergeCells count="3">
     <mergeCell ref="B3:I3"/>

</xml_diff>

<commit_message>
update of results using corrected deinition of apr
</commit_message>
<xml_diff>
--- a/Tables/SS.xlsx
+++ b/Tables/SS.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24827"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25629"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\isaac\Dropbox\Apps\ShareLaTeX\Donde2020\Tables\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\isaac\Dropbox\Apps\Overleaf\Donde2020\Tables\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5137F4EA-E541-4770-B5C6-9B9358049491}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B3EAE4A7-3AD2-4386-A93E-B2B14DF81CFF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-10695" windowWidth="29040" windowHeight="15720" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-19215" yWindow="-13410" windowWidth="19185" windowHeight="11265" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="SS_admin" sheetId="1" r:id="rId1"/>
@@ -30,6 +30,7 @@
         <xcalcf:feature name="microsoft.com:CNMTM"/>
         <xcalcf:feature name="microsoft.com:LET_WF"/>
         <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -37,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="20">
   <si>
     <t>Choice</t>
   </si>
@@ -81,9 +82,6 @@
     <t xml:space="preserve">Choice </t>
   </si>
   <si>
-    <t>% ended up pawning</t>
-  </si>
-  <si>
     <t>Number of branch-day pawns</t>
   </si>
   <si>
@@ -99,10 +97,7 @@
     <t>Commitment arms</t>
   </si>
   <si>
-    <t>Panel C : Survey Data (conditional on pawning)</t>
-  </si>
-  <si>
-    <t>Panel B : Survey Data (unconditional)</t>
+    <t>Panel B : Survey Data</t>
   </si>
 </sst>
 </file>
@@ -184,7 +179,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="19">
+  <cellXfs count="20">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
@@ -223,6 +218,9 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -556,135 +554,135 @@
   <sheetData>
     <row r="2" spans="2:13" x14ac:dyDescent="0.35">
       <c r="B2">
-        <v>2279.9653846153847</v>
+        <v>2267.4576271186438</v>
       </c>
       <c r="C2">
-        <v>2147.1437198067633</v>
+        <v>2162.484646878198</v>
       </c>
       <c r="D2">
-        <v>2132.9021789522485</v>
+        <v>2258.353741496599</v>
       </c>
       <c r="E2">
-        <v>2164.8011644832604</v>
+        <v>2222.993023255814</v>
       </c>
       <c r="F2">
-        <v>2089.2792630057802</v>
+        <v>2099.3119747899159</v>
       </c>
       <c r="G2">
-        <v>2057.1111111111113</v>
+        <v>2247.7777777777778</v>
       </c>
       <c r="H2">
-        <v>2161.7426600117442</v>
+        <v>2200.8203489551629</v>
       </c>
       <c r="K2">
-        <v>0.46124979356012857</v>
+        <v>0.76620124290554692</v>
       </c>
       <c r="L2">
-        <v>0.37612637612186028</v>
+        <v>0.64447263875811633</v>
       </c>
       <c r="M2">
-        <v>0.14718551370824021</v>
+        <v>0.17277180983385451</v>
       </c>
     </row>
     <row r="3" spans="2:13" x14ac:dyDescent="0.35">
       <c r="B3">
-        <v>76.146605585818605</v>
+        <v>75.874088260545236</v>
       </c>
       <c r="C3">
-        <v>71.911953944693479</v>
+        <v>83.127592776594469</v>
       </c>
       <c r="D3">
-        <v>73.985411575168982</v>
+        <v>90.589984100427486</v>
       </c>
       <c r="E3">
-        <v>57.575004627999661</v>
+        <v>65.750426103453577</v>
       </c>
       <c r="F3">
-        <v>64.541278696715779</v>
+        <v>66.084751832379908</v>
       </c>
       <c r="G3">
-        <v>140.8140183528381</v>
+        <v>157.45014986681429</v>
       </c>
       <c r="H3">
-        <v>30.154263574554555</v>
+        <v>33.462527085377637</v>
       </c>
     </row>
     <row r="4" spans="2:13" x14ac:dyDescent="0.35">
       <c r="B4">
-        <v>0.87807692307692309</v>
+        <v>0.87966101694915255</v>
       </c>
       <c r="C4">
-        <v>0.89130434782608692</v>
+        <v>0.89406345957011257</v>
       </c>
       <c r="D4">
-        <v>0.88317107093184977</v>
+        <v>0.89863945578231297</v>
       </c>
       <c r="E4">
-        <v>0.84657933042212519</v>
+        <v>0.83100775193798448</v>
       </c>
       <c r="F4">
-        <v>0.82947976878612717</v>
+        <v>0.81355042016806722</v>
       </c>
       <c r="G4">
         <v>0.83333331677648759</v>
       </c>
       <c r="H4">
-        <v>0.86288901915882033</v>
+        <v>0.8589977680076859</v>
       </c>
       <c r="K4">
-        <v>0.52376627821867361</v>
+        <v>0.58496630583942488</v>
       </c>
       <c r="L4">
-        <v>0.70502590236959217</v>
+        <v>0.55956661802877306</v>
       </c>
       <c r="M4">
-        <v>0.64444779531836671</v>
+        <v>0.42690043197119448</v>
       </c>
     </row>
     <row r="5" spans="2:13" x14ac:dyDescent="0.35">
       <c r="B5">
-        <v>3.9975841310504141E-2</v>
+        <v>4.3632089264598002E-2</v>
       </c>
       <c r="C5">
-        <v>3.3776765366283587E-2</v>
+        <v>3.487149126010651E-2</v>
       </c>
       <c r="D5">
-        <v>3.6353445955306977E-2</v>
+        <v>3.3294156485300951E-2</v>
       </c>
       <c r="E5">
-        <v>4.2147068344393836E-2</v>
+        <v>4.7901996328697877E-2</v>
       </c>
       <c r="F5">
-        <v>4.836901048168215E-2</v>
+        <v>5.6448359867079613E-2</v>
       </c>
       <c r="G5">
-        <v>4.3154986380046355E-2</v>
+        <v>4.3154986380046348E-2</v>
       </c>
       <c r="H5">
-        <v>1.8446251080789934E-2</v>
+        <v>2.0450829661416529E-2</v>
       </c>
     </row>
     <row r="6" spans="2:13" x14ac:dyDescent="0.35">
       <c r="B6">
-        <v>2600</v>
+        <v>1770</v>
       </c>
       <c r="C6">
-        <v>2484</v>
+        <v>1954</v>
       </c>
       <c r="D6">
-        <v>2157</v>
+        <v>1470</v>
       </c>
       <c r="E6">
-        <v>3435</v>
+        <v>2580</v>
       </c>
       <c r="F6">
-        <v>2768</v>
+        <v>1904</v>
       </c>
       <c r="G6">
         <v>180</v>
       </c>
       <c r="H6">
-        <v>13624</v>
+        <v>9858</v>
       </c>
     </row>
   </sheetData>
@@ -704,57 +702,57 @@
   <sheetData>
     <row r="2" spans="2:13" x14ac:dyDescent="0.35">
       <c r="B2">
-        <v>30.892857142857142</v>
+        <v>30.98245614035088</v>
       </c>
       <c r="C2">
-        <v>31</v>
+        <v>32.757575757575758</v>
       </c>
       <c r="D2">
-        <v>31.691176470588236</v>
+        <v>33.375</v>
       </c>
       <c r="E2">
-        <v>36.892473118279568</v>
+        <v>39.591549295774648</v>
       </c>
       <c r="F2">
-        <v>33.731707317073173</v>
+        <v>33.719298245614027</v>
       </c>
       <c r="G2">
-        <v>36.021871704525417</v>
+        <v>36.085999441146853</v>
       </c>
       <c r="H2">
-        <v>33.919824372767593</v>
+        <v>34.986388098969591</v>
       </c>
       <c r="K2">
-        <v>0.72947061051374762</v>
+        <v>0.85840438797708241</v>
       </c>
       <c r="L2">
-        <v>0.15905141841818249</v>
+        <v>0.13505108292256951</v>
       </c>
       <c r="M2">
-        <v>0.56873437132818427</v>
+        <v>0.75529327588176964</v>
       </c>
     </row>
     <row r="3" spans="2:13" x14ac:dyDescent="0.35">
       <c r="B3">
-        <v>2.1952210296988395</v>
+        <v>3.011516244813532</v>
       </c>
       <c r="C3">
-        <v>2.3418320211300112</v>
+        <v>2.7222694328990138</v>
       </c>
       <c r="D3">
-        <v>2.3739752054504661</v>
+        <v>3.1713233305146709</v>
       </c>
       <c r="E3">
-        <v>2.6475381476904647</v>
+        <v>3.3261706893428289</v>
       </c>
       <c r="F3">
-        <v>1.7640090781652411</v>
+        <v>2.243027959544043</v>
       </c>
       <c r="G3">
-        <v>1.2524285128627448</v>
+        <v>1.2515869857807671</v>
       </c>
       <c r="H3">
-        <v>0.81507699640653886</v>
+        <v>0.95341813798153385</v>
       </c>
     </row>
     <row r="4" spans="2:13" x14ac:dyDescent="0.35">
@@ -777,7 +775,7 @@
         <v>180</v>
       </c>
       <c r="H4">
-        <v>83.868687610099826</v>
+        <v>84.543315074051534</v>
       </c>
     </row>
     <row r="5" spans="2:13" x14ac:dyDescent="0.35">
@@ -800,122 +798,116 @@
         <v>0</v>
       </c>
       <c r="H5">
-        <v>0.48192768037495048</v>
+        <v>0.52547058877336872</v>
       </c>
     </row>
     <row r="6" spans="2:13" x14ac:dyDescent="0.35">
       <c r="B6">
-        <v>2600</v>
+        <v>1770</v>
       </c>
       <c r="C6">
-        <v>2484</v>
+        <v>1954</v>
       </c>
       <c r="D6">
-        <v>2157</v>
+        <v>1470</v>
       </c>
       <c r="E6">
-        <v>3435</v>
+        <v>2580</v>
       </c>
       <c r="F6">
-        <v>2768</v>
+        <v>1904</v>
       </c>
       <c r="G6">
         <v>180</v>
       </c>
       <c r="H6">
-        <v>13624</v>
+        <v>9858</v>
       </c>
     </row>
     <row r="8" spans="2:13" x14ac:dyDescent="0.35">
       <c r="B8">
-        <v>0.98280098280098283</v>
+        <v>1</v>
       </c>
       <c r="C8">
-        <v>0.97222222222222221</v>
+        <v>1</v>
       </c>
       <c r="D8">
-        <v>0.9869020501138952</v>
+        <v>1</v>
       </c>
       <c r="E8">
-        <v>0.97823681298413867</v>
+        <v>1</v>
       </c>
       <c r="F8">
-        <v>0.9887285843101894</v>
+        <v>1</v>
       </c>
       <c r="G8">
-        <v>0.98165223936770796</v>
-      </c>
-      <c r="L8">
-        <v>0.42791260083165938</v>
-      </c>
-      <c r="M8">
-        <v>0.48848581421085902</v>
+        <v>1</v>
       </c>
     </row>
     <row r="9" spans="2:13" x14ac:dyDescent="0.35">
       <c r="B9">
-        <v>4.0156175496241656E-3</v>
+        <v>0</v>
       </c>
       <c r="C9">
-        <v>7.3612074334708771E-3</v>
+        <v>0</v>
       </c>
       <c r="D9">
-        <v>3.3401981602603032E-3</v>
+        <v>0</v>
       </c>
       <c r="E9">
-        <v>5.982955141978775E-3</v>
+        <v>0</v>
       </c>
       <c r="F9">
-        <v>2.9388029720992899E-3</v>
+        <v>0</v>
       </c>
       <c r="G9">
-        <v>2.3323583385866185E-3</v>
+        <v>0</v>
       </c>
     </row>
     <row r="10" spans="2:13" x14ac:dyDescent="0.35">
       <c r="B10">
-        <v>0.76923076923076927</v>
+        <v>0.7830508474576271</v>
       </c>
       <c r="C10">
-        <v>0.74738114423851731</v>
+        <v>0.75153688524590168</v>
       </c>
       <c r="D10">
-        <v>0.80380333951762528</v>
+        <v>0.80054458815520757</v>
       </c>
       <c r="E10">
-        <v>0.77205240174672485</v>
+        <v>0.7682170542635659</v>
       </c>
       <c r="F10">
-        <v>0.79284164859002171</v>
+        <v>0.80567226890756305</v>
       </c>
       <c r="G10">
-        <v>0.77632264305379861</v>
+        <v>0.77984496124031011</v>
       </c>
       <c r="L10">
-        <v>0.73706312919069306</v>
+        <v>0.5875424157118081</v>
       </c>
       <c r="M10">
-        <v>0.50303070678483697</v>
+        <v>0.69470752921424106</v>
       </c>
     </row>
     <row r="11" spans="2:13" x14ac:dyDescent="0.35">
       <c r="B11">
-        <v>1.9842184742342475E-2</v>
+        <v>1.811130220026428E-2</v>
       </c>
       <c r="C11">
-        <v>2.5623636641152012E-2</v>
+        <v>2.5108514489635889E-2</v>
       </c>
       <c r="D11">
-        <v>2.3871935695980506E-2</v>
+        <v>2.7914848140193949E-2</v>
       </c>
       <c r="E11">
-        <v>2.3676825836405423E-2</v>
+        <v>2.5590462389769891E-2</v>
       </c>
       <c r="F11">
-        <v>2.2472107685513335E-2</v>
+        <v>2.1239282926013531E-2</v>
       </c>
       <c r="G11">
-        <v>1.0493470680901324E-2</v>
+        <v>1.099794824214932E-2</v>
       </c>
     </row>
   </sheetData>
@@ -935,375 +927,375 @@
   <sheetData>
     <row r="2" spans="2:13" x14ac:dyDescent="0.35">
       <c r="B2">
-        <v>0.75514266755142667</v>
+        <v>0.72671443193449337</v>
       </c>
       <c r="C2">
-        <v>0.72237196765498657</v>
+        <v>0.71376481312670925</v>
       </c>
       <c r="D2">
-        <v>0.72635983263598325</v>
+        <v>0.69873417721518982</v>
       </c>
       <c r="E2">
-        <v>0.71811414392059558</v>
+        <v>0.6984240687679083</v>
       </c>
       <c r="F2">
-        <v>0.74058060531192094</v>
+        <v>0.72718052738336714</v>
       </c>
       <c r="G2">
-        <v>0.74980252764612954</v>
+        <v>0.33333333333333331</v>
       </c>
       <c r="H2">
-        <v>0.73897857808134115</v>
+        <v>0.71191926884996193</v>
       </c>
       <c r="K2">
-        <v>0.1237099015269276</v>
+        <v>6.9274793783455094E-2</v>
       </c>
       <c r="L2">
-        <v>0.20316365915662801</v>
+        <v>0.65951689489423038</v>
       </c>
       <c r="M2">
-        <v>0.53421473315735013</v>
+        <v>0.55340910471649929</v>
       </c>
     </row>
     <row r="3" spans="2:13" x14ac:dyDescent="0.35">
       <c r="B3">
-        <v>1.6425991245592318E-2</v>
+        <v>2.3496909134917761E-2</v>
       </c>
       <c r="C3">
-        <v>1.6091100265249757E-2</v>
+        <v>1.9399821328008521E-2</v>
       </c>
       <c r="D3">
-        <v>2.0324180320801292E-2</v>
+        <v>2.1841268197077331E-2</v>
       </c>
       <c r="E3">
-        <v>1.5140443704992812E-2</v>
+        <v>2.0803474242117068E-2</v>
       </c>
       <c r="F3">
-        <v>1.2828726752602795E-2</v>
+        <v>1.8069885724529701E-2</v>
       </c>
       <c r="G3">
-        <v>9.0149695175873682E-3</v>
+        <v>0.25458753860865779</v>
       </c>
       <c r="H3">
-        <v>5.6750398759389097E-3</v>
+        <v>9.5164117247609793E-3</v>
       </c>
     </row>
     <row r="4" spans="2:13" x14ac:dyDescent="0.35">
       <c r="B4">
-        <v>43.197583511016347</v>
+        <v>43.216245883644348</v>
       </c>
       <c r="C4">
-        <v>43.214285714285715</v>
+        <v>42.728862973760933</v>
       </c>
       <c r="D4">
-        <v>43.014652014652015</v>
+        <v>42.0979020979021</v>
       </c>
       <c r="E4">
-        <v>44.068119891008173</v>
+        <v>43.164274322169057</v>
       </c>
       <c r="F4">
-        <v>43.085413929040733</v>
+        <v>42.27398720682303</v>
       </c>
       <c r="G4">
-        <v>43.05681818181818</v>
+        <v>52.666666666666657</v>
       </c>
       <c r="H4">
-        <v>43.246039686509924</v>
+        <v>42.764269524005769</v>
       </c>
       <c r="K4">
-        <v>0.45869706596643522</v>
+        <v>7.8021215238789701E-2</v>
       </c>
       <c r="L4">
-        <v>0.51811943398266214</v>
+        <v>0.9128006774409122</v>
       </c>
       <c r="M4">
-        <v>0.97646568723149618</v>
+        <v>0.49205056096718142</v>
       </c>
     </row>
     <row r="5" spans="2:13" x14ac:dyDescent="0.35">
       <c r="B5">
-        <v>0.56359423339355952</v>
+        <v>0.72156527591038777</v>
       </c>
       <c r="C5">
-        <v>0.77069700997930013</v>
+        <v>0.97569774213318905</v>
       </c>
       <c r="D5">
-        <v>0.66004082042892609</v>
+        <v>0.71345918257971452</v>
       </c>
       <c r="E5">
-        <v>0.6046553749281488</v>
+        <v>0.63716196516581103</v>
       </c>
       <c r="F5">
-        <v>0.51619884617405898</v>
+        <v>0.69379757689913479</v>
       </c>
       <c r="G5">
-        <v>0.31582069920051548</v>
+        <v>6.8664509135468341</v>
       </c>
       <c r="H5">
-        <v>0.21148102499151927</v>
+        <v>0.34249915365843758</v>
       </c>
     </row>
     <row r="6" spans="2:13" x14ac:dyDescent="0.35">
       <c r="B6">
-        <v>3145.352544966549</v>
+        <v>3006.2437898038552</v>
       </c>
       <c r="C6">
-        <v>2984.9842439870736</v>
+        <v>2821.7948068237311</v>
       </c>
       <c r="D6">
-        <v>3010.3149184642348</v>
+        <v>2888.7710581766569</v>
       </c>
       <c r="E6">
-        <v>3110.9508585695362</v>
+        <v>3070.6324083174259</v>
       </c>
       <c r="F6">
-        <v>3082.6830472633487</v>
+        <v>2848.878149354538</v>
       </c>
       <c r="G6">
-        <v>3192.3481642889119</v>
+        <v>1831.914347330729</v>
       </c>
       <c r="H6">
-        <v>3111.7356224371706</v>
+        <v>2935.5698940123771</v>
       </c>
       <c r="K6">
-        <v>0.15545089802205039</v>
+        <v>9.4502397916000006E-6</v>
       </c>
       <c r="L6">
-        <v>0.34170888107806208</v>
+        <v>0.1139644273456603</v>
       </c>
       <c r="M6">
-        <v>0.41658255644769909</v>
+        <v>0.33670897301853492</v>
       </c>
     </row>
     <row r="7" spans="2:13" x14ac:dyDescent="0.35">
       <c r="B7">
-        <v>68.222299405324407</v>
+        <v>71.0158895041953</v>
       </c>
       <c r="C7">
-        <v>88.234047660960769</v>
+        <v>89.643425666912151</v>
       </c>
       <c r="D7">
-        <v>76.470442299269322</v>
+        <v>84.523872524705041</v>
       </c>
       <c r="E7">
-        <v>84.469381845420926</v>
+        <v>86.812031935256002</v>
       </c>
       <c r="F7">
-        <v>99.031452584314081</v>
+        <v>92.351196197717485</v>
       </c>
       <c r="G7">
-        <v>75.187897820076472</v>
+        <v>295.6326676245713</v>
       </c>
       <c r="H7">
-        <v>35.735445672018784</v>
+        <v>39.601137495357207</v>
       </c>
     </row>
     <row r="8" spans="2:13" x14ac:dyDescent="0.35">
       <c r="B8">
-        <v>0.89052631578947372</v>
+        <v>0.86188436830835113</v>
       </c>
       <c r="C8">
-        <v>0.89978828510938602</v>
+        <v>0.88392007611798284</v>
       </c>
       <c r="D8">
-        <v>0.89132420091324205</v>
+        <v>0.87533875338753386</v>
       </c>
       <c r="E8">
-        <v>0.91070467993544912</v>
+        <v>0.89315910837817059</v>
       </c>
       <c r="F8">
-        <v>0.89414114513981358</v>
+        <v>0.87152034261241973</v>
       </c>
       <c r="G8">
-        <v>0.88422131147540983</v>
+        <v>1</v>
       </c>
       <c r="H8">
-        <v>0.89267531614386597</v>
+        <v>0.878726833199033</v>
       </c>
       <c r="K8">
-        <v>0.225273760595539</v>
+        <v>1.53589704353E-55</v>
       </c>
       <c r="L8">
-        <v>0.40550231444286589</v>
+        <v>0.29145305872640548</v>
       </c>
       <c r="M8">
-        <v>0.96738092930936537</v>
+        <v>0.83969621922048276</v>
       </c>
     </row>
     <row r="9" spans="2:13" x14ac:dyDescent="0.35">
       <c r="B9">
-        <v>1.1504362429475282E-2</v>
+        <v>1.5973031642757742E-2</v>
       </c>
       <c r="C9">
-        <v>1.057909469617015E-2</v>
+        <v>1.341267379134994E-2</v>
       </c>
       <c r="D9">
-        <v>1.4535413795478427E-2</v>
+        <v>1.838390551064947E-2</v>
       </c>
       <c r="E9">
-        <v>9.9323761115656124E-3</v>
+        <v>1.2110784938116809E-2</v>
       </c>
       <c r="F9">
-        <v>9.4836902763061059E-3</v>
+        <v>1.473996510102527E-2</v>
       </c>
       <c r="G9">
-        <v>1.0533724370448033E-2</v>
+        <v>0</v>
       </c>
       <c r="H9">
-        <v>5.2054873450900745E-3</v>
+        <v>6.5508164953812578E-3</v>
       </c>
     </row>
     <row r="10" spans="2:13" x14ac:dyDescent="0.35">
       <c r="B10">
-        <v>92.725089422585597</v>
+        <v>91.886692015209121</v>
       </c>
       <c r="C10">
-        <v>92.197490452809603</v>
+        <v>91.646175839885629</v>
       </c>
       <c r="D10">
-        <v>93.655192532088677</v>
+        <v>93.240561896400351</v>
       </c>
       <c r="E10">
-        <v>93.716412213740455</v>
+        <v>93.610994764397901</v>
       </c>
       <c r="F10">
-        <v>93.339202965708992</v>
+        <v>92.704377104377102</v>
       </c>
       <c r="G10">
-        <v>91.835829749369722</v>
+        <v>100</v>
       </c>
       <c r="H10">
-        <v>92.6401174743025</v>
+        <v>92.679994485040666</v>
       </c>
       <c r="K10">
-        <v>1.1912823211479E-3</v>
+        <v>2.0673023913799999E-66</v>
       </c>
       <c r="L10">
-        <v>0.17622289997028059</v>
+        <v>9.1780872572990599E-2</v>
       </c>
       <c r="M10">
-        <v>0.48869909187268379</v>
+        <v>0.40650021553621668</v>
       </c>
     </row>
     <row r="11" spans="2:13" x14ac:dyDescent="0.35">
       <c r="B11">
-        <v>0.54084732630950216</v>
+        <v>0.72142723064601466</v>
       </c>
       <c r="C11">
-        <v>0.8381790132481084</v>
+        <v>1.0318898299456749</v>
       </c>
       <c r="D11">
-        <v>0.59030374500190863</v>
+        <v>0.72033173811356188</v>
       </c>
       <c r="E11">
-        <v>0.45517920772459858</v>
+        <v>0.58165693064045443</v>
       </c>
       <c r="F11">
-        <v>0.59487333389159291</v>
+        <v>0.79716566856601923</v>
       </c>
       <c r="G11">
-        <v>0.30818777366122263</v>
+        <v>0</v>
       </c>
       <c r="H11">
-        <v>0.20475253752404457</v>
+        <v>0.3490781329319485</v>
       </c>
     </row>
     <row r="12" spans="2:13" x14ac:dyDescent="0.35">
       <c r="B12">
-        <v>0.6597421203438395</v>
+        <v>0.65555555555555556</v>
       </c>
       <c r="C12">
-        <v>0.66884057971014488</v>
+        <v>0.66243902439024394</v>
       </c>
       <c r="D12">
-        <v>0.64716805942432687</v>
+        <v>0.63961485557083908</v>
       </c>
       <c r="E12">
-        <v>0.66276477146042367</v>
+        <v>0.6508447304907482</v>
       </c>
       <c r="F12">
-        <v>0.643598615916955</v>
+        <v>0.65260821309655936</v>
       </c>
       <c r="G12">
-        <v>0.59694943585457583</v>
+        <v>1</v>
       </c>
       <c r="H12">
-        <v>0.63285064825728232</v>
+        <v>0.65326947105372757</v>
       </c>
       <c r="K12">
-        <v>1.115253817344E-4</v>
+        <v>4.4758712593999997E-119</v>
       </c>
       <c r="L12">
-        <v>0.94338858432257489</v>
+        <v>0.92740950159320434</v>
       </c>
       <c r="M12">
-        <v>0.81166552956809146</v>
+        <v>0.90254130390463971</v>
       </c>
     </row>
     <row r="13" spans="2:13" x14ac:dyDescent="0.35">
       <c r="B13">
-        <v>1.938204739007152E-2</v>
+        <v>2.693662515942892E-2</v>
       </c>
       <c r="C13">
-        <v>1.9329841394817811E-2</v>
+        <v>2.2998521361771971E-2</v>
       </c>
       <c r="D13">
-        <v>2.4251483945742537E-2</v>
+        <v>2.7499668962467121E-2</v>
       </c>
       <c r="E13">
-        <v>1.6843213086678365E-2</v>
+        <v>1.9253409433816052E-2</v>
       </c>
       <c r="F13">
-        <v>1.6646508216829121E-2</v>
+        <v>1.95439236041129E-2</v>
       </c>
       <c r="G13">
-        <v>1.2957951584969644E-2</v>
+        <v>0</v>
       </c>
       <c r="H13">
-        <v>7.4824965608947022E-3</v>
+        <v>1.023896608416211E-2</v>
       </c>
     </row>
     <row r="14" spans="2:13" x14ac:dyDescent="0.35">
       <c r="B14">
-        <v>2635</v>
+        <v>1770</v>
       </c>
       <c r="C14">
-        <v>2535</v>
+        <v>1952</v>
       </c>
       <c r="D14">
-        <v>2179</v>
+        <v>1469</v>
       </c>
       <c r="E14">
-        <v>3494</v>
+        <v>2580</v>
       </c>
       <c r="F14">
-        <v>2791</v>
+        <v>1904</v>
       </c>
       <c r="G14">
-        <v>6919</v>
+        <v>6</v>
       </c>
       <c r="H14">
-        <v>20553</v>
+        <v>9681</v>
       </c>
     </row>
     <row r="16" spans="2:13" x14ac:dyDescent="0.35">
       <c r="B16">
-        <v>2035</v>
+        <v>1386</v>
       </c>
       <c r="C16">
-        <v>1908</v>
+        <v>1467</v>
       </c>
       <c r="D16">
-        <v>1756</v>
+        <v>1176</v>
       </c>
       <c r="E16">
-        <v>2711</v>
+        <v>1982</v>
       </c>
       <c r="F16">
-        <v>2218</v>
+        <v>1534</v>
       </c>
       <c r="G16">
-        <v>6919</v>
+        <v>6</v>
       </c>
     </row>
   </sheetData>
@@ -1323,315 +1315,315 @@
   <sheetData>
     <row r="2" spans="2:11" x14ac:dyDescent="0.35">
       <c r="B2">
-        <v>0.75706594885598921</v>
+        <v>0.72671443193449337</v>
       </c>
       <c r="C2">
-        <v>0.72451790633608815</v>
+        <v>0.71376481312670925</v>
       </c>
       <c r="D2">
-        <v>0.72527472527472525</v>
+        <v>0.69873417721518982</v>
       </c>
       <c r="E2">
-        <v>0.71761133603238869</v>
+        <v>0.6984240687679083</v>
       </c>
       <c r="F2">
-        <v>0.74111041796631316</v>
+        <v>0.72718052738336714</v>
       </c>
       <c r="G2">
-        <v>0.73259740259740258</v>
+        <v>0.71235226839496757</v>
       </c>
       <c r="J2">
-        <v>0.18200741924100611</v>
+        <v>0.65951689489423015</v>
       </c>
       <c r="K2">
-        <v>0.47018827911332062</v>
+        <v>0.55340910471649962</v>
       </c>
     </row>
     <row r="3" spans="2:11" x14ac:dyDescent="0.35">
       <c r="B3">
-        <v>1.6329938660297399E-2</v>
+        <v>2.3496909134917761E-2</v>
       </c>
       <c r="C3">
-        <v>1.6037712453979818E-2</v>
+        <v>1.9399821328008521E-2</v>
       </c>
       <c r="D3">
-        <v>2.0704066804602263E-2</v>
+        <v>2.1841268197077331E-2</v>
       </c>
       <c r="E3">
-        <v>1.5859952936583335E-2</v>
+        <v>2.0803474242117068E-2</v>
       </c>
       <c r="F3">
-        <v>1.2945207155944547E-2</v>
+        <v>1.8069885724529701E-2</v>
       </c>
       <c r="G3">
-        <v>7.382530362813145E-3</v>
+        <v>9.5223325342266418E-3</v>
       </c>
     </row>
     <row r="4" spans="2:11" x14ac:dyDescent="0.35">
       <c r="B4">
-        <v>43.164866810655148</v>
+        <v>43.216245883644348</v>
       </c>
       <c r="C4">
-        <v>43.174778761061944</v>
+        <v>42.728862973760933</v>
       </c>
       <c r="D4">
-        <v>42.960185185185182</v>
+        <v>42.0979020979021</v>
       </c>
       <c r="E4">
-        <v>43.963272120200337</v>
+        <v>43.164274322169057</v>
       </c>
       <c r="F4">
-        <v>43.072377158034527</v>
+        <v>42.27398720682303</v>
       </c>
       <c r="G4">
-        <v>43.317480359147027</v>
+        <v>42.752011553538267</v>
       </c>
       <c r="J4">
-        <v>0.58299404675484134</v>
+        <v>0.91280067744091231</v>
       </c>
       <c r="K4">
-        <v>0.97226330730205768</v>
+        <v>0.49205056096718119</v>
       </c>
     </row>
     <row r="5" spans="2:11" x14ac:dyDescent="0.35">
       <c r="B5">
-        <v>0.57302039418728534</v>
+        <v>0.72156527591038799</v>
       </c>
       <c r="C5">
-        <v>0.7869341141204792</v>
+        <v>0.97569774213318883</v>
       </c>
       <c r="D5">
-        <v>0.65161383087213032</v>
+        <v>0.71345918257971475</v>
       </c>
       <c r="E5">
-        <v>0.61260005153338226</v>
+        <v>0.63716196516581114</v>
       </c>
       <c r="F5">
-        <v>0.5175395496028099</v>
+        <v>0.69379757689913468</v>
       </c>
       <c r="G5">
-        <v>0.28326816453393761</v>
+        <v>0.34297930661234749</v>
       </c>
     </row>
     <row r="6" spans="2:11" x14ac:dyDescent="0.35">
       <c r="B6">
-        <v>3151.8311879330831</v>
+        <v>3006.2437898038552</v>
       </c>
       <c r="C6">
-        <v>2977.8080010068757</v>
+        <v>2821.7948068237311</v>
       </c>
       <c r="D6">
-        <v>2987.6091755578368</v>
+        <v>2888.7710581766569</v>
       </c>
       <c r="E6">
-        <v>3114.8420998012557</v>
+        <v>3070.6324083174259</v>
       </c>
       <c r="F6">
-        <v>3080.6487658710303</v>
+        <v>2848.878149354538</v>
       </c>
       <c r="G6">
-        <v>3069.2245258990883</v>
+        <v>2936.5790273985531</v>
       </c>
       <c r="J6">
-        <v>0.29805537908350199</v>
+        <v>0.1139644273456602</v>
       </c>
       <c r="K6">
-        <v>0.27369802702174151</v>
+        <v>0.33670897301853531</v>
       </c>
     </row>
     <row r="7" spans="2:11" x14ac:dyDescent="0.35">
       <c r="B7">
-        <v>68.633705702668763</v>
+        <v>71.0158895041953</v>
       </c>
       <c r="C7">
-        <v>90.821567649747067</v>
+        <v>89.643425666912151</v>
       </c>
       <c r="D7">
-        <v>76.019238973365518</v>
+        <v>84.523872524705027</v>
       </c>
       <c r="E7">
-        <v>84.55291310515976</v>
+        <v>86.812031935256016</v>
       </c>
       <c r="F7">
-        <v>99.417675983085019</v>
+        <v>92.351196197717485</v>
       </c>
       <c r="G7">
-        <v>38.649480296696282</v>
+        <v>39.608754453128327</v>
       </c>
     </row>
     <row r="8" spans="2:11" x14ac:dyDescent="0.35">
       <c r="B8">
-        <v>0.89102564102564108</v>
+        <v>0.86188436830835113</v>
       </c>
       <c r="C8">
-        <v>0.89841498559077815</v>
+        <v>0.88392007611798284</v>
       </c>
       <c r="D8">
-        <v>0.89289012003693446</v>
+        <v>0.87533875338753386</v>
       </c>
       <c r="E8">
-        <v>0.91058694459681844</v>
+        <v>0.89315910837817059</v>
       </c>
       <c r="F8">
-        <v>0.89374579690652323</v>
+        <v>0.87152034261241973</v>
       </c>
       <c r="G8">
-        <v>0.89826026443980511</v>
+        <v>0.87858007260992332</v>
       </c>
       <c r="J8">
-        <v>0.42375394960748619</v>
+        <v>0.29145305872640559</v>
       </c>
       <c r="K8">
-        <v>0.98364695363089938</v>
+        <v>0.83969621922048276</v>
       </c>
     </row>
     <row r="9" spans="2:11" x14ac:dyDescent="0.35">
       <c r="B9">
-        <v>1.1699017063997981E-2</v>
+        <v>1.5973031642757742E-2</v>
       </c>
       <c r="C9">
-        <v>1.0536449576402311E-2</v>
+        <v>1.341267379134994E-2</v>
       </c>
       <c r="D9">
-        <v>1.4414244480650894E-2</v>
+        <v>1.838390551064947E-2</v>
       </c>
       <c r="E9">
-        <v>9.9989344362034476E-3</v>
+        <v>1.2110784938116809E-2</v>
       </c>
       <c r="F9">
-        <v>9.5382524633601719E-3</v>
+        <v>1.473996510102527E-2</v>
       </c>
       <c r="G9">
-        <v>4.9491419759811308E-3</v>
+        <v>6.5608352967268828E-3</v>
       </c>
     </row>
     <row r="10" spans="2:11" x14ac:dyDescent="0.35">
       <c r="B10">
-        <v>92.740644490644485</v>
+        <v>91.886692015209121</v>
       </c>
       <c r="C10">
-        <v>92.156950672645735</v>
+        <v>91.646175839885629</v>
       </c>
       <c r="D10">
-        <v>93.604376108811351</v>
+        <v>93.240561896400351</v>
       </c>
       <c r="E10">
-        <v>93.670308232539995</v>
+        <v>93.610994764397901</v>
       </c>
       <c r="F10">
-        <v>93.290866510538635</v>
+        <v>92.704377104377102</v>
       </c>
       <c r="G10">
-        <v>93.134495394671688</v>
+        <v>92.674944812362028</v>
       </c>
       <c r="J10">
-        <v>0.21062078261948161</v>
+        <v>9.1780872572990599E-2</v>
       </c>
       <c r="K10">
-        <v>0.55369821967704347</v>
+        <v>0.40650021553621629</v>
       </c>
     </row>
     <row r="11" spans="2:11" x14ac:dyDescent="0.35">
       <c r="B11">
-        <v>0.55282250572746661</v>
+        <v>0.72142723064601466</v>
       </c>
       <c r="C11">
-        <v>0.85746436976065976</v>
+        <v>1.031889829945674</v>
       </c>
       <c r="D11">
-        <v>0.59648670007090754</v>
+        <v>0.72033173811356166</v>
       </c>
       <c r="E11">
-        <v>0.47054474058339091</v>
+        <v>0.58165693064045443</v>
       </c>
       <c r="F11">
-        <v>0.59891547015170432</v>
+        <v>0.79716566856601956</v>
       </c>
       <c r="G11">
-        <v>0.27434924538180411</v>
+        <v>0.34925879876304872</v>
       </c>
     </row>
     <row r="12" spans="2:11" x14ac:dyDescent="0.35">
       <c r="B12">
-        <v>0.66084425036390104</v>
+        <v>0.65555555555555556</v>
       </c>
       <c r="C12">
-        <v>0.6723372781065089</v>
+        <v>0.66243902439024394</v>
       </c>
       <c r="D12">
-        <v>0.64694835680751173</v>
+        <v>0.63961485557083908</v>
       </c>
       <c r="E12">
-        <v>0.66590779738190098</v>
+        <v>0.6508447304907482</v>
       </c>
       <c r="F12">
-        <v>0.64220824598183091</v>
+        <v>0.65260821309655936</v>
       </c>
       <c r="G12">
-        <v>0.65840378277690215</v>
+        <v>0.65283569641367811</v>
       </c>
       <c r="J12">
-        <v>0.91190770005625166</v>
+        <v>0.92740950159320423</v>
       </c>
       <c r="K12">
-        <v>0.75438829625622084</v>
+        <v>0.90254130390463971</v>
       </c>
     </row>
     <row r="13" spans="2:11" x14ac:dyDescent="0.35">
       <c r="B13">
-        <v>1.9264793906698385E-2</v>
+        <v>2.693662515942892E-2</v>
       </c>
       <c r="C13">
-        <v>1.8898567915395067E-2</v>
+        <v>2.2998521361771971E-2</v>
       </c>
       <c r="D13">
-        <v>2.4289475036466852E-2</v>
+        <v>2.7499668962467121E-2</v>
       </c>
       <c r="E13">
-        <v>1.6402036310363216E-2</v>
+        <v>1.9253409433816052E-2</v>
       </c>
       <c r="F13">
-        <v>1.6248832152705936E-2</v>
+        <v>1.95439236041129E-2</v>
       </c>
       <c r="G13">
-        <v>8.3758892114355592E-3</v>
+        <v>1.024460360708169E-2</v>
       </c>
     </row>
     <row r="14" spans="2:11" x14ac:dyDescent="0.35">
       <c r="B14">
-        <v>2600</v>
+        <v>1770</v>
       </c>
       <c r="C14">
-        <v>2482</v>
+        <v>1952</v>
       </c>
       <c r="D14">
-        <v>2156</v>
+        <v>1469</v>
       </c>
       <c r="E14">
-        <v>3435</v>
+        <v>2580</v>
       </c>
       <c r="F14">
-        <v>2766</v>
+        <v>1904</v>
       </c>
       <c r="G14">
-        <v>13439</v>
+        <v>9675</v>
       </c>
     </row>
     <row r="16" spans="2:11" x14ac:dyDescent="0.35">
       <c r="B16">
-        <v>2000</v>
+        <v>1386</v>
       </c>
       <c r="C16">
-        <v>1855</v>
+        <v>1467</v>
       </c>
       <c r="D16">
-        <v>1733</v>
+        <v>1176</v>
       </c>
       <c r="E16">
-        <v>2652</v>
+        <v>1982</v>
       </c>
       <c r="F16">
-        <v>2193</v>
+        <v>1534</v>
       </c>
     </row>
   </sheetData>
@@ -1641,10 +1633,10 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3B054637-0760-4807-B01C-4419EACB0C14}">
-  <dimension ref="A2:I39"/>
+  <dimension ref="A2:I25"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3:I38"/>
+      <selection activeCell="L8" sqref="L8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1661,29 +1653,29 @@
   <sheetData>
     <row r="2" spans="1:9" s="10" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A2" s="15"/>
-      <c r="B2" s="16"/>
-      <c r="C2" s="16"/>
-      <c r="D2" s="16"/>
-      <c r="E2" s="16"/>
-      <c r="F2" s="16"/>
-      <c r="G2" s="16"/>
-      <c r="H2" s="16"/>
-      <c r="I2" s="16"/>
+      <c r="B2" s="17"/>
+      <c r="C2" s="17"/>
+      <c r="D2" s="17"/>
+      <c r="E2" s="17"/>
+      <c r="F2" s="17"/>
+      <c r="G2" s="17"/>
+      <c r="H2" s="17"/>
+      <c r="I2" s="17"/>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A3" s="10"/>
       <c r="B3" s="11"/>
-      <c r="C3" s="18" t="s">
-        <v>19</v>
-      </c>
-      <c r="D3" s="18"/>
-      <c r="E3" s="18"/>
+      <c r="C3" s="19" t="s">
+        <v>18</v>
+      </c>
+      <c r="D3" s="19"/>
+      <c r="E3" s="19"/>
       <c r="F3" s="11"/>
-      <c r="G3" s="18" t="s">
-        <v>18</v>
-      </c>
-      <c r="H3" s="18"/>
-      <c r="I3" s="18"/>
+      <c r="G3" s="19" t="s">
+        <v>17</v>
+      </c>
+      <c r="H3" s="19"/>
+      <c r="I3" s="19"/>
     </row>
     <row r="4" spans="1:9" s="6" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A4" s="12"/>
@@ -1712,16 +1704,16 @@
     </row>
     <row r="5" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A5" s="2"/>
-      <c r="B5" s="17" t="s">
+      <c r="B5" s="18" t="s">
         <v>3</v>
       </c>
-      <c r="C5" s="17"/>
-      <c r="D5" s="17"/>
-      <c r="E5" s="17"/>
-      <c r="F5" s="17"/>
-      <c r="G5" s="17"/>
-      <c r="H5" s="17"/>
-      <c r="I5" s="17"/>
+      <c r="C5" s="18"/>
+      <c r="D5" s="18"/>
+      <c r="E5" s="18"/>
+      <c r="F5" s="18"/>
+      <c r="G5" s="18"/>
+      <c r="H5" s="18"/>
+      <c r="I5" s="18"/>
     </row>
     <row r="6" spans="1:9" ht="15" thickTop="1" x14ac:dyDescent="0.35">
       <c r="A6" s="10" t="s">
@@ -1729,32 +1721,32 @@
       </c>
       <c r="B6" s="11">
         <f>ROUND(SS_admin!B2,0)</f>
-        <v>2280</v>
+        <v>2267</v>
       </c>
       <c r="C6" s="11">
         <f>ROUND(SS_admin!C2,0)</f>
-        <v>2147</v>
+        <v>2162</v>
       </c>
       <c r="D6" s="11">
         <f>ROUND(SS_admin!E2,0)</f>
-        <v>2165</v>
+        <v>2223</v>
       </c>
       <c r="E6" s="11">
         <f>ROUND(SS_admin!L2,2)</f>
-        <v>0.38</v>
+        <v>0.64</v>
       </c>
       <c r="F6" s="11"/>
       <c r="G6" s="11">
         <f>ROUND(SS_admin!D2,0)</f>
-        <v>2133</v>
+        <v>2258</v>
       </c>
       <c r="H6" s="11">
         <f>ROUND(SS_admin!F2,0)</f>
-        <v>2089</v>
+        <v>2099</v>
       </c>
       <c r="I6" s="11">
         <f>ROUND(SS_admin!M2,2)</f>
-        <v>0.15</v>
+        <v>0.17</v>
       </c>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.35">
@@ -1765,27 +1757,27 @@
       </c>
       <c r="C7" s="11" t="str">
         <f>CONCATENATE("(",ROUND(SS_admin!C3,0),")")</f>
-        <v>(72)</v>
+        <v>(83)</v>
       </c>
       <c r="D7" s="11" t="str">
         <f>CONCATENATE("(",ROUND(SS_admin!E3,0),")")</f>
-        <v>(58)</v>
+        <v>(66)</v>
       </c>
       <c r="E7" s="11"/>
       <c r="F7" s="11"/>
       <c r="G7" s="11" t="str">
         <f>CONCATENATE("(",ROUND(SS_admin!D3,0),")")</f>
-        <v>(74)</v>
+        <v>(91)</v>
       </c>
       <c r="H7" s="11" t="str">
         <f>CONCATENATE("(",ROUND(SS_admin!F3,0),")")</f>
-        <v>(65)</v>
+        <v>(66)</v>
       </c>
       <c r="I7" s="11"/>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A8" s="10" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B8" s="11">
         <f>ROUND(SS_admin!B4,2)</f>
@@ -1797,49 +1789,49 @@
       </c>
       <c r="D8" s="11">
         <f>ROUND(SS_admin!E4,2)</f>
-        <v>0.85</v>
+        <v>0.83</v>
       </c>
       <c r="E8" s="11">
         <f>ROUND(SS_admin!L4,2)</f>
-        <v>0.71</v>
+        <v>0.56000000000000005</v>
       </c>
       <c r="F8" s="11"/>
       <c r="G8" s="11">
         <f>ROUND(SS_admin!D4,2)</f>
-        <v>0.88</v>
+        <v>0.9</v>
       </c>
       <c r="H8" s="11">
         <f>ROUND(SS_admin!F4,2)</f>
-        <v>0.83</v>
+        <v>0.81</v>
       </c>
       <c r="I8" s="11">
         <f>ROUND(SS_admin!M4,2)</f>
-        <v>0.64</v>
+        <v>0.43</v>
       </c>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A9" s="10"/>
       <c r="B9" s="11" t="str">
         <f>CONCATENATE("(",ROUND(SS_admin!B5,3),")")</f>
-        <v>(0.04)</v>
+        <v>(0.044)</v>
       </c>
       <c r="C9" s="11" t="str">
         <f>CONCATENATE("(",ROUND(SS_admin!C5,3),")")</f>
-        <v>(0.034)</v>
+        <v>(0.035)</v>
       </c>
       <c r="D9" s="11" t="str">
         <f>CONCATENATE("(",ROUND(SS_admin!E5,3),")")</f>
-        <v>(0.042)</v>
+        <v>(0.048)</v>
       </c>
       <c r="E9" s="11"/>
       <c r="F9" s="11"/>
       <c r="G9" s="11" t="str">
         <f>CONCATENATE("(",ROUND(SS_admin!D5,3),")")</f>
-        <v>(0.036)</v>
+        <v>(0.033)</v>
       </c>
       <c r="H9" s="11" t="str">
         <f>CONCATENATE("(",ROUND(SS_admin!F5,3),")")</f>
-        <v>(0.048)</v>
+        <v>(0.056)</v>
       </c>
       <c r="I9" s="11"/>
     </row>
@@ -1849,40 +1841,40 @@
       </c>
       <c r="B10" s="4">
         <f>SS_admin!B6</f>
-        <v>2600</v>
+        <v>1770</v>
       </c>
       <c r="C10" s="4">
         <f>SS_admin!C6</f>
-        <v>2484</v>
+        <v>1954</v>
       </c>
       <c r="D10" s="4">
         <f>SS_admin!E6</f>
-        <v>3435</v>
+        <v>2580</v>
       </c>
       <c r="E10" s="4"/>
       <c r="F10" s="4"/>
       <c r="G10" s="4">
         <f>SS_admin!D6</f>
-        <v>2157</v>
+        <v>1470</v>
       </c>
       <c r="H10" s="4">
         <f>SS_admin!F6</f>
-        <v>2768</v>
+        <v>1904</v>
       </c>
       <c r="I10" s="4"/>
     </row>
     <row r="11" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A11" s="2"/>
-      <c r="B11" s="17" t="s">
-        <v>21</v>
-      </c>
-      <c r="C11" s="17"/>
-      <c r="D11" s="17"/>
-      <c r="E11" s="17"/>
-      <c r="F11" s="17"/>
-      <c r="G11" s="17"/>
-      <c r="H11" s="17"/>
-      <c r="I11" s="17"/>
+      <c r="B11" s="18" t="s">
+        <v>19</v>
+      </c>
+      <c r="C11" s="18"/>
+      <c r="D11" s="18"/>
+      <c r="E11" s="18"/>
+      <c r="F11" s="18"/>
+      <c r="G11" s="18"/>
+      <c r="H11" s="18"/>
+      <c r="I11" s="18"/>
     </row>
     <row r="12" spans="1:9" ht="15" thickTop="1" x14ac:dyDescent="0.35">
       <c r="A12" s="10" t="s">
@@ -1890,57 +1882,57 @@
       </c>
       <c r="B12" s="11">
         <f>ROUND(SS_survey_uncond!B2,2)</f>
-        <v>0.76</v>
+        <v>0.73</v>
       </c>
       <c r="C12" s="11">
         <f>ROUND(SS_survey_uncond!C2,2)</f>
-        <v>0.72</v>
+        <v>0.71</v>
       </c>
       <c r="D12" s="11">
         <f>ROUND(SS_survey_uncond!E2,2)</f>
-        <v>0.72</v>
+        <v>0.7</v>
       </c>
       <c r="E12" s="11">
         <f>ROUND(SS_survey_uncond!L2,2)</f>
-        <v>0.2</v>
+        <v>0.66</v>
       </c>
       <c r="F12" s="11"/>
       <c r="G12" s="11">
         <f>ROUND(SS_survey_uncond!D2,2)</f>
-        <v>0.73</v>
+        <v>0.7</v>
       </c>
       <c r="H12" s="11">
         <f>ROUND(SS_survey_uncond!F2,2)</f>
-        <v>0.74</v>
+        <v>0.73</v>
       </c>
       <c r="I12" s="11">
         <f>ROUND(SS_survey_uncond!M2,2)</f>
-        <v>0.53</v>
+        <v>0.55000000000000004</v>
       </c>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A13" s="10"/>
       <c r="B13" s="11" t="str">
         <f>CONCATENATE("(",ROUND(SS_survey_uncond!B3,3),")")</f>
-        <v>(0.016)</v>
+        <v>(0.023)</v>
       </c>
       <c r="C13" s="11" t="str">
         <f>CONCATENATE("(",ROUND(SS_survey_uncond!C3,3),")")</f>
-        <v>(0.016)</v>
+        <v>(0.019)</v>
       </c>
       <c r="D13" s="11" t="str">
         <f>CONCATENATE("(",ROUND(SS_survey_uncond!E3,3),")")</f>
-        <v>(0.015)</v>
+        <v>(0.021)</v>
       </c>
       <c r="E13" s="11"/>
       <c r="F13" s="11"/>
       <c r="G13" s="11" t="str">
         <f>CONCATENATE("(",ROUND(SS_survey_uncond!D3,3),")")</f>
-        <v>(0.02)</v>
+        <v>(0.022)</v>
       </c>
       <c r="H13" s="11" t="str">
         <f>CONCATENATE("(",ROUND(SS_survey_uncond!F3,3),")")</f>
-        <v>(0.013)</v>
+        <v>(0.018)</v>
       </c>
       <c r="I13" s="11"/>
     </row>
@@ -1950,57 +1942,57 @@
       </c>
       <c r="B14" s="11">
         <f>ROUND(SS_survey_uncond!B4,2)</f>
-        <v>43.2</v>
+        <v>43.22</v>
       </c>
       <c r="C14" s="11">
         <f>ROUND(SS_survey_uncond!C4,2)</f>
-        <v>43.21</v>
+        <v>42.73</v>
       </c>
       <c r="D14" s="11">
         <f>ROUND(SS_survey_uncond!E4,2)</f>
-        <v>44.07</v>
+        <v>43.16</v>
       </c>
       <c r="E14" s="11">
         <f>ROUND(SS_survey_uncond!L4,2)</f>
-        <v>0.52</v>
+        <v>0.91</v>
       </c>
       <c r="F14" s="11"/>
       <c r="G14" s="11">
         <f>ROUND(SS_survey_uncond!D4,2)</f>
-        <v>43.01</v>
+        <v>42.1</v>
       </c>
       <c r="H14" s="11">
         <f>ROUND(SS_survey_uncond!F4,2)</f>
-        <v>43.09</v>
+        <v>42.27</v>
       </c>
       <c r="I14" s="11">
         <f>ROUND(SS_survey_uncond!M4,2)</f>
-        <v>0.98</v>
+        <v>0.49</v>
       </c>
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A15" s="10"/>
       <c r="B15" s="11" t="str">
         <f>CONCATENATE("(",ROUND(SS_survey_uncond!B5,3),")")</f>
-        <v>(0.564)</v>
+        <v>(0.722)</v>
       </c>
       <c r="C15" s="11" t="str">
         <f>CONCATENATE("(",ROUND(SS_survey_uncond!C5,3),")")</f>
-        <v>(0.771)</v>
+        <v>(0.976)</v>
       </c>
       <c r="D15" s="11" t="str">
         <f>CONCATENATE("(",ROUND(SS_survey_uncond!E5,3),")")</f>
-        <v>(0.605)</v>
+        <v>(0.637)</v>
       </c>
       <c r="E15" s="11"/>
       <c r="F15" s="11"/>
       <c r="G15" s="11" t="str">
         <f>CONCATENATE("(",ROUND(SS_survey_uncond!D5,3),")")</f>
-        <v>(0.66)</v>
+        <v>(0.713)</v>
       </c>
       <c r="H15" s="11" t="str">
         <f>CONCATENATE("(",ROUND(SS_survey_uncond!F5,3),")")</f>
-        <v>(0.516)</v>
+        <v>(0.694)</v>
       </c>
       <c r="I15" s="11"/>
     </row>
@@ -2010,57 +2002,57 @@
       </c>
       <c r="B16" s="11">
         <f>ROUND(SS_survey_uncond!B6,0)</f>
-        <v>3145</v>
+        <v>3006</v>
       </c>
       <c r="C16" s="11">
         <f>ROUND(SS_survey_uncond!C6,0)</f>
-        <v>2985</v>
+        <v>2822</v>
       </c>
       <c r="D16" s="11">
         <f>ROUND(SS_survey_uncond!E6,0)</f>
-        <v>3111</v>
+        <v>3071</v>
       </c>
       <c r="E16" s="11">
         <f>ROUND(SS_survey_uncond!L6,2)</f>
-        <v>0.34</v>
+        <v>0.11</v>
       </c>
       <c r="F16" s="11"/>
       <c r="G16" s="11">
         <f>ROUND(SS_survey_uncond!D6,0)</f>
-        <v>3010</v>
+        <v>2889</v>
       </c>
       <c r="H16" s="11">
         <f>ROUND(SS_survey_uncond!F6,0)</f>
-        <v>3083</v>
+        <v>2849</v>
       </c>
       <c r="I16" s="11">
         <f>ROUND(SS_survey_uncond!M6,2)</f>
-        <v>0.42</v>
+        <v>0.34</v>
       </c>
     </row>
     <row r="17" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A17" s="10"/>
       <c r="B17" s="11" t="str">
         <f>CONCATENATE("(",ROUND(SS_survey_uncond!B7,0),")")</f>
-        <v>(68)</v>
+        <v>(71)</v>
       </c>
       <c r="C17" s="11" t="str">
         <f>CONCATENATE("(",ROUND(SS_survey_uncond!C7,0),")")</f>
-        <v>(88)</v>
+        <v>(90)</v>
       </c>
       <c r="D17" s="11" t="str">
         <f>CONCATENATE("(",ROUND(SS_survey_uncond!E7,0),")")</f>
-        <v>(84)</v>
+        <v>(87)</v>
       </c>
       <c r="E17" s="11"/>
       <c r="F17" s="11"/>
       <c r="G17" s="11" t="str">
         <f>CONCATENATE("(",ROUND(SS_survey_uncond!D7,0),")")</f>
-        <v>(76)</v>
+        <v>(85)</v>
       </c>
       <c r="H17" s="11" t="str">
         <f>CONCATENATE("(",ROUND(SS_survey_uncond!F7,0),")")</f>
-        <v>(99)</v>
+        <v>(92)</v>
       </c>
       <c r="I17" s="11"/>
     </row>
@@ -2070,57 +2062,57 @@
       </c>
       <c r="B18" s="11">
         <f>ROUND(SS_survey_uncond!B8,2)</f>
-        <v>0.89</v>
+        <v>0.86</v>
       </c>
       <c r="C18" s="11">
         <f>ROUND(SS_survey_uncond!C8,2)</f>
-        <v>0.9</v>
+        <v>0.88</v>
       </c>
       <c r="D18" s="11">
         <f>ROUND(SS_survey_uncond!E8,2)</f>
-        <v>0.91</v>
+        <v>0.89</v>
       </c>
       <c r="E18" s="11">
         <f>ROUND(SS_survey_uncond!L8,2)</f>
-        <v>0.41</v>
+        <v>0.28999999999999998</v>
       </c>
       <c r="F18" s="11"/>
       <c r="G18" s="11">
         <f>ROUND(SS_survey_uncond!D8,2)</f>
-        <v>0.89</v>
+        <v>0.88</v>
       </c>
       <c r="H18" s="11">
         <f>ROUND(SS_survey_uncond!F8,2)</f>
-        <v>0.89</v>
+        <v>0.87</v>
       </c>
       <c r="I18" s="11">
         <f>ROUND(SS_survey_uncond!M8,2)</f>
-        <v>0.97</v>
+        <v>0.84</v>
       </c>
     </row>
     <row r="19" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A19" s="10"/>
       <c r="B19" s="11" t="str">
         <f>CONCATENATE("(",ROUND(SS_survey_uncond!B9,3),")")</f>
-        <v>(0.012)</v>
+        <v>(0.016)</v>
       </c>
       <c r="C19" s="11" t="str">
         <f>CONCATENATE("(",ROUND(SS_survey_uncond!C9,3),")")</f>
-        <v>(0.011)</v>
+        <v>(0.013)</v>
       </c>
       <c r="D19" s="11" t="str">
         <f>CONCATENATE("(",ROUND(SS_survey_uncond!E9,3),")")</f>
-        <v>(0.01)</v>
+        <v>(0.012)</v>
       </c>
       <c r="E19" s="11"/>
       <c r="F19" s="11"/>
       <c r="G19" s="11" t="str">
         <f>CONCATENATE("(",ROUND(SS_survey_uncond!D9,3),")")</f>
-        <v>(0.015)</v>
+        <v>(0.018)</v>
       </c>
       <c r="H19" s="11" t="str">
         <f>CONCATENATE("(",ROUND(SS_survey_uncond!F9,3),")")</f>
-        <v>(0.009)</v>
+        <v>(0.015)</v>
       </c>
       <c r="I19" s="11"/>
     </row>
@@ -2130,57 +2122,57 @@
       </c>
       <c r="B20" s="11">
         <f>ROUND(SS_survey_uncond!B10,2)</f>
-        <v>92.73</v>
+        <v>91.89</v>
       </c>
       <c r="C20" s="11">
         <f>ROUND(SS_survey_uncond!C10,2)</f>
-        <v>92.2</v>
+        <v>91.65</v>
       </c>
       <c r="D20" s="11">
         <f>ROUND(SS_survey_uncond!E10,2)</f>
-        <v>93.72</v>
+        <v>93.61</v>
       </c>
       <c r="E20" s="11">
         <f>ROUND(SS_survey_uncond!L10,2)</f>
-        <v>0.18</v>
+        <v>0.09</v>
       </c>
       <c r="F20" s="11"/>
       <c r="G20" s="11">
         <f>ROUND(SS_survey_uncond!D10,2)</f>
-        <v>93.66</v>
+        <v>93.24</v>
       </c>
       <c r="H20" s="11">
         <f>ROUND(SS_survey_uncond!F10,2)</f>
-        <v>93.34</v>
+        <v>92.7</v>
       </c>
       <c r="I20" s="11">
         <f>ROUND(SS_survey_uncond!M10,2)</f>
-        <v>0.49</v>
+        <v>0.41</v>
       </c>
     </row>
     <row r="21" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A21" s="10"/>
       <c r="B21" s="11" t="str">
         <f>CONCATENATE("(",ROUND(SS_survey_uncond!B11,3),")")</f>
-        <v>(0.541)</v>
+        <v>(0.721)</v>
       </c>
       <c r="C21" s="11" t="str">
         <f>CONCATENATE("(",ROUND(SS_survey_uncond!C11,3),")")</f>
-        <v>(0.838)</v>
+        <v>(1.032)</v>
       </c>
       <c r="D21" s="11" t="str">
         <f>CONCATENATE("(",ROUND(SS_survey_uncond!E11,3),")")</f>
-        <v>(0.455)</v>
+        <v>(0.582)</v>
       </c>
       <c r="E21" s="11"/>
       <c r="F21" s="11"/>
       <c r="G21" s="11" t="str">
         <f>CONCATENATE("(",ROUND(SS_survey_uncond!D11,3),")")</f>
-        <v>(0.59)</v>
+        <v>(0.72)</v>
       </c>
       <c r="H21" s="11" t="str">
         <f>CONCATENATE("(",ROUND(SS_survey_uncond!F11,3),")")</f>
-        <v>(0.595)</v>
+        <v>(0.797)</v>
       </c>
       <c r="I21" s="11"/>
     </row>
@@ -2194,491 +2186,89 @@
       </c>
       <c r="C22" s="11">
         <f>ROUND(SS_survey_uncond!C12,2)</f>
-        <v>0.67</v>
+        <v>0.66</v>
       </c>
       <c r="D22" s="11">
         <f>ROUND(SS_survey_uncond!E12,2)</f>
-        <v>0.66</v>
+        <v>0.65</v>
       </c>
       <c r="E22" s="11">
         <f>ROUND(SS_survey_uncond!L12,2)</f>
-        <v>0.94</v>
+        <v>0.93</v>
       </c>
       <c r="F22" s="11"/>
       <c r="G22" s="11">
         <f>ROUND(SS_survey_uncond!D12,2)</f>
-        <v>0.65</v>
+        <v>0.64</v>
       </c>
       <c r="H22" s="11">
         <f>ROUND(SS_survey_uncond!F12,2)</f>
-        <v>0.64</v>
+        <v>0.65</v>
       </c>
       <c r="I22" s="11">
         <f>ROUND(SS_survey_uncond!M12,2)</f>
-        <v>0.81</v>
+        <v>0.9</v>
       </c>
     </row>
     <row r="23" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A23" s="10"/>
       <c r="B23" s="11" t="str">
         <f>CONCATENATE("(",ROUND(SS_survey_uncond!B13,3),")")</f>
-        <v>(0.019)</v>
+        <v>(0.027)</v>
       </c>
       <c r="C23" s="11" t="str">
         <f>CONCATENATE("(",ROUND(SS_survey_uncond!C13,3),")")</f>
-        <v>(0.019)</v>
+        <v>(0.023)</v>
       </c>
       <c r="D23" s="11" t="str">
         <f>CONCATENATE("(",ROUND(SS_survey_uncond!E13,3),")")</f>
-        <v>(0.017)</v>
+        <v>(0.019)</v>
       </c>
       <c r="E23" s="11"/>
       <c r="F23" s="11"/>
       <c r="G23" s="11" t="str">
         <f>CONCATENATE("(",ROUND(SS_survey_uncond!D13,3),")")</f>
-        <v>(0.024)</v>
+        <v>(0.027)</v>
       </c>
       <c r="H23" s="11" t="str">
         <f>CONCATENATE("(",ROUND(SS_survey_uncond!F13,3),")")</f>
-        <v>(0.017)</v>
+        <v>(0.02)</v>
       </c>
       <c r="I23" s="11"/>
     </row>
-    <row r="24" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A24" s="1" t="s">
+    <row r="24" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A24" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="B24" s="4">
+      <c r="B24" s="16">
         <f>SS_survey_uncond!B16</f>
-        <v>2035</v>
-      </c>
-      <c r="C24" s="4">
+        <v>1386</v>
+      </c>
+      <c r="C24" s="16">
         <f>SS_survey_uncond!C16</f>
-        <v>1908</v>
-      </c>
-      <c r="D24" s="4">
+        <v>1467</v>
+      </c>
+      <c r="D24" s="16">
         <f>SS_survey_uncond!E16</f>
-        <v>2711</v>
-      </c>
-      <c r="E24" s="4"/>
-      <c r="F24" s="4"/>
-      <c r="G24" s="4">
+        <v>1982</v>
+      </c>
+      <c r="E24" s="16"/>
+      <c r="F24" s="16"/>
+      <c r="G24" s="16">
         <f>SS_survey_uncond!D16</f>
-        <v>1756</v>
-      </c>
-      <c r="H24" s="4">
+        <v>1176</v>
+      </c>
+      <c r="H24" s="16">
         <f>SS_survey_uncond!F16</f>
-        <v>2218</v>
-      </c>
-      <c r="I24" s="4"/>
-    </row>
-    <row r="25" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A25" s="2"/>
-      <c r="B25" s="17" t="s">
-        <v>20</v>
-      </c>
-      <c r="C25" s="17"/>
-      <c r="D25" s="17"/>
-      <c r="E25" s="17"/>
-      <c r="F25" s="17"/>
-      <c r="G25" s="17"/>
-      <c r="H25" s="17"/>
-      <c r="I25" s="17"/>
-    </row>
-    <row r="26" spans="1:9" ht="15" thickTop="1" x14ac:dyDescent="0.35">
-      <c r="A26" s="10" t="s">
-        <v>6</v>
-      </c>
-      <c r="B26" s="11">
-        <f>ROUND(SS_survey!B2,2)</f>
-        <v>0.76</v>
-      </c>
-      <c r="C26" s="11">
-        <f>ROUND(SS_survey!C2,2)</f>
-        <v>0.72</v>
-      </c>
-      <c r="D26" s="11">
-        <f>ROUND(SS_survey!E2,2)</f>
-        <v>0.72</v>
-      </c>
-      <c r="E26" s="11">
-        <f>ROUND(SS_survey!J2,2)</f>
-        <v>0.18</v>
-      </c>
-      <c r="F26" s="11"/>
-      <c r="G26" s="11">
-        <f>ROUND(SS_survey!D2,2)</f>
-        <v>0.73</v>
-      </c>
-      <c r="H26" s="11">
-        <f>ROUND(SS_survey!F2,2)</f>
-        <v>0.74</v>
-      </c>
-      <c r="I26" s="11">
-        <f>ROUND(SS_survey!K2,2)</f>
-        <v>0.47</v>
-      </c>
-    </row>
-    <row r="27" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A27" s="10"/>
-      <c r="B27" s="11" t="str">
-        <f>CONCATENATE("(",ROUND(SS_survey!B3,3),")")</f>
-        <v>(0.016)</v>
-      </c>
-      <c r="C27" s="11" t="str">
-        <f>CONCATENATE("(",ROUND(SS_survey!C3,3),")")</f>
-        <v>(0.016)</v>
-      </c>
-      <c r="D27" s="11" t="str">
-        <f>CONCATENATE("(",ROUND(SS_survey!E3,3),")")</f>
-        <v>(0.016)</v>
-      </c>
-      <c r="E27" s="11"/>
-      <c r="F27" s="11"/>
-      <c r="G27" s="11" t="str">
-        <f>CONCATENATE("(",ROUND(SS_survey!D3,3),")")</f>
-        <v>(0.021)</v>
-      </c>
-      <c r="H27" s="11" t="str">
-        <f>CONCATENATE("(",ROUND(SS_survey!F3,3),")")</f>
-        <v>(0.013)</v>
-      </c>
-      <c r="I27" s="11"/>
-    </row>
-    <row r="28" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A28" s="10" t="s">
-        <v>7</v>
-      </c>
-      <c r="B28" s="11">
-        <f>ROUND(SS_survey!B4,2)</f>
-        <v>43.16</v>
-      </c>
-      <c r="C28" s="11" t="str">
-        <f>CONCATENATE("(",ROUND(SS_survey!C4,3),")")</f>
-        <v>(43.175)</v>
-      </c>
-      <c r="D28" s="11" t="str">
-        <f>CONCATENATE("(",ROUND(SS_survey!E4,3),")")</f>
-        <v>(43.963)</v>
-      </c>
-      <c r="E28" s="11">
-        <f>ROUND(SS_survey!J4,2)</f>
-        <v>0.57999999999999996</v>
-      </c>
-      <c r="F28" s="11"/>
-      <c r="G28" s="11" t="str">
-        <f>CONCATENATE("(",ROUND(SS_survey!D4,3),")")</f>
-        <v>(42.96)</v>
-      </c>
-      <c r="H28" s="11" t="str">
-        <f>CONCATENATE("(",ROUND(SS_survey!F4,3),")")</f>
-        <v>(43.072)</v>
-      </c>
-      <c r="I28" s="11">
-        <f>ROUND(SS_survey!K4,2)</f>
-        <v>0.97</v>
-      </c>
-    </row>
-    <row r="29" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A29" s="10"/>
-      <c r="B29" s="11" t="str">
-        <f>CONCATENATE("(",ROUND(SS_survey!B5,3),")")</f>
-        <v>(0.573)</v>
-      </c>
-      <c r="C29" s="11" t="str">
-        <f>CONCATENATE("(",ROUND(SS_survey!C5,3),")")</f>
-        <v>(0.787)</v>
-      </c>
-      <c r="D29" s="11" t="str">
-        <f>CONCATENATE("(",ROUND(SS_survey!E5,3),")")</f>
-        <v>(0.613)</v>
-      </c>
-      <c r="E29" s="11"/>
-      <c r="F29" s="11"/>
-      <c r="G29" s="11" t="str">
-        <f>CONCATENATE("(",ROUND(SS_survey!D5,3),")")</f>
-        <v>(0.652)</v>
-      </c>
-      <c r="H29" s="11" t="str">
-        <f>CONCATENATE("(",ROUND(SS_survey!F5,3),")")</f>
-        <v>(0.518)</v>
-      </c>
-      <c r="I29" s="11"/>
-    </row>
-    <row r="30" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A30" s="10" t="s">
-        <v>8</v>
-      </c>
-      <c r="B30" s="11">
-        <f>ROUND(SS_survey!B6,0)</f>
-        <v>3152</v>
-      </c>
-      <c r="C30" s="11">
-        <f>ROUND(SS_survey!C6,0)</f>
-        <v>2978</v>
-      </c>
-      <c r="D30" s="11">
-        <f>ROUND(SS_survey!E6,0)</f>
-        <v>3115</v>
-      </c>
-      <c r="E30" s="11">
-        <f>ROUND(SS_survey!J6,2)</f>
-        <v>0.3</v>
-      </c>
-      <c r="F30" s="11"/>
-      <c r="G30" s="11">
-        <f>ROUND(SS_survey!D6,0)</f>
-        <v>2988</v>
-      </c>
-      <c r="H30" s="11">
-        <f>ROUND(SS_survey!F6,0)</f>
-        <v>3081</v>
-      </c>
-      <c r="I30" s="11">
-        <f>ROUND(SS_survey!K6,2)</f>
-        <v>0.27</v>
-      </c>
-    </row>
-    <row r="31" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A31" s="10"/>
-      <c r="B31" s="11" t="str">
-        <f>CONCATENATE("(",ROUND(SS_survey!B7,0),")")</f>
-        <v>(69)</v>
-      </c>
-      <c r="C31" s="11" t="str">
-        <f>CONCATENATE("(",ROUND(SS_survey!C7,0),")")</f>
-        <v>(91)</v>
-      </c>
-      <c r="D31" s="11" t="str">
-        <f>CONCATENATE("(",ROUND(SS_survey!E7,0),")")</f>
-        <v>(85)</v>
-      </c>
-      <c r="E31" s="11"/>
-      <c r="F31" s="11"/>
-      <c r="G31" s="11" t="str">
-        <f>CONCATENATE("(",ROUND(SS_survey!D7,0),")")</f>
-        <v>(76)</v>
-      </c>
-      <c r="H31" s="11" t="str">
-        <f>CONCATENATE("(",ROUND(SS_survey!F7,0),")")</f>
-        <v>(99)</v>
-      </c>
-      <c r="I31" s="11"/>
-    </row>
-    <row r="32" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A32" s="10" t="s">
-        <v>9</v>
-      </c>
-      <c r="B32" s="11">
-        <f>ROUND(SS_survey!B8,2)</f>
-        <v>0.89</v>
-      </c>
-      <c r="C32" s="11">
-        <f>ROUND(SS_survey!C8,2)</f>
-        <v>0.9</v>
-      </c>
-      <c r="D32" s="11">
-        <f>ROUND(SS_survey!E8,2)</f>
-        <v>0.91</v>
-      </c>
-      <c r="E32" s="11">
-        <f>ROUND(SS_survey!J8,2)</f>
-        <v>0.42</v>
-      </c>
-      <c r="F32" s="11"/>
-      <c r="G32" s="11">
-        <f>ROUND(SS_survey!D8,2)</f>
-        <v>0.89</v>
-      </c>
-      <c r="H32" s="11">
-        <f>ROUND(SS_survey!F8,2)</f>
-        <v>0.89</v>
-      </c>
-      <c r="I32" s="11">
-        <f>ROUND(SS_survey!K8,2)</f>
-        <v>0.98</v>
-      </c>
-    </row>
-    <row r="33" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A33" s="10"/>
-      <c r="B33" s="11" t="str">
-        <f>CONCATENATE("(",ROUND(SS_survey!B9,3),")")</f>
-        <v>(0.012)</v>
-      </c>
-      <c r="C33" s="11" t="str">
-        <f>CONCATENATE("(",ROUND(SS_survey!C9,3),")")</f>
-        <v>(0.011)</v>
-      </c>
-      <c r="D33" s="11" t="str">
-        <f>CONCATENATE("(",ROUND(SS_survey!E9,3),")")</f>
-        <v>(0.01)</v>
-      </c>
-      <c r="E33" s="11"/>
-      <c r="F33" s="11"/>
-      <c r="G33" s="11" t="str">
-        <f>CONCATENATE("(",ROUND(SS_survey!D9,3),")")</f>
-        <v>(0.014)</v>
-      </c>
-      <c r="H33" s="11" t="str">
-        <f>CONCATENATE("(",ROUND(SS_survey!F9,3),")")</f>
-        <v>(0.01)</v>
-      </c>
-      <c r="I33" s="11"/>
-    </row>
-    <row r="34" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A34" s="10" t="s">
-        <v>10</v>
-      </c>
-      <c r="B34" s="11">
-        <f>ROUND(SS_survey!B10,2)</f>
-        <v>92.74</v>
-      </c>
-      <c r="C34" s="11">
-        <f>ROUND(SS_survey!C10,2)</f>
-        <v>92.16</v>
-      </c>
-      <c r="D34" s="11">
-        <f>ROUND(SS_survey!E10,2)</f>
-        <v>93.67</v>
-      </c>
-      <c r="E34" s="11">
-        <f>ROUND(SS_survey!J10,2)</f>
-        <v>0.21</v>
-      </c>
-      <c r="F34" s="11"/>
-      <c r="G34" s="11">
-        <f>ROUND(SS_survey!D10,2)</f>
-        <v>93.6</v>
-      </c>
-      <c r="H34" s="11">
-        <f>ROUND(SS_survey!F10,2)</f>
-        <v>93.29</v>
-      </c>
-      <c r="I34" s="11">
-        <f>ROUND(SS_survey!K10,2)</f>
-        <v>0.55000000000000004</v>
-      </c>
-    </row>
-    <row r="35" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A35" s="10"/>
-      <c r="B35" s="11" t="str">
-        <f>CONCATENATE("(",ROUND(SS_survey!B11,3),")")</f>
-        <v>(0.553)</v>
-      </c>
-      <c r="C35" s="11" t="str">
-        <f>CONCATENATE("(",ROUND(SS_survey!C11,3),")")</f>
-        <v>(0.857)</v>
-      </c>
-      <c r="D35" s="11" t="str">
-        <f>CONCATENATE("(",ROUND(SS_survey!E11,3),")")</f>
-        <v>(0.471)</v>
-      </c>
-      <c r="E35" s="11"/>
-      <c r="F35" s="11"/>
-      <c r="G35" s="11" t="str">
-        <f>CONCATENATE("(",ROUND(SS_survey!D11,3),")")</f>
-        <v>(0.596)</v>
-      </c>
-      <c r="H35" s="11" t="str">
-        <f>CONCATENATE("(",ROUND(SS_survey!F11,3),")")</f>
-        <v>(0.599)</v>
-      </c>
-      <c r="I35" s="11"/>
-    </row>
-    <row r="36" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A36" s="10" t="s">
-        <v>11</v>
-      </c>
-      <c r="B36" s="11">
-        <f>ROUND(SS_survey!B12,2)</f>
-        <v>0.66</v>
-      </c>
-      <c r="C36" s="11">
-        <f>ROUND(SS_survey!C12,2)</f>
-        <v>0.67</v>
-      </c>
-      <c r="D36" s="11">
-        <f>ROUND(SS_survey!E12,2)</f>
-        <v>0.67</v>
-      </c>
-      <c r="E36" s="11">
-        <f>ROUND(SS_survey!J12,2)</f>
-        <v>0.91</v>
-      </c>
-      <c r="F36" s="11"/>
-      <c r="G36" s="11">
-        <f>ROUND(SS_survey!D12,2)</f>
-        <v>0.65</v>
-      </c>
-      <c r="H36" s="11">
-        <f>ROUND(SS_survey!F12,2)</f>
-        <v>0.64</v>
-      </c>
-      <c r="I36" s="11">
-        <f>ROUND(SS_survey!K12,2)</f>
-        <v>0.75</v>
-      </c>
-    </row>
-    <row r="37" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A37" s="10"/>
-      <c r="B37" s="11" t="str">
-        <f>CONCATENATE("(",ROUND(SS_survey!B13,3),")")</f>
-        <v>(0.019)</v>
-      </c>
-      <c r="C37" s="11" t="str">
-        <f>CONCATENATE("(",ROUND(SS_survey!C13,3),")")</f>
-        <v>(0.019)</v>
-      </c>
-      <c r="D37" s="11" t="str">
-        <f>CONCATENATE("(",ROUND(SS_survey!E13,3),")")</f>
-        <v>(0.016)</v>
-      </c>
-      <c r="E37" s="11"/>
-      <c r="F37" s="11"/>
-      <c r="G37" s="11" t="str">
-        <f>CONCATENATE("(",ROUND(SS_survey!D13,3),")")</f>
-        <v>(0.024)</v>
-      </c>
-      <c r="H37" s="11" t="str">
-        <f>CONCATENATE("(",ROUND(SS_survey!F13,3),")")</f>
-        <v>(0.016)</v>
-      </c>
-      <c r="I37" s="11"/>
-    </row>
-    <row r="38" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A38" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="B38" s="9">
-        <f>SS_survey!B16</f>
-        <v>2000</v>
-      </c>
-      <c r="C38" s="9">
-        <f>SS_survey!C16</f>
-        <v>1855</v>
-      </c>
-      <c r="D38" s="9">
-        <f>SS_survey!E16</f>
-        <v>2652</v>
-      </c>
-      <c r="E38" s="9"/>
-      <c r="F38" s="9"/>
-      <c r="G38" s="9">
-        <f>SS_survey!D16</f>
-        <v>1733</v>
-      </c>
-      <c r="H38" s="9">
-        <f>SS_survey!F16</f>
-        <v>2193</v>
-      </c>
-      <c r="I38" s="9"/>
-    </row>
-    <row r="39" spans="1:9" ht="15" thickTop="1" x14ac:dyDescent="0.35"/>
+        <v>1534</v>
+      </c>
+      <c r="I24" s="16"/>
+    </row>
+    <row r="25" spans="1:9" ht="15" thickTop="1" x14ac:dyDescent="0.35"/>
   </sheetData>
-  <mergeCells count="6">
+  <mergeCells count="5">
     <mergeCell ref="B2:I2"/>
     <mergeCell ref="B11:I11"/>
-    <mergeCell ref="B25:I25"/>
     <mergeCell ref="B5:I5"/>
     <mergeCell ref="C3:E3"/>
     <mergeCell ref="G3:I3"/>
@@ -2689,10 +2279,10 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{754403B8-1DA5-4CBA-B8B6-94BFF0A849DB}">
-  <dimension ref="A1:K13"/>
+  <dimension ref="A1:K11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A4" sqref="A4:I12"/>
+      <selection activeCell="M18" sqref="M18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -2736,31 +2326,31 @@
     </row>
     <row r="3" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A3" s="15"/>
-      <c r="B3" s="16"/>
-      <c r="C3" s="16"/>
-      <c r="D3" s="16"/>
-      <c r="E3" s="16"/>
-      <c r="F3" s="16"/>
-      <c r="G3" s="16"/>
-      <c r="H3" s="16"/>
-      <c r="I3" s="16"/>
+      <c r="B3" s="17"/>
+      <c r="C3" s="17"/>
+      <c r="D3" s="17"/>
+      <c r="E3" s="17"/>
+      <c r="F3" s="17"/>
+      <c r="G3" s="17"/>
+      <c r="H3" s="17"/>
+      <c r="I3" s="17"/>
       <c r="J3" s="10"/>
       <c r="K3" s="10"/>
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A4" s="10"/>
       <c r="B4" s="11"/>
-      <c r="C4" s="18" t="s">
-        <v>19</v>
-      </c>
-      <c r="D4" s="18"/>
-      <c r="E4" s="18"/>
+      <c r="C4" s="19" t="s">
+        <v>18</v>
+      </c>
+      <c r="D4" s="19"/>
+      <c r="E4" s="19"/>
       <c r="F4" s="11"/>
-      <c r="G4" s="18" t="s">
-        <v>18</v>
-      </c>
-      <c r="H4" s="18"/>
-      <c r="I4" s="18"/>
+      <c r="G4" s="19" t="s">
+        <v>17</v>
+      </c>
+      <c r="H4" s="19"/>
+      <c r="I4" s="19"/>
       <c r="J4" s="10"/>
       <c r="K4" s="10"/>
     </row>
@@ -2793,7 +2383,7 @@
     </row>
     <row r="6" spans="1:11" ht="15" thickTop="1" x14ac:dyDescent="0.35">
       <c r="A6" s="10" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B6" s="11">
         <f>ROUND(SS_att!B2,0)</f>
@@ -2801,20 +2391,20 @@
       </c>
       <c r="C6" s="11">
         <f>ROUND(SS_att!C2,0)</f>
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="D6" s="11">
         <f>ROUND(SS_att!E2,0)</f>
-        <v>37</v>
+        <v>40</v>
       </c>
       <c r="E6" s="11">
         <f>ROUND(SS_att!L2,2)</f>
-        <v>0.16</v>
+        <v>0.14000000000000001</v>
       </c>
       <c r="F6" s="11"/>
       <c r="G6" s="11">
         <f>ROUND(SS_att!D2,0)</f>
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="H6" s="11">
         <f>ROUND(SS_att!F2,0)</f>
@@ -2822,7 +2412,7 @@
       </c>
       <c r="I6" s="11">
         <f>ROUND(SS_att!M2,2)</f>
-        <v>0.56999999999999995</v>
+        <v>0.76</v>
       </c>
       <c r="J6" s="10"/>
       <c r="K6" s="10"/>
@@ -2831,25 +2421,25 @@
       <c r="A7" s="10"/>
       <c r="B7" s="11" t="str">
         <f>CONCATENATE("(",ROUND(SS_att!B3,1),")")</f>
-        <v>(2.2)</v>
+        <v>(3)</v>
       </c>
       <c r="C7" s="11" t="str">
         <f>CONCATENATE("(",ROUND(SS_att!C3,1),")")</f>
-        <v>(2.3)</v>
+        <v>(2.7)</v>
       </c>
       <c r="D7" s="11" t="str">
         <f>CONCATENATE("(",ROUND(SS_att!E3,1),")")</f>
-        <v>(2.6)</v>
+        <v>(3.3)</v>
       </c>
       <c r="E7" s="11"/>
       <c r="F7" s="11"/>
       <c r="G7" s="11" t="str">
         <f>CONCATENATE("(",ROUND(SS_att!D3,1),")")</f>
-        <v>(2.4)</v>
+        <v>(3.2)</v>
       </c>
       <c r="H7" s="11" t="str">
         <f>CONCATENATE("(",ROUND(SS_att!F3,1),")")</f>
-        <v>(1.8)</v>
+        <v>(2.2)</v>
       </c>
       <c r="I7" s="11"/>
       <c r="J7" s="10"/>
@@ -2857,11 +2447,11 @@
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B8" s="3">
         <f>ROUND(SS_att!B10,2)</f>
-        <v>0.77</v>
+        <v>0.78</v>
       </c>
       <c r="C8" s="3">
         <f>ROUND(SS_att!C10,2)</f>
@@ -2873,7 +2463,7 @@
       </c>
       <c r="E8" s="3">
         <f>ROUND(SS_att!L10,2)</f>
-        <v>0.74</v>
+        <v>0.59</v>
       </c>
       <c r="G8" s="3">
         <f>ROUND(SS_att!D10,2)</f>
@@ -2881,11 +2471,11 @@
       </c>
       <c r="H8" s="3">
         <f>ROUND(SS_att!F10,2)</f>
-        <v>0.79</v>
+        <v>0.81</v>
       </c>
       <c r="I8" s="3">
         <f>ROUND(SS_att!M10,2)</f>
-        <v>0.5</v>
+        <v>0.69</v>
       </c>
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.35">
@@ -2899,101 +2489,46 @@
       </c>
       <c r="D9" s="3" t="str">
         <f>CONCATENATE("(",ROUND(SS_att!E11,2),")")</f>
-        <v>(0.02)</v>
+        <v>(0.03)</v>
       </c>
       <c r="G9" s="3" t="str">
         <f>CONCATENATE("(",ROUND(SS_att!D11,2),")")</f>
-        <v>(0.02)</v>
+        <v>(0.03)</v>
       </c>
       <c r="H9" s="3" t="str">
         <f>CONCATENATE("(",ROUND(SS_att!F11,2),")")</f>
         <v>(0.02)</v>
       </c>
     </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A10" t="s">
-        <v>14</v>
-      </c>
-      <c r="B10" s="3">
-        <f>ROUND(SS_att!B8,2)</f>
-        <v>0.98</v>
-      </c>
-      <c r="C10" s="3">
-        <f>ROUND(SS_att!C8,2)</f>
-        <v>0.97</v>
-      </c>
-      <c r="D10" s="3">
-        <f>ROUND(SS_att!E8,2)</f>
-        <v>0.98</v>
-      </c>
-      <c r="E10" s="3">
-        <f>ROUND(SS_att!L8,2)</f>
-        <v>0.43</v>
-      </c>
-      <c r="G10" s="3">
-        <f>ROUND(SS_att!D8,2)</f>
-        <v>0.99</v>
-      </c>
-      <c r="H10" s="3">
-        <f>ROUND(SS_att!F8,2)</f>
-        <v>0.99</v>
-      </c>
-      <c r="I10" s="3">
-        <f>ROUND(SS_att!M8,2)</f>
-        <v>0.49</v>
-      </c>
-    </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="B11" s="3" t="str">
-        <f>CONCATENATE("(",ROUND(SS_att!B9,3),")")</f>
-        <v>(0.004)</v>
-      </c>
-      <c r="C11" s="3" t="str">
-        <f>CONCATENATE("(",ROUND(SS_att!C9,3),")")</f>
-        <v>(0.007)</v>
-      </c>
-      <c r="D11" s="3" t="str">
-        <f>CONCATENATE("(",ROUND(SS_att!E9,3),")")</f>
-        <v>(0.006)</v>
-      </c>
-      <c r="G11" s="3" t="str">
-        <f>CONCATENATE("(",ROUND(SS_att!D9,3),")")</f>
-        <v>(0.003)</v>
-      </c>
-      <c r="H11" s="3" t="str">
-        <f>CONCATENATE("(",ROUND(SS_att!F9,3),")")</f>
-        <v>(0.003)</v>
-      </c>
-    </row>
-    <row r="12" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A12" s="2" t="s">
+    <row r="10" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A10" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="B12" s="5">
+      <c r="B10" s="5">
         <f>SS_att!B6</f>
-        <v>2600</v>
-      </c>
-      <c r="C12" s="5">
+        <v>1770</v>
+      </c>
+      <c r="C10" s="5">
         <f>SS_att!C6</f>
-        <v>2484</v>
-      </c>
-      <c r="D12" s="5">
+        <v>1954</v>
+      </c>
+      <c r="D10" s="5">
         <f>SS_att!E6</f>
-        <v>3435</v>
-      </c>
-      <c r="E12" s="8"/>
-      <c r="F12" s="9"/>
-      <c r="G12" s="5">
+        <v>2580</v>
+      </c>
+      <c r="E10" s="8"/>
+      <c r="F10" s="9"/>
+      <c r="G10" s="5">
         <f>SS_att!D6</f>
-        <v>2157</v>
-      </c>
-      <c r="H12" s="5">
+        <v>1470</v>
+      </c>
+      <c r="H10" s="5">
         <f>SS_att!F6</f>
-        <v>2768</v>
-      </c>
-      <c r="I12" s="5"/>
-    </row>
-    <row r="13" spans="1:11" ht="15" thickTop="1" x14ac:dyDescent="0.35"/>
+        <v>1904</v>
+      </c>
+      <c r="I10" s="5"/>
+    </row>
+    <row r="11" spans="1:11" ht="15" thickTop="1" x14ac:dyDescent="0.35"/>
   </sheetData>
   <mergeCells count="3">
     <mergeCell ref="B3:I3"/>

</xml_diff>

<commit_message>
tut conditional on survey & results with NA in causal RF
</commit_message>
<xml_diff>
--- a/Tables/SS.xlsx
+++ b/Tables/SS.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26327"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26529"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\isaac\Dropbox\Apps\Overleaf\Donde2022\Tables\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F16C3369-17AB-4E0F-A517-9F0EEFC252FF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{81E3DE23-7774-481C-8739-DC27504D8DD5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-22815" yWindow="-16320" windowWidth="29040" windowHeight="15720" firstSheet="1" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-22395" yWindow="3615" windowWidth="21600" windowHeight="11175" firstSheet="2" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="SS_admin" sheetId="1" r:id="rId1"/>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="28">
   <si>
     <t>Choice</t>
   </si>
@@ -90,9 +90,6 @@
     <t>Panel B : Survey Data</t>
   </si>
   <si>
-    <t>Income index</t>
-  </si>
-  <si>
     <t>Present bias</t>
   </si>
   <si>
@@ -133,7 +130,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="1">
     <font>
       <sz val="11"/>
       <name val="Calibri"/>
@@ -565,9 +562,9 @@
       <selection activeCell="M11" sqref="A1:M11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="2" spans="2:12" x14ac:dyDescent="0.35">
+    <row r="2" spans="2:12">
       <c r="B2">
         <v>2267.4576271186438</v>
       </c>
@@ -584,7 +581,7 @@
         <v>0.64503108323202074</v>
       </c>
     </row>
-    <row r="3" spans="2:12" x14ac:dyDescent="0.35">
+    <row r="3" spans="2:12">
       <c r="B3">
         <v>75.874088260545236</v>
       </c>
@@ -598,7 +595,7 @@
         <v>42.936615450474939</v>
       </c>
     </row>
-    <row r="4" spans="2:12" x14ac:dyDescent="0.35">
+    <row r="4" spans="2:12">
       <c r="B4">
         <v>0.87966101694915255</v>
       </c>
@@ -615,7 +612,7 @@
         <v>0.56027324425210501</v>
       </c>
     </row>
-    <row r="5" spans="2:12" x14ac:dyDescent="0.35">
+    <row r="5" spans="2:12">
       <c r="B5">
         <v>4.3632089264598002E-2</v>
       </c>
@@ -629,7 +626,7 @@
         <v>2.5577577893366659E-2</v>
       </c>
     </row>
-    <row r="6" spans="2:12" x14ac:dyDescent="0.35">
+    <row r="6" spans="2:12">
       <c r="B6">
         <v>1770</v>
       </c>
@@ -656,9 +653,9 @@
       <selection activeCell="P21" sqref="A1:P21"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="2" spans="2:12" x14ac:dyDescent="0.35">
+    <row r="2" spans="2:12">
       <c r="B2">
         <v>34.385964912280699</v>
       </c>
@@ -675,7 +672,7 @@
         <v>0.51863884752020373</v>
       </c>
     </row>
-    <row r="3" spans="2:12" x14ac:dyDescent="0.35">
+    <row r="3" spans="2:12">
       <c r="B3">
         <v>3.0011228460479158</v>
       </c>
@@ -689,7 +686,7 @@
         <v>1.8380690486041</v>
       </c>
     </row>
-    <row r="4" spans="2:12" x14ac:dyDescent="0.35">
+    <row r="4" spans="2:12">
       <c r="B4">
         <v>1770</v>
       </c>
@@ -703,7 +700,7 @@
         <v>6304</v>
       </c>
     </row>
-    <row r="8" spans="2:12" x14ac:dyDescent="0.35">
+    <row r="8" spans="2:12">
       <c r="B8">
         <v>0.97536945812807885</v>
       </c>
@@ -720,7 +717,7 @@
         <v>0.61894128114173319</v>
       </c>
     </row>
-    <row r="9" spans="2:12" x14ac:dyDescent="0.35">
+    <row r="9" spans="2:12">
       <c r="B9">
         <v>5.5641049658199894E-3</v>
       </c>
@@ -734,7 +731,7 @@
         <v>4.4762159277795602E-3</v>
       </c>
     </row>
-    <row r="10" spans="2:12" x14ac:dyDescent="0.35">
+    <row r="10" spans="2:12">
       <c r="B10">
         <v>0.78725761772853187</v>
       </c>
@@ -751,7 +748,7 @@
         <v>0.61700341260717884</v>
       </c>
     </row>
-    <row r="11" spans="2:12" x14ac:dyDescent="0.35">
+    <row r="11" spans="2:12">
       <c r="B11">
         <v>1.787061830945753E-2</v>
       </c>
@@ -778,9 +775,9 @@
       <selection activeCell="N31" sqref="B1:N31"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="2" spans="2:12" x14ac:dyDescent="0.35">
+    <row r="2" spans="2:12">
       <c r="B2">
         <v>4084.044748373869</v>
       </c>
@@ -797,7 +794,7 @@
         <v>0.50741363647763404</v>
       </c>
     </row>
-    <row r="3" spans="2:12" x14ac:dyDescent="0.35">
+    <row r="3" spans="2:12">
       <c r="B3">
         <v>186.32530822216469</v>
       </c>
@@ -811,7 +808,7 @@
         <v>106.6210974172742</v>
       </c>
     </row>
-    <row r="4" spans="2:12" x14ac:dyDescent="0.35">
+    <row r="4" spans="2:12">
       <c r="B4">
         <v>0.1870631315668515</v>
       </c>
@@ -828,7 +825,7 @@
         <v>0.67256604845929213</v>
       </c>
     </row>
-    <row r="5" spans="2:12" x14ac:dyDescent="0.35">
+    <row r="5" spans="2:12">
       <c r="B5">
         <v>2.4433091346626679E-2</v>
       </c>
@@ -842,7 +839,7 @@
         <v>1.2895102797403321E-2</v>
       </c>
     </row>
-    <row r="6" spans="2:12" x14ac:dyDescent="0.35">
+    <row r="6" spans="2:12">
       <c r="B6">
         <v>0.13815789473684209</v>
       </c>
@@ -859,7 +856,7 @@
         <v>0.88964950426016531</v>
       </c>
     </row>
-    <row r="7" spans="2:12" x14ac:dyDescent="0.35">
+    <row r="7" spans="2:12">
       <c r="B7">
         <v>2.0646396595072281E-2</v>
       </c>
@@ -873,7 +870,7 @@
         <v>9.0357611917287195E-3</v>
       </c>
     </row>
-    <row r="8" spans="2:12" x14ac:dyDescent="0.35">
+    <row r="8" spans="2:12">
       <c r="B8">
         <v>0.62474437627811863</v>
       </c>
@@ -890,7 +887,7 @@
         <v>0.29259959707503702</v>
       </c>
     </row>
-    <row r="9" spans="2:12" x14ac:dyDescent="0.35">
+    <row r="9" spans="2:12">
       <c r="B9">
         <v>2.8080273403161181E-2</v>
       </c>
@@ -904,7 +901,7 @@
         <v>1.6701632404580391E-2</v>
       </c>
     </row>
-    <row r="10" spans="2:12" x14ac:dyDescent="0.35">
+    <row r="10" spans="2:12">
       <c r="B10">
         <v>91.886692015209121</v>
       </c>
@@ -921,7 +918,7 @@
         <v>9.3375432500356903E-2</v>
       </c>
     </row>
-    <row r="11" spans="2:12" x14ac:dyDescent="0.35">
+    <row r="11" spans="2:12">
       <c r="B11">
         <v>0.72142723064601477</v>
       </c>
@@ -935,7 +932,7 @@
         <v>0.4502856911185264</v>
       </c>
     </row>
-    <row r="12" spans="2:12" x14ac:dyDescent="0.35">
+    <row r="12" spans="2:12">
       <c r="B12">
         <v>0.8693877551020408</v>
       </c>
@@ -952,7 +949,7 @@
         <v>0.2521838227756053</v>
       </c>
     </row>
-    <row r="13" spans="2:12" x14ac:dyDescent="0.35">
+    <row r="13" spans="2:12">
       <c r="B13">
         <v>1.5429549670760771E-2</v>
       </c>
@@ -966,7 +963,7 @@
         <v>7.5100652933181586E-3</v>
       </c>
     </row>
-    <row r="14" spans="2:12" x14ac:dyDescent="0.35">
+    <row r="14" spans="2:12">
       <c r="B14">
         <v>43.316996871741402</v>
       </c>
@@ -983,7 +980,7 @@
         <v>0.72947420733682788</v>
       </c>
     </row>
-    <row r="15" spans="2:12" x14ac:dyDescent="0.35">
+    <row r="15" spans="2:12">
       <c r="B15">
         <v>0.68765705993205639</v>
       </c>
@@ -997,7 +994,7 @@
         <v>0.47585898339836669</v>
       </c>
     </row>
-    <row r="16" spans="2:12" x14ac:dyDescent="0.35">
+    <row r="16" spans="2:12">
       <c r="B16">
         <v>0.7275390625</v>
       </c>
@@ -1014,7 +1011,7 @@
         <v>0.87880547636069528</v>
       </c>
     </row>
-    <row r="17" spans="2:12" x14ac:dyDescent="0.35">
+    <row r="17" spans="2:12">
       <c r="B17">
         <v>2.2722829871839111E-2</v>
       </c>
@@ -1028,7 +1025,7 @@
         <v>1.1899628511819889E-2</v>
       </c>
     </row>
-    <row r="18" spans="2:12" x14ac:dyDescent="0.35">
+    <row r="18" spans="2:12">
       <c r="B18">
         <v>0.65861344537815125</v>
       </c>
@@ -1045,7 +1042,7 @@
         <v>0.83627432511379829</v>
       </c>
     </row>
-    <row r="19" spans="2:12" x14ac:dyDescent="0.35">
+    <row r="19" spans="2:12">
       <c r="B19">
         <v>2.7084494536168069E-2</v>
       </c>
@@ -1059,7 +1056,7 @@
         <v>1.264015748271608E-2</v>
       </c>
     </row>
-    <row r="20" spans="2:12" x14ac:dyDescent="0.35">
+    <row r="20" spans="2:12">
       <c r="B20">
         <v>1770</v>
       </c>
@@ -1073,7 +1070,7 @@
         <v>6304</v>
       </c>
     </row>
-    <row r="23" spans="2:12" x14ac:dyDescent="0.35">
+    <row r="23" spans="2:12">
       <c r="B23">
         <v>1386</v>
       </c>
@@ -1097,9 +1094,9 @@
       <selection activeCell="L3" sqref="L3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="2" spans="2:12" x14ac:dyDescent="0.35">
+    <row r="2" spans="2:12">
       <c r="B2">
         <v>2199.2352092352089</v>
       </c>
@@ -1116,7 +1113,7 @@
         <v>0.98415991070079034</v>
       </c>
     </row>
-    <row r="3" spans="2:12" x14ac:dyDescent="0.35">
+    <row r="3" spans="2:12">
       <c r="B3">
         <v>85.691617474481063</v>
       </c>
@@ -1130,7 +1127,7 @@
         <v>51.996675747123149</v>
       </c>
     </row>
-    <row r="4" spans="2:12" x14ac:dyDescent="0.35">
+    <row r="4" spans="2:12">
       <c r="B4">
         <v>0.87590187590187585</v>
       </c>
@@ -1147,7 +1144,7 @@
         <v>0.80262123234967087</v>
       </c>
     </row>
-    <row r="5" spans="2:12" x14ac:dyDescent="0.35">
+    <row r="5" spans="2:12">
       <c r="B5">
         <v>4.4829425630513037E-2</v>
       </c>
@@ -1161,7 +1158,7 @@
         <v>2.5337910106350281E-2</v>
       </c>
     </row>
-    <row r="6" spans="2:12" x14ac:dyDescent="0.35">
+    <row r="6" spans="2:12">
       <c r="B6">
         <v>1386</v>
       </c>
@@ -1188,14 +1185,14 @@
       <selection activeCell="Q2" sqref="Q2:S11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="17" max="17" width="9.54296875" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="10.453125" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="7.36328125" customWidth="1"/>
+    <col min="17" max="17" width="9.5703125" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="10.42578125" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="7.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:19" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="2" spans="2:19" ht="15.75" thickBot="1">
       <c r="B2">
         <v>0.73333333333333328</v>
       </c>
@@ -1218,16 +1215,16 @@
         <v>33</v>
       </c>
       <c r="Q2" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="R2" s="5" t="s">
         <v>24</v>
       </c>
-      <c r="R2" s="5" t="s">
+      <c r="S2" s="5" t="s">
         <v>25</v>
       </c>
-      <c r="S2" s="5" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="3" spans="2:19" ht="15" thickTop="1" x14ac:dyDescent="0.35">
+    </row>
+    <row r="3" spans="2:19" ht="15.75" thickTop="1">
       <c r="B3">
         <v>2.2227133407258709E-2</v>
       </c>
@@ -1258,7 +1255,7 @@
         <v>4.6399999999999997</v>
       </c>
     </row>
-    <row r="4" spans="2:19" x14ac:dyDescent="0.35">
+    <row r="4" spans="2:19">
       <c r="B4">
         <v>0.49265536723163839</v>
       </c>
@@ -1292,7 +1289,7 @@
         <v>28.1</v>
       </c>
     </row>
-    <row r="5" spans="2:19" x14ac:dyDescent="0.35">
+    <row r="5" spans="2:19">
       <c r="B5">
         <v>2.30962400955886E-2</v>
       </c>
@@ -1323,7 +1320,7 @@
         <v>28.85</v>
       </c>
     </row>
-    <row r="6" spans="2:19" x14ac:dyDescent="0.35">
+    <row r="6" spans="2:19">
       <c r="B6">
         <v>0.42937853107344631</v>
       </c>
@@ -1357,7 +1354,7 @@
         <v>30.830000000000002</v>
       </c>
     </row>
-    <row r="7" spans="2:19" x14ac:dyDescent="0.35">
+    <row r="7" spans="2:19">
       <c r="B7">
         <v>2.2539581021475689E-2</v>
       </c>
@@ -1388,7 +1385,7 @@
         <v>32.39</v>
       </c>
     </row>
-    <row r="8" spans="2:19" x14ac:dyDescent="0.35">
+    <row r="8" spans="2:19">
       <c r="B8">
         <v>0.55254237288135588</v>
       </c>
@@ -1422,7 +1419,7 @@
         <v>35.1</v>
       </c>
     </row>
-    <row r="9" spans="2:19" x14ac:dyDescent="0.35">
+    <row r="9" spans="2:19">
       <c r="B9">
         <v>2.3021717142206809E-2</v>
       </c>
@@ -1453,7 +1450,7 @@
         <v>41.34</v>
       </c>
     </row>
-    <row r="10" spans="2:19" x14ac:dyDescent="0.35">
+    <row r="10" spans="2:19">
       <c r="B10">
         <v>0.74293785310734461</v>
       </c>
@@ -1487,7 +1484,7 @@
         <v>56.49</v>
       </c>
     </row>
-    <row r="11" spans="2:19" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="11" spans="2:19" ht="15.75" thickBot="1">
       <c r="B11">
         <v>2.3824936806509319E-2</v>
       </c>
@@ -1518,7 +1515,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="12" spans="2:19" ht="15" thickTop="1" x14ac:dyDescent="0.35">
+    <row r="12" spans="2:19" ht="15.75" thickTop="1">
       <c r="B12">
         <v>0.5536723163841808</v>
       </c>
@@ -1535,7 +1532,7 @@
         <v>0.56579109636169034</v>
       </c>
     </row>
-    <row r="13" spans="2:19" x14ac:dyDescent="0.35">
+    <row r="13" spans="2:19">
       <c r="B13">
         <v>2.3197736740832291E-2</v>
       </c>
@@ -1549,7 +1546,7 @@
         <v>1.2812478832268839E-2</v>
       </c>
     </row>
-    <row r="14" spans="2:19" x14ac:dyDescent="0.35">
+    <row r="14" spans="2:19">
       <c r="B14">
         <v>0.54180790960451974</v>
       </c>
@@ -1566,7 +1563,7 @@
         <v>0.59041645057610981</v>
       </c>
     </row>
-    <row r="15" spans="2:19" x14ac:dyDescent="0.35">
+    <row r="15" spans="2:19">
       <c r="B15">
         <v>2.3028825848404249E-2</v>
       </c>
@@ -1580,7 +1577,7 @@
         <v>1.215151264408409E-2</v>
       </c>
     </row>
-    <row r="16" spans="2:19" x14ac:dyDescent="0.35">
+    <row r="16" spans="2:19">
       <c r="B16">
         <v>0.5785310734463277</v>
       </c>
@@ -1597,7 +1594,7 @@
         <v>0.93267269990982249</v>
       </c>
     </row>
-    <row r="17" spans="2:12" x14ac:dyDescent="0.35">
+    <row r="17" spans="2:12">
       <c r="B17">
         <v>2.4804932440873621E-2</v>
       </c>
@@ -1611,7 +1608,7 @@
         <v>1.316677672471577E-2</v>
       </c>
     </row>
-    <row r="18" spans="2:12" x14ac:dyDescent="0.35">
+    <row r="18" spans="2:12">
       <c r="B18">
         <v>0.53785310734463276</v>
       </c>
@@ -1628,7 +1625,7 @@
         <v>0.38649070048922801</v>
       </c>
     </row>
-    <row r="19" spans="2:12" x14ac:dyDescent="0.35">
+    <row r="19" spans="2:12">
       <c r="B19">
         <v>2.497582090269404E-2</v>
       </c>
@@ -1642,7 +1639,7 @@
         <v>1.314890352713889E-2</v>
       </c>
     </row>
-    <row r="20" spans="2:12" x14ac:dyDescent="0.35">
+    <row r="20" spans="2:12">
       <c r="B20">
         <v>1770</v>
       </c>
@@ -1665,34 +1662,34 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{67FF63D4-14D6-4F54-BD0D-751B1AD5E68C}">
   <dimension ref="A2:E31"/>
   <sheetViews>
-    <sheetView topLeftCell="A8" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
       <selection activeCell="A3" sqref="A3:E30"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="18.1796875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="9.7265625" style="3" customWidth="1"/>
-    <col min="3" max="3" width="10.54296875" style="3" customWidth="1"/>
-    <col min="4" max="4" width="7.54296875" style="3" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="7.54296875" style="3" customWidth="1"/>
+    <col min="1" max="1" width="18.140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="9.7109375" style="3" customWidth="1"/>
+    <col min="3" max="3" width="10.5703125" style="3" customWidth="1"/>
+    <col min="4" max="4" width="7.5703125" style="3" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="7.5703125" style="3" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="2" spans="1:5" ht="15.75" thickBot="1">
       <c r="A2" s="10"/>
       <c r="B2" s="13"/>
       <c r="C2" s="13"/>
       <c r="D2" s="13"/>
       <c r="E2" s="13"/>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:5">
       <c r="C3" s="14" t="s">
         <v>14</v>
       </c>
       <c r="D3" s="14"/>
       <c r="E3" s="14"/>
     </row>
-    <row r="4" spans="1:5" s="6" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:5" s="6" customFormat="1" ht="30">
       <c r="B4" s="8" t="s">
         <v>1</v>
       </c>
@@ -1706,16 +1703,16 @@
         <v>2</v>
       </c>
     </row>
-    <row r="5" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="5" spans="1:5" ht="15.75" thickBot="1">
       <c r="A5" s="2"/>
       <c r="B5" s="15" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C5" s="15"/>
       <c r="D5" s="15"/>
       <c r="E5" s="15"/>
     </row>
-    <row r="6" spans="1:5" ht="15" thickTop="1" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:5" ht="15.75" thickTop="1">
       <c r="A6" t="s">
         <v>4</v>
       </c>
@@ -1736,7 +1733,7 @@
         <v>0.98</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:5">
       <c r="B7" s="3" t="str">
         <f>CONCATENATE("(",ROUND(SS_admin_survey!B3,0),")")</f>
         <v>(86)</v>
@@ -1750,7 +1747,7 @@
         <v>(81)</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:5">
       <c r="A8" t="s">
         <v>13</v>
       </c>
@@ -1771,7 +1768,7 @@
         <v>0.8</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:5">
       <c r="B9" s="3" t="str">
         <f>CONCATENATE("(",ROUND(SS_admin_survey!B5,3),")")</f>
         <v>(0.045)</v>
@@ -1785,7 +1782,7 @@
         <v>(0.045)</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:5">
       <c r="A10" s="1" t="s">
         <v>5</v>
       </c>
@@ -1803,16 +1800,16 @@
       </c>
       <c r="E10" s="4"/>
     </row>
-    <row r="11" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="11" spans="1:5" ht="15.75" thickBot="1">
       <c r="A11" s="2"/>
       <c r="B11" s="15" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C11" s="15"/>
       <c r="D11" s="15"/>
       <c r="E11" s="15"/>
     </row>
-    <row r="12" spans="1:5" ht="15" thickTop="1" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:5" ht="15.75" thickTop="1">
       <c r="A12" t="s">
         <v>8</v>
       </c>
@@ -1833,7 +1830,7 @@
         <v>0.39</v>
       </c>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:5">
       <c r="B13" s="3" t="str">
         <f>CONCATENATE("(",ROUND(survey_response_rate!B3,3),")")</f>
         <v>(0.022)</v>
@@ -1847,9 +1844,9 @@
         <v>(0.024)</v>
       </c>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:5">
       <c r="A14" t="s">
-        <v>16</v>
+        <v>26</v>
       </c>
       <c r="B14" s="3">
         <f>ROUND(survey_response_rate!B4,2)</f>
@@ -1868,7 +1865,7 @@
         <v>0.28999999999999998</v>
       </c>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:5">
       <c r="B15" s="3" t="str">
         <f>CONCATENATE("(",ROUND(survey_response_rate!B5,3),")")</f>
         <v>(0.023)</v>
@@ -1882,9 +1879,9 @@
         <v>(0.022)</v>
       </c>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:5">
       <c r="A16" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B16" s="3">
         <f>ROUND(survey_response_rate!B6,2)</f>
@@ -1903,7 +1900,7 @@
         <v>0.17</v>
       </c>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:5">
       <c r="B17" s="3" t="str">
         <f>CONCATENATE("(",ROUND(survey_response_rate!B7,2),")")</f>
         <v>(0.02)</v>
@@ -1917,9 +1914,9 @@
         <v>(0.02)</v>
       </c>
     </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:5">
       <c r="A18" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B18" s="3">
         <f>ROUND(survey_response_rate!B8,2)</f>
@@ -1938,7 +1935,7 @@
         <v>0.56000000000000005</v>
       </c>
     </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:5">
       <c r="B19" s="3" t="str">
         <f>CONCATENATE("(",ROUND(survey_response_rate!B9,3),")")</f>
         <v>(0.023)</v>
@@ -1952,7 +1949,7 @@
         <v>(0.019)</v>
       </c>
     </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:5">
       <c r="A20" t="s">
         <v>9</v>
       </c>
@@ -1973,7 +1970,7 @@
         <v>0.71</v>
       </c>
     </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:5">
       <c r="B21" s="3" t="str">
         <f>CONCATENATE("(",ROUND(survey_response_rate!B11,3),")")</f>
         <v>(0.024)</v>
@@ -1987,9 +1984,9 @@
         <v>(0.025)</v>
       </c>
     </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:5">
       <c r="A22" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B22" s="3">
         <f>ROUND(survey_response_rate!B12,2)</f>
@@ -2008,7 +2005,7 @@
         <v>0.56999999999999995</v>
       </c>
     </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:5">
       <c r="B23" s="3" t="str">
         <f>CONCATENATE("(",ROUND(survey_response_rate!B13,3),")")</f>
         <v>(0.023)</v>
@@ -2022,7 +2019,7 @@
         <v>(0.02)</v>
       </c>
     </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:5">
       <c r="A24" t="s">
         <v>7</v>
       </c>
@@ -2043,7 +2040,7 @@
         <v>0.59</v>
       </c>
     </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:5">
       <c r="B25" s="3" t="str">
         <f>CONCATENATE("(",ROUND(survey_response_rate!B15,3),")")</f>
         <v>(0.023)</v>
@@ -2057,7 +2054,7 @@
         <v>(0.018)</v>
       </c>
     </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:5">
       <c r="A26" t="s">
         <v>6</v>
       </c>
@@ -2078,7 +2075,7 @@
         <v>0.93</v>
       </c>
     </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:5">
       <c r="B27" s="3" t="str">
         <f>CONCATENATE("(",ROUND(survey_response_rate!B17,3),")")</f>
         <v>(0.025)</v>
@@ -2092,9 +2089,9 @@
         <v>(0.02)</v>
       </c>
     </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:5">
       <c r="A28" s="11" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B28" s="3">
         <f>ROUND(survey_response_rate!B18,2)</f>
@@ -2113,7 +2110,7 @@
         <v>0.39</v>
       </c>
     </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:5">
       <c r="B29" s="3" t="str">
         <f>CONCATENATE("(",ROUND(survey_response_rate!B19,3),")")</f>
         <v>(0.025)</v>
@@ -2127,7 +2124,7 @@
         <v>(0.019)</v>
       </c>
     </row>
-    <row r="30" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="30" spans="1:5" ht="15.75" thickBot="1">
       <c r="A30" s="2" t="s">
         <v>5</v>
       </c>
@@ -2145,7 +2142,7 @@
       </c>
       <c r="E30" s="5"/>
     </row>
-    <row r="31" spans="1:5" ht="15" thickTop="1" x14ac:dyDescent="0.35"/>
+    <row r="31" spans="1:5" ht="15.75" thickTop="1"/>
   </sheetData>
   <mergeCells count="4">
     <mergeCell ref="B2:E2"/>
@@ -2161,34 +2158,34 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3B054637-0760-4807-B01C-4419EACB0C14}">
   <dimension ref="A2:E31"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
+    <sheetView topLeftCell="A6" workbookViewId="0">
       <selection activeCell="A3" sqref="A3:E30"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="18.1796875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="9.7265625" style="3" customWidth="1"/>
-    <col min="3" max="3" width="10.54296875" style="3" customWidth="1"/>
-    <col min="4" max="4" width="7.54296875" style="3" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="7.54296875" style="3" customWidth="1"/>
+    <col min="1" max="1" width="18.140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="9.7109375" style="3" customWidth="1"/>
+    <col min="3" max="3" width="10.5703125" style="3" customWidth="1"/>
+    <col min="4" max="4" width="7.5703125" style="3" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="7.5703125" style="3" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="2" spans="1:5" ht="15.75" thickBot="1">
       <c r="A2" s="10"/>
       <c r="B2" s="13"/>
       <c r="C2" s="13"/>
       <c r="D2" s="13"/>
       <c r="E2" s="13"/>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:5">
       <c r="C3" s="14" t="s">
         <v>14</v>
       </c>
       <c r="D3" s="14"/>
       <c r="E3" s="14"/>
     </row>
-    <row r="4" spans="1:5" s="6" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:5" s="6" customFormat="1" ht="30">
       <c r="B4" s="8" t="s">
         <v>1</v>
       </c>
@@ -2202,7 +2199,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="5" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="5" spans="1:5" ht="15.75" thickBot="1">
       <c r="A5" s="2"/>
       <c r="B5" s="15" t="s">
         <v>3</v>
@@ -2211,7 +2208,7 @@
       <c r="D5" s="15"/>
       <c r="E5" s="15"/>
     </row>
-    <row r="6" spans="1:5" ht="15" thickTop="1" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:5" ht="15.75" thickTop="1">
       <c r="A6" t="s">
         <v>4</v>
       </c>
@@ -2232,7 +2229,7 @@
         <v>0.65</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:5">
       <c r="B7" s="3" t="str">
         <f>CONCATENATE("(",ROUND(SS_admin!B3,0),")")</f>
         <v>(76)</v>
@@ -2246,7 +2243,7 @@
         <v>(66)</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:5">
       <c r="A8" t="s">
         <v>13</v>
       </c>
@@ -2267,7 +2264,7 @@
         <v>0.56000000000000005</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:5">
       <c r="B9" s="3" t="str">
         <f>CONCATENATE("(",ROUND(SS_admin!B5,3),")")</f>
         <v>(0.044)</v>
@@ -2281,7 +2278,7 @@
         <v>(0.048)</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:5">
       <c r="A10" s="1" t="s">
         <v>5</v>
       </c>
@@ -2299,7 +2296,7 @@
       </c>
       <c r="E10" s="4"/>
     </row>
-    <row r="11" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="11" spans="1:5" ht="15.75" thickBot="1">
       <c r="A11" s="2"/>
       <c r="B11" s="15" t="s">
         <v>15</v>
@@ -2308,7 +2305,7 @@
       <c r="D11" s="15"/>
       <c r="E11" s="15"/>
     </row>
-    <row r="12" spans="1:5" ht="15" thickTop="1" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:5" ht="15.75" thickTop="1">
       <c r="A12" t="s">
         <v>8</v>
       </c>
@@ -2329,7 +2326,7 @@
         <v>0.51</v>
       </c>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:5">
       <c r="B13" s="3" t="str">
         <f>CONCATENATE("(",ROUND(SS_survey!B3,0),")")</f>
         <v>(186)</v>
@@ -2343,9 +2340,9 @@
         <v>(172)</v>
       </c>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:5">
       <c r="A14" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B14" s="3">
         <f>ROUND(SS_survey!B4,2)</f>
@@ -2364,7 +2361,7 @@
         <v>0.67</v>
       </c>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:5">
       <c r="B15" s="3" t="str">
         <f>CONCATENATE("(",ROUND(SS_survey!B5,3),")")</f>
         <v>(0.024)</v>
@@ -2378,9 +2375,9 @@
         <v>(0.02)</v>
       </c>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:5">
       <c r="A16" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B16" s="3">
         <f>ROUND(SS_survey!B6,2)</f>
@@ -2399,7 +2396,7 @@
         <v>0.89</v>
       </c>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:5">
       <c r="B17" s="3" t="str">
         <f>CONCATENATE("(",ROUND(SS_survey!B7,2),")")</f>
         <v>(0.02)</v>
@@ -2413,9 +2410,9 @@
         <v>(0.01)</v>
       </c>
     </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:5">
       <c r="A18" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B18" s="3">
         <f>ROUND(SS_survey!B8,2)</f>
@@ -2434,7 +2431,7 @@
         <v>0.28999999999999998</v>
       </c>
     </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:5">
       <c r="B19" s="3" t="str">
         <f>CONCATENATE("(",ROUND(SS_survey!B9,3),")")</f>
         <v>(0.028)</v>
@@ -2448,7 +2445,7 @@
         <v>(0.021)</v>
       </c>
     </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:5">
       <c r="A20" t="s">
         <v>9</v>
       </c>
@@ -2469,7 +2466,7 @@
         <v>0.09</v>
       </c>
     </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:5">
       <c r="B21" s="3" t="str">
         <f>CONCATENATE("(",ROUND(SS_survey!B11,3),")")</f>
         <v>(0.721)</v>
@@ -2483,9 +2480,9 @@
         <v>(0.582)</v>
       </c>
     </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:5">
       <c r="A22" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B22" s="3">
         <f>ROUND(SS_survey!B12,2)</f>
@@ -2504,7 +2501,7 @@
         <v>0.25</v>
       </c>
     </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:5">
       <c r="B23" s="3">
         <f>ROUND(SS_survey!B13,2)</f>
         <v>0.02</v>
@@ -2518,7 +2515,7 @@
         <v>(0.011)</v>
       </c>
     </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:5">
       <c r="A24" t="s">
         <v>7</v>
       </c>
@@ -2539,7 +2536,7 @@
         <v>0.73</v>
       </c>
     </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:5">
       <c r="B25" s="3" t="str">
         <f>CONCATENATE("(",ROUND(SS_survey!B15,3),")")</f>
         <v>(0.688)</v>
@@ -2553,9 +2550,9 @@
         <v>(0.792)</v>
       </c>
     </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:5">
       <c r="A26" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B26" s="3">
         <f>ROUND(SS_survey!B16,2)</f>
@@ -2574,7 +2571,7 @@
         <v>0.88</v>
       </c>
     </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:5">
       <c r="B27" s="3" t="str">
         <f>CONCATENATE("(",ROUND(SS_survey!B17,3),")")</f>
         <v>(0.023)</v>
@@ -2588,9 +2585,9 @@
         <v>(0.02)</v>
       </c>
     </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:5">
       <c r="A28" s="11" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B28" s="3">
         <f>ROUND(SS_survey!B18,2)</f>
@@ -2609,7 +2606,7 @@
         <v>0.84</v>
       </c>
     </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:5">
       <c r="B29" s="3" t="str">
         <f>CONCATENATE("(",ROUND(SS_survey!B19,3),")")</f>
         <v>(0.027)</v>
@@ -2623,7 +2620,7 @@
         <v>(0.018)</v>
       </c>
     </row>
-    <row r="30" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="30" spans="1:5" ht="15.75" thickBot="1">
       <c r="A30" s="2" t="s">
         <v>5</v>
       </c>
@@ -2641,7 +2638,7 @@
       </c>
       <c r="E30" s="5"/>
     </row>
-    <row r="31" spans="1:5" ht="15" thickTop="1" x14ac:dyDescent="0.35"/>
+    <row r="31" spans="1:5" ht="15.75" thickTop="1"/>
   </sheetData>
   <mergeCells count="4">
     <mergeCell ref="B2:E2"/>
@@ -2661,30 +2658,30 @@
       <selection activeCell="A4" sqref="A4:E12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="26.26953125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="7.1796875" style="3" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="10.1796875" style="3" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="6.54296875" style="3" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="6.54296875" style="3" customWidth="1"/>
+    <col min="1" max="1" width="26.28515625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="7.140625" style="3" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10.140625" style="3" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="6.5703125" style="3" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="6.5703125" style="3" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="3" spans="1:5" ht="15.75" thickBot="1">
       <c r="A3" s="10"/>
       <c r="B3" s="13"/>
       <c r="C3" s="13"/>
       <c r="D3" s="13"/>
       <c r="E3" s="13"/>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:5">
       <c r="C4" s="14" t="s">
         <v>14</v>
       </c>
       <c r="D4" s="14"/>
       <c r="E4" s="14"/>
     </row>
-    <row r="5" spans="1:5" ht="16.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="5" spans="1:5" ht="16.5" customHeight="1" thickBot="1">
       <c r="A5" s="9"/>
       <c r="B5" s="7" t="s">
         <v>1</v>
@@ -2699,7 +2696,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="6" spans="1:5" ht="16.5" customHeight="1" thickTop="1" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:5" ht="16.5" customHeight="1" thickTop="1">
       <c r="A6" t="s">
         <v>11</v>
       </c>
@@ -2720,7 +2717,7 @@
         <v>0.52</v>
       </c>
     </row>
-    <row r="7" spans="1:5" ht="16.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:5" ht="16.5" customHeight="1">
       <c r="B7" s="3" t="str">
         <f>CONCATENATE("(",ROUND(SS_att!B3,1),")")</f>
         <v>(3)</v>
@@ -2734,9 +2731,9 @@
         <v>(1.8)</v>
       </c>
     </row>
-    <row r="8" spans="1:5" ht="16.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:5" ht="16.5" customHeight="1">
       <c r="A8" s="6" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B8" s="3">
         <f>ROUND(SS_att!B8,2)</f>
@@ -2755,7 +2752,7 @@
         <v>0.62</v>
       </c>
     </row>
-    <row r="9" spans="1:5" ht="16.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:5" ht="16.5" customHeight="1">
       <c r="A9" s="6"/>
       <c r="B9" s="3" t="str">
         <f>CONCATENATE("(",ROUND(SS_att!B9,2),")")</f>
@@ -2770,7 +2767,7 @@
         <v>(0.01)</v>
       </c>
     </row>
-    <row r="10" spans="1:5" ht="16.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:5" ht="16.5" customHeight="1">
       <c r="A10" t="s">
         <v>12</v>
       </c>
@@ -2791,7 +2788,7 @@
         <v>0.62</v>
       </c>
     </row>
-    <row r="11" spans="1:5" ht="16.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:5" ht="16.5" customHeight="1">
       <c r="B11" s="3" t="str">
         <f>CONCATENATE("(",ROUND(SS_att!B11,2),")")</f>
         <v>(0.02)</v>
@@ -2805,7 +2802,7 @@
         <v>(0.01)</v>
       </c>
     </row>
-    <row r="12" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="12" spans="1:5" ht="15.75" thickBot="1">
       <c r="A12" s="2" t="s">
         <v>5</v>
       </c>
@@ -2823,7 +2820,7 @@
       </c>
       <c r="E12" s="5"/>
     </row>
-    <row r="13" spans="1:5" ht="15" thickTop="1" x14ac:dyDescent="0.35"/>
+    <row r="13" spans="1:5" ht="15.75" thickTop="1"/>
   </sheetData>
   <mergeCells count="2">
     <mergeCell ref="B3:E3"/>

</xml_diff>

<commit_message>
tot_tut_validity & edits to the main paper
</commit_message>
<xml_diff>
--- a/Tables/SS.xlsx
+++ b/Tables/SS.xlsx
@@ -1,6 +1,6 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26529"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
@@ -10,7 +10,7 @@
   </mc:AlternateContent>
   <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{81E3DE23-7774-481C-8739-DC27504D8DD5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-22395" yWindow="3615" windowWidth="21600" windowHeight="11175" firstSheet="2" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-22395" yWindow="3615" windowWidth="21600" windowHeight="11175" firstSheet="2" activeTab="5"/>
   </bookViews>
   <sheets>
     <sheet name="SS_admin" sheetId="1" r:id="rId1"/>
@@ -22,7 +22,7 @@
     <sheet name="SS" sheetId="5" r:id="rId7"/>
     <sheet name="Attrition" sheetId="6" r:id="rId8"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="191029" fullCalcOnLoad="true"/>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" count="52" uniqueCount="28">
   <si>
     <t>Choice</t>
   </si>
@@ -129,7 +129,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing">
   <fonts count="1">
     <font>
       <sz val="11"/>
@@ -207,39 +207,39 @@
   </cellStyleXfs>
   <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="true"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="true"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="true">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="true" applyAlignment="true">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="true" applyAlignment="true">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment wrapText="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="true">
+      <alignment wrapText="true"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="true" applyAlignment="true">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="true">
+      <alignment horizontal="center" wrapText="true"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="true" applyAlignment="true">
+      <alignment wrapText="true"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="true"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="true"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="true"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="true" applyAlignment="true">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="true" applyAlignment="true">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="true" applyAlignment="true">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -260,7 +260,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -411,7 +411,7 @@
         <a:solidFill>
           <a:schemeClr val="phClr"/>
         </a:solidFill>
-        <a:gradFill rotWithShape="1">
+        <a:gradFill rotWithShape="true">
           <a:gsLst>
             <a:gs pos="0">
               <a:schemeClr val="phClr">
@@ -435,9 +435,9 @@
               </a:schemeClr>
             </a:gs>
           </a:gsLst>
-          <a:lin ang="5400000" scaled="0"/>
+          <a:lin ang="5400000" scaled="false"/>
         </a:gradFill>
-        <a:gradFill rotWithShape="1">
+        <a:gradFill rotWithShape="true">
           <a:gsLst>
             <a:gs pos="0">
               <a:schemeClr val="phClr">
@@ -461,7 +461,7 @@
               </a:schemeClr>
             </a:gs>
           </a:gsLst>
-          <a:lin ang="5400000" scaled="0"/>
+          <a:lin ang="5400000" scaled="false"/>
         </a:gradFill>
       </a:fillStyleLst>
       <a:lnStyleLst>
@@ -496,7 +496,7 @@
         </a:effectStyle>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="0">
+            <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="false">
               <a:srgbClr val="000000">
                 <a:alpha val="63000"/>
               </a:srgbClr>
@@ -514,7 +514,7 @@
             <a:satMod val="170000"/>
           </a:schemeClr>
         </a:solidFill>
-        <a:gradFill rotWithShape="1">
+        <a:gradFill rotWithShape="true">
           <a:gsLst>
             <a:gs pos="0">
               <a:schemeClr val="phClr">
@@ -539,7 +539,7 @@
               </a:schemeClr>
             </a:gs>
           </a:gsLst>
-          <a:lin ang="5400000" scaled="0"/>
+          <a:lin ang="5400000" scaled="false"/>
         </a:gradFill>
       </a:bgFillStyleLst>
     </a:fmtScheme>
@@ -555,7 +555,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="B2:L6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -564,9 +564,9 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="2" spans="2:12">
+    <row r="2">
       <c r="B2">
-        <v>2267.4576271186438</v>
+        <v>2267.457627118644</v>
       </c>
       <c r="C2">
         <v>2162.484646878198</v>
@@ -575,58 +575,58 @@
         <v>2222.993023255814</v>
       </c>
       <c r="E2">
-        <v>2216.7222398477161</v>
+        <v>2216.722239847716</v>
       </c>
       <c r="L2">
-        <v>0.64503108323202074</v>
-      </c>
-    </row>
-    <row r="3" spans="2:12">
+        <v>0.6450310832320212</v>
+      </c>
+    </row>
+    <row r="3">
       <c r="B3">
-        <v>75.874088260545236</v>
+        <v>75.87408826054524</v>
       </c>
       <c r="C3">
-        <v>83.127592776594469</v>
+        <v>83.12759277659441</v>
       </c>
       <c r="D3">
-        <v>65.750426103453577</v>
+        <v>65.75042610345361</v>
       </c>
       <c r="E3">
-        <v>42.936615450474939</v>
-      </c>
-    </row>
-    <row r="4" spans="2:12">
+        <v>42.93661545047494</v>
+      </c>
+    </row>
+    <row r="4">
       <c r="B4">
-        <v>0.87966101694915255</v>
+        <v>0.8796610169491526</v>
       </c>
       <c r="C4">
-        <v>0.89406345957011257</v>
+        <v>0.8940634595701126</v>
       </c>
       <c r="D4">
-        <v>0.83100775193798448</v>
+        <v>0.8310077519379845</v>
       </c>
       <c r="E4">
         <v>0.8642131979695431</v>
       </c>
       <c r="L4">
-        <v>0.56027324425210501</v>
-      </c>
-    </row>
-    <row r="5" spans="2:12">
+        <v>0.560273244252105</v>
+      </c>
+    </row>
+    <row r="5">
       <c r="B5">
-        <v>4.3632089264598002E-2</v>
+        <v>0.043632089264598</v>
       </c>
       <c r="C5">
-        <v>3.4871491260106517E-2</v>
+        <v>0.03487149126010652</v>
       </c>
       <c r="D5">
-        <v>4.7901996328697877E-2</v>
+        <v>0.04790199632869788</v>
       </c>
       <c r="E5">
-        <v>2.5577577893366659E-2</v>
-      </c>
-    </row>
-    <row r="6" spans="2:12">
+        <v>0.02557757789336666</v>
+      </c>
+    </row>
+    <row r="6">
       <c r="B6">
         <v>1770</v>
       </c>
@@ -646,7 +646,7 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="B2:L11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -655,38 +655,38 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="2" spans="2:12">
+    <row r="2">
       <c r="B2">
-        <v>34.385964912280699</v>
+        <v>30.46153846153846</v>
       </c>
       <c r="C2">
-        <v>33.56666666666667</v>
+        <v>33.76666666666667</v>
       </c>
       <c r="D2">
-        <v>38.634920634920633</v>
+        <v>38.82857142857143</v>
       </c>
       <c r="E2">
-        <v>35.6</v>
+        <v>34.76923076923077</v>
       </c>
       <c r="L2">
-        <v>0.51863884752020373</v>
-      </c>
-    </row>
-    <row r="3" spans="2:12">
+        <v>0.1584710080897333</v>
+      </c>
+    </row>
+    <row r="3">
       <c r="B3">
-        <v>3.0011228460479158</v>
+        <v>2.790776331556584</v>
       </c>
       <c r="C3">
-        <v>2.8780649755984449</v>
+        <v>2.906583863434686</v>
       </c>
       <c r="D3">
-        <v>3.5731906673108398</v>
+        <v>3.320491085220305</v>
       </c>
       <c r="E3">
-        <v>1.8380690486041</v>
-      </c>
-    </row>
-    <row r="4" spans="2:12">
+        <v>1.79376807323629</v>
+      </c>
+    </row>
+    <row r="4">
       <c r="B4">
         <v>1770</v>
       </c>
@@ -700,66 +700,66 @@
         <v>6304</v>
       </c>
     </row>
-    <row r="8" spans="2:12">
+    <row r="8">
       <c r="B8">
-        <v>0.97536945812807885</v>
+        <v>0.9753694581280788</v>
       </c>
       <c r="C8">
-        <v>0.96513157894736845</v>
+        <v>0.9651315789473685</v>
       </c>
       <c r="D8">
         <v>0.9710926016658501</v>
       </c>
       <c r="E8">
-        <v>0.97049377759935773</v>
+        <v>0.9704937775993577</v>
       </c>
       <c r="L8">
-        <v>0.61894128114173319</v>
-      </c>
-    </row>
-    <row r="9" spans="2:12">
+        <v>0.6189412811417327</v>
+      </c>
+    </row>
+    <row r="9">
       <c r="B9">
-        <v>5.5641049658199894E-3</v>
+        <v>0.00556410496581999</v>
       </c>
       <c r="C9">
-        <v>9.0558404602785851E-3</v>
+        <v>0.009055840460278583</v>
       </c>
       <c r="D9">
-        <v>7.7705794497818937E-3</v>
+        <v>0.007770579449781894</v>
       </c>
       <c r="E9">
-        <v>4.4762159277795602E-3</v>
-      </c>
-    </row>
-    <row r="10" spans="2:12">
+        <v>0.00447621592777956</v>
+      </c>
+    </row>
+    <row r="10">
       <c r="B10">
-        <v>0.78725761772853187</v>
+        <v>0.7872576177285319</v>
       </c>
       <c r="C10">
-        <v>0.75810473815461343</v>
+        <v>0.7581047381546134</v>
       </c>
       <c r="D10">
-        <v>0.77339901477832518</v>
+        <v>0.7733990147783252</v>
       </c>
       <c r="E10">
         <v>0.772522871763064</v>
       </c>
       <c r="L10">
-        <v>0.61700341260717884</v>
-      </c>
-    </row>
-    <row r="11" spans="2:12">
+        <v>0.6170034126071788</v>
+      </c>
+    </row>
+    <row r="11">
       <c r="B11">
-        <v>1.787061830945753E-2</v>
+        <v>0.01787061830945753</v>
       </c>
       <c r="C11">
-        <v>2.4082154914125339E-2</v>
+        <v>0.02408215491412533</v>
       </c>
       <c r="D11">
-        <v>2.495667269143001E-2</v>
+        <v>0.02495667269143001</v>
       </c>
       <c r="E11">
-        <v>1.365506059590319E-2</v>
+        <v>0.01365506059590319</v>
       </c>
     </row>
   </sheetData>
@@ -768,7 +768,7 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="B2:L23"/>
   <sheetViews>
     <sheetView topLeftCell="A20" workbookViewId="0">
@@ -777,7 +777,7 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="2" spans="2:12">
+    <row r="2">
       <c r="B2">
         <v>4084.044748373869</v>
       </c>
@@ -785,278 +785,278 @@
         <v>3876.572927111064</v>
       </c>
       <c r="D2">
-        <v>4173.1413633660959</v>
+        <v>4173.141363366096</v>
       </c>
       <c r="E2">
-        <v>4057.7718023592788</v>
+        <v>4057.771802359279</v>
       </c>
       <c r="L2">
-        <v>0.50741363647763404</v>
-      </c>
-    </row>
-    <row r="3" spans="2:12">
+        <v>0.5074136364776338</v>
+      </c>
+    </row>
+    <row r="3">
       <c r="B3">
-        <v>186.32530822216469</v>
+        <v>186.3253082221647</v>
       </c>
       <c r="C3">
-        <v>193.32407154060641</v>
+        <v>193.3240715406064</v>
       </c>
       <c r="D3">
-        <v>171.58152340909879</v>
+        <v>171.5815234090987</v>
       </c>
       <c r="E3">
-        <v>106.6210974172742</v>
-      </c>
-    </row>
-    <row r="4" spans="2:12">
+        <v>106.6210974172743</v>
+      </c>
+    </row>
+    <row r="4">
       <c r="B4">
         <v>0.1870631315668515</v>
       </c>
       <c r="C4">
-        <v>0.20947016543776689</v>
+        <v>0.2094701654377669</v>
       </c>
       <c r="D4">
-        <v>0.18374126248217959</v>
+        <v>0.1837412624821796</v>
       </c>
       <c r="E4">
-        <v>0.19285795427201721</v>
+        <v>0.1928579542720172</v>
       </c>
       <c r="L4">
-        <v>0.67256604845929213</v>
-      </c>
-    </row>
-    <row r="5" spans="2:12">
+        <v>0.6725660484592921</v>
+      </c>
+    </row>
+    <row r="5">
       <c r="B5">
-        <v>2.4433091346626679E-2</v>
+        <v>0.02443309134662668</v>
       </c>
       <c r="C5">
-        <v>2.2831240521491838E-2</v>
+        <v>0.02283124052149185</v>
       </c>
       <c r="D5">
-        <v>2.0246312642953609E-2</v>
+        <v>0.02024631264295361</v>
       </c>
       <c r="E5">
-        <v>1.2895102797403321E-2</v>
-      </c>
-    </row>
-    <row r="6" spans="2:12">
+        <v>0.01289510279740332</v>
+      </c>
+    </row>
+    <row r="6">
       <c r="B6">
-        <v>0.13815789473684209</v>
+        <v>0.1381578947368421</v>
       </c>
       <c r="C6">
-        <v>0.12823529411764709</v>
+        <v>0.1282352941176471</v>
       </c>
       <c r="D6">
         <v>0.1266201395812562</v>
       </c>
       <c r="E6">
-        <v>0.13050133945656331</v>
+        <v>0.1305013394565633</v>
       </c>
       <c r="L6">
-        <v>0.88964950426016531</v>
-      </c>
-    </row>
-    <row r="7" spans="2:12">
+        <v>0.8896495042601654</v>
+      </c>
+    </row>
+    <row r="7">
       <c r="B7">
-        <v>2.0646396595072281E-2</v>
+        <v>0.02064639659507228</v>
       </c>
       <c r="C7">
-        <v>1.427153837750952E-2</v>
+        <v>0.01427153837750952</v>
       </c>
       <c r="D7">
-        <v>1.2989025875656869E-2</v>
+        <v>0.01298902587565687</v>
       </c>
       <c r="E7">
-        <v>9.0357611917287195E-3</v>
-      </c>
-    </row>
-    <row r="8" spans="2:12">
+        <v>0.009035761191728721</v>
+      </c>
+    </row>
+    <row r="8">
       <c r="B8">
-        <v>0.62474437627811863</v>
+        <v>0.6247443762781186</v>
       </c>
       <c r="C8">
-        <v>0.58845096241979833</v>
+        <v>0.5884509624197983</v>
       </c>
       <c r="D8">
-        <v>0.65175953079178883</v>
+        <v>0.6517595307917888</v>
       </c>
       <c r="E8">
-        <v>0.62394407224002335</v>
+        <v>0.6239440722400234</v>
       </c>
       <c r="L8">
-        <v>0.29259959707503702</v>
-      </c>
-    </row>
-    <row r="9" spans="2:12">
+        <v>0.2925995970750369</v>
+      </c>
+    </row>
+    <row r="9">
       <c r="B9">
-        <v>2.8080273403161181E-2</v>
+        <v>0.02808027340316118</v>
       </c>
       <c r="C9">
-        <v>3.5546721070160617E-2</v>
+        <v>0.03554672107016062</v>
       </c>
       <c r="D9">
-        <v>2.101418987928844E-2</v>
+        <v>0.02101418987928844</v>
       </c>
       <c r="E9">
-        <v>1.6701632404580391E-2</v>
-      </c>
-    </row>
-    <row r="10" spans="2:12">
+        <v>0.01670163240458039</v>
+      </c>
+    </row>
+    <row r="10">
       <c r="B10">
-        <v>91.886692015209121</v>
+        <v>91.88669201520912</v>
       </c>
       <c r="C10">
-        <v>91.652142857142863</v>
+        <v>91.65214285714286</v>
       </c>
       <c r="D10">
-        <v>93.610994764397901</v>
+        <v>93.6109947643979</v>
       </c>
       <c r="E10">
-        <v>92.527783783783789</v>
+        <v>92.52778378378379</v>
       </c>
       <c r="L10">
-        <v>9.3375432500356903E-2</v>
-      </c>
-    </row>
-    <row r="11" spans="2:12">
+        <v>0.093375432500357</v>
+      </c>
+    </row>
+    <row r="11">
       <c r="B11">
-        <v>0.72142723064601477</v>
+        <v>0.7214272306460148</v>
       </c>
       <c r="C11">
         <v>1.031496976703081</v>
       </c>
       <c r="D11">
-        <v>0.58165693064045443</v>
+        <v>0.5816569306404544</v>
       </c>
       <c r="E11">
-        <v>0.4502856911185264</v>
-      </c>
-    </row>
-    <row r="12" spans="2:12">
+        <v>0.4502856911185265</v>
+      </c>
+    </row>
+    <row r="12">
       <c r="B12">
         <v>0.8693877551020408</v>
       </c>
       <c r="C12">
-        <v>0.88718411552346566</v>
+        <v>0.8871841155234657</v>
       </c>
       <c r="D12">
         <v>0.9007246376811594</v>
       </c>
       <c r="E12">
-        <v>0.88754325259515576</v>
+        <v>0.8875432525951558</v>
       </c>
       <c r="L12">
         <v>0.2521838227756053</v>
       </c>
     </row>
-    <row r="13" spans="2:12">
+    <row r="13">
       <c r="B13">
-        <v>1.5429549670760771E-2</v>
+        <v>0.01542954967076077</v>
       </c>
       <c r="C13">
-        <v>1.2769905653078379E-2</v>
+        <v>0.01276990565307838</v>
       </c>
       <c r="D13">
-        <v>1.1107505082691109E-2</v>
+        <v>0.01110750508269111</v>
       </c>
       <c r="E13">
-        <v>7.5100652933181586E-3</v>
-      </c>
-    </row>
-    <row r="14" spans="2:12">
+        <v>0.007510065293318159</v>
+      </c>
+    </row>
+    <row r="14">
       <c r="B14">
-        <v>43.316996871741402</v>
+        <v>43.3169968717414</v>
       </c>
       <c r="C14">
-        <v>42.852913968547639</v>
+        <v>42.85291396854764</v>
       </c>
       <c r="D14">
-        <v>43.821138211382113</v>
+        <v>43.82113821138211</v>
       </c>
       <c r="E14">
         <v>43.37017388741527</v>
       </c>
       <c r="L14">
-        <v>0.72947420733682788</v>
-      </c>
-    </row>
-    <row r="15" spans="2:12">
+        <v>0.7294742073368279</v>
+      </c>
+    </row>
+    <row r="15">
       <c r="B15">
-        <v>0.68765705993205639</v>
+        <v>0.6876570599320564</v>
       </c>
       <c r="C15">
-        <v>0.94934692018880429</v>
+        <v>0.9493469201888045</v>
       </c>
       <c r="D15">
-        <v>0.79169967129326269</v>
+        <v>0.7916996712932627</v>
       </c>
       <c r="E15">
-        <v>0.47585898339836669</v>
-      </c>
-    </row>
-    <row r="16" spans="2:12">
+        <v>0.4758589833983667</v>
+      </c>
+    </row>
+    <row r="16">
       <c r="B16">
         <v>0.7275390625</v>
       </c>
       <c r="C16">
-        <v>0.72097053726169846</v>
+        <v>0.7209705372616985</v>
       </c>
       <c r="D16">
-        <v>0.71247498332221482</v>
+        <v>0.7124749833222148</v>
       </c>
       <c r="E16">
         <v>0.7193364155561599</v>
       </c>
       <c r="L16">
-        <v>0.87880547636069528</v>
-      </c>
-    </row>
-    <row r="17" spans="2:12">
+        <v>0.8788054763606953</v>
+      </c>
+    </row>
+    <row r="17">
       <c r="B17">
-        <v>2.2722829871839111E-2</v>
+        <v>0.02272282987183911</v>
       </c>
       <c r="C17">
-        <v>1.8719850717439711E-2</v>
+        <v>0.01871985071743971</v>
       </c>
       <c r="D17">
-        <v>1.9807350620927651E-2</v>
+        <v>0.01980735062092765</v>
       </c>
       <c r="E17">
-        <v>1.1899628511819889E-2</v>
-      </c>
-    </row>
-    <row r="18" spans="2:12">
+        <v>0.01189962851181989</v>
+      </c>
+    </row>
+    <row r="18">
       <c r="B18">
-        <v>0.65861344537815125</v>
+        <v>0.6586134453781513</v>
       </c>
       <c r="C18">
-        <v>0.66851851851851851</v>
+        <v>0.6685185185185185</v>
       </c>
       <c r="D18">
-        <v>0.65151515151515149</v>
+        <v>0.6515151515151515</v>
       </c>
       <c r="E18">
-        <v>0.65900954653937949</v>
+        <v>0.6590095465393795</v>
       </c>
       <c r="L18">
-        <v>0.83627432511379829</v>
-      </c>
-    </row>
-    <row r="19" spans="2:12">
+        <v>0.8362743251137983</v>
+      </c>
+    </row>
+    <row r="19">
       <c r="B19">
-        <v>2.7084494536168069E-2</v>
+        <v>0.02708449453616807</v>
       </c>
       <c r="C19">
-        <v>2.245117168137609E-2</v>
+        <v>0.02245117168137609</v>
       </c>
       <c r="D19">
-        <v>1.7630212971503322E-2</v>
+        <v>0.01763021297150332</v>
       </c>
       <c r="E19">
-        <v>1.264015748271608E-2</v>
-      </c>
-    </row>
-    <row r="20" spans="2:12">
+        <v>0.01264015748271608</v>
+      </c>
+    </row>
+    <row r="20">
       <c r="B20">
         <v>1770</v>
       </c>
@@ -1070,7 +1070,7 @@
         <v>6304</v>
       </c>
     </row>
-    <row r="23" spans="2:12">
+    <row r="23">
       <c r="B23">
         <v>1386</v>
       </c>
@@ -1087,7 +1087,7 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
   <dimension ref="B2:L6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -1096,69 +1096,69 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="2" spans="2:12">
+    <row r="2">
       <c r="B2">
-        <v>2199.2352092352089</v>
+        <v>2199.235209235209</v>
       </c>
       <c r="C2">
-        <v>2196.0415248468339</v>
+        <v>2196.041524846834</v>
       </c>
       <c r="D2">
-        <v>2216.4177598385472</v>
+        <v>2216.417759838547</v>
       </c>
       <c r="E2">
-        <v>2205.3059747777552</v>
+        <v>2205.305974777755</v>
       </c>
       <c r="L2">
-        <v>0.98415991070079034</v>
-      </c>
-    </row>
-    <row r="3" spans="2:12">
+        <v>0.9841599107007903</v>
+      </c>
+    </row>
+    <row r="3">
       <c r="B3">
-        <v>85.691617474481063</v>
+        <v>85.69161747448106</v>
       </c>
       <c r="C3">
-        <v>105.62668921394879</v>
+        <v>105.6266892139488</v>
       </c>
       <c r="D3">
-        <v>80.611977579989215</v>
+        <v>80.61197757998926</v>
       </c>
       <c r="E3">
-        <v>51.996675747123149</v>
-      </c>
-    </row>
-    <row r="4" spans="2:12">
+        <v>51.99667574712315</v>
+      </c>
+    </row>
+    <row r="4">
       <c r="B4">
-        <v>0.87590187590187585</v>
+        <v>0.8759018759018758</v>
       </c>
       <c r="C4">
-        <v>0.88563648740639889</v>
+        <v>0.8856364874063989</v>
       </c>
       <c r="D4">
-        <v>0.84712411705348134</v>
+        <v>0.8471241170534813</v>
       </c>
       <c r="E4">
-        <v>0.86706636344841848</v>
+        <v>0.8670663634484185</v>
       </c>
       <c r="L4">
-        <v>0.80262123234967087</v>
-      </c>
-    </row>
-    <row r="5" spans="2:12">
+        <v>0.8026212323496709</v>
+      </c>
+    </row>
+    <row r="5">
       <c r="B5">
-        <v>4.4829425630513037E-2</v>
+        <v>0.04482942563051304</v>
       </c>
       <c r="C5">
-        <v>3.8037392189498608E-2</v>
+        <v>0.03803739218949861</v>
       </c>
       <c r="D5">
-        <v>4.5323633701885309E-2</v>
+        <v>0.04532363370188531</v>
       </c>
       <c r="E5">
-        <v>2.5337910106350281E-2</v>
-      </c>
-    </row>
-    <row r="6" spans="2:12">
+        <v>0.02533791010635028</v>
+      </c>
+    </row>
+    <row r="6">
       <c r="B6">
         <v>1386</v>
       </c>
@@ -1178,7 +1178,7 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
   <dimension ref="B2:S20"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -1187,26 +1187,26 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="17" max="17" width="9.5703125" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="10.42578125" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="7.42578125" customWidth="1"/>
+    <col min="17" max="17" width="9.5703125" bestFit="true" customWidth="true"/>
+    <col min="18" max="18" width="10.42578125" bestFit="true" customWidth="true"/>
+    <col min="19" max="19" width="7.42578125" customWidth="true"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:19" ht="15.75" thickBot="1">
+    <row r="2" ht="15.75" thickBot="true">
       <c r="B2">
-        <v>0.73333333333333328</v>
+        <v>0.7333333333333333</v>
       </c>
       <c r="C2">
-        <v>0.68935516888433979</v>
+        <v>0.6893551688843398</v>
       </c>
       <c r="D2">
-        <v>0.70542635658914732</v>
+        <v>0.7054263565891473</v>
       </c>
       <c r="E2">
-        <v>0.70828045685279184</v>
+        <v>0.7082804568527918</v>
       </c>
       <c r="L2">
-        <v>0.38947230579030429</v>
+        <v>0.3894723057903044</v>
       </c>
       <c r="N2">
         <v>0</v>
@@ -1224,18 +1224,18 @@
         <v>25</v>
       </c>
     </row>
-    <row r="3" spans="2:19" ht="15.75" thickTop="1">
+    <row r="3" ht="15.75" thickTop="true">
       <c r="B3">
-        <v>2.2227133407258709E-2</v>
+        <v>0.02222713340725871</v>
       </c>
       <c r="C3">
-        <v>2.3945559259684199E-2</v>
+        <v>0.02394555925968419</v>
       </c>
       <c r="D3">
-        <v>2.448740630667276E-2</v>
+        <v>0.02448740630667276</v>
       </c>
       <c r="E3">
-        <v>1.405414443820463E-2</v>
+        <v>0.01405414443820463</v>
       </c>
       <c r="N3">
         <v>1</v>
@@ -1255,18 +1255,18 @@
         <v>4.6399999999999997</v>
       </c>
     </row>
-    <row r="4" spans="2:19">
+    <row r="4">
       <c r="B4">
-        <v>0.49265536723163839</v>
+        <v>0.4926553672316384</v>
       </c>
       <c r="C4">
-        <v>0.47697031729785061</v>
+        <v>0.4769703172978506</v>
       </c>
       <c r="D4">
-        <v>0.44341085271317832</v>
+        <v>0.4434108527131783</v>
       </c>
       <c r="E4">
-        <v>0.46763959390862941</v>
+        <v>0.4676395939086294</v>
       </c>
       <c r="L4">
         <v>0.2875593605623547</v>
@@ -1289,18 +1289,18 @@
         <v>28.1</v>
       </c>
     </row>
-    <row r="5" spans="2:19">
+    <row r="5">
       <c r="B5">
-        <v>2.30962400955886E-2</v>
+        <v>0.02309624009558859</v>
       </c>
       <c r="C5">
-        <v>2.2430876785456681E-2</v>
+        <v>0.02243087678545668</v>
       </c>
       <c r="D5">
-        <v>2.2238865610497351E-2</v>
+        <v>0.02223886561049735</v>
       </c>
       <c r="E5">
-        <v>1.3451909622314609E-2</v>
+        <v>0.01345190962231461</v>
       </c>
       <c r="N5">
         <v>3</v>
@@ -1320,21 +1320,21 @@
         <v>28.85</v>
       </c>
     </row>
-    <row r="6" spans="2:19">
+    <row r="6">
       <c r="B6">
-        <v>0.42937853107344631</v>
+        <v>0.4293785310734463</v>
       </c>
       <c r="C6">
-        <v>0.43500511770726707</v>
+        <v>0.4350051177072671</v>
       </c>
       <c r="D6">
-        <v>0.38875968992248061</v>
+        <v>0.3887596899224806</v>
       </c>
       <c r="E6">
-        <v>0.41449873096446699</v>
+        <v>0.414498730964467</v>
       </c>
       <c r="L6">
-        <v>0.16570447921258691</v>
+        <v>0.1657044792125869</v>
       </c>
       <c r="N6">
         <v>4</v>
@@ -1354,18 +1354,18 @@
         <v>30.830000000000002</v>
       </c>
     </row>
-    <row r="7" spans="2:19">
+    <row r="7">
       <c r="B7">
-        <v>2.2539581021475689E-2</v>
+        <v>0.02253958102147569</v>
       </c>
       <c r="C7">
-        <v>2.1272764353621978E-2</v>
+        <v>0.02127276435362197</v>
       </c>
       <c r="D7">
-        <v>1.7156228789498341E-2</v>
+        <v>0.01715622878949833</v>
       </c>
       <c r="E7">
-        <v>1.185696393078531E-2</v>
+        <v>0.01185696393078531</v>
       </c>
       <c r="N7">
         <v>5</v>
@@ -1385,21 +1385,21 @@
         <v>32.39</v>
       </c>
     </row>
-    <row r="8" spans="2:19">
+    <row r="8">
       <c r="B8">
-        <v>0.55254237288135588</v>
+        <v>0.5525423728813559</v>
       </c>
       <c r="C8">
-        <v>0.55834186284544529</v>
+        <v>0.5583418628454453</v>
       </c>
       <c r="D8">
-        <v>0.52868217054263567</v>
+        <v>0.5286821705426357</v>
       </c>
       <c r="E8">
         <v>0.5445748730964467</v>
       </c>
       <c r="L8">
-        <v>0.56094587102663473</v>
+        <v>0.5609458710266343</v>
       </c>
       <c r="N8">
         <v>6</v>
@@ -1419,18 +1419,18 @@
         <v>35.1</v>
       </c>
     </row>
-    <row r="9" spans="2:19">
+    <row r="9">
       <c r="B9">
-        <v>2.3021717142206809E-2</v>
+        <v>0.02302171714220681</v>
       </c>
       <c r="C9">
-        <v>2.284086769741038E-2</v>
+        <v>0.02284086769741038</v>
       </c>
       <c r="D9">
-        <v>1.9453047006242681E-2</v>
+        <v>0.01945304700624268</v>
       </c>
       <c r="E9">
-        <v>1.259298623720528E-2</v>
+        <v>0.01259298623720528</v>
       </c>
       <c r="N9">
         <v>7</v>
@@ -1450,21 +1450,21 @@
         <v>41.34</v>
       </c>
     </row>
-    <row r="10" spans="2:19">
+    <row r="10">
       <c r="B10">
-        <v>0.74293785310734461</v>
+        <v>0.7429378531073446</v>
       </c>
       <c r="C10">
         <v>0.7164790174002047</v>
       </c>
       <c r="D10">
-        <v>0.74031007751937983</v>
+        <v>0.7403100775193798</v>
       </c>
       <c r="E10">
-        <v>0.73366116751269039</v>
+        <v>0.7336611675126904</v>
       </c>
       <c r="L10">
-        <v>0.71186933052406198</v>
+        <v>0.711869330524062</v>
       </c>
       <c r="N10">
         <v>8</v>
@@ -1484,18 +1484,18 @@
         <v>56.49</v>
       </c>
     </row>
-    <row r="11" spans="2:19" ht="15.75" thickBot="1">
+    <row r="11" ht="15.75" thickBot="true">
       <c r="B11">
-        <v>2.3824936806509319E-2</v>
+        <v>0.02382493680650932</v>
       </c>
       <c r="C11">
-        <v>2.5477564039296342E-2</v>
+        <v>0.02547756403929634</v>
       </c>
       <c r="D11">
-        <v>2.5358148430980949E-2</v>
+        <v>0.02535814843098096</v>
       </c>
       <c r="E11">
-        <v>1.462507287141228E-2</v>
+        <v>0.01462507287141228</v>
       </c>
       <c r="N11">
         <v>9</v>
@@ -1515,7 +1515,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="12" spans="2:19" ht="15.75" thickTop="1">
+    <row r="12" ht="15.75" thickTop="true">
       <c r="B12">
         <v>0.5536723163841808</v>
       </c>
@@ -1523,123 +1523,123 @@
         <v>0.5670419651995906</v>
       </c>
       <c r="D12">
-        <v>0.53488372093023251</v>
+        <v>0.5348837209302325</v>
       </c>
       <c r="E12">
-        <v>0.55012690355329952</v>
+        <v>0.5501269035532995</v>
       </c>
       <c r="L12">
-        <v>0.56579109636169034</v>
-      </c>
-    </row>
-    <row r="13" spans="2:19">
+        <v>0.5657910963616903</v>
+      </c>
+    </row>
+    <row r="13">
       <c r="B13">
-        <v>2.3197736740832291E-2</v>
+        <v>0.02319773674083229</v>
       </c>
       <c r="C13">
-        <v>2.3802739213909081E-2</v>
+        <v>0.02380273921390908</v>
       </c>
       <c r="D13">
-        <v>1.9572399449557739E-2</v>
+        <v>0.01957239944955774</v>
       </c>
       <c r="E13">
-        <v>1.2812478832268839E-2</v>
-      </c>
-    </row>
-    <row r="14" spans="2:19">
+        <v>0.01281247883226884</v>
+      </c>
+    </row>
+    <row r="14">
       <c r="B14">
-        <v>0.54180790960451974</v>
+        <v>0.5418079096045197</v>
       </c>
       <c r="C14">
-        <v>0.55322415557830096</v>
+        <v>0.553224155578301</v>
       </c>
       <c r="D14">
-        <v>0.52441860465116275</v>
+        <v>0.5244186046511627</v>
       </c>
       <c r="E14">
-        <v>0.53822969543147203</v>
+        <v>0.538229695431472</v>
       </c>
       <c r="L14">
-        <v>0.59041645057610981</v>
-      </c>
-    </row>
-    <row r="15" spans="2:19">
+        <v>0.5904164505761096</v>
+      </c>
+    </row>
+    <row r="15">
       <c r="B15">
-        <v>2.3028825848404249E-2</v>
+        <v>0.02302882584840425</v>
       </c>
       <c r="C15">
-        <v>2.263762438473425E-2</v>
+        <v>0.02263762438473425</v>
       </c>
       <c r="D15">
-        <v>1.7949107537719389E-2</v>
+        <v>0.01794910753771939</v>
       </c>
       <c r="E15">
-        <v>1.215151264408409E-2</v>
-      </c>
-    </row>
-    <row r="16" spans="2:19">
+        <v>0.0121515126440841</v>
+      </c>
+    </row>
+    <row r="16">
       <c r="B16">
         <v>0.5785310734463277</v>
       </c>
       <c r="C16">
-        <v>0.59058341862845443</v>
+        <v>0.5905834186284544</v>
       </c>
       <c r="D16">
-        <v>0.58100775193798448</v>
+        <v>0.5810077519379845</v>
       </c>
       <c r="E16">
-        <v>0.58328045685279184</v>
+        <v>0.5832804568527918</v>
       </c>
       <c r="L16">
-        <v>0.93267269990982249</v>
-      </c>
-    </row>
-    <row r="17" spans="2:12">
+        <v>0.9326726999098225</v>
+      </c>
+    </row>
+    <row r="17">
       <c r="B17">
-        <v>2.4804932440873621E-2</v>
+        <v>0.02480493244087363</v>
       </c>
       <c r="C17">
-        <v>2.4454339740942709E-2</v>
+        <v>0.0244543397409427</v>
       </c>
       <c r="D17">
-        <v>2.0184205552730611E-2</v>
+        <v>0.02018420555273061</v>
       </c>
       <c r="E17">
-        <v>1.316677672471577E-2</v>
-      </c>
-    </row>
-    <row r="18" spans="2:12">
+        <v>0.01316677672471577</v>
+      </c>
+    </row>
+    <row r="18">
       <c r="B18">
-        <v>0.53785310734463276</v>
+        <v>0.5378531073446328</v>
       </c>
       <c r="C18">
-        <v>0.55271238485158647</v>
+        <v>0.5527123848515865</v>
       </c>
       <c r="D18">
-        <v>0.51162790697674421</v>
+        <v>0.5116279069767442</v>
       </c>
       <c r="E18">
-        <v>0.53172588832487311</v>
+        <v>0.5317258883248731</v>
       </c>
       <c r="L18">
-        <v>0.38649070048922801</v>
-      </c>
-    </row>
-    <row r="19" spans="2:12">
+        <v>0.3864907004892281</v>
+      </c>
+    </row>
+    <row r="19">
       <c r="B19">
-        <v>2.497582090269404E-2</v>
+        <v>0.02497582090269404</v>
       </c>
       <c r="C19">
-        <v>2.4730039627438721E-2</v>
+        <v>0.02473003962743872</v>
       </c>
       <c r="D19">
-        <v>1.882401910494624E-2</v>
+        <v>0.01882401910494625</v>
       </c>
       <c r="E19">
-        <v>1.314890352713889E-2</v>
-      </c>
-    </row>
-    <row r="20" spans="2:12">
+        <v>0.01314890352713889</v>
+      </c>
+    </row>
+    <row r="20">
       <c r="B20">
         <v>1770</v>
       </c>
@@ -1659,37 +1659,37 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{67FF63D4-14D6-4F54-BD0D-751B1AD5E68C}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{67FF63D4-14D6-4F54-BD0D-751B1AD5E68C}">
   <dimension ref="A2:E31"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+    <sheetView tabSelected="true" topLeftCell="A10" workbookViewId="0">
       <selection activeCell="A3" sqref="A3:E30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="18.140625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="9.7109375" style="3" customWidth="1"/>
-    <col min="3" max="3" width="10.5703125" style="3" customWidth="1"/>
-    <col min="4" max="4" width="7.5703125" style="3" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="7.5703125" style="3" customWidth="1"/>
+    <col min="1" max="1" width="18.140625" bestFit="true" customWidth="true"/>
+    <col min="2" max="2" width="9.7109375" style="3" customWidth="true"/>
+    <col min="3" max="3" width="10.5703125" style="3" customWidth="true"/>
+    <col min="4" max="4" width="7.5703125" style="3" bestFit="true" customWidth="true"/>
+    <col min="5" max="5" width="7.5703125" style="3" customWidth="true"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:5" ht="15.75" thickBot="1">
+    <row r="2" ht="15.75" thickBot="true">
       <c r="A2" s="10"/>
       <c r="B2" s="13"/>
       <c r="C2" s="13"/>
       <c r="D2" s="13"/>
       <c r="E2" s="13"/>
     </row>
-    <row r="3" spans="1:5">
+    <row r="3">
       <c r="C3" s="14" t="s">
         <v>14</v>
       </c>
       <c r="D3" s="14"/>
       <c r="E3" s="14"/>
     </row>
-    <row r="4" spans="1:5" s="6" customFormat="1" ht="30">
+    <row r="4" s="6" customFormat="true" ht="30">
       <c r="B4" s="8" t="s">
         <v>1</v>
       </c>
@@ -1703,7 +1703,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="5" spans="1:5" ht="15.75" thickBot="1">
+    <row r="5" ht="15.75" thickBot="true">
       <c r="A5" s="2"/>
       <c r="B5" s="15" t="s">
         <v>20</v>
@@ -1712,7 +1712,7 @@
       <c r="D5" s="15"/>
       <c r="E5" s="15"/>
     </row>
-    <row r="6" spans="1:5" ht="15.75" thickTop="1">
+    <row r="6" ht="15.75" thickTop="true">
       <c r="A6" t="s">
         <v>4</v>
       </c>
@@ -1733,7 +1733,7 @@
         <v>0.98</v>
       </c>
     </row>
-    <row r="7" spans="1:5">
+    <row r="7">
       <c r="B7" s="3" t="str">
         <f>CONCATENATE("(",ROUND(SS_admin_survey!B3,0),")")</f>
         <v>(86)</v>
@@ -1747,7 +1747,7 @@
         <v>(81)</v>
       </c>
     </row>
-    <row r="8" spans="1:5">
+    <row r="8">
       <c r="A8" t="s">
         <v>13</v>
       </c>
@@ -1768,7 +1768,7 @@
         <v>0.8</v>
       </c>
     </row>
-    <row r="9" spans="1:5">
+    <row r="9">
       <c r="B9" s="3" t="str">
         <f>CONCATENATE("(",ROUND(SS_admin_survey!B5,3),")")</f>
         <v>(0.045)</v>
@@ -1782,7 +1782,7 @@
         <v>(0.045)</v>
       </c>
     </row>
-    <row r="10" spans="1:5">
+    <row r="10">
       <c r="A10" s="1" t="s">
         <v>5</v>
       </c>
@@ -1800,7 +1800,7 @@
       </c>
       <c r="E10" s="4"/>
     </row>
-    <row r="11" spans="1:5" ht="15.75" thickBot="1">
+    <row r="11" ht="15.75" thickBot="true">
       <c r="A11" s="2"/>
       <c r="B11" s="15" t="s">
         <v>21</v>
@@ -1809,7 +1809,7 @@
       <c r="D11" s="15"/>
       <c r="E11" s="15"/>
     </row>
-    <row r="12" spans="1:5" ht="15.75" thickTop="1">
+    <row r="12" ht="15.75" thickTop="true">
       <c r="A12" t="s">
         <v>8</v>
       </c>
@@ -1830,7 +1830,7 @@
         <v>0.39</v>
       </c>
     </row>
-    <row r="13" spans="1:5">
+    <row r="13">
       <c r="B13" s="3" t="str">
         <f>CONCATENATE("(",ROUND(survey_response_rate!B3,3),")")</f>
         <v>(0.022)</v>
@@ -1844,7 +1844,7 @@
         <v>(0.024)</v>
       </c>
     </row>
-    <row r="14" spans="1:5">
+    <row r="14">
       <c r="A14" t="s">
         <v>26</v>
       </c>
@@ -1865,7 +1865,7 @@
         <v>0.28999999999999998</v>
       </c>
     </row>
-    <row r="15" spans="1:5">
+    <row r="15">
       <c r="B15" s="3" t="str">
         <f>CONCATENATE("(",ROUND(survey_response_rate!B5,3),")")</f>
         <v>(0.023)</v>
@@ -1879,7 +1879,7 @@
         <v>(0.022)</v>
       </c>
     </row>
-    <row r="16" spans="1:5">
+    <row r="16">
       <c r="A16" t="s">
         <v>16</v>
       </c>
@@ -1900,7 +1900,7 @@
         <v>0.17</v>
       </c>
     </row>
-    <row r="17" spans="1:5">
+    <row r="17">
       <c r="B17" s="3" t="str">
         <f>CONCATENATE("(",ROUND(survey_response_rate!B7,2),")")</f>
         <v>(0.02)</v>
@@ -1914,7 +1914,7 @@
         <v>(0.02)</v>
       </c>
     </row>
-    <row r="18" spans="1:5">
+    <row r="18">
       <c r="A18" t="s">
         <v>17</v>
       </c>
@@ -1935,7 +1935,7 @@
         <v>0.56000000000000005</v>
       </c>
     </row>
-    <row r="19" spans="1:5">
+    <row r="19">
       <c r="B19" s="3" t="str">
         <f>CONCATENATE("(",ROUND(survey_response_rate!B9,3),")")</f>
         <v>(0.023)</v>
@@ -1949,7 +1949,7 @@
         <v>(0.019)</v>
       </c>
     </row>
-    <row r="20" spans="1:5">
+    <row r="20">
       <c r="A20" t="s">
         <v>9</v>
       </c>
@@ -1970,7 +1970,7 @@
         <v>0.71</v>
       </c>
     </row>
-    <row r="21" spans="1:5">
+    <row r="21">
       <c r="B21" s="3" t="str">
         <f>CONCATENATE("(",ROUND(survey_response_rate!B11,3),")")</f>
         <v>(0.024)</v>
@@ -1984,7 +1984,7 @@
         <v>(0.025)</v>
       </c>
     </row>
-    <row r="22" spans="1:5">
+    <row r="22">
       <c r="A22" t="s">
         <v>18</v>
       </c>
@@ -2005,7 +2005,7 @@
         <v>0.56999999999999995</v>
       </c>
     </row>
-    <row r="23" spans="1:5">
+    <row r="23">
       <c r="B23" s="3" t="str">
         <f>CONCATENATE("(",ROUND(survey_response_rate!B13,3),")")</f>
         <v>(0.023)</v>
@@ -2019,7 +2019,7 @@
         <v>(0.02)</v>
       </c>
     </row>
-    <row r="24" spans="1:5">
+    <row r="24">
       <c r="A24" t="s">
         <v>7</v>
       </c>
@@ -2040,7 +2040,7 @@
         <v>0.59</v>
       </c>
     </row>
-    <row r="25" spans="1:5">
+    <row r="25">
       <c r="B25" s="3" t="str">
         <f>CONCATENATE("(",ROUND(survey_response_rate!B15,3),")")</f>
         <v>(0.023)</v>
@@ -2054,7 +2054,7 @@
         <v>(0.018)</v>
       </c>
     </row>
-    <row r="26" spans="1:5">
+    <row r="26">
       <c r="A26" t="s">
         <v>6</v>
       </c>
@@ -2075,7 +2075,7 @@
         <v>0.93</v>
       </c>
     </row>
-    <row r="27" spans="1:5">
+    <row r="27">
       <c r="B27" s="3" t="str">
         <f>CONCATENATE("(",ROUND(survey_response_rate!B17,3),")")</f>
         <v>(0.025)</v>
@@ -2089,7 +2089,7 @@
         <v>(0.02)</v>
       </c>
     </row>
-    <row r="28" spans="1:5">
+    <row r="28">
       <c r="A28" s="11" t="s">
         <v>19</v>
       </c>
@@ -2110,7 +2110,7 @@
         <v>0.39</v>
       </c>
     </row>
-    <row r="29" spans="1:5">
+    <row r="29">
       <c r="B29" s="3" t="str">
         <f>CONCATENATE("(",ROUND(survey_response_rate!B19,3),")")</f>
         <v>(0.025)</v>
@@ -2124,7 +2124,7 @@
         <v>(0.019)</v>
       </c>
     </row>
-    <row r="30" spans="1:5" ht="15.75" thickBot="1">
+    <row r="30" ht="15.75" thickBot="true">
       <c r="A30" s="2" t="s">
         <v>5</v>
       </c>
@@ -2142,7 +2142,7 @@
       </c>
       <c r="E30" s="5"/>
     </row>
-    <row r="31" spans="1:5" ht="15.75" thickTop="1"/>
+    <row r="31" ht="15.75" thickTop="true"/>
   </sheetData>
   <mergeCells count="4">
     <mergeCell ref="B2:E2"/>
@@ -2155,7 +2155,7 @@
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3B054637-0760-4807-B01C-4419EACB0C14}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3B054637-0760-4807-B01C-4419EACB0C14}">
   <dimension ref="A2:E31"/>
   <sheetViews>
     <sheetView topLeftCell="A6" workbookViewId="0">
@@ -2164,28 +2164,28 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="18.140625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="9.7109375" style="3" customWidth="1"/>
-    <col min="3" max="3" width="10.5703125" style="3" customWidth="1"/>
-    <col min="4" max="4" width="7.5703125" style="3" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="7.5703125" style="3" customWidth="1"/>
+    <col min="1" max="1" width="18.140625" bestFit="true" customWidth="true"/>
+    <col min="2" max="2" width="9.7109375" style="3" customWidth="true"/>
+    <col min="3" max="3" width="10.5703125" style="3" customWidth="true"/>
+    <col min="4" max="4" width="7.5703125" style="3" bestFit="true" customWidth="true"/>
+    <col min="5" max="5" width="7.5703125" style="3" customWidth="true"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:5" ht="15.75" thickBot="1">
+    <row r="2" ht="15.75" thickBot="true">
       <c r="A2" s="10"/>
       <c r="B2" s="13"/>
       <c r="C2" s="13"/>
       <c r="D2" s="13"/>
       <c r="E2" s="13"/>
     </row>
-    <row r="3" spans="1:5">
+    <row r="3">
       <c r="C3" s="14" t="s">
         <v>14</v>
       </c>
       <c r="D3" s="14"/>
       <c r="E3" s="14"/>
     </row>
-    <row r="4" spans="1:5" s="6" customFormat="1" ht="30">
+    <row r="4" s="6" customFormat="true" ht="30">
       <c r="B4" s="8" t="s">
         <v>1</v>
       </c>
@@ -2199,7 +2199,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="5" spans="1:5" ht="15.75" thickBot="1">
+    <row r="5" ht="15.75" thickBot="true">
       <c r="A5" s="2"/>
       <c r="B5" s="15" t="s">
         <v>3</v>
@@ -2208,7 +2208,7 @@
       <c r="D5" s="15"/>
       <c r="E5" s="15"/>
     </row>
-    <row r="6" spans="1:5" ht="15.75" thickTop="1">
+    <row r="6" ht="15.75" thickTop="true">
       <c r="A6" t="s">
         <v>4</v>
       </c>
@@ -2229,7 +2229,7 @@
         <v>0.65</v>
       </c>
     </row>
-    <row r="7" spans="1:5">
+    <row r="7">
       <c r="B7" s="3" t="str">
         <f>CONCATENATE("(",ROUND(SS_admin!B3,0),")")</f>
         <v>(76)</v>
@@ -2243,7 +2243,7 @@
         <v>(66)</v>
       </c>
     </row>
-    <row r="8" spans="1:5">
+    <row r="8">
       <c r="A8" t="s">
         <v>13</v>
       </c>
@@ -2264,7 +2264,7 @@
         <v>0.56000000000000005</v>
       </c>
     </row>
-    <row r="9" spans="1:5">
+    <row r="9">
       <c r="B9" s="3" t="str">
         <f>CONCATENATE("(",ROUND(SS_admin!B5,3),")")</f>
         <v>(0.044)</v>
@@ -2278,7 +2278,7 @@
         <v>(0.048)</v>
       </c>
     </row>
-    <row r="10" spans="1:5">
+    <row r="10">
       <c r="A10" s="1" t="s">
         <v>5</v>
       </c>
@@ -2296,7 +2296,7 @@
       </c>
       <c r="E10" s="4"/>
     </row>
-    <row r="11" spans="1:5" ht="15.75" thickBot="1">
+    <row r="11" ht="15.75" thickBot="true">
       <c r="A11" s="2"/>
       <c r="B11" s="15" t="s">
         <v>15</v>
@@ -2305,7 +2305,7 @@
       <c r="D11" s="15"/>
       <c r="E11" s="15"/>
     </row>
-    <row r="12" spans="1:5" ht="15.75" thickTop="1">
+    <row r="12" ht="15.75" thickTop="true">
       <c r="A12" t="s">
         <v>8</v>
       </c>
@@ -2326,7 +2326,7 @@
         <v>0.51</v>
       </c>
     </row>
-    <row r="13" spans="1:5">
+    <row r="13">
       <c r="B13" s="3" t="str">
         <f>CONCATENATE("(",ROUND(SS_survey!B3,0),")")</f>
         <v>(186)</v>
@@ -2340,7 +2340,7 @@
         <v>(172)</v>
       </c>
     </row>
-    <row r="14" spans="1:5">
+    <row r="14">
       <c r="A14" t="s">
         <v>26</v>
       </c>
@@ -2361,7 +2361,7 @@
         <v>0.67</v>
       </c>
     </row>
-    <row r="15" spans="1:5">
+    <row r="15">
       <c r="B15" s="3" t="str">
         <f>CONCATENATE("(",ROUND(SS_survey!B5,3),")")</f>
         <v>(0.024)</v>
@@ -2375,7 +2375,7 @@
         <v>(0.02)</v>
       </c>
     </row>
-    <row r="16" spans="1:5">
+    <row r="16">
       <c r="A16" t="s">
         <v>16</v>
       </c>
@@ -2396,7 +2396,7 @@
         <v>0.89</v>
       </c>
     </row>
-    <row r="17" spans="1:5">
+    <row r="17">
       <c r="B17" s="3" t="str">
         <f>CONCATENATE("(",ROUND(SS_survey!B7,2),")")</f>
         <v>(0.02)</v>
@@ -2410,7 +2410,7 @@
         <v>(0.01)</v>
       </c>
     </row>
-    <row r="18" spans="1:5">
+    <row r="18">
       <c r="A18" t="s">
         <v>17</v>
       </c>
@@ -2431,7 +2431,7 @@
         <v>0.28999999999999998</v>
       </c>
     </row>
-    <row r="19" spans="1:5">
+    <row r="19">
       <c r="B19" s="3" t="str">
         <f>CONCATENATE("(",ROUND(SS_survey!B9,3),")")</f>
         <v>(0.028)</v>
@@ -2445,7 +2445,7 @@
         <v>(0.021)</v>
       </c>
     </row>
-    <row r="20" spans="1:5">
+    <row r="20">
       <c r="A20" t="s">
         <v>9</v>
       </c>
@@ -2466,7 +2466,7 @@
         <v>0.09</v>
       </c>
     </row>
-    <row r="21" spans="1:5">
+    <row r="21">
       <c r="B21" s="3" t="str">
         <f>CONCATENATE("(",ROUND(SS_survey!B11,3),")")</f>
         <v>(0.721)</v>
@@ -2480,7 +2480,7 @@
         <v>(0.582)</v>
       </c>
     </row>
-    <row r="22" spans="1:5">
+    <row r="22">
       <c r="A22" t="s">
         <v>18</v>
       </c>
@@ -2501,7 +2501,7 @@
         <v>0.25</v>
       </c>
     </row>
-    <row r="23" spans="1:5">
+    <row r="23">
       <c r="B23" s="3">
         <f>ROUND(SS_survey!B13,2)</f>
         <v>0.02</v>
@@ -2515,7 +2515,7 @@
         <v>(0.011)</v>
       </c>
     </row>
-    <row r="24" spans="1:5">
+    <row r="24">
       <c r="A24" t="s">
         <v>7</v>
       </c>
@@ -2536,7 +2536,7 @@
         <v>0.73</v>
       </c>
     </row>
-    <row r="25" spans="1:5">
+    <row r="25">
       <c r="B25" s="3" t="str">
         <f>CONCATENATE("(",ROUND(SS_survey!B15,3),")")</f>
         <v>(0.688)</v>
@@ -2550,7 +2550,7 @@
         <v>(0.792)</v>
       </c>
     </row>
-    <row r="26" spans="1:5">
+    <row r="26">
       <c r="A26" t="s">
         <v>27</v>
       </c>
@@ -2571,7 +2571,7 @@
         <v>0.88</v>
       </c>
     </row>
-    <row r="27" spans="1:5">
+    <row r="27">
       <c r="B27" s="3" t="str">
         <f>CONCATENATE("(",ROUND(SS_survey!B17,3),")")</f>
         <v>(0.023)</v>
@@ -2585,7 +2585,7 @@
         <v>(0.02)</v>
       </c>
     </row>
-    <row r="28" spans="1:5">
+    <row r="28">
       <c r="A28" s="11" t="s">
         <v>19</v>
       </c>
@@ -2606,7 +2606,7 @@
         <v>0.84</v>
       </c>
     </row>
-    <row r="29" spans="1:5">
+    <row r="29">
       <c r="B29" s="3" t="str">
         <f>CONCATENATE("(",ROUND(SS_survey!B19,3),")")</f>
         <v>(0.027)</v>
@@ -2620,7 +2620,7 @@
         <v>(0.018)</v>
       </c>
     </row>
-    <row r="30" spans="1:5" ht="15.75" thickBot="1">
+    <row r="30" ht="15.75" thickBot="true">
       <c r="A30" s="2" t="s">
         <v>5</v>
       </c>
@@ -2638,7 +2638,7 @@
       </c>
       <c r="E30" s="5"/>
     </row>
-    <row r="31" spans="1:5" ht="15.75" thickTop="1"/>
+    <row r="31" ht="15.75" thickTop="true"/>
   </sheetData>
   <mergeCells count="4">
     <mergeCell ref="B2:E2"/>
@@ -2651,7 +2651,7 @@
 </file>
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{754403B8-1DA5-4CBA-B8B6-94BFF0A849DB}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{754403B8-1DA5-4CBA-B8B6-94BFF0A849DB}">
   <dimension ref="A3:E13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -2660,28 +2660,28 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="26.28515625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="7.140625" style="3" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="10.140625" style="3" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="6.5703125" style="3" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="6.5703125" style="3" customWidth="1"/>
+    <col min="1" max="1" width="26.28515625" bestFit="true" customWidth="true"/>
+    <col min="2" max="2" width="7.140625" style="3" bestFit="true" customWidth="true"/>
+    <col min="3" max="3" width="10.140625" style="3" bestFit="true" customWidth="true"/>
+    <col min="4" max="4" width="6.5703125" style="3" bestFit="true" customWidth="true"/>
+    <col min="5" max="5" width="6.5703125" style="3" customWidth="true"/>
   </cols>
   <sheetData>
-    <row r="3" spans="1:5" ht="15.75" thickBot="1">
+    <row r="3" ht="15.75" thickBot="true">
       <c r="A3" s="10"/>
       <c r="B3" s="13"/>
       <c r="C3" s="13"/>
       <c r="D3" s="13"/>
       <c r="E3" s="13"/>
     </row>
-    <row r="4" spans="1:5">
+    <row r="4">
       <c r="C4" s="14" t="s">
         <v>14</v>
       </c>
       <c r="D4" s="14"/>
       <c r="E4" s="14"/>
     </row>
-    <row r="5" spans="1:5" ht="16.5" customHeight="1" thickBot="1">
+    <row r="5" ht="16.5" customHeight="true" thickBot="true">
       <c r="A5" s="9"/>
       <c r="B5" s="7" t="s">
         <v>1</v>
@@ -2696,7 +2696,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="6" spans="1:5" ht="16.5" customHeight="1" thickTop="1">
+    <row r="6" ht="16.5" customHeight="true" thickTop="true">
       <c r="A6" t="s">
         <v>11</v>
       </c>
@@ -2717,7 +2717,7 @@
         <v>0.52</v>
       </c>
     </row>
-    <row r="7" spans="1:5" ht="16.5" customHeight="1">
+    <row r="7" ht="16.5" customHeight="true">
       <c r="B7" s="3" t="str">
         <f>CONCATENATE("(",ROUND(SS_att!B3,1),")")</f>
         <v>(3)</v>
@@ -2731,7 +2731,7 @@
         <v>(1.8)</v>
       </c>
     </row>
-    <row r="8" spans="1:5" ht="16.5" customHeight="1">
+    <row r="8" ht="16.5" customHeight="true">
       <c r="A8" s="6" t="s">
         <v>22</v>
       </c>
@@ -2752,7 +2752,7 @@
         <v>0.62</v>
       </c>
     </row>
-    <row r="9" spans="1:5" ht="16.5" customHeight="1">
+    <row r="9" ht="16.5" customHeight="true">
       <c r="A9" s="6"/>
       <c r="B9" s="3" t="str">
         <f>CONCATENATE("(",ROUND(SS_att!B9,2),")")</f>
@@ -2767,7 +2767,7 @@
         <v>(0.01)</v>
       </c>
     </row>
-    <row r="10" spans="1:5" ht="16.5" customHeight="1">
+    <row r="10" ht="16.5" customHeight="true">
       <c r="A10" t="s">
         <v>12</v>
       </c>
@@ -2788,7 +2788,7 @@
         <v>0.62</v>
       </c>
     </row>
-    <row r="11" spans="1:5" ht="16.5" customHeight="1">
+    <row r="11" ht="16.5" customHeight="true">
       <c r="B11" s="3" t="str">
         <f>CONCATENATE("(",ROUND(SS_att!B11,2),")")</f>
         <v>(0.02)</v>
@@ -2802,7 +2802,7 @@
         <v>(0.01)</v>
       </c>
     </row>
-    <row r="12" spans="1:5" ht="15.75" thickBot="1">
+    <row r="12" ht="15.75" thickBot="true">
       <c r="A12" s="2" t="s">
         <v>5</v>
       </c>
@@ -2820,7 +2820,7 @@
       </c>
       <c r="E12" s="5"/>
     </row>
-    <row r="13" spans="1:5" ht="15.75" thickTop="1"/>
+    <row r="13" ht="15.75" thickTop="true"/>
   </sheetData>
   <mergeCells count="2">
     <mergeCell ref="B3:E3"/>

</xml_diff>

<commit_message>
revision after jpe submission
</commit_message>
<xml_diff>
--- a/Tables/SS.xlsx
+++ b/Tables/SS.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26529"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26827"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\isaac\Dropbox\Apps\Overleaf\Donde2022\Tables\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{81E3DE23-7774-481C-8739-DC27504D8DD5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9EFB68CC-00D9-4501-9F3E-C7918637F11C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-22395" yWindow="3615" windowWidth="21600" windowHeight="11175" firstSheet="2" activeTab="5"/>
+    <workbookView xWindow="-22815" yWindow="-16320" windowWidth="29040" windowHeight="15720" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="SS_admin" sheetId="1" r:id="rId1"/>
@@ -22,7 +22,7 @@
     <sheet name="SS" sheetId="5" r:id="rId7"/>
     <sheet name="Attrition" sheetId="6" r:id="rId8"/>
   </sheets>
-  <calcPr calcId="191029" fullCalcOnLoad="true"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" count="52" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="28">
   <si>
     <t>Choice</t>
   </si>
@@ -129,8 +129,8 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing">
-  <fonts count="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <name val="Calibri"/>
@@ -207,39 +207,39 @@
   </cellStyleXfs>
   <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="true"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="true"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="true">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="true" applyAlignment="true">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="true" applyAlignment="true">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="true">
-      <alignment wrapText="true"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="true" applyAlignment="true">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="true">
-      <alignment horizontal="center" wrapText="true"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="true" applyAlignment="true">
-      <alignment wrapText="true"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="true"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="true"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="true"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="true" applyAlignment="true">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="true" applyAlignment="true">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="true" applyAlignment="true">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -260,7 +260,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -411,7 +411,7 @@
         <a:solidFill>
           <a:schemeClr val="phClr"/>
         </a:solidFill>
-        <a:gradFill rotWithShape="true">
+        <a:gradFill rotWithShape="1">
           <a:gsLst>
             <a:gs pos="0">
               <a:schemeClr val="phClr">
@@ -435,9 +435,9 @@
               </a:schemeClr>
             </a:gs>
           </a:gsLst>
-          <a:lin ang="5400000" scaled="false"/>
+          <a:lin ang="5400000" scaled="0"/>
         </a:gradFill>
-        <a:gradFill rotWithShape="true">
+        <a:gradFill rotWithShape="1">
           <a:gsLst>
             <a:gs pos="0">
               <a:schemeClr val="phClr">
@@ -461,7 +461,7 @@
               </a:schemeClr>
             </a:gs>
           </a:gsLst>
-          <a:lin ang="5400000" scaled="false"/>
+          <a:lin ang="5400000" scaled="0"/>
         </a:gradFill>
       </a:fillStyleLst>
       <a:lnStyleLst>
@@ -496,7 +496,7 @@
         </a:effectStyle>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="false">
+            <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="0">
               <a:srgbClr val="000000">
                 <a:alpha val="63000"/>
               </a:srgbClr>
@@ -514,7 +514,7 @@
             <a:satMod val="170000"/>
           </a:schemeClr>
         </a:solidFill>
-        <a:gradFill rotWithShape="true">
+        <a:gradFill rotWithShape="1">
           <a:gsLst>
             <a:gs pos="0">
               <a:schemeClr val="phClr">
@@ -539,7 +539,7 @@
               </a:schemeClr>
             </a:gs>
           </a:gsLst>
-          <a:lin ang="5400000" scaled="false"/>
+          <a:lin ang="5400000" scaled="0"/>
         </a:gradFill>
       </a:bgFillStyleLst>
     </a:fmtScheme>
@@ -555,78 +555,78 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="B2:L6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="M11" sqref="A1:M11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData>
-    <row r="2">
+    <row r="2" spans="2:12" x14ac:dyDescent="0.35">
       <c r="B2">
-        <v>2267.457627118644</v>
+        <v>2267.4576271186443</v>
       </c>
       <c r="C2">
-        <v>2162.484646878198</v>
+        <v>2162.4846468781984</v>
       </c>
       <c r="D2">
         <v>2222.993023255814</v>
       </c>
       <c r="E2">
-        <v>2216.722239847716</v>
+        <v>2216.7222398477156</v>
       </c>
       <c r="L2">
-        <v>0.6450310832320212</v>
-      </c>
-    </row>
-    <row r="3">
+        <v>0.64503108323202052</v>
+      </c>
+    </row>
+    <row r="3" spans="2:12" x14ac:dyDescent="0.35">
       <c r="B3">
-        <v>75.87408826054524</v>
+        <v>75.874088260545236</v>
       </c>
       <c r="C3">
-        <v>83.12759277659441</v>
+        <v>83.127592776594426</v>
       </c>
       <c r="D3">
-        <v>65.75042610345361</v>
+        <v>65.750426103453577</v>
       </c>
       <c r="E3">
-        <v>42.93661545047494</v>
-      </c>
-    </row>
-    <row r="4">
+        <v>42.936615450474939</v>
+      </c>
+    </row>
+    <row r="4" spans="2:12" x14ac:dyDescent="0.35">
       <c r="B4">
-        <v>0.8796610169491526</v>
+        <v>0.87966101694915255</v>
       </c>
       <c r="C4">
-        <v>0.8940634595701126</v>
+        <v>0.89406345957011257</v>
       </c>
       <c r="D4">
-        <v>0.8310077519379845</v>
+        <v>0.83100775193798448</v>
       </c>
       <c r="E4">
         <v>0.8642131979695431</v>
       </c>
       <c r="L4">
-        <v>0.560273244252105</v>
-      </c>
-    </row>
-    <row r="5">
+        <v>0.56027324425210501</v>
+      </c>
+    </row>
+    <row r="5" spans="2:12" x14ac:dyDescent="0.35">
       <c r="B5">
-        <v>0.043632089264598</v>
+        <v>4.3632089264597995E-2</v>
       </c>
       <c r="C5">
-        <v>0.03487149126010652</v>
+        <v>3.4871491260106517E-2</v>
       </c>
       <c r="D5">
-        <v>0.04790199632869788</v>
+        <v>4.7901996328697884E-2</v>
       </c>
       <c r="E5">
-        <v>0.02557757789336666</v>
-      </c>
-    </row>
-    <row r="6">
+        <v>2.5577577893366663E-2</v>
+      </c>
+    </row>
+    <row r="6" spans="2:12" x14ac:dyDescent="0.35">
       <c r="B6">
         <v>1770</v>
       </c>
@@ -646,47 +646,47 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="B2:L11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="P21" sqref="A1:P21"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData>
-    <row r="2">
+    <row r="2" spans="2:12" x14ac:dyDescent="0.35">
       <c r="B2">
-        <v>30.46153846153846</v>
+        <v>32.333333333333336</v>
       </c>
       <c r="C2">
-        <v>33.76666666666667</v>
+        <v>34.15</v>
       </c>
       <c r="D2">
-        <v>38.82857142857143</v>
+        <v>37.134328358208954</v>
       </c>
       <c r="E2">
-        <v>34.76923076923077</v>
+        <v>34.752808988764045</v>
       </c>
       <c r="L2">
-        <v>0.1584710080897333</v>
-      </c>
-    </row>
-    <row r="3">
+        <v>0.572023905328648</v>
+      </c>
+    </row>
+    <row r="3" spans="2:12" x14ac:dyDescent="0.35">
       <c r="B3">
-        <v>2.790776331556584</v>
+        <v>3.3381533778207677</v>
       </c>
       <c r="C3">
-        <v>2.906583863434686</v>
+        <v>2.9165246131670202</v>
       </c>
       <c r="D3">
-        <v>3.320491085220305</v>
+        <v>3.1781063232804376</v>
       </c>
       <c r="E3">
-        <v>1.79376807323629</v>
-      </c>
-    </row>
-    <row r="4">
+        <v>1.8159027540097266</v>
+      </c>
+    </row>
+    <row r="4" spans="2:12" x14ac:dyDescent="0.35">
       <c r="B4">
         <v>1770</v>
       </c>
@@ -700,66 +700,66 @@
         <v>6304</v>
       </c>
     </row>
-    <row r="8">
+    <row r="8" spans="2:12" x14ac:dyDescent="0.35">
       <c r="B8">
-        <v>0.9753694581280788</v>
+        <v>0.97536945812807885</v>
       </c>
       <c r="C8">
-        <v>0.9651315789473685</v>
+        <v>0.96513157894736845</v>
       </c>
       <c r="D8">
         <v>0.9710926016658501</v>
       </c>
       <c r="E8">
-        <v>0.9704937775993577</v>
+        <v>0.97049377759935773</v>
       </c>
       <c r="L8">
-        <v>0.6189412811417327</v>
-      </c>
-    </row>
-    <row r="9">
+        <v>0.61894128114173319</v>
+      </c>
+    </row>
+    <row r="9" spans="2:12" x14ac:dyDescent="0.35">
       <c r="B9">
-        <v>0.00556410496581999</v>
+        <v>5.564104965819992E-3</v>
       </c>
       <c r="C9">
-        <v>0.009055840460278583</v>
+        <v>9.0558404602785851E-3</v>
       </c>
       <c r="D9">
-        <v>0.007770579449781894</v>
+        <v>7.7705794497818937E-3</v>
       </c>
       <c r="E9">
-        <v>0.00447621592777956</v>
-      </c>
-    </row>
-    <row r="10">
+        <v>4.4762159277795593E-3</v>
+      </c>
+    </row>
+    <row r="10" spans="2:12" x14ac:dyDescent="0.35">
       <c r="B10">
-        <v>0.7872576177285319</v>
+        <v>0.78725761772853187</v>
       </c>
       <c r="C10">
-        <v>0.7581047381546134</v>
+        <v>0.75810473815461343</v>
       </c>
       <c r="D10">
-        <v>0.7733990147783252</v>
+        <v>0.77339901477832518</v>
       </c>
       <c r="E10">
         <v>0.772522871763064</v>
       </c>
       <c r="L10">
-        <v>0.6170034126071788</v>
-      </c>
-    </row>
-    <row r="11">
+        <v>0.61700341260717884</v>
+      </c>
+    </row>
+    <row r="11" spans="2:12" x14ac:dyDescent="0.35">
       <c r="B11">
-        <v>0.01787061830945753</v>
+        <v>1.7870618309457527E-2</v>
       </c>
       <c r="C11">
-        <v>0.02408215491412533</v>
+        <v>2.4082154914125332E-2</v>
       </c>
       <c r="D11">
-        <v>0.02495667269143001</v>
+        <v>2.4956672691430013E-2</v>
       </c>
       <c r="E11">
-        <v>0.01365506059590319</v>
+        <v>1.3655060595903191E-2</v>
       </c>
     </row>
   </sheetData>
@@ -768,295 +768,295 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="B2:L23"/>
   <sheetViews>
-    <sheetView topLeftCell="A20" workbookViewId="0">
-      <selection activeCell="N31" sqref="B1:N31"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D15" sqref="D15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData>
-    <row r="2">
+    <row r="2" spans="2:12" x14ac:dyDescent="0.35">
       <c r="B2">
-        <v>4084.044748373869</v>
+        <v>4084.0447483738694</v>
       </c>
       <c r="C2">
         <v>3876.572927111064</v>
       </c>
       <c r="D2">
-        <v>4173.141363366096</v>
+        <v>4173.1413633660959</v>
       </c>
       <c r="E2">
-        <v>4057.771802359279</v>
+        <v>4057.7718023592788</v>
       </c>
       <c r="L2">
-        <v>0.5074136364776338</v>
-      </c>
-    </row>
-    <row r="3">
+        <v>0.50741363647763404</v>
+      </c>
+    </row>
+    <row r="3" spans="2:12" x14ac:dyDescent="0.35">
       <c r="B3">
-        <v>186.3253082221647</v>
+        <v>186.32530822216472</v>
       </c>
       <c r="C3">
-        <v>193.3240715406064</v>
+        <v>193.32407154060641</v>
       </c>
       <c r="D3">
-        <v>171.5815234090987</v>
+        <v>171.58152340909876</v>
       </c>
       <c r="E3">
-        <v>106.6210974172743</v>
-      </c>
-    </row>
-    <row r="4">
+        <v>106.62109741727424</v>
+      </c>
+    </row>
+    <row r="4" spans="2:12" x14ac:dyDescent="0.35">
       <c r="B4">
         <v>0.1870631315668515</v>
       </c>
       <c r="C4">
-        <v>0.2094701654377669</v>
+        <v>0.20947016543776692</v>
       </c>
       <c r="D4">
-        <v>0.1837412624821796</v>
+        <v>0.18374126248217962</v>
       </c>
       <c r="E4">
-        <v>0.1928579542720172</v>
+        <v>0.19285795427201724</v>
       </c>
       <c r="L4">
-        <v>0.6725660484592921</v>
-      </c>
-    </row>
-    <row r="5">
+        <v>0.67256604845929213</v>
+      </c>
+    </row>
+    <row r="5" spans="2:12" x14ac:dyDescent="0.35">
       <c r="B5">
-        <v>0.02443309134662668</v>
+        <v>2.4433091346626679E-2</v>
       </c>
       <c r="C5">
-        <v>0.02283124052149185</v>
+        <v>2.2831240521491845E-2</v>
       </c>
       <c r="D5">
-        <v>0.02024631264295361</v>
+        <v>2.0246312642953609E-2</v>
       </c>
       <c r="E5">
-        <v>0.01289510279740332</v>
-      </c>
-    </row>
-    <row r="6">
+        <v>1.2895102797403319E-2</v>
+      </c>
+    </row>
+    <row r="6" spans="2:12" x14ac:dyDescent="0.35">
       <c r="B6">
-        <v>0.1381578947368421</v>
+        <v>0.13815789473684212</v>
       </c>
       <c r="C6">
-        <v>0.1282352941176471</v>
+        <v>0.12823529411764706</v>
       </c>
       <c r="D6">
-        <v>0.1266201395812562</v>
+        <v>0.12662013958125623</v>
       </c>
       <c r="E6">
-        <v>0.1305013394565633</v>
+        <v>0.13050133945656334</v>
       </c>
       <c r="L6">
-        <v>0.8896495042601654</v>
-      </c>
-    </row>
-    <row r="7">
+        <v>0.88964950426016542</v>
+      </c>
+    </row>
+    <row r="7" spans="2:12" x14ac:dyDescent="0.35">
       <c r="B7">
-        <v>0.02064639659507228</v>
+        <v>2.0646396595072284E-2</v>
       </c>
       <c r="C7">
-        <v>0.01427153837750952</v>
+        <v>1.4271538377509519E-2</v>
       </c>
       <c r="D7">
-        <v>0.01298902587565687</v>
+        <v>1.2989025875656875E-2</v>
       </c>
       <c r="E7">
-        <v>0.009035761191728721</v>
-      </c>
-    </row>
-    <row r="8">
+        <v>9.0357611917287195E-3</v>
+      </c>
+    </row>
+    <row r="8" spans="2:12" x14ac:dyDescent="0.35">
       <c r="B8">
-        <v>0.6247443762781186</v>
+        <v>0.62474437627811863</v>
       </c>
       <c r="C8">
-        <v>0.5884509624197983</v>
+        <v>0.58845096241979833</v>
       </c>
       <c r="D8">
-        <v>0.6517595307917888</v>
+        <v>0.65175953079178883</v>
       </c>
       <c r="E8">
-        <v>0.6239440722400234</v>
+        <v>0.62394407224002335</v>
       </c>
       <c r="L8">
-        <v>0.2925995970750369</v>
-      </c>
-    </row>
-    <row r="9">
+        <v>0.29259959707503691</v>
+      </c>
+    </row>
+    <row r="9" spans="2:12" x14ac:dyDescent="0.35">
       <c r="B9">
-        <v>0.02808027340316118</v>
+        <v>2.8080273403161184E-2</v>
       </c>
       <c r="C9">
-        <v>0.03554672107016062</v>
+        <v>3.5546721070160631E-2</v>
       </c>
       <c r="D9">
-        <v>0.02101418987928844</v>
+        <v>2.101418987928844E-2</v>
       </c>
       <c r="E9">
-        <v>0.01670163240458039</v>
-      </c>
-    </row>
-    <row r="10">
+        <v>1.6701632404580391E-2</v>
+      </c>
+    </row>
+    <row r="10" spans="2:12" x14ac:dyDescent="0.35">
       <c r="B10">
-        <v>91.88669201520912</v>
+        <v>91.886692015209121</v>
       </c>
       <c r="C10">
-        <v>91.65214285714286</v>
+        <v>91.652142857142863</v>
       </c>
       <c r="D10">
-        <v>93.6109947643979</v>
+        <v>93.610994764397901</v>
       </c>
       <c r="E10">
-        <v>92.52778378378379</v>
+        <v>92.527783783783789</v>
       </c>
       <c r="L10">
-        <v>0.093375432500357</v>
-      </c>
-    </row>
-    <row r="11">
+        <v>9.3375432500357E-2</v>
+      </c>
+    </row>
+    <row r="11" spans="2:12" x14ac:dyDescent="0.35">
       <c r="B11">
-        <v>0.7214272306460148</v>
+        <v>0.72142723064601477</v>
       </c>
       <c r="C11">
-        <v>1.031496976703081</v>
+        <v>1.0314969767030806</v>
       </c>
       <c r="D11">
-        <v>0.5816569306404544</v>
+        <v>0.58165693064045443</v>
       </c>
       <c r="E11">
-        <v>0.4502856911185265</v>
-      </c>
-    </row>
-    <row r="12">
+        <v>0.45028569111852645</v>
+      </c>
+    </row>
+    <row r="12" spans="2:12" x14ac:dyDescent="0.35">
       <c r="B12">
         <v>0.8693877551020408</v>
       </c>
       <c r="C12">
-        <v>0.8871841155234657</v>
+        <v>0.88718411552346566</v>
       </c>
       <c r="D12">
         <v>0.9007246376811594</v>
       </c>
       <c r="E12">
-        <v>0.8875432525951558</v>
+        <v>0.88754325259515576</v>
       </c>
       <c r="L12">
         <v>0.2521838227756053</v>
       </c>
     </row>
-    <row r="13">
+    <row r="13" spans="2:12" x14ac:dyDescent="0.35">
       <c r="B13">
-        <v>0.01542954967076077</v>
+        <v>1.5429549670760771E-2</v>
       </c>
       <c r="C13">
-        <v>0.01276990565307838</v>
+        <v>1.2769905653078381E-2</v>
       </c>
       <c r="D13">
-        <v>0.01110750508269111</v>
+        <v>1.1107505082691111E-2</v>
       </c>
       <c r="E13">
-        <v>0.007510065293318159</v>
-      </c>
-    </row>
-    <row r="14">
+        <v>7.5100652933181595E-3</v>
+      </c>
+    </row>
+    <row r="14" spans="2:12" x14ac:dyDescent="0.35">
       <c r="B14">
-        <v>43.3169968717414</v>
+        <v>43.316996871741395</v>
       </c>
       <c r="C14">
-        <v>42.85291396854764</v>
+        <v>42.852913968547639</v>
       </c>
       <c r="D14">
-        <v>43.82113821138211</v>
+        <v>43.821138211382113</v>
       </c>
       <c r="E14">
         <v>43.37017388741527</v>
       </c>
       <c r="L14">
-        <v>0.7294742073368279</v>
-      </c>
-    </row>
-    <row r="15">
+        <v>0.72947420733682788</v>
+      </c>
+    </row>
+    <row r="15" spans="2:12" x14ac:dyDescent="0.35">
       <c r="B15">
-        <v>0.6876570599320564</v>
+        <v>0.68765705993205639</v>
       </c>
       <c r="C15">
-        <v>0.9493469201888045</v>
+        <v>0.94934692018880396</v>
       </c>
       <c r="D15">
-        <v>0.7916996712932627</v>
+        <v>0.79169967129326257</v>
       </c>
       <c r="E15">
-        <v>0.4758589833983667</v>
-      </c>
-    </row>
-    <row r="16">
+        <v>0.47585898339836669</v>
+      </c>
+    </row>
+    <row r="16" spans="2:12" x14ac:dyDescent="0.35">
       <c r="B16">
         <v>0.7275390625</v>
       </c>
       <c r="C16">
-        <v>0.7209705372616985</v>
+        <v>0.72097053726169846</v>
       </c>
       <c r="D16">
-        <v>0.7124749833222148</v>
+        <v>0.71247498332221482</v>
       </c>
       <c r="E16">
         <v>0.7193364155561599</v>
       </c>
       <c r="L16">
-        <v>0.8788054763606953</v>
-      </c>
-    </row>
-    <row r="17">
+        <v>0.87880547636069528</v>
+      </c>
+    </row>
+    <row r="17" spans="2:12" x14ac:dyDescent="0.35">
       <c r="B17">
-        <v>0.02272282987183911</v>
+        <v>2.2722829871839111E-2</v>
       </c>
       <c r="C17">
-        <v>0.01871985071743971</v>
+        <v>1.8719850717439725E-2</v>
       </c>
       <c r="D17">
-        <v>0.01980735062092765</v>
+        <v>1.9807350620927644E-2</v>
       </c>
       <c r="E17">
-        <v>0.01189962851181989</v>
-      </c>
-    </row>
-    <row r="18">
+        <v>1.1899628511819891E-2</v>
+      </c>
+    </row>
+    <row r="18" spans="2:12" x14ac:dyDescent="0.35">
       <c r="B18">
-        <v>0.6586134453781513</v>
+        <v>0.65861344537815125</v>
       </c>
       <c r="C18">
-        <v>0.6685185185185185</v>
+        <v>0.66851851851851851</v>
       </c>
       <c r="D18">
-        <v>0.6515151515151515</v>
+        <v>0.65151515151515149</v>
       </c>
       <c r="E18">
-        <v>0.6590095465393795</v>
+        <v>0.65900954653937949</v>
       </c>
       <c r="L18">
-        <v>0.8362743251137983</v>
-      </c>
-    </row>
-    <row r="19">
+        <v>0.83627432511379829</v>
+      </c>
+    </row>
+    <row r="19" spans="2:12" x14ac:dyDescent="0.35">
       <c r="B19">
-        <v>0.02708449453616807</v>
+        <v>2.7084494536168072E-2</v>
       </c>
       <c r="C19">
-        <v>0.02245117168137609</v>
+        <v>2.245117168137609E-2</v>
       </c>
       <c r="D19">
-        <v>0.01763021297150332</v>
+        <v>1.7630212971503318E-2</v>
       </c>
       <c r="E19">
-        <v>0.01264015748271608</v>
-      </c>
-    </row>
-    <row r="20">
+        <v>1.2640157482716076E-2</v>
+      </c>
+    </row>
+    <row r="20" spans="2:12" x14ac:dyDescent="0.35">
       <c r="B20">
         <v>1770</v>
       </c>
@@ -1070,7 +1070,7 @@
         <v>6304</v>
       </c>
     </row>
-    <row r="23">
+    <row r="23" spans="2:12" x14ac:dyDescent="0.35">
       <c r="B23">
         <v>1386</v>
       </c>
@@ -1087,78 +1087,78 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
   <dimension ref="B2:L6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="L3" sqref="L3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData>
-    <row r="2">
+    <row r="2" spans="2:12" x14ac:dyDescent="0.35">
       <c r="B2">
-        <v>2199.235209235209</v>
+        <v>2199.2352092352094</v>
       </c>
       <c r="C2">
-        <v>2196.041524846834</v>
+        <v>2196.0415248468344</v>
       </c>
       <c r="D2">
-        <v>2216.417759838547</v>
+        <v>2216.4177598385468</v>
       </c>
       <c r="E2">
-        <v>2205.305974777755</v>
+        <v>2205.3059747777547</v>
       </c>
       <c r="L2">
-        <v>0.9841599107007903</v>
-      </c>
-    </row>
-    <row r="3">
+        <v>0.98415991070079034</v>
+      </c>
+    </row>
+    <row r="3" spans="2:12" x14ac:dyDescent="0.35">
       <c r="B3">
-        <v>85.69161747448106</v>
+        <v>85.691617474481063</v>
       </c>
       <c r="C3">
-        <v>105.6266892139488</v>
+        <v>105.62668921394878</v>
       </c>
       <c r="D3">
-        <v>80.61197757998926</v>
+        <v>80.611977579989215</v>
       </c>
       <c r="E3">
-        <v>51.99667574712315</v>
-      </c>
-    </row>
-    <row r="4">
+        <v>51.996675747123149</v>
+      </c>
+    </row>
+    <row r="4" spans="2:12" x14ac:dyDescent="0.35">
       <c r="B4">
-        <v>0.8759018759018758</v>
+        <v>0.87590187590187585</v>
       </c>
       <c r="C4">
-        <v>0.8856364874063989</v>
+        <v>0.88563648740639889</v>
       </c>
       <c r="D4">
-        <v>0.8471241170534813</v>
+        <v>0.84712411705348134</v>
       </c>
       <c r="E4">
-        <v>0.8670663634484185</v>
+        <v>0.86706636344841848</v>
       </c>
       <c r="L4">
-        <v>0.8026212323496709</v>
-      </c>
-    </row>
-    <row r="5">
+        <v>0.80262123234967087</v>
+      </c>
+    </row>
+    <row r="5" spans="2:12" x14ac:dyDescent="0.35">
       <c r="B5">
-        <v>0.04482942563051304</v>
+        <v>4.4829425630513044E-2</v>
       </c>
       <c r="C5">
-        <v>0.03803739218949861</v>
+        <v>3.8037392189498614E-2</v>
       </c>
       <c r="D5">
-        <v>0.04532363370188531</v>
+        <v>4.5323633701885309E-2</v>
       </c>
       <c r="E5">
-        <v>0.02533791010635028</v>
-      </c>
-    </row>
-    <row r="6">
+        <v>2.5337910106350277E-2</v>
+      </c>
+    </row>
+    <row r="6" spans="2:12" x14ac:dyDescent="0.35">
       <c r="B6">
         <v>1386</v>
       </c>
@@ -1178,32 +1178,32 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
   <dimension ref="B2:S20"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="Q2" sqref="Q2:S11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="17" max="17" width="9.5703125" bestFit="true" customWidth="true"/>
-    <col min="18" max="18" width="10.42578125" bestFit="true" customWidth="true"/>
-    <col min="19" max="19" width="7.42578125" customWidth="true"/>
+    <col min="17" max="17" width="9.54296875" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="10.453125" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="7.453125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" ht="15.75" thickBot="true">
+    <row r="2" spans="2:19" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B2">
-        <v>0.7333333333333333</v>
+        <v>0.73333333333333328</v>
       </c>
       <c r="C2">
-        <v>0.6893551688843398</v>
+        <v>0.68935516888433979</v>
       </c>
       <c r="D2">
-        <v>0.7054263565891473</v>
+        <v>0.70542635658914732</v>
       </c>
       <c r="E2">
-        <v>0.7082804568527918</v>
+        <v>0.70828045685279184</v>
       </c>
       <c r="L2">
         <v>0.3894723057903044</v>
@@ -1224,18 +1224,18 @@
         <v>25</v>
       </c>
     </row>
-    <row r="3" ht="15.75" thickTop="true">
+    <row r="3" spans="2:19" ht="15" thickTop="1" x14ac:dyDescent="0.35">
       <c r="B3">
-        <v>0.02222713340725871</v>
+        <v>2.2227133407258709E-2</v>
       </c>
       <c r="C3">
-        <v>0.02394555925968419</v>
+        <v>2.3945559259684196E-2</v>
       </c>
       <c r="D3">
-        <v>0.02448740630667276</v>
+        <v>2.4487406306672753E-2</v>
       </c>
       <c r="E3">
-        <v>0.01405414443820463</v>
+        <v>1.4054144438204628E-2</v>
       </c>
       <c r="N3">
         <v>1</v>
@@ -1255,18 +1255,18 @@
         <v>4.6399999999999997</v>
       </c>
     </row>
-    <row r="4">
+    <row r="4" spans="2:19" x14ac:dyDescent="0.35">
       <c r="B4">
-        <v>0.4926553672316384</v>
+        <v>0.49265536723163844</v>
       </c>
       <c r="C4">
-        <v>0.4769703172978506</v>
+        <v>0.47697031729785055</v>
       </c>
       <c r="D4">
-        <v>0.4434108527131783</v>
+        <v>0.44341085271317832</v>
       </c>
       <c r="E4">
-        <v>0.4676395939086294</v>
+        <v>0.46763959390862941</v>
       </c>
       <c r="L4">
         <v>0.2875593605623547</v>
@@ -1289,18 +1289,18 @@
         <v>28.1</v>
       </c>
     </row>
-    <row r="5">
+    <row r="5" spans="2:19" x14ac:dyDescent="0.35">
       <c r="B5">
-        <v>0.02309624009558859</v>
+        <v>2.3096240095588593E-2</v>
       </c>
       <c r="C5">
-        <v>0.02243087678545668</v>
+        <v>2.2430876785456685E-2</v>
       </c>
       <c r="D5">
-        <v>0.02223886561049735</v>
+        <v>2.2238865610497347E-2</v>
       </c>
       <c r="E5">
-        <v>0.01345190962231461</v>
+        <v>1.3451909622314613E-2</v>
       </c>
       <c r="N5">
         <v>3</v>
@@ -1320,21 +1320,21 @@
         <v>28.85</v>
       </c>
     </row>
-    <row r="6">
+    <row r="6" spans="2:19" x14ac:dyDescent="0.35">
       <c r="B6">
-        <v>0.4293785310734463</v>
+        <v>0.42937853107344631</v>
       </c>
       <c r="C6">
-        <v>0.4350051177072671</v>
+        <v>0.43500511770726713</v>
       </c>
       <c r="D6">
-        <v>0.3887596899224806</v>
+        <v>0.38875968992248061</v>
       </c>
       <c r="E6">
-        <v>0.414498730964467</v>
+        <v>0.41449873096446699</v>
       </c>
       <c r="L6">
-        <v>0.1657044792125869</v>
+        <v>0.16570447921258699</v>
       </c>
       <c r="N6">
         <v>4</v>
@@ -1354,18 +1354,18 @@
         <v>30.830000000000002</v>
       </c>
     </row>
-    <row r="7">
+    <row r="7" spans="2:19" x14ac:dyDescent="0.35">
       <c r="B7">
-        <v>0.02253958102147569</v>
+        <v>2.2539581021475692E-2</v>
       </c>
       <c r="C7">
-        <v>0.02127276435362197</v>
+        <v>2.1272764353621975E-2</v>
       </c>
       <c r="D7">
-        <v>0.01715622878949833</v>
+        <v>1.7156228789498337E-2</v>
       </c>
       <c r="E7">
-        <v>0.01185696393078531</v>
+        <v>1.1856963930785313E-2</v>
       </c>
       <c r="N7">
         <v>5</v>
@@ -1385,21 +1385,21 @@
         <v>32.39</v>
       </c>
     </row>
-    <row r="8">
+    <row r="8" spans="2:19" x14ac:dyDescent="0.35">
       <c r="B8">
-        <v>0.5525423728813559</v>
+        <v>0.55254237288135588</v>
       </c>
       <c r="C8">
-        <v>0.5583418628454453</v>
+        <v>0.55834186284544529</v>
       </c>
       <c r="D8">
-        <v>0.5286821705426357</v>
+        <v>0.52868217054263567</v>
       </c>
       <c r="E8">
         <v>0.5445748730964467</v>
       </c>
       <c r="L8">
-        <v>0.5609458710266343</v>
+        <v>0.56094587102663429</v>
       </c>
       <c r="N8">
         <v>6</v>
@@ -1419,18 +1419,18 @@
         <v>35.1</v>
       </c>
     </row>
-    <row r="9">
+    <row r="9" spans="2:19" x14ac:dyDescent="0.35">
       <c r="B9">
-        <v>0.02302171714220681</v>
+        <v>2.3021717142206806E-2</v>
       </c>
       <c r="C9">
-        <v>0.02284086769741038</v>
+        <v>2.284086769741038E-2</v>
       </c>
       <c r="D9">
-        <v>0.01945304700624268</v>
+        <v>1.9453047006242685E-2</v>
       </c>
       <c r="E9">
-        <v>0.01259298623720528</v>
+        <v>1.2592986237205277E-2</v>
       </c>
       <c r="N9">
         <v>7</v>
@@ -1450,21 +1450,21 @@
         <v>41.34</v>
       </c>
     </row>
-    <row r="10">
+    <row r="10" spans="2:19" x14ac:dyDescent="0.35">
       <c r="B10">
-        <v>0.7429378531073446</v>
+        <v>0.74293785310734461</v>
       </c>
       <c r="C10">
         <v>0.7164790174002047</v>
       </c>
       <c r="D10">
-        <v>0.7403100775193798</v>
+        <v>0.74031007751937983</v>
       </c>
       <c r="E10">
-        <v>0.7336611675126904</v>
+        <v>0.73366116751269039</v>
       </c>
       <c r="L10">
-        <v>0.711869330524062</v>
+        <v>0.71186933052406198</v>
       </c>
       <c r="N10">
         <v>8</v>
@@ -1484,18 +1484,18 @@
         <v>56.49</v>
       </c>
     </row>
-    <row r="11" ht="15.75" thickBot="true">
+    <row r="11" spans="2:19" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B11">
-        <v>0.02382493680650932</v>
+        <v>2.3824936806509319E-2</v>
       </c>
       <c r="C11">
-        <v>0.02547756403929634</v>
+        <v>2.5477564039296352E-2</v>
       </c>
       <c r="D11">
-        <v>0.02535814843098096</v>
+        <v>2.5358148430980946E-2</v>
       </c>
       <c r="E11">
-        <v>0.01462507287141228</v>
+        <v>1.4625072871412275E-2</v>
       </c>
       <c r="N11">
         <v>9</v>
@@ -1515,7 +1515,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="12" ht="15.75" thickTop="true">
+    <row r="12" spans="2:19" ht="15" thickTop="1" x14ac:dyDescent="0.35">
       <c r="B12">
         <v>0.5536723163841808</v>
       </c>
@@ -1523,123 +1523,123 @@
         <v>0.5670419651995906</v>
       </c>
       <c r="D12">
-        <v>0.5348837209302325</v>
+        <v>0.53488372093023251</v>
       </c>
       <c r="E12">
-        <v>0.5501269035532995</v>
+        <v>0.55012690355329952</v>
       </c>
       <c r="L12">
-        <v>0.5657910963616903</v>
-      </c>
-    </row>
-    <row r="13">
+        <v>0.56579109636169034</v>
+      </c>
+    </row>
+    <row r="13" spans="2:19" x14ac:dyDescent="0.35">
       <c r="B13">
-        <v>0.02319773674083229</v>
+        <v>2.3197736740832288E-2</v>
       </c>
       <c r="C13">
-        <v>0.02380273921390908</v>
+        <v>2.3802739213909081E-2</v>
       </c>
       <c r="D13">
-        <v>0.01957239944955774</v>
+        <v>1.9572399449557739E-2</v>
       </c>
       <c r="E13">
-        <v>0.01281247883226884</v>
-      </c>
-    </row>
-    <row r="14">
+        <v>1.2812478832268841E-2</v>
+      </c>
+    </row>
+    <row r="14" spans="2:19" x14ac:dyDescent="0.35">
       <c r="B14">
-        <v>0.5418079096045197</v>
+        <v>0.54180790960451974</v>
       </c>
       <c r="C14">
-        <v>0.553224155578301</v>
+        <v>0.55322415557830096</v>
       </c>
       <c r="D14">
-        <v>0.5244186046511627</v>
+        <v>0.52441860465116275</v>
       </c>
       <c r="E14">
-        <v>0.538229695431472</v>
+        <v>0.53822969543147203</v>
       </c>
       <c r="L14">
-        <v>0.5904164505761096</v>
-      </c>
-    </row>
-    <row r="15">
+        <v>0.59041645057610959</v>
+      </c>
+    </row>
+    <row r="15" spans="2:19" x14ac:dyDescent="0.35">
       <c r="B15">
-        <v>0.02302882584840425</v>
+        <v>2.3028825848404249E-2</v>
       </c>
       <c r="C15">
-        <v>0.02263762438473425</v>
+        <v>2.2637624384734246E-2</v>
       </c>
       <c r="D15">
-        <v>0.01794910753771939</v>
+        <v>1.7949107537719389E-2</v>
       </c>
       <c r="E15">
-        <v>0.0121515126440841</v>
-      </c>
-    </row>
-    <row r="16">
+        <v>1.2151512644084097E-2</v>
+      </c>
+    </row>
+    <row r="16" spans="2:19" x14ac:dyDescent="0.35">
       <c r="B16">
         <v>0.5785310734463277</v>
       </c>
       <c r="C16">
-        <v>0.5905834186284544</v>
+        <v>0.59058341862845443</v>
       </c>
       <c r="D16">
-        <v>0.5810077519379845</v>
+        <v>0.58100775193798448</v>
       </c>
       <c r="E16">
-        <v>0.5832804568527918</v>
+        <v>0.58328045685279184</v>
       </c>
       <c r="L16">
-        <v>0.9326726999098225</v>
-      </c>
-    </row>
-    <row r="17">
+        <v>0.93267269990982249</v>
+      </c>
+    </row>
+    <row r="17" spans="2:12" x14ac:dyDescent="0.35">
       <c r="B17">
-        <v>0.02480493244087363</v>
+        <v>2.4804932440873628E-2</v>
       </c>
       <c r="C17">
-        <v>0.0244543397409427</v>
+        <v>2.4454339740942695E-2</v>
       </c>
       <c r="D17">
-        <v>0.02018420555273061</v>
+        <v>2.0184205552730608E-2</v>
       </c>
       <c r="E17">
-        <v>0.01316677672471577</v>
-      </c>
-    </row>
-    <row r="18">
+        <v>1.3166776724715765E-2</v>
+      </c>
+    </row>
+    <row r="18" spans="2:12" x14ac:dyDescent="0.35">
       <c r="B18">
-        <v>0.5378531073446328</v>
+        <v>0.53785310734463276</v>
       </c>
       <c r="C18">
-        <v>0.5527123848515865</v>
+        <v>0.55271238485158647</v>
       </c>
       <c r="D18">
-        <v>0.5116279069767442</v>
+        <v>0.51162790697674421</v>
       </c>
       <c r="E18">
-        <v>0.5317258883248731</v>
+        <v>0.53172588832487311</v>
       </c>
       <c r="L18">
-        <v>0.3864907004892281</v>
-      </c>
-    </row>
-    <row r="19">
+        <v>0.38649070048922801</v>
+      </c>
+    </row>
+    <row r="19" spans="2:12" x14ac:dyDescent="0.35">
       <c r="B19">
-        <v>0.02497582090269404</v>
+        <v>2.497582090269404E-2</v>
       </c>
       <c r="C19">
-        <v>0.02473003962743872</v>
+        <v>2.4730039627438711E-2</v>
       </c>
       <c r="D19">
-        <v>0.01882401910494625</v>
+        <v>1.8824019104946247E-2</v>
       </c>
       <c r="E19">
-        <v>0.01314890352713889</v>
-      </c>
-    </row>
-    <row r="20">
+        <v>1.3148903527138892E-2</v>
+      </c>
+    </row>
+    <row r="20" spans="2:12" x14ac:dyDescent="0.35">
       <c r="B20">
         <v>1770</v>
       </c>
@@ -1659,37 +1659,37 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{67FF63D4-14D6-4F54-BD0D-751B1AD5E68C}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{67FF63D4-14D6-4F54-BD0D-751B1AD5E68C}">
   <dimension ref="A2:E31"/>
   <sheetViews>
-    <sheetView tabSelected="true" topLeftCell="A10" workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="A3" sqref="A3:E30"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="18.140625" bestFit="true" customWidth="true"/>
-    <col min="2" max="2" width="9.7109375" style="3" customWidth="true"/>
-    <col min="3" max="3" width="10.5703125" style="3" customWidth="true"/>
-    <col min="4" max="4" width="7.5703125" style="3" bestFit="true" customWidth="true"/>
-    <col min="5" max="5" width="7.5703125" style="3" customWidth="true"/>
+    <col min="1" max="1" width="18.1796875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="9.7265625" style="3" customWidth="1"/>
+    <col min="3" max="3" width="10.54296875" style="3" customWidth="1"/>
+    <col min="4" max="4" width="7.54296875" style="3" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="7.54296875" style="3" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" ht="15.75" thickBot="true">
+    <row r="2" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A2" s="10"/>
       <c r="B2" s="13"/>
       <c r="C2" s="13"/>
       <c r="D2" s="13"/>
       <c r="E2" s="13"/>
     </row>
-    <row r="3">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.35">
       <c r="C3" s="14" t="s">
         <v>14</v>
       </c>
       <c r="D3" s="14"/>
       <c r="E3" s="14"/>
     </row>
-    <row r="4" s="6" customFormat="true" ht="30">
+    <row r="4" spans="1:5" s="6" customFormat="1" x14ac:dyDescent="0.35">
       <c r="B4" s="8" t="s">
         <v>1</v>
       </c>
@@ -1703,7 +1703,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="5" ht="15.75" thickBot="true">
+    <row r="5" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A5" s="2"/>
       <c r="B5" s="15" t="s">
         <v>20</v>
@@ -1712,7 +1712,7 @@
       <c r="D5" s="15"/>
       <c r="E5" s="15"/>
     </row>
-    <row r="6" ht="15.75" thickTop="true">
+    <row r="6" spans="1:5" ht="15" thickTop="1" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>4</v>
       </c>
@@ -1733,7 +1733,7 @@
         <v>0.98</v>
       </c>
     </row>
-    <row r="7">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.35">
       <c r="B7" s="3" t="str">
         <f>CONCATENATE("(",ROUND(SS_admin_survey!B3,0),")")</f>
         <v>(86)</v>
@@ -1747,7 +1747,7 @@
         <v>(81)</v>
       </c>
     </row>
-    <row r="8">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
         <v>13</v>
       </c>
@@ -1768,7 +1768,7 @@
         <v>0.8</v>
       </c>
     </row>
-    <row r="9">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.35">
       <c r="B9" s="3" t="str">
         <f>CONCATENATE("(",ROUND(SS_admin_survey!B5,3),")")</f>
         <v>(0.045)</v>
@@ -1782,7 +1782,7 @@
         <v>(0.045)</v>
       </c>
     </row>
-    <row r="10">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A10" s="1" t="s">
         <v>5</v>
       </c>
@@ -1800,7 +1800,7 @@
       </c>
       <c r="E10" s="4"/>
     </row>
-    <row r="11" ht="15.75" thickBot="true">
+    <row r="11" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A11" s="2"/>
       <c r="B11" s="15" t="s">
         <v>21</v>
@@ -1809,7 +1809,7 @@
       <c r="D11" s="15"/>
       <c r="E11" s="15"/>
     </row>
-    <row r="12" ht="15.75" thickTop="true">
+    <row r="12" spans="1:5" ht="15" thickTop="1" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
         <v>8</v>
       </c>
@@ -1830,7 +1830,7 @@
         <v>0.39</v>
       </c>
     </row>
-    <row r="13">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.35">
       <c r="B13" s="3" t="str">
         <f>CONCATENATE("(",ROUND(survey_response_rate!B3,3),")")</f>
         <v>(0.022)</v>
@@ -1844,7 +1844,7 @@
         <v>(0.024)</v>
       </c>
     </row>
-    <row r="14">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
         <v>26</v>
       </c>
@@ -1865,7 +1865,7 @@
         <v>0.28999999999999998</v>
       </c>
     </row>
-    <row r="15">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.35">
       <c r="B15" s="3" t="str">
         <f>CONCATENATE("(",ROUND(survey_response_rate!B5,3),")")</f>
         <v>(0.023)</v>
@@ -1879,7 +1879,7 @@
         <v>(0.022)</v>
       </c>
     </row>
-    <row r="16">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A16" t="s">
         <v>16</v>
       </c>
@@ -1900,7 +1900,7 @@
         <v>0.17</v>
       </c>
     </row>
-    <row r="17">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.35">
       <c r="B17" s="3" t="str">
         <f>CONCATENATE("(",ROUND(survey_response_rate!B7,2),")")</f>
         <v>(0.02)</v>
@@ -1914,7 +1914,7 @@
         <v>(0.02)</v>
       </c>
     </row>
-    <row r="18">
+    <row r="18" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A18" t="s">
         <v>17</v>
       </c>
@@ -1935,7 +1935,7 @@
         <v>0.56000000000000005</v>
       </c>
     </row>
-    <row r="19">
+    <row r="19" spans="1:5" x14ac:dyDescent="0.35">
       <c r="B19" s="3" t="str">
         <f>CONCATENATE("(",ROUND(survey_response_rate!B9,3),")")</f>
         <v>(0.023)</v>
@@ -1949,7 +1949,7 @@
         <v>(0.019)</v>
       </c>
     </row>
-    <row r="20">
+    <row r="20" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A20" t="s">
         <v>9</v>
       </c>
@@ -1970,7 +1970,7 @@
         <v>0.71</v>
       </c>
     </row>
-    <row r="21">
+    <row r="21" spans="1:5" x14ac:dyDescent="0.35">
       <c r="B21" s="3" t="str">
         <f>CONCATENATE("(",ROUND(survey_response_rate!B11,3),")")</f>
         <v>(0.024)</v>
@@ -1984,7 +1984,7 @@
         <v>(0.025)</v>
       </c>
     </row>
-    <row r="22">
+    <row r="22" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A22" t="s">
         <v>18</v>
       </c>
@@ -2005,7 +2005,7 @@
         <v>0.56999999999999995</v>
       </c>
     </row>
-    <row r="23">
+    <row r="23" spans="1:5" x14ac:dyDescent="0.35">
       <c r="B23" s="3" t="str">
         <f>CONCATENATE("(",ROUND(survey_response_rate!B13,3),")")</f>
         <v>(0.023)</v>
@@ -2019,7 +2019,7 @@
         <v>(0.02)</v>
       </c>
     </row>
-    <row r="24">
+    <row r="24" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A24" t="s">
         <v>7</v>
       </c>
@@ -2040,7 +2040,7 @@
         <v>0.59</v>
       </c>
     </row>
-    <row r="25">
+    <row r="25" spans="1:5" x14ac:dyDescent="0.35">
       <c r="B25" s="3" t="str">
         <f>CONCATENATE("(",ROUND(survey_response_rate!B15,3),")")</f>
         <v>(0.023)</v>
@@ -2054,7 +2054,7 @@
         <v>(0.018)</v>
       </c>
     </row>
-    <row r="26">
+    <row r="26" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A26" t="s">
         <v>6</v>
       </c>
@@ -2075,7 +2075,7 @@
         <v>0.93</v>
       </c>
     </row>
-    <row r="27">
+    <row r="27" spans="1:5" x14ac:dyDescent="0.35">
       <c r="B27" s="3" t="str">
         <f>CONCATENATE("(",ROUND(survey_response_rate!B17,3),")")</f>
         <v>(0.025)</v>
@@ -2089,7 +2089,7 @@
         <v>(0.02)</v>
       </c>
     </row>
-    <row r="28">
+    <row r="28" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A28" s="11" t="s">
         <v>19</v>
       </c>
@@ -2110,7 +2110,7 @@
         <v>0.39</v>
       </c>
     </row>
-    <row r="29">
+    <row r="29" spans="1:5" x14ac:dyDescent="0.35">
       <c r="B29" s="3" t="str">
         <f>CONCATENATE("(",ROUND(survey_response_rate!B19,3),")")</f>
         <v>(0.025)</v>
@@ -2124,7 +2124,7 @@
         <v>(0.019)</v>
       </c>
     </row>
-    <row r="30" ht="15.75" thickBot="true">
+    <row r="30" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A30" s="2" t="s">
         <v>5</v>
       </c>
@@ -2142,7 +2142,7 @@
       </c>
       <c r="E30" s="5"/>
     </row>
-    <row r="31" ht="15.75" thickTop="true"/>
+    <row r="31" spans="1:5" ht="15" thickTop="1" x14ac:dyDescent="0.35"/>
   </sheetData>
   <mergeCells count="4">
     <mergeCell ref="B2:E2"/>
@@ -2155,37 +2155,37 @@
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3B054637-0760-4807-B01C-4419EACB0C14}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3B054637-0760-4807-B01C-4419EACB0C14}">
   <dimension ref="A2:E31"/>
   <sheetViews>
-    <sheetView topLeftCell="A6" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A3" sqref="A3:E30"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="18.140625" bestFit="true" customWidth="true"/>
-    <col min="2" max="2" width="9.7109375" style="3" customWidth="true"/>
-    <col min="3" max="3" width="10.5703125" style="3" customWidth="true"/>
-    <col min="4" max="4" width="7.5703125" style="3" bestFit="true" customWidth="true"/>
-    <col min="5" max="5" width="7.5703125" style="3" customWidth="true"/>
+    <col min="1" max="1" width="18.1796875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="9.7265625" style="3" customWidth="1"/>
+    <col min="3" max="3" width="10.54296875" style="3" customWidth="1"/>
+    <col min="4" max="4" width="7.54296875" style="3" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="7.54296875" style="3" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" ht="15.75" thickBot="true">
+    <row r="2" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A2" s="10"/>
       <c r="B2" s="13"/>
       <c r="C2" s="13"/>
       <c r="D2" s="13"/>
       <c r="E2" s="13"/>
     </row>
-    <row r="3">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.35">
       <c r="C3" s="14" t="s">
         <v>14</v>
       </c>
       <c r="D3" s="14"/>
       <c r="E3" s="14"/>
     </row>
-    <row r="4" s="6" customFormat="true" ht="30">
+    <row r="4" spans="1:5" s="6" customFormat="1" x14ac:dyDescent="0.35">
       <c r="B4" s="8" t="s">
         <v>1</v>
       </c>
@@ -2199,7 +2199,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="5" ht="15.75" thickBot="true">
+    <row r="5" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A5" s="2"/>
       <c r="B5" s="15" t="s">
         <v>3</v>
@@ -2208,7 +2208,7 @@
       <c r="D5" s="15"/>
       <c r="E5" s="15"/>
     </row>
-    <row r="6" ht="15.75" thickTop="true">
+    <row r="6" spans="1:5" ht="15" thickTop="1" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>4</v>
       </c>
@@ -2229,7 +2229,7 @@
         <v>0.65</v>
       </c>
     </row>
-    <row r="7">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.35">
       <c r="B7" s="3" t="str">
         <f>CONCATENATE("(",ROUND(SS_admin!B3,0),")")</f>
         <v>(76)</v>
@@ -2243,7 +2243,7 @@
         <v>(66)</v>
       </c>
     </row>
-    <row r="8">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
         <v>13</v>
       </c>
@@ -2264,7 +2264,7 @@
         <v>0.56000000000000005</v>
       </c>
     </row>
-    <row r="9">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.35">
       <c r="B9" s="3" t="str">
         <f>CONCATENATE("(",ROUND(SS_admin!B5,3),")")</f>
         <v>(0.044)</v>
@@ -2278,7 +2278,7 @@
         <v>(0.048)</v>
       </c>
     </row>
-    <row r="10">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A10" s="1" t="s">
         <v>5</v>
       </c>
@@ -2296,7 +2296,7 @@
       </c>
       <c r="E10" s="4"/>
     </row>
-    <row r="11" ht="15.75" thickBot="true">
+    <row r="11" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A11" s="2"/>
       <c r="B11" s="15" t="s">
         <v>15</v>
@@ -2305,7 +2305,7 @@
       <c r="D11" s="15"/>
       <c r="E11" s="15"/>
     </row>
-    <row r="12" ht="15.75" thickTop="true">
+    <row r="12" spans="1:5" ht="15" thickTop="1" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
         <v>8</v>
       </c>
@@ -2326,7 +2326,7 @@
         <v>0.51</v>
       </c>
     </row>
-    <row r="13">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.35">
       <c r="B13" s="3" t="str">
         <f>CONCATENATE("(",ROUND(SS_survey!B3,0),")")</f>
         <v>(186)</v>
@@ -2340,7 +2340,7 @@
         <v>(172)</v>
       </c>
     </row>
-    <row r="14">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
         <v>26</v>
       </c>
@@ -2361,7 +2361,7 @@
         <v>0.67</v>
       </c>
     </row>
-    <row r="15">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.35">
       <c r="B15" s="3" t="str">
         <f>CONCATENATE("(",ROUND(SS_survey!B5,3),")")</f>
         <v>(0.024)</v>
@@ -2375,7 +2375,7 @@
         <v>(0.02)</v>
       </c>
     </row>
-    <row r="16">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A16" t="s">
         <v>16</v>
       </c>
@@ -2396,7 +2396,7 @@
         <v>0.89</v>
       </c>
     </row>
-    <row r="17">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.35">
       <c r="B17" s="3" t="str">
         <f>CONCATENATE("(",ROUND(SS_survey!B7,2),")")</f>
         <v>(0.02)</v>
@@ -2410,7 +2410,7 @@
         <v>(0.01)</v>
       </c>
     </row>
-    <row r="18">
+    <row r="18" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A18" t="s">
         <v>17</v>
       </c>
@@ -2431,7 +2431,7 @@
         <v>0.28999999999999998</v>
       </c>
     </row>
-    <row r="19">
+    <row r="19" spans="1:5" x14ac:dyDescent="0.35">
       <c r="B19" s="3" t="str">
         <f>CONCATENATE("(",ROUND(SS_survey!B9,3),")")</f>
         <v>(0.028)</v>
@@ -2445,7 +2445,7 @@
         <v>(0.021)</v>
       </c>
     </row>
-    <row r="20">
+    <row r="20" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A20" t="s">
         <v>9</v>
       </c>
@@ -2466,7 +2466,7 @@
         <v>0.09</v>
       </c>
     </row>
-    <row r="21">
+    <row r="21" spans="1:5" x14ac:dyDescent="0.35">
       <c r="B21" s="3" t="str">
         <f>CONCATENATE("(",ROUND(SS_survey!B11,3),")")</f>
         <v>(0.721)</v>
@@ -2480,7 +2480,7 @@
         <v>(0.582)</v>
       </c>
     </row>
-    <row r="22">
+    <row r="22" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A22" t="s">
         <v>18</v>
       </c>
@@ -2501,7 +2501,7 @@
         <v>0.25</v>
       </c>
     </row>
-    <row r="23">
+    <row r="23" spans="1:5" x14ac:dyDescent="0.35">
       <c r="B23" s="3">
         <f>ROUND(SS_survey!B13,2)</f>
         <v>0.02</v>
@@ -2515,7 +2515,7 @@
         <v>(0.011)</v>
       </c>
     </row>
-    <row r="24">
+    <row r="24" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A24" t="s">
         <v>7</v>
       </c>
@@ -2536,7 +2536,7 @@
         <v>0.73</v>
       </c>
     </row>
-    <row r="25">
+    <row r="25" spans="1:5" x14ac:dyDescent="0.35">
       <c r="B25" s="3" t="str">
         <f>CONCATENATE("(",ROUND(SS_survey!B15,3),")")</f>
         <v>(0.688)</v>
@@ -2550,7 +2550,7 @@
         <v>(0.792)</v>
       </c>
     </row>
-    <row r="26">
+    <row r="26" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A26" t="s">
         <v>27</v>
       </c>
@@ -2571,7 +2571,7 @@
         <v>0.88</v>
       </c>
     </row>
-    <row r="27">
+    <row r="27" spans="1:5" x14ac:dyDescent="0.35">
       <c r="B27" s="3" t="str">
         <f>CONCATENATE("(",ROUND(SS_survey!B17,3),")")</f>
         <v>(0.023)</v>
@@ -2585,7 +2585,7 @@
         <v>(0.02)</v>
       </c>
     </row>
-    <row r="28">
+    <row r="28" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A28" s="11" t="s">
         <v>19</v>
       </c>
@@ -2606,7 +2606,7 @@
         <v>0.84</v>
       </c>
     </row>
-    <row r="29">
+    <row r="29" spans="1:5" x14ac:dyDescent="0.35">
       <c r="B29" s="3" t="str">
         <f>CONCATENATE("(",ROUND(SS_survey!B19,3),")")</f>
         <v>(0.027)</v>
@@ -2620,7 +2620,7 @@
         <v>(0.018)</v>
       </c>
     </row>
-    <row r="30" ht="15.75" thickBot="true">
+    <row r="30" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A30" s="2" t="s">
         <v>5</v>
       </c>
@@ -2638,7 +2638,7 @@
       </c>
       <c r="E30" s="5"/>
     </row>
-    <row r="31" ht="15.75" thickTop="true"/>
+    <row r="31" spans="1:5" ht="15" thickTop="1" x14ac:dyDescent="0.35"/>
   </sheetData>
   <mergeCells count="4">
     <mergeCell ref="B2:E2"/>
@@ -2651,37 +2651,37 @@
 </file>
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{754403B8-1DA5-4CBA-B8B6-94BFF0A849DB}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{754403B8-1DA5-4CBA-B8B6-94BFF0A849DB}">
   <dimension ref="A3:E13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A4" sqref="A4:E12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="26.28515625" bestFit="true" customWidth="true"/>
-    <col min="2" max="2" width="7.140625" style="3" bestFit="true" customWidth="true"/>
-    <col min="3" max="3" width="10.140625" style="3" bestFit="true" customWidth="true"/>
-    <col min="4" max="4" width="6.5703125" style="3" bestFit="true" customWidth="true"/>
-    <col min="5" max="5" width="6.5703125" style="3" customWidth="true"/>
+    <col min="1" max="1" width="26.26953125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="7.1796875" style="3" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10.1796875" style="3" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="6.54296875" style="3" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="6.54296875" style="3" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" ht="15.75" thickBot="true">
+    <row r="3" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A3" s="10"/>
       <c r="B3" s="13"/>
       <c r="C3" s="13"/>
       <c r="D3" s="13"/>
       <c r="E3" s="13"/>
     </row>
-    <row r="4">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.35">
       <c r="C4" s="14" t="s">
         <v>14</v>
       </c>
       <c r="D4" s="14"/>
       <c r="E4" s="14"/>
     </row>
-    <row r="5" ht="16.5" customHeight="true" thickBot="true">
+    <row r="5" spans="1:5" ht="16.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A5" s="9"/>
       <c r="B5" s="7" t="s">
         <v>1</v>
@@ -2696,42 +2696,42 @@
         <v>2</v>
       </c>
     </row>
-    <row r="6" ht="16.5" customHeight="true" thickTop="true">
+    <row r="6" spans="1:5" ht="16.5" customHeight="1" thickTop="1" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>11</v>
       </c>
       <c r="B6" s="3">
         <f>ROUND(SS_att!B2,0)</f>
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="C6" s="3">
         <f>ROUND(SS_att!C2,0)</f>
         <v>34</v>
       </c>
       <c r="D6" s="3">
-        <f>ROUND(SS_att!E2,0)</f>
-        <v>36</v>
+        <f>ROUND(SS_att!D2,0)</f>
+        <v>37</v>
       </c>
       <c r="E6" s="3">
         <f>ROUND(SS_att!L2,2)</f>
-        <v>0.52</v>
-      </c>
-    </row>
-    <row r="7" ht="16.5" customHeight="true">
+        <v>0.56999999999999995</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" ht="16.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B7" s="3" t="str">
         <f>CONCATENATE("(",ROUND(SS_att!B3,1),")")</f>
-        <v>(3)</v>
+        <v>(3.3)</v>
       </c>
       <c r="C7" s="3" t="str">
         <f>CONCATENATE("(",ROUND(SS_att!C3,1),")")</f>
         <v>(2.9)</v>
       </c>
       <c r="D7" s="3" t="str">
-        <f>CONCATENATE("(",ROUND(SS_att!E3,1),")")</f>
-        <v>(1.8)</v>
-      </c>
-    </row>
-    <row r="8" ht="16.5" customHeight="true">
+        <f>CONCATENATE("(",ROUND(SS_att!D3,1),")")</f>
+        <v>(3.2)</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" ht="16.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A8" s="6" t="s">
         <v>22</v>
       </c>
@@ -2752,7 +2752,7 @@
         <v>0.62</v>
       </c>
     </row>
-    <row r="9" ht="16.5" customHeight="true">
+    <row r="9" spans="1:5" ht="16.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A9" s="6"/>
       <c r="B9" s="3" t="str">
         <f>CONCATENATE("(",ROUND(SS_att!B9,2),")")</f>
@@ -2767,7 +2767,7 @@
         <v>(0.01)</v>
       </c>
     </row>
-    <row r="10" ht="16.5" customHeight="true">
+    <row r="10" spans="1:5" ht="16.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
         <v>12</v>
       </c>
@@ -2780,7 +2780,7 @@
         <v>0.76</v>
       </c>
       <c r="D10" s="3">
-        <f>ROUND(SS_att!E10,2)</f>
+        <f>ROUND(SS_att!D10,2)</f>
         <v>0.77</v>
       </c>
       <c r="E10" s="3">
@@ -2788,7 +2788,7 @@
         <v>0.62</v>
       </c>
     </row>
-    <row r="11" ht="16.5" customHeight="true">
+    <row r="11" spans="1:5" ht="16.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B11" s="3" t="str">
         <f>CONCATENATE("(",ROUND(SS_att!B11,2),")")</f>
         <v>(0.02)</v>
@@ -2798,11 +2798,11 @@
         <v>(0.02)</v>
       </c>
       <c r="D11" s="3" t="str">
-        <f>CONCATENATE("(",ROUND(SS_att!E11,2),")")</f>
-        <v>(0.01)</v>
-      </c>
-    </row>
-    <row r="12" ht="15.75" thickBot="true">
+        <f>CONCATENATE("(",ROUND(SS_att!D11,2),")")</f>
+        <v>(0.02)</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A12" s="2" t="s">
         <v>5</v>
       </c>
@@ -2820,7 +2820,7 @@
       </c>
       <c r="E12" s="5"/>
     </row>
-    <row r="13" ht="15.75" thickTop="true"/>
+    <row r="13" spans="1:5" ht="15" thickTop="1" x14ac:dyDescent="0.35"/>
   </sheetData>
   <mergeCells count="2">
     <mergeCell ref="B3:E3"/>

</xml_diff>

<commit_message>
cleaning of project folder - build replication files
</commit_message>
<xml_diff>
--- a/Tables/SS.xlsx
+++ b/Tables/SS.xlsx
@@ -1,6 +1,6 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26827"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\isaac\Dropbox\Apps\Overleaf\Donde2022\Tables\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9EFB68CC-00D9-4501-9F3E-C7918637F11C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9A031DCF-B88B-48F5-9ECB-1A1ADFB74B5B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-22815" yWindow="-16320" windowWidth="29040" windowHeight="15720" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-13995" yWindow="-12600" windowWidth="14400" windowHeight="8175" activeTab="5"/>
   </bookViews>
   <sheets>
     <sheet name="SS_admin" sheetId="1" r:id="rId1"/>
@@ -22,7 +22,7 @@
     <sheet name="SS" sheetId="5" r:id="rId7"/>
     <sheet name="Attrition" sheetId="6" r:id="rId8"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="191029" fullCalcOnLoad="true"/>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" count="52" uniqueCount="28">
   <si>
     <t>Choice</t>
   </si>
@@ -129,8 +129,8 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing">
+  <fonts count="1">
     <font>
       <sz val="11"/>
       <name val="Calibri"/>
@@ -207,39 +207,39 @@
   </cellStyleXfs>
   <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="true"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="true"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="true">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="true" applyAlignment="true">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="true" applyAlignment="true">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment wrapText="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="true">
+      <alignment wrapText="true"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="true" applyAlignment="true">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="true">
+      <alignment horizontal="center" wrapText="true"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="true" applyAlignment="true">
+      <alignment wrapText="true"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="true"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="true"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="true"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="true" applyAlignment="true">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="true" applyAlignment="true">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="true" applyAlignment="true">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -260,7 +260,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -411,7 +411,7 @@
         <a:solidFill>
           <a:schemeClr val="phClr"/>
         </a:solidFill>
-        <a:gradFill rotWithShape="1">
+        <a:gradFill rotWithShape="true">
           <a:gsLst>
             <a:gs pos="0">
               <a:schemeClr val="phClr">
@@ -435,9 +435,9 @@
               </a:schemeClr>
             </a:gs>
           </a:gsLst>
-          <a:lin ang="5400000" scaled="0"/>
+          <a:lin ang="5400000" scaled="false"/>
         </a:gradFill>
-        <a:gradFill rotWithShape="1">
+        <a:gradFill rotWithShape="true">
           <a:gsLst>
             <a:gs pos="0">
               <a:schemeClr val="phClr">
@@ -461,7 +461,7 @@
               </a:schemeClr>
             </a:gs>
           </a:gsLst>
-          <a:lin ang="5400000" scaled="0"/>
+          <a:lin ang="5400000" scaled="false"/>
         </a:gradFill>
       </a:fillStyleLst>
       <a:lnStyleLst>
@@ -496,7 +496,7 @@
         </a:effectStyle>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="0">
+            <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="false">
               <a:srgbClr val="000000">
                 <a:alpha val="63000"/>
               </a:srgbClr>
@@ -514,7 +514,7 @@
             <a:satMod val="170000"/>
           </a:schemeClr>
         </a:solidFill>
-        <a:gradFill rotWithShape="1">
+        <a:gradFill rotWithShape="true">
           <a:gsLst>
             <a:gs pos="0">
               <a:schemeClr val="phClr">
@@ -539,7 +539,7 @@
               </a:schemeClr>
             </a:gs>
           </a:gsLst>
-          <a:lin ang="5400000" scaled="0"/>
+          <a:lin ang="5400000" scaled="false"/>
         </a:gradFill>
       </a:bgFillStyleLst>
     </a:fmtScheme>
@@ -555,16 +555,16 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="B2:L6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="M11" sqref="A1:M11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData>
-    <row r="2" spans="2:12" x14ac:dyDescent="0.35">
+    <row xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" r="2" x14ac:dyDescent="0.35">
       <c r="B2">
         <v>2267.4576271186443</v>
       </c>
@@ -578,15 +578,15 @@
         <v>2216.7222398477156</v>
       </c>
       <c r="L2">
-        <v>0.64503108323202052</v>
-      </c>
-    </row>
-    <row r="3" spans="2:12" x14ac:dyDescent="0.35">
+        <v>0.64503108323202074</v>
+      </c>
+    </row>
+    <row xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" r="3" x14ac:dyDescent="0.35">
       <c r="B3">
-        <v>75.874088260545236</v>
+        <v>75.874088260545221</v>
       </c>
       <c r="C3">
-        <v>83.127592776594426</v>
+        <v>83.127592776594455</v>
       </c>
       <c r="D3">
         <v>65.750426103453577</v>
@@ -595,7 +595,7 @@
         <v>42.936615450474939</v>
       </c>
     </row>
-    <row r="4" spans="2:12" x14ac:dyDescent="0.35">
+    <row xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" r="4" x14ac:dyDescent="0.35">
       <c r="B4">
         <v>0.87966101694915255</v>
       </c>
@@ -603,7 +603,7 @@
         <v>0.89406345957011257</v>
       </c>
       <c r="D4">
-        <v>0.83100775193798448</v>
+        <v>0.83100775193798449</v>
       </c>
       <c r="E4">
         <v>0.8642131979695431</v>
@@ -612,21 +612,21 @@
         <v>0.56027324425210501</v>
       </c>
     </row>
-    <row r="5" spans="2:12" x14ac:dyDescent="0.35">
+    <row xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" r="5" x14ac:dyDescent="0.35">
       <c r="B5">
-        <v>4.3632089264597995E-2</v>
+        <v>0.043632089264597995</v>
       </c>
       <c r="C5">
-        <v>3.4871491260106517E-2</v>
+        <v>0.034871491260106517</v>
       </c>
       <c r="D5">
-        <v>4.7901996328697884E-2</v>
+        <v>0.047901996328697884</v>
       </c>
       <c r="E5">
-        <v>2.5577577893366663E-2</v>
-      </c>
-    </row>
-    <row r="6" spans="2:12" x14ac:dyDescent="0.35">
+        <v>0.025577577893366663</v>
+      </c>
+    </row>
+    <row xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" r="6" x14ac:dyDescent="0.35">
       <c r="B6">
         <v>1770</v>
       </c>
@@ -646,47 +646,47 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="B2:L11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="P21" sqref="A1:P21"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData>
-    <row r="2" spans="2:12" x14ac:dyDescent="0.35">
+    <row xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" r="2" x14ac:dyDescent="0.35">
       <c r="B2">
-        <v>32.333333333333336</v>
+        <v>35.404255319148938</v>
       </c>
       <c r="C2">
-        <v>34.15</v>
+        <v>32.322580645161288</v>
       </c>
       <c r="D2">
-        <v>37.134328358208954</v>
+        <v>37.324324324324323</v>
       </c>
       <c r="E2">
-        <v>34.752808988764045</v>
+        <v>35.136612021857921</v>
       </c>
       <c r="L2">
-        <v>0.572023905328648</v>
-      </c>
-    </row>
-    <row r="3" spans="2:12" x14ac:dyDescent="0.35">
+        <v>0.46218569349467797</v>
+      </c>
+    </row>
+    <row xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" r="3" x14ac:dyDescent="0.35">
       <c r="B3">
-        <v>3.3381533778207677</v>
+        <v>3.4834961191702076</v>
       </c>
       <c r="C3">
-        <v>2.9165246131670202</v>
+        <v>2.6504216953471356</v>
       </c>
       <c r="D3">
-        <v>3.1781063232804376</v>
+        <v>3.1208005093831628</v>
       </c>
       <c r="E3">
-        <v>1.8159027540097266</v>
-      </c>
-    </row>
-    <row r="4" spans="2:12" x14ac:dyDescent="0.35">
+        <v>1.7862037315142396</v>
+      </c>
+    </row>
+    <row xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" r="4" x14ac:dyDescent="0.35">
       <c r="B4">
         <v>1770</v>
       </c>
@@ -700,7 +700,7 @@
         <v>6304</v>
       </c>
     </row>
-    <row r="8" spans="2:12" x14ac:dyDescent="0.35">
+    <row xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" r="8" x14ac:dyDescent="0.35">
       <c r="B8">
         <v>0.97536945812807885</v>
       </c>
@@ -717,21 +717,21 @@
         <v>0.61894128114173319</v>
       </c>
     </row>
-    <row r="9" spans="2:12" x14ac:dyDescent="0.35">
+    <row xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" r="9" x14ac:dyDescent="0.35">
       <c r="B9">
-        <v>5.564104965819992E-3</v>
+        <v>0.0055641049658199876</v>
       </c>
       <c r="C9">
-        <v>9.0558404602785851E-3</v>
+        <v>0.0090558404602785834</v>
       </c>
       <c r="D9">
-        <v>7.7705794497818937E-3</v>
+        <v>0.0077705794497818937</v>
       </c>
       <c r="E9">
-        <v>4.4762159277795593E-3</v>
-      </c>
-    </row>
-    <row r="10" spans="2:12" x14ac:dyDescent="0.35">
+        <v>0.0044762159277795602</v>
+      </c>
+    </row>
+    <row xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" r="10" x14ac:dyDescent="0.35">
       <c r="B10">
         <v>0.78725761772853187</v>
       </c>
@@ -748,18 +748,18 @@
         <v>0.61700341260717884</v>
       </c>
     </row>
-    <row r="11" spans="2:12" x14ac:dyDescent="0.35">
+    <row xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" r="11" x14ac:dyDescent="0.35">
       <c r="B11">
-        <v>1.7870618309457527E-2</v>
+        <v>0.017870618309457527</v>
       </c>
       <c r="C11">
-        <v>2.4082154914125332E-2</v>
+        <v>0.024082154914125336</v>
       </c>
       <c r="D11">
-        <v>2.4956672691430013E-2</v>
+        <v>0.024956672691430013</v>
       </c>
       <c r="E11">
-        <v>1.3655060595903191E-2</v>
+        <v>0.01365506059590319</v>
       </c>
     </row>
   </sheetData>
@@ -768,16 +768,16 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="B2:L23"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="D15" sqref="D15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData>
-    <row r="2" spans="2:12" x14ac:dyDescent="0.35">
+    <row xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" r="2" x14ac:dyDescent="0.35">
       <c r="B2">
         <v>4084.0447483738694</v>
       </c>
@@ -791,10 +791,10 @@
         <v>4057.7718023592788</v>
       </c>
       <c r="L2">
-        <v>0.50741363647763404</v>
-      </c>
-    </row>
-    <row r="3" spans="2:12" x14ac:dyDescent="0.35">
+        <v>0.50741363647763405</v>
+      </c>
+    </row>
+    <row xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" r="3" x14ac:dyDescent="0.35">
       <c r="B3">
         <v>186.32530822216472</v>
       </c>
@@ -805,10 +805,10 @@
         <v>171.58152340909876</v>
       </c>
       <c r="E3">
-        <v>106.62109741727424</v>
-      </c>
-    </row>
-    <row r="4" spans="2:12" x14ac:dyDescent="0.35">
+        <v>106.62109741727427</v>
+      </c>
+    </row>
+    <row xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" r="4" x14ac:dyDescent="0.35">
       <c r="B4">
         <v>0.1870631315668515</v>
       </c>
@@ -822,24 +822,24 @@
         <v>0.19285795427201724</v>
       </c>
       <c r="L4">
-        <v>0.67256604845929213</v>
-      </c>
-    </row>
-    <row r="5" spans="2:12" x14ac:dyDescent="0.35">
+        <v>0.67256604845929191</v>
+      </c>
+    </row>
+    <row xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" r="5" x14ac:dyDescent="0.35">
       <c r="B5">
-        <v>2.4433091346626679E-2</v>
+        <v>0.024433091346626676</v>
       </c>
       <c r="C5">
-        <v>2.2831240521491845E-2</v>
+        <v>0.022831240521491839</v>
       </c>
       <c r="D5">
-        <v>2.0246312642953609E-2</v>
+        <v>0.02024631264295361</v>
       </c>
       <c r="E5">
-        <v>1.2895102797403319E-2</v>
-      </c>
-    </row>
-    <row r="6" spans="2:12" x14ac:dyDescent="0.35">
+        <v>0.012895102797403319</v>
+      </c>
+    </row>
+    <row xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" r="6" x14ac:dyDescent="0.35">
       <c r="B6">
         <v>0.13815789473684212</v>
       </c>
@@ -853,24 +853,24 @@
         <v>0.13050133945656334</v>
       </c>
       <c r="L6">
-        <v>0.88964950426016542</v>
-      </c>
-    </row>
-    <row r="7" spans="2:12" x14ac:dyDescent="0.35">
+        <v>0.88964950426016531</v>
+      </c>
+    </row>
+    <row xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" r="7" x14ac:dyDescent="0.35">
       <c r="B7">
-        <v>2.0646396595072284E-2</v>
+        <v>0.020646396595072281</v>
       </c>
       <c r="C7">
-        <v>1.4271538377509519E-2</v>
+        <v>0.014271538377509522</v>
       </c>
       <c r="D7">
-        <v>1.2989025875656875E-2</v>
+        <v>0.012989025875656875</v>
       </c>
       <c r="E7">
-        <v>9.0357611917287195E-3</v>
-      </c>
-    </row>
-    <row r="8" spans="2:12" x14ac:dyDescent="0.35">
+        <v>0.0090357611917287212</v>
+      </c>
+    </row>
+    <row xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" r="8" x14ac:dyDescent="0.35">
       <c r="B8">
         <v>0.62474437627811863</v>
       </c>
@@ -884,24 +884,24 @@
         <v>0.62394407224002335</v>
       </c>
       <c r="L8">
-        <v>0.29259959707503691</v>
-      </c>
-    </row>
-    <row r="9" spans="2:12" x14ac:dyDescent="0.35">
+        <v>0.29259959707503708</v>
+      </c>
+    </row>
+    <row xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" r="9" x14ac:dyDescent="0.35">
       <c r="B9">
-        <v>2.8080273403161184E-2</v>
+        <v>0.028080273403161174</v>
       </c>
       <c r="C9">
-        <v>3.5546721070160631E-2</v>
+        <v>0.035546721070160624</v>
       </c>
       <c r="D9">
-        <v>2.101418987928844E-2</v>
+        <v>0.021014189879288447</v>
       </c>
       <c r="E9">
-        <v>1.6701632404580391E-2</v>
-      </c>
-    </row>
-    <row r="10" spans="2:12" x14ac:dyDescent="0.35">
+        <v>0.016701632404580388</v>
+      </c>
+    </row>
+    <row xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" r="10" x14ac:dyDescent="0.35">
       <c r="B10">
         <v>91.886692015209121</v>
       </c>
@@ -915,26 +915,26 @@
         <v>92.527783783783789</v>
       </c>
       <c r="L10">
-        <v>9.3375432500357E-2</v>
-      </c>
-    </row>
-    <row r="11" spans="2:12" x14ac:dyDescent="0.35">
+        <v>0.093375432500357</v>
+      </c>
+    </row>
+    <row xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" r="11" x14ac:dyDescent="0.35">
       <c r="B11">
         <v>0.72142723064601477</v>
       </c>
       <c r="C11">
-        <v>1.0314969767030806</v>
+        <v>1.0314969767030808</v>
       </c>
       <c r="D11">
         <v>0.58165693064045443</v>
       </c>
       <c r="E11">
-        <v>0.45028569111852645</v>
-      </c>
-    </row>
-    <row r="12" spans="2:12" x14ac:dyDescent="0.35">
+        <v>0.45028569111852646</v>
+      </c>
+    </row>
+    <row xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" r="12" x14ac:dyDescent="0.35">
       <c r="B12">
-        <v>0.8693877551020408</v>
+        <v>0.86938775510204081</v>
       </c>
       <c r="C12">
         <v>0.88718411552346566</v>
@@ -946,29 +946,29 @@
         <v>0.88754325259515576</v>
       </c>
       <c r="L12">
-        <v>0.2521838227756053</v>
-      </c>
-    </row>
-    <row r="13" spans="2:12" x14ac:dyDescent="0.35">
+        <v>0.25218382277560531</v>
+      </c>
+    </row>
+    <row xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" r="13" x14ac:dyDescent="0.35">
       <c r="B13">
-        <v>1.5429549670760771E-2</v>
+        <v>0.015429549670760771</v>
       </c>
       <c r="C13">
-        <v>1.2769905653078381E-2</v>
+        <v>0.012769905653078385</v>
       </c>
       <c r="D13">
-        <v>1.1107505082691111E-2</v>
+        <v>0.011107505082691113</v>
       </c>
       <c r="E13">
-        <v>7.5100652933181595E-3</v>
-      </c>
-    </row>
-    <row r="14" spans="2:12" x14ac:dyDescent="0.35">
+        <v>0.0075100652933181595</v>
+      </c>
+    </row>
+    <row xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" r="14" x14ac:dyDescent="0.35">
       <c r="B14">
         <v>43.316996871741395</v>
       </c>
       <c r="C14">
-        <v>42.852913968547639</v>
+        <v>42.85291396854764</v>
       </c>
       <c r="D14">
         <v>43.821138211382113</v>
@@ -977,24 +977,24 @@
         <v>43.37017388741527</v>
       </c>
       <c r="L14">
-        <v>0.72947420733682788</v>
-      </c>
-    </row>
-    <row r="15" spans="2:12" x14ac:dyDescent="0.35">
+        <v>0.72947420733682766</v>
+      </c>
+    </row>
+    <row xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" r="15" x14ac:dyDescent="0.35">
       <c r="B15">
-        <v>0.68765705993205639</v>
+        <v>0.68765705993205628</v>
       </c>
       <c r="C15">
-        <v>0.94934692018880396</v>
+        <v>0.94934692018880451</v>
       </c>
       <c r="D15">
-        <v>0.79169967129326257</v>
+        <v>0.79169967129326269</v>
       </c>
       <c r="E15">
-        <v>0.47585898339836669</v>
-      </c>
-    </row>
-    <row r="16" spans="2:12" x14ac:dyDescent="0.35">
+        <v>0.47585898339836674</v>
+      </c>
+    </row>
+    <row xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" r="16" x14ac:dyDescent="0.35">
       <c r="B16">
         <v>0.7275390625</v>
       </c>
@@ -1011,21 +1011,21 @@
         <v>0.87880547636069528</v>
       </c>
     </row>
-    <row r="17" spans="2:12" x14ac:dyDescent="0.35">
+    <row xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" r="17" x14ac:dyDescent="0.35">
       <c r="B17">
-        <v>2.2722829871839111E-2</v>
+        <v>0.022722829871839111</v>
       </c>
       <c r="C17">
-        <v>1.8719850717439725E-2</v>
+        <v>0.018719850717439715</v>
       </c>
       <c r="D17">
-        <v>1.9807350620927644E-2</v>
+        <v>0.019807350620927648</v>
       </c>
       <c r="E17">
-        <v>1.1899628511819891E-2</v>
-      </c>
-    </row>
-    <row r="18" spans="2:12" x14ac:dyDescent="0.35">
+        <v>0.011899628511819889</v>
+      </c>
+    </row>
+    <row xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" r="18" x14ac:dyDescent="0.35">
       <c r="B18">
         <v>0.65861344537815125</v>
       </c>
@@ -1042,21 +1042,21 @@
         <v>0.83627432511379829</v>
       </c>
     </row>
-    <row r="19" spans="2:12" x14ac:dyDescent="0.35">
+    <row xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" r="19" x14ac:dyDescent="0.35">
       <c r="B19">
-        <v>2.7084494536168072E-2</v>
+        <v>0.027084494536168072</v>
       </c>
       <c r="C19">
-        <v>2.245117168137609E-2</v>
+        <v>0.02245117168137609</v>
       </c>
       <c r="D19">
-        <v>1.7630212971503318E-2</v>
+        <v>0.017630212971503318</v>
       </c>
       <c r="E19">
-        <v>1.2640157482716076E-2</v>
-      </c>
-    </row>
-    <row r="20" spans="2:12" x14ac:dyDescent="0.35">
+        <v>0.01264015748271608</v>
+      </c>
+    </row>
+    <row xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" r="20" x14ac:dyDescent="0.35">
       <c r="B20">
         <v>1770</v>
       </c>
@@ -1070,7 +1070,7 @@
         <v>6304</v>
       </c>
     </row>
-    <row r="23" spans="2:12" x14ac:dyDescent="0.35">
+    <row xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" r="23" x14ac:dyDescent="0.35">
       <c r="B23">
         <v>1386</v>
       </c>
@@ -1087,16 +1087,16 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
   <dimension ref="B2:L6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="L3" sqref="L3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData>
-    <row r="2" spans="2:12" x14ac:dyDescent="0.35">
+    <row xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" r="2" x14ac:dyDescent="0.35">
       <c r="B2">
         <v>2199.2352092352094</v>
       </c>
@@ -1113,9 +1113,9 @@
         <v>0.98415991070079034</v>
       </c>
     </row>
-    <row r="3" spans="2:12" x14ac:dyDescent="0.35">
+    <row xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" r="3" x14ac:dyDescent="0.35">
       <c r="B3">
-        <v>85.691617474481063</v>
+        <v>85.691617474481077</v>
       </c>
       <c r="C3">
         <v>105.62668921394878</v>
@@ -1124,10 +1124,10 @@
         <v>80.611977579989215</v>
       </c>
       <c r="E3">
-        <v>51.996675747123149</v>
-      </c>
-    </row>
-    <row r="4" spans="2:12" x14ac:dyDescent="0.35">
+        <v>51.996675747123135</v>
+      </c>
+    </row>
+    <row xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" r="4" x14ac:dyDescent="0.35">
       <c r="B4">
         <v>0.87590187590187585</v>
       </c>
@@ -1144,21 +1144,21 @@
         <v>0.80262123234967087</v>
       </c>
     </row>
-    <row r="5" spans="2:12" x14ac:dyDescent="0.35">
+    <row xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" r="5" x14ac:dyDescent="0.35">
       <c r="B5">
-        <v>4.4829425630513044E-2</v>
+        <v>0.044829425630513044</v>
       </c>
       <c r="C5">
-        <v>3.8037392189498614E-2</v>
+        <v>0.038037392189498615</v>
       </c>
       <c r="D5">
-        <v>4.5323633701885309E-2</v>
+        <v>0.045323633701885309</v>
       </c>
       <c r="E5">
-        <v>2.5337910106350277E-2</v>
-      </c>
-    </row>
-    <row r="6" spans="2:12" x14ac:dyDescent="0.35">
+        <v>0.025337910106350278</v>
+      </c>
+    </row>
+    <row xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" r="6" x14ac:dyDescent="0.35">
       <c r="B6">
         <v>1386</v>
       </c>
@@ -1178,21 +1178,21 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
   <dimension ref="B2:S20"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="Q2" sqref="Q2:S11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="17" max="17" width="9.54296875" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="10.453125" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="7.453125" customWidth="1"/>
+    <col min="17" max="17" width="9.54296875" bestFit="true" customWidth="true"/>
+    <col min="18" max="18" width="10.453125" bestFit="true" customWidth="true"/>
+    <col min="19" max="19" width="7.453125" customWidth="true"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:19" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" r="2" ht="15" thickBot="true" x14ac:dyDescent="0.4">
       <c r="B2">
         <v>0.73333333333333328</v>
       </c>
@@ -1224,18 +1224,18 @@
         <v>25</v>
       </c>
     </row>
-    <row r="3" spans="2:19" ht="15" thickTop="1" x14ac:dyDescent="0.35">
+    <row xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" r="3" ht="15" thickTop="true" x14ac:dyDescent="0.35">
       <c r="B3">
-        <v>2.2227133407258709E-2</v>
+        <v>0.022227133407258709</v>
       </c>
       <c r="C3">
-        <v>2.3945559259684196E-2</v>
+        <v>0.023945559259684192</v>
       </c>
       <c r="D3">
-        <v>2.4487406306672753E-2</v>
+        <v>0.024487406306672753</v>
       </c>
       <c r="E3">
-        <v>1.4054144438204628E-2</v>
+        <v>0.014054144438204628</v>
       </c>
       <c r="N3">
         <v>1</v>
@@ -1255,21 +1255,21 @@
         <v>4.6399999999999997</v>
       </c>
     </row>
-    <row r="4" spans="2:19" x14ac:dyDescent="0.35">
+    <row xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" r="4" x14ac:dyDescent="0.35">
       <c r="B4">
         <v>0.49265536723163844</v>
       </c>
       <c r="C4">
-        <v>0.47697031729785055</v>
+        <v>0.47697031729785056</v>
       </c>
       <c r="D4">
         <v>0.44341085271317832</v>
       </c>
       <c r="E4">
-        <v>0.46763959390862941</v>
+        <v>0.46763959390862942</v>
       </c>
       <c r="L4">
-        <v>0.2875593605623547</v>
+        <v>0.28755936056235471</v>
       </c>
       <c r="N4">
         <v>2</v>
@@ -1289,18 +1289,18 @@
         <v>28.1</v>
       </c>
     </row>
-    <row r="5" spans="2:19" x14ac:dyDescent="0.35">
+    <row xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" r="5" x14ac:dyDescent="0.35">
       <c r="B5">
-        <v>2.3096240095588593E-2</v>
+        <v>0.023096240095588593</v>
       </c>
       <c r="C5">
-        <v>2.2430876785456685E-2</v>
+        <v>0.022430876785456685</v>
       </c>
       <c r="D5">
-        <v>2.2238865610497347E-2</v>
+        <v>0.022238865610497347</v>
       </c>
       <c r="E5">
-        <v>1.3451909622314613E-2</v>
+        <v>0.013451909622314613</v>
       </c>
       <c r="N5">
         <v>3</v>
@@ -1320,7 +1320,7 @@
         <v>28.85</v>
       </c>
     </row>
-    <row r="6" spans="2:19" x14ac:dyDescent="0.35">
+    <row xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" r="6" x14ac:dyDescent="0.35">
       <c r="B6">
         <v>0.42937853107344631</v>
       </c>
@@ -1354,18 +1354,18 @@
         <v>30.830000000000002</v>
       </c>
     </row>
-    <row r="7" spans="2:19" x14ac:dyDescent="0.35">
+    <row xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" r="7" x14ac:dyDescent="0.35">
       <c r="B7">
-        <v>2.2539581021475692E-2</v>
+        <v>0.022539581021475692</v>
       </c>
       <c r="C7">
-        <v>2.1272764353621975E-2</v>
+        <v>0.021272764353621985</v>
       </c>
       <c r="D7">
-        <v>1.7156228789498337E-2</v>
+        <v>0.017156228789498337</v>
       </c>
       <c r="E7">
-        <v>1.1856963930785313E-2</v>
+        <v>0.011856963930785313</v>
       </c>
       <c r="N7">
         <v>5</v>
@@ -1385,7 +1385,7 @@
         <v>32.39</v>
       </c>
     </row>
-    <row r="8" spans="2:19" x14ac:dyDescent="0.35">
+    <row xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" r="8" x14ac:dyDescent="0.35">
       <c r="B8">
         <v>0.55254237288135588</v>
       </c>
@@ -1419,18 +1419,18 @@
         <v>35.1</v>
       </c>
     </row>
-    <row r="9" spans="2:19" x14ac:dyDescent="0.35">
+    <row xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" r="9" x14ac:dyDescent="0.35">
       <c r="B9">
-        <v>2.3021717142206806E-2</v>
+        <v>0.023021717142206799</v>
       </c>
       <c r="C9">
-        <v>2.284086769741038E-2</v>
+        <v>0.02284086769741038</v>
       </c>
       <c r="D9">
-        <v>1.9453047006242685E-2</v>
+        <v>0.019453047006242681</v>
       </c>
       <c r="E9">
-        <v>1.2592986237205277E-2</v>
+        <v>0.012592986237205277</v>
       </c>
       <c r="N9">
         <v>7</v>
@@ -1450,9 +1450,9 @@
         <v>41.34</v>
       </c>
     </row>
-    <row r="10" spans="2:19" x14ac:dyDescent="0.35">
+    <row xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" r="10" x14ac:dyDescent="0.35">
       <c r="B10">
-        <v>0.74293785310734461</v>
+        <v>0.74293785310734462</v>
       </c>
       <c r="C10">
         <v>0.7164790174002047</v>
@@ -1484,18 +1484,18 @@
         <v>56.49</v>
       </c>
     </row>
-    <row r="11" spans="2:19" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" r="11" ht="15" thickBot="true" x14ac:dyDescent="0.4">
       <c r="B11">
-        <v>2.3824936806509319E-2</v>
+        <v>0.023824936806509316</v>
       </c>
       <c r="C11">
-        <v>2.5477564039296352E-2</v>
+        <v>0.025477564039296345</v>
       </c>
       <c r="D11">
-        <v>2.5358148430980946E-2</v>
+        <v>0.025358148430980946</v>
       </c>
       <c r="E11">
-        <v>1.4625072871412275E-2</v>
+        <v>0.014625072871412275</v>
       </c>
       <c r="N11">
         <v>9</v>
@@ -1515,7 +1515,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="12" spans="2:19" ht="15" thickTop="1" x14ac:dyDescent="0.35">
+    <row xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" r="12" ht="15" thickTop="true" x14ac:dyDescent="0.35">
       <c r="B12">
         <v>0.5536723163841808</v>
       </c>
@@ -1532,21 +1532,21 @@
         <v>0.56579109636169034</v>
       </c>
     </row>
-    <row r="13" spans="2:19" x14ac:dyDescent="0.35">
+    <row xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" r="13" x14ac:dyDescent="0.35">
       <c r="B13">
-        <v>2.3197736740832288E-2</v>
+        <v>0.023197736740832281</v>
       </c>
       <c r="C13">
-        <v>2.3802739213909081E-2</v>
+        <v>0.023802739213909085</v>
       </c>
       <c r="D13">
-        <v>1.9572399449557739E-2</v>
+        <v>0.019572399449557746</v>
       </c>
       <c r="E13">
-        <v>1.2812478832268841E-2</v>
-      </c>
-    </row>
-    <row r="14" spans="2:19" x14ac:dyDescent="0.35">
+        <v>0.012812478832268839</v>
+      </c>
+    </row>
+    <row xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" r="14" x14ac:dyDescent="0.35">
       <c r="B14">
         <v>0.54180790960451974</v>
       </c>
@@ -1563,21 +1563,21 @@
         <v>0.59041645057610959</v>
       </c>
     </row>
-    <row r="15" spans="2:19" x14ac:dyDescent="0.35">
+    <row xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" r="15" x14ac:dyDescent="0.35">
       <c r="B15">
-        <v>2.3028825848404249E-2</v>
+        <v>0.023028825848404246</v>
       </c>
       <c r="C15">
-        <v>2.2637624384734246E-2</v>
+        <v>0.022637624384734246</v>
       </c>
       <c r="D15">
-        <v>1.7949107537719389E-2</v>
+        <v>0.017949107537719385</v>
       </c>
       <c r="E15">
-        <v>1.2151512644084097E-2</v>
-      </c>
-    </row>
-    <row r="16" spans="2:19" x14ac:dyDescent="0.35">
+        <v>0.012151512644084097</v>
+      </c>
+    </row>
+    <row xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" r="16" x14ac:dyDescent="0.35">
       <c r="B16">
         <v>0.5785310734463277</v>
       </c>
@@ -1585,7 +1585,7 @@
         <v>0.59058341862845443</v>
       </c>
       <c r="D16">
-        <v>0.58100775193798448</v>
+        <v>0.58100775193798449</v>
       </c>
       <c r="E16">
         <v>0.58328045685279184</v>
@@ -1594,21 +1594,21 @@
         <v>0.93267269990982249</v>
       </c>
     </row>
-    <row r="17" spans="2:12" x14ac:dyDescent="0.35">
+    <row xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" r="17" x14ac:dyDescent="0.35">
       <c r="B17">
-        <v>2.4804932440873628E-2</v>
+        <v>0.024804932440873628</v>
       </c>
       <c r="C17">
-        <v>2.4454339740942695E-2</v>
+        <v>0.024454339740942702</v>
       </c>
       <c r="D17">
-        <v>2.0184205552730608E-2</v>
+        <v>0.020184205552730605</v>
       </c>
       <c r="E17">
-        <v>1.3166776724715765E-2</v>
-      </c>
-    </row>
-    <row r="18" spans="2:12" x14ac:dyDescent="0.35">
+        <v>0.013166776724715766</v>
+      </c>
+    </row>
+    <row xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" r="18" x14ac:dyDescent="0.35">
       <c r="B18">
         <v>0.53785310734463276</v>
       </c>
@@ -1625,21 +1625,21 @@
         <v>0.38649070048922801</v>
       </c>
     </row>
-    <row r="19" spans="2:12" x14ac:dyDescent="0.35">
+    <row xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" r="19" x14ac:dyDescent="0.35">
       <c r="B19">
-        <v>2.497582090269404E-2</v>
+        <v>0.024975820902694037</v>
       </c>
       <c r="C19">
-        <v>2.4730039627438711E-2</v>
+        <v>0.024730039627438711</v>
       </c>
       <c r="D19">
-        <v>1.8824019104946247E-2</v>
+        <v>0.018824019104946247</v>
       </c>
       <c r="E19">
-        <v>1.3148903527138892E-2</v>
-      </c>
-    </row>
-    <row r="20" spans="2:12" x14ac:dyDescent="0.35">
+        <v>0.013148903527138892</v>
+      </c>
+    </row>
+    <row xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" r="20" x14ac:dyDescent="0.35">
       <c r="B20">
         <v>1770</v>
       </c>
@@ -1659,37 +1659,37 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{67FF63D4-14D6-4F54-BD0D-751B1AD5E68C}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{67FF63D4-14D6-4F54-BD0D-751B1AD5E68C}">
   <dimension ref="A2:E31"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView tabSelected="true" workbookViewId="0">
       <selection activeCell="A3" sqref="A3:E30"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="18.1796875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="9.7265625" style="3" customWidth="1"/>
-    <col min="3" max="3" width="10.54296875" style="3" customWidth="1"/>
-    <col min="4" max="4" width="7.54296875" style="3" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="7.54296875" style="3" customWidth="1"/>
+    <col min="1" max="1" width="18.1796875" bestFit="true" customWidth="true"/>
+    <col min="2" max="2" width="9.7265625" style="3" customWidth="true"/>
+    <col min="3" max="3" width="10.54296875" style="3" customWidth="true"/>
+    <col min="4" max="4" width="7.54296875" style="3" bestFit="true" customWidth="true"/>
+    <col min="5" max="5" width="7.54296875" style="3" customWidth="true"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" r="2" ht="15" thickBot="true" x14ac:dyDescent="0.4">
       <c r="A2" s="10"/>
       <c r="B2" s="13"/>
       <c r="C2" s="13"/>
       <c r="D2" s="13"/>
       <c r="E2" s="13"/>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.35">
+    <row xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" r="3" x14ac:dyDescent="0.35">
       <c r="C3" s="14" t="s">
         <v>14</v>
       </c>
       <c r="D3" s="14"/>
       <c r="E3" s="14"/>
     </row>
-    <row r="4" spans="1:5" s="6" customFormat="1" x14ac:dyDescent="0.35">
+    <row xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" r="4" s="6" customFormat="true" x14ac:dyDescent="0.35">
       <c r="B4" s="8" t="s">
         <v>1</v>
       </c>
@@ -1703,7 +1703,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="5" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" r="5" ht="15" thickBot="true" x14ac:dyDescent="0.4">
       <c r="A5" s="2"/>
       <c r="B5" s="15" t="s">
         <v>20</v>
@@ -1712,7 +1712,7 @@
       <c r="D5" s="15"/>
       <c r="E5" s="15"/>
     </row>
-    <row r="6" spans="1:5" ht="15" thickTop="1" x14ac:dyDescent="0.35">
+    <row xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" r="6" ht="15" thickTop="true" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>4</v>
       </c>
@@ -1733,7 +1733,7 @@
         <v>0.98</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.35">
+    <row xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" r="7" x14ac:dyDescent="0.35">
       <c r="B7" s="3" t="str">
         <f>CONCATENATE("(",ROUND(SS_admin_survey!B3,0),")")</f>
         <v>(86)</v>
@@ -1747,7 +1747,7 @@
         <v>(81)</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.35">
+    <row xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" r="8" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
         <v>13</v>
       </c>
@@ -1768,7 +1768,7 @@
         <v>0.8</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.35">
+    <row xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" r="9" x14ac:dyDescent="0.35">
       <c r="B9" s="3" t="str">
         <f>CONCATENATE("(",ROUND(SS_admin_survey!B5,3),")")</f>
         <v>(0.045)</v>
@@ -1782,7 +1782,7 @@
         <v>(0.045)</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.35">
+    <row xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" r="10" x14ac:dyDescent="0.35">
       <c r="A10" s="1" t="s">
         <v>5</v>
       </c>
@@ -1800,7 +1800,7 @@
       </c>
       <c r="E10" s="4"/>
     </row>
-    <row r="11" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" r="11" ht="15" thickBot="true" x14ac:dyDescent="0.4">
       <c r="A11" s="2"/>
       <c r="B11" s="15" t="s">
         <v>21</v>
@@ -1809,7 +1809,7 @@
       <c r="D11" s="15"/>
       <c r="E11" s="15"/>
     </row>
-    <row r="12" spans="1:5" ht="15" thickTop="1" x14ac:dyDescent="0.35">
+    <row xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" r="12" ht="15" thickTop="true" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
         <v>8</v>
       </c>
@@ -1830,7 +1830,7 @@
         <v>0.39</v>
       </c>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.35">
+    <row xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" r="13" x14ac:dyDescent="0.35">
       <c r="B13" s="3" t="str">
         <f>CONCATENATE("(",ROUND(survey_response_rate!B3,3),")")</f>
         <v>(0.022)</v>
@@ -1844,7 +1844,7 @@
         <v>(0.024)</v>
       </c>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.35">
+    <row xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" r="14" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
         <v>26</v>
       </c>
@@ -1865,7 +1865,7 @@
         <v>0.28999999999999998</v>
       </c>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.35">
+    <row xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" r="15" x14ac:dyDescent="0.35">
       <c r="B15" s="3" t="str">
         <f>CONCATENATE("(",ROUND(survey_response_rate!B5,3),")")</f>
         <v>(0.023)</v>
@@ -1879,7 +1879,7 @@
         <v>(0.022)</v>
       </c>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.35">
+    <row xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" r="16" x14ac:dyDescent="0.35">
       <c r="A16" t="s">
         <v>16</v>
       </c>
@@ -1900,7 +1900,7 @@
         <v>0.17</v>
       </c>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.35">
+    <row xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" r="17" x14ac:dyDescent="0.35">
       <c r="B17" s="3" t="str">
         <f>CONCATENATE("(",ROUND(survey_response_rate!B7,2),")")</f>
         <v>(0.02)</v>
@@ -1914,7 +1914,7 @@
         <v>(0.02)</v>
       </c>
     </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.35">
+    <row xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" r="18" x14ac:dyDescent="0.35">
       <c r="A18" t="s">
         <v>17</v>
       </c>
@@ -1935,7 +1935,7 @@
         <v>0.56000000000000005</v>
       </c>
     </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.35">
+    <row xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" r="19" x14ac:dyDescent="0.35">
       <c r="B19" s="3" t="str">
         <f>CONCATENATE("(",ROUND(survey_response_rate!B9,3),")")</f>
         <v>(0.023)</v>
@@ -1949,7 +1949,7 @@
         <v>(0.019)</v>
       </c>
     </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.35">
+    <row xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" r="20" x14ac:dyDescent="0.35">
       <c r="A20" t="s">
         <v>9</v>
       </c>
@@ -1970,7 +1970,7 @@
         <v>0.71</v>
       </c>
     </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.35">
+    <row xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" r="21" x14ac:dyDescent="0.35">
       <c r="B21" s="3" t="str">
         <f>CONCATENATE("(",ROUND(survey_response_rate!B11,3),")")</f>
         <v>(0.024)</v>
@@ -1984,7 +1984,7 @@
         <v>(0.025)</v>
       </c>
     </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.35">
+    <row xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" r="22" x14ac:dyDescent="0.35">
       <c r="A22" t="s">
         <v>18</v>
       </c>
@@ -2005,7 +2005,7 @@
         <v>0.56999999999999995</v>
       </c>
     </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.35">
+    <row xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" r="23" x14ac:dyDescent="0.35">
       <c r="B23" s="3" t="str">
         <f>CONCATENATE("(",ROUND(survey_response_rate!B13,3),")")</f>
         <v>(0.023)</v>
@@ -2019,7 +2019,7 @@
         <v>(0.02)</v>
       </c>
     </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.35">
+    <row xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" r="24" x14ac:dyDescent="0.35">
       <c r="A24" t="s">
         <v>7</v>
       </c>
@@ -2040,7 +2040,7 @@
         <v>0.59</v>
       </c>
     </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.35">
+    <row xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" r="25" x14ac:dyDescent="0.35">
       <c r="B25" s="3" t="str">
         <f>CONCATENATE("(",ROUND(survey_response_rate!B15,3),")")</f>
         <v>(0.023)</v>
@@ -2054,7 +2054,7 @@
         <v>(0.018)</v>
       </c>
     </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.35">
+    <row xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" r="26" x14ac:dyDescent="0.35">
       <c r="A26" t="s">
         <v>6</v>
       </c>
@@ -2075,7 +2075,7 @@
         <v>0.93</v>
       </c>
     </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.35">
+    <row xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" r="27" x14ac:dyDescent="0.35">
       <c r="B27" s="3" t="str">
         <f>CONCATENATE("(",ROUND(survey_response_rate!B17,3),")")</f>
         <v>(0.025)</v>
@@ -2089,7 +2089,7 @@
         <v>(0.02)</v>
       </c>
     </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.35">
+    <row xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" r="28" x14ac:dyDescent="0.35">
       <c r="A28" s="11" t="s">
         <v>19</v>
       </c>
@@ -2110,7 +2110,7 @@
         <v>0.39</v>
       </c>
     </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.35">
+    <row xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" r="29" x14ac:dyDescent="0.35">
       <c r="B29" s="3" t="str">
         <f>CONCATENATE("(",ROUND(survey_response_rate!B19,3),")")</f>
         <v>(0.025)</v>
@@ -2124,7 +2124,7 @@
         <v>(0.019)</v>
       </c>
     </row>
-    <row r="30" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" r="30" ht="15" thickBot="true" x14ac:dyDescent="0.4">
       <c r="A30" s="2" t="s">
         <v>5</v>
       </c>
@@ -2142,7 +2142,7 @@
       </c>
       <c r="E30" s="5"/>
     </row>
-    <row r="31" spans="1:5" ht="15" thickTop="1" x14ac:dyDescent="0.35"/>
+    <row xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" r="31" ht="15" thickTop="true" x14ac:dyDescent="0.35"/>
   </sheetData>
   <mergeCells count="4">
     <mergeCell ref="B2:E2"/>
@@ -2155,37 +2155,37 @@
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3B054637-0760-4807-B01C-4419EACB0C14}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3B054637-0760-4807-B01C-4419EACB0C14}">
   <dimension ref="A2:E31"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A3" sqref="A3:E30"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="18.1796875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="9.7265625" style="3" customWidth="1"/>
-    <col min="3" max="3" width="10.54296875" style="3" customWidth="1"/>
-    <col min="4" max="4" width="7.54296875" style="3" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="7.54296875" style="3" customWidth="1"/>
+    <col min="1" max="1" width="18.1796875" bestFit="true" customWidth="true"/>
+    <col min="2" max="2" width="9.7265625" style="3" customWidth="true"/>
+    <col min="3" max="3" width="10.54296875" style="3" customWidth="true"/>
+    <col min="4" max="4" width="7.54296875" style="3" bestFit="true" customWidth="true"/>
+    <col min="5" max="5" width="7.54296875" style="3" customWidth="true"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" r="2" ht="15" thickBot="true" x14ac:dyDescent="0.4">
       <c r="A2" s="10"/>
       <c r="B2" s="13"/>
       <c r="C2" s="13"/>
       <c r="D2" s="13"/>
       <c r="E2" s="13"/>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.35">
+    <row xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" r="3" x14ac:dyDescent="0.35">
       <c r="C3" s="14" t="s">
         <v>14</v>
       </c>
       <c r="D3" s="14"/>
       <c r="E3" s="14"/>
     </row>
-    <row r="4" spans="1:5" s="6" customFormat="1" x14ac:dyDescent="0.35">
+    <row xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" r="4" s="6" customFormat="true" x14ac:dyDescent="0.35">
       <c r="B4" s="8" t="s">
         <v>1</v>
       </c>
@@ -2199,7 +2199,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="5" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" r="5" ht="15" thickBot="true" x14ac:dyDescent="0.4">
       <c r="A5" s="2"/>
       <c r="B5" s="15" t="s">
         <v>3</v>
@@ -2208,7 +2208,7 @@
       <c r="D5" s="15"/>
       <c r="E5" s="15"/>
     </row>
-    <row r="6" spans="1:5" ht="15" thickTop="1" x14ac:dyDescent="0.35">
+    <row xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" r="6" ht="15" thickTop="true" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>4</v>
       </c>
@@ -2229,7 +2229,7 @@
         <v>0.65</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.35">
+    <row xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" r="7" x14ac:dyDescent="0.35">
       <c r="B7" s="3" t="str">
         <f>CONCATENATE("(",ROUND(SS_admin!B3,0),")")</f>
         <v>(76)</v>
@@ -2243,7 +2243,7 @@
         <v>(66)</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.35">
+    <row xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" r="8" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
         <v>13</v>
       </c>
@@ -2264,7 +2264,7 @@
         <v>0.56000000000000005</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.35">
+    <row xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" r="9" x14ac:dyDescent="0.35">
       <c r="B9" s="3" t="str">
         <f>CONCATENATE("(",ROUND(SS_admin!B5,3),")")</f>
         <v>(0.044)</v>
@@ -2278,7 +2278,7 @@
         <v>(0.048)</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.35">
+    <row xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" r="10" x14ac:dyDescent="0.35">
       <c r="A10" s="1" t="s">
         <v>5</v>
       </c>
@@ -2296,7 +2296,7 @@
       </c>
       <c r="E10" s="4"/>
     </row>
-    <row r="11" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" r="11" ht="15" thickBot="true" x14ac:dyDescent="0.4">
       <c r="A11" s="2"/>
       <c r="B11" s="15" t="s">
         <v>15</v>
@@ -2305,7 +2305,7 @@
       <c r="D11" s="15"/>
       <c r="E11" s="15"/>
     </row>
-    <row r="12" spans="1:5" ht="15" thickTop="1" x14ac:dyDescent="0.35">
+    <row xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" r="12" ht="15" thickTop="true" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
         <v>8</v>
       </c>
@@ -2326,7 +2326,7 @@
         <v>0.51</v>
       </c>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.35">
+    <row xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" r="13" x14ac:dyDescent="0.35">
       <c r="B13" s="3" t="str">
         <f>CONCATENATE("(",ROUND(SS_survey!B3,0),")")</f>
         <v>(186)</v>
@@ -2340,7 +2340,7 @@
         <v>(172)</v>
       </c>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.35">
+    <row xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" r="14" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
         <v>26</v>
       </c>
@@ -2361,7 +2361,7 @@
         <v>0.67</v>
       </c>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.35">
+    <row xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" r="15" x14ac:dyDescent="0.35">
       <c r="B15" s="3" t="str">
         <f>CONCATENATE("(",ROUND(SS_survey!B5,3),")")</f>
         <v>(0.024)</v>
@@ -2375,7 +2375,7 @@
         <v>(0.02)</v>
       </c>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.35">
+    <row xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" r="16" x14ac:dyDescent="0.35">
       <c r="A16" t="s">
         <v>16</v>
       </c>
@@ -2396,7 +2396,7 @@
         <v>0.89</v>
       </c>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.35">
+    <row xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" r="17" x14ac:dyDescent="0.35">
       <c r="B17" s="3" t="str">
         <f>CONCATENATE("(",ROUND(SS_survey!B7,2),")")</f>
         <v>(0.02)</v>
@@ -2410,7 +2410,7 @@
         <v>(0.01)</v>
       </c>
     </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.35">
+    <row xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" r="18" x14ac:dyDescent="0.35">
       <c r="A18" t="s">
         <v>17</v>
       </c>
@@ -2431,7 +2431,7 @@
         <v>0.28999999999999998</v>
       </c>
     </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.35">
+    <row xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" r="19" x14ac:dyDescent="0.35">
       <c r="B19" s="3" t="str">
         <f>CONCATENATE("(",ROUND(SS_survey!B9,3),")")</f>
         <v>(0.028)</v>
@@ -2445,7 +2445,7 @@
         <v>(0.021)</v>
       </c>
     </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.35">
+    <row xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" r="20" x14ac:dyDescent="0.35">
       <c r="A20" t="s">
         <v>9</v>
       </c>
@@ -2466,7 +2466,7 @@
         <v>0.09</v>
       </c>
     </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.35">
+    <row xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" r="21" x14ac:dyDescent="0.35">
       <c r="B21" s="3" t="str">
         <f>CONCATENATE("(",ROUND(SS_survey!B11,3),")")</f>
         <v>(0.721)</v>
@@ -2480,7 +2480,7 @@
         <v>(0.582)</v>
       </c>
     </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.35">
+    <row xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" r="22" x14ac:dyDescent="0.35">
       <c r="A22" t="s">
         <v>18</v>
       </c>
@@ -2501,7 +2501,7 @@
         <v>0.25</v>
       </c>
     </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.35">
+    <row xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" r="23" x14ac:dyDescent="0.35">
       <c r="B23" s="3">
         <f>ROUND(SS_survey!B13,2)</f>
         <v>0.02</v>
@@ -2515,7 +2515,7 @@
         <v>(0.011)</v>
       </c>
     </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.35">
+    <row xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" r="24" x14ac:dyDescent="0.35">
       <c r="A24" t="s">
         <v>7</v>
       </c>
@@ -2536,7 +2536,7 @@
         <v>0.73</v>
       </c>
     </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.35">
+    <row xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" r="25" x14ac:dyDescent="0.35">
       <c r="B25" s="3" t="str">
         <f>CONCATENATE("(",ROUND(SS_survey!B15,3),")")</f>
         <v>(0.688)</v>
@@ -2550,7 +2550,7 @@
         <v>(0.792)</v>
       </c>
     </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.35">
+    <row xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" r="26" x14ac:dyDescent="0.35">
       <c r="A26" t="s">
         <v>27</v>
       </c>
@@ -2571,7 +2571,7 @@
         <v>0.88</v>
       </c>
     </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.35">
+    <row xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" r="27" x14ac:dyDescent="0.35">
       <c r="B27" s="3" t="str">
         <f>CONCATENATE("(",ROUND(SS_survey!B17,3),")")</f>
         <v>(0.023)</v>
@@ -2585,7 +2585,7 @@
         <v>(0.02)</v>
       </c>
     </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.35">
+    <row xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" r="28" x14ac:dyDescent="0.35">
       <c r="A28" s="11" t="s">
         <v>19</v>
       </c>
@@ -2606,7 +2606,7 @@
         <v>0.84</v>
       </c>
     </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.35">
+    <row xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" r="29" x14ac:dyDescent="0.35">
       <c r="B29" s="3" t="str">
         <f>CONCATENATE("(",ROUND(SS_survey!B19,3),")")</f>
         <v>(0.027)</v>
@@ -2620,7 +2620,7 @@
         <v>(0.018)</v>
       </c>
     </row>
-    <row r="30" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" r="30" ht="15" thickBot="true" x14ac:dyDescent="0.4">
       <c r="A30" s="2" t="s">
         <v>5</v>
       </c>
@@ -2638,7 +2638,7 @@
       </c>
       <c r="E30" s="5"/>
     </row>
-    <row r="31" spans="1:5" ht="15" thickTop="1" x14ac:dyDescent="0.35"/>
+    <row xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" r="31" ht="15" thickTop="true" x14ac:dyDescent="0.35"/>
   </sheetData>
   <mergeCells count="4">
     <mergeCell ref="B2:E2"/>
@@ -2651,37 +2651,37 @@
 </file>
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{754403B8-1DA5-4CBA-B8B6-94BFF0A849DB}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{754403B8-1DA5-4CBA-B8B6-94BFF0A849DB}">
   <dimension ref="A3:E13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A4" sqref="A4:E12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="26.26953125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="7.1796875" style="3" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="10.1796875" style="3" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="6.54296875" style="3" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="6.54296875" style="3" customWidth="1"/>
+    <col min="1" max="1" width="26.26953125" bestFit="true" customWidth="true"/>
+    <col min="2" max="2" width="7.1796875" style="3" bestFit="true" customWidth="true"/>
+    <col min="3" max="3" width="10.1796875" style="3" bestFit="true" customWidth="true"/>
+    <col min="4" max="4" width="6.54296875" style="3" bestFit="true" customWidth="true"/>
+    <col min="5" max="5" width="6.54296875" style="3" customWidth="true"/>
   </cols>
   <sheetData>
-    <row r="3" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" r="3" ht="15" thickBot="true" x14ac:dyDescent="0.4">
       <c r="A3" s="10"/>
       <c r="B3" s="13"/>
       <c r="C3" s="13"/>
       <c r="D3" s="13"/>
       <c r="E3" s="13"/>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.35">
+    <row xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" r="4" x14ac:dyDescent="0.35">
       <c r="C4" s="14" t="s">
         <v>14</v>
       </c>
       <c r="D4" s="14"/>
       <c r="E4" s="14"/>
     </row>
-    <row r="5" spans="1:5" ht="16.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" r="5" ht="16.5" customHeight="true" thickBot="true" x14ac:dyDescent="0.4">
       <c r="A5" s="9"/>
       <c r="B5" s="7" t="s">
         <v>1</v>
@@ -2696,42 +2696,42 @@
         <v>2</v>
       </c>
     </row>
-    <row r="6" spans="1:5" ht="16.5" customHeight="1" thickTop="1" x14ac:dyDescent="0.35">
+    <row xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" r="6" ht="16.5" customHeight="true" thickTop="true" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>11</v>
       </c>
       <c r="B6" s="3">
         <f>ROUND(SS_att!B2,0)</f>
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C6" s="3">
         <f>ROUND(SS_att!C2,0)</f>
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="D6" s="3">
         <f>ROUND(SS_att!D2,0)</f>
-        <v>37</v>
+        <v>41</v>
       </c>
       <c r="E6" s="3">
         <f>ROUND(SS_att!L2,2)</f>
-        <v>0.56999999999999995</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5" ht="16.5" customHeight="1" x14ac:dyDescent="0.35">
+        <v>7.0000000000000007E-2</v>
+      </c>
+    </row>
+    <row xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" r="7" ht="16.5" customHeight="true" x14ac:dyDescent="0.35">
       <c r="B7" s="3" t="str">
         <f>CONCATENATE("(",ROUND(SS_att!B3,1),")")</f>
-        <v>(3.3)</v>
+        <v>(2.7)</v>
       </c>
       <c r="C7" s="3" t="str">
         <f>CONCATENATE("(",ROUND(SS_att!C3,1),")")</f>
-        <v>(2.9)</v>
+        <v>(3.1)</v>
       </c>
       <c r="D7" s="3" t="str">
         <f>CONCATENATE("(",ROUND(SS_att!D3,1),")")</f>
-        <v>(3.2)</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5" ht="16.5" customHeight="1" x14ac:dyDescent="0.35">
+        <v>(3.4)</v>
+      </c>
+    </row>
+    <row xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" r="8" ht="16.5" customHeight="true" x14ac:dyDescent="0.35">
       <c r="A8" s="6" t="s">
         <v>22</v>
       </c>
@@ -2752,7 +2752,7 @@
         <v>0.62</v>
       </c>
     </row>
-    <row r="9" spans="1:5" ht="16.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" r="9" ht="16.5" customHeight="true" x14ac:dyDescent="0.35">
       <c r="A9" s="6"/>
       <c r="B9" s="3" t="str">
         <f>CONCATENATE("(",ROUND(SS_att!B9,2),")")</f>
@@ -2767,7 +2767,7 @@
         <v>(0.01)</v>
       </c>
     </row>
-    <row r="10" spans="1:5" ht="16.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" r="10" ht="16.5" customHeight="true" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
         <v>12</v>
       </c>
@@ -2788,7 +2788,7 @@
         <v>0.62</v>
       </c>
     </row>
-    <row r="11" spans="1:5" ht="16.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" r="11" ht="16.5" customHeight="true" x14ac:dyDescent="0.35">
       <c r="B11" s="3" t="str">
         <f>CONCATENATE("(",ROUND(SS_att!B11,2),")")</f>
         <v>(0.02)</v>
@@ -2802,7 +2802,7 @@
         <v>(0.02)</v>
       </c>
     </row>
-    <row r="12" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" r="12" ht="15" thickBot="true" x14ac:dyDescent="0.4">
       <c r="A12" s="2" t="s">
         <v>5</v>
       </c>
@@ -2820,7 +2820,7 @@
       </c>
       <c r="E12" s="5"/>
     </row>
-    <row r="13" spans="1:5" ht="15" thickTop="1" x14ac:dyDescent="0.35"/>
+    <row xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" r="13" ht="15" thickTop="true" x14ac:dyDescent="0.35"/>
   </sheetData>
   <mergeCells count="2">
     <mergeCell ref="B3:E3"/>

</xml_diff>